<commit_message>
Finished the equipment section.
- Fixed a few issues.
- Adventures can now give XP bonuses.
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
   <si>
     <t>name</t>
   </si>
@@ -192,6 +192,36 @@
   </si>
   <si>
     <t>Squires always have hopes of one day becoming a gallant knight. They train, and train and train and .... Does it ever get them what they truly want?</t>
+  </si>
+  <si>
+    <t>Dark Hopes</t>
+  </si>
+  <si>
+    <t>The darkest of dreams and hopes imbue this item for all shadows will hide deep in the hearts of men and women.</t>
+  </si>
+  <si>
+    <t>Festering Doubt</t>
+  </si>
+  <si>
+    <t>Let it fester, let the doubt take over and let it make you run from battle.</t>
+  </si>
+  <si>
+    <t>Treasures Winds</t>
+  </si>
+  <si>
+    <t>Follow the winds to the treasure.</t>
+  </si>
+  <si>
+    <t>Swfit Beat</t>
+  </si>
+  <si>
+    <t>The music is upbeat and the drums pound with the sounds of war. Move quickly my child.</t>
+  </si>
+  <si>
+    <t>Take Aim</t>
+  </si>
+  <si>
+    <t>Take aim at the enemy. Truly, they are vile. Never miss your mark, srtike em dead the first time. Right through the eyes.</t>
   </si>
 </sst>
 </file>
@@ -530,7 +560,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1091,6 +1121,187 @@
         <v>20</v>
       </c>
     </row>
+    <row r="17" spans="1:18">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17">
+        <v>0.15</v>
+      </c>
+      <c r="D17">
+        <v>0.15</v>
+      </c>
+      <c r="E17">
+        <v>0.15</v>
+      </c>
+      <c r="F17">
+        <v>0.13</v>
+      </c>
+      <c r="G17">
+        <v>0.13</v>
+      </c>
+      <c r="H17">
+        <v>0.13</v>
+      </c>
+      <c r="I17">
+        <v>0.13</v>
+      </c>
+      <c r="J17">
+        <v>0.13</v>
+      </c>
+      <c r="K17">
+        <v>23</v>
+      </c>
+      <c r="L17">
+        <v>12</v>
+      </c>
+      <c r="M17">
+        <v>40</v>
+      </c>
+      <c r="Q17">
+        <v>5000</v>
+      </c>
+      <c r="R17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18">
+        <v>0.05</v>
+      </c>
+      <c r="D18">
+        <v>0.05</v>
+      </c>
+      <c r="E18">
+        <v>0.05</v>
+      </c>
+      <c r="G18">
+        <v>0.3</v>
+      </c>
+      <c r="H18">
+        <v>0.3</v>
+      </c>
+      <c r="K18">
+        <v>24</v>
+      </c>
+      <c r="L18">
+        <v>15</v>
+      </c>
+      <c r="M18">
+        <v>40</v>
+      </c>
+      <c r="Q18">
+        <v>5000</v>
+      </c>
+      <c r="R18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="K19">
+        <v>28</v>
+      </c>
+      <c r="L19">
+        <v>16</v>
+      </c>
+      <c r="M19">
+        <v>40</v>
+      </c>
+      <c r="N19" t="s">
+        <v>31</v>
+      </c>
+      <c r="O19">
+        <v>0.15</v>
+      </c>
+      <c r="P19">
+        <v>0.05</v>
+      </c>
+      <c r="Q19">
+        <v>5000</v>
+      </c>
+      <c r="R19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="K20">
+        <v>28</v>
+      </c>
+      <c r="L20">
+        <v>18</v>
+      </c>
+      <c r="M20">
+        <v>40</v>
+      </c>
+      <c r="N20" t="s">
+        <v>38</v>
+      </c>
+      <c r="O20">
+        <v>0.15</v>
+      </c>
+      <c r="P20">
+        <v>0.05</v>
+      </c>
+      <c r="Q20">
+        <v>5000</v>
+      </c>
+      <c r="R20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+      <c r="K21">
+        <v>29</v>
+      </c>
+      <c r="L21">
+        <v>20</v>
+      </c>
+      <c r="M21">
+        <v>40</v>
+      </c>
+      <c r="N21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O21">
+        <v>0.15</v>
+      </c>
+      <c r="P21">
+        <v>0.05</v>
+      </c>
+      <c r="Q21">
+        <v>5000</v>
+      </c>
+      <c r="R21" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>

<commit_message>
Updated items and affixes
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
   <si>
     <t>name</t>
   </si>
@@ -71,223 +71,211 @@
     <t>type</t>
   </si>
   <si>
-    <t>Goblin War Cry</t>
-  </si>
-  <si>
-    <t>The cry and the drums of goblins heard in the distance only get louder as they approach to swarm, overwhelm and kill their enemies.</t>
+    <t>Balanced Energies</t>
+  </si>
+  <si>
+    <t>Balance your energies and feel on top of the world.</t>
   </si>
   <si>
     <t>suffix</t>
   </si>
   <si>
-    <t>Mages Defiance</t>
-  </si>
-  <si>
-    <t>Defy the rules and cast the unspeakable, illegal and darkest of magics.</t>
+    <t>Fighters Strength</t>
+  </si>
+  <si>
+    <t>Sometimes all you need is a little extra strength</t>
   </si>
   <si>
     <t>Archers Bane</t>
   </si>
   <si>
-    <t>See the target, hit the target. Kill the target.</t>
+    <t>Try and find your mark child. Take aim!</t>
   </si>
   <si>
     <t>Blood Lust</t>
   </si>
   <si>
-    <t>Crave blood do ya? Seek it out in the victims. Feed upon their fear.</t>
-  </si>
-  <si>
-    <t>Prayer Of Faith</t>
-  </si>
-  <si>
-    <t>Pray as hard as you might, it all comes down to faith.</t>
-  </si>
-  <si>
-    <t>Golden Touch</t>
-  </si>
-  <si>
-    <t>Your lust for the treasure is over taking your thoughts, causing you to go crazy.</t>
+    <t>The lust for the enemies life is strong.</t>
+  </si>
+  <si>
+    <t>Mages Inspiration</t>
+  </si>
+  <si>
+    <t>Be a little better, Be a lot smarter</t>
+  </si>
+  <si>
+    <t>Clerics Blessing</t>
+  </si>
+  <si>
+    <t>Call on your holy power to smite down your own enemies.</t>
+  </si>
+  <si>
+    <t>Deaths Accuracy</t>
+  </si>
+  <si>
+    <t>Death has remarkable aim</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>prefix</t>
+  </si>
+  <si>
+    <t>Dancers Moves</t>
+  </si>
+  <si>
+    <t>Dodge the swipes. Doge the spells. Dodge it all as you dance around the enemy.</t>
+  </si>
+  <si>
+    <t>Dodge</t>
+  </si>
+  <si>
+    <t>Thieves Eye</t>
+  </si>
+  <si>
+    <t>Steel from the enemies, find the hidden treasure.</t>
   </si>
   <si>
     <t>Looting</t>
   </si>
   <si>
-    <t>prefix</t>
-  </si>
-  <si>
-    <t>Never Miss</t>
-  </si>
-  <si>
-    <t>Never miss your target. never. You hear me?</t>
-  </si>
-  <si>
-    <t>Accuracy</t>
-  </si>
-  <si>
-    <t>Quick Foot</t>
-  </si>
-  <si>
-    <t>Be quick about it! Get out the way!</t>
-  </si>
-  <si>
-    <t>Dodge</t>
-  </si>
-  <si>
-    <t>Weapon Crafters Sigil</t>
-  </si>
-  <si>
-    <t>Craft the weapons, all the weapons. Feel good about your accomplishments.</t>
+    <t>Weapon Crafter Spell</t>
+  </si>
+  <si>
+    <t>Enchantment to help you craft weapons better.</t>
   </si>
   <si>
     <t>Weapon Crafting</t>
   </si>
   <si>
-    <t>Smiths Blood</t>
-  </si>
-  <si>
-    <t>How many smithies do you think it will take before I have enough blood to enchant their skill into your soul?</t>
+    <t>Blacksmiths Heart</t>
+  </si>
+  <si>
+    <t>The heart of the blacksmith went into making this enchantment. Literally.</t>
   </si>
   <si>
     <t>Armour Crafting</t>
   </si>
   <si>
-    <t>Mages Weaving</t>
-  </si>
-  <si>
-    <t>Weave the spells together and create dangerous magics.</t>
+    <t>Spell Weavers Thoughts</t>
+  </si>
+  <si>
+    <t>Helps with creating new spells. Coming up with ideas and inspiration.</t>
   </si>
   <si>
     <t>Spell Crafting</t>
   </si>
   <si>
-    <t>Enchantresses Heart</t>
-  </si>
-  <si>
-    <t>She placed her heart into her work, literally.</t>
+    <t>Ring Makers Inspiration</t>
+  </si>
+  <si>
+    <t>Let the inspiration of the worlds greatest ring maker flow through you.</t>
+  </si>
+  <si>
+    <t>Ring Crafting</t>
+  </si>
+  <si>
+    <t>Artifact Hunter</t>
+  </si>
+  <si>
+    <t>Hunt down and search for new artifacts with the eye of a hawk for glistening metals.</t>
   </si>
   <si>
     <t>Enchanting</t>
   </si>
   <si>
-    <t>Ring Crafters Thoughts</t>
-  </si>
-  <si>
-    <t>The thoughts of a ring crafter flow through the item giving it an eerie glow of perfection and magic.</t>
-  </si>
-  <si>
-    <t>Ring Crafting</t>
-  </si>
-  <si>
-    <t>Artifact Hunter</t>
-  </si>
-  <si>
-    <t>The materials needed to create artifacts of great power are hard to find and few and far between. The magics needed are deadly and not to be trifled with.</t>
+    <t>Natures Balancing Bliss</t>
+  </si>
+  <si>
+    <t>Nature has a way of balancing it's self out, and those around it.</t>
+  </si>
+  <si>
+    <t>Soldiers Resilance</t>
+  </si>
+  <si>
+    <t>Let the strength of a soldier, seasoned with war, flow through you.</t>
+  </si>
+  <si>
+    <t>Hawk Eye</t>
+  </si>
+  <si>
+    <t>See the enemy from miles away, see them better then they see them selves.</t>
+  </si>
+  <si>
+    <t>Life Stealer</t>
+  </si>
+  <si>
+    <t>Steal the soul and life right out of your enemy.</t>
+  </si>
+  <si>
+    <t>Sorcerers Magic</t>
+  </si>
+  <si>
+    <t>Sorcerers are strange beings, wickedly intelligent and born of dragon magic, they're intelligence will inspire you.</t>
+  </si>
+  <si>
+    <t>Archbishops Prayer</t>
+  </si>
+  <si>
+    <t>The Archbishop once prayed for the end to a nasty plague. His prayer was answered when they stopped dying. But they're was a side effect, they all rose.</t>
+  </si>
+  <si>
+    <t>Devils Arrow</t>
+  </si>
+  <si>
+    <t>Let the devils arrow guide your aim.</t>
+  </si>
+  <si>
+    <t>Sinister Dance</t>
+  </si>
+  <si>
+    <t>Do a sinister dance around the already confused enemy.</t>
+  </si>
+  <si>
+    <t>Eye For Gold</t>
+  </si>
+  <si>
+    <t>You now have the eye for gold. All that glistens will be yours.</t>
+  </si>
+  <si>
+    <t>Weapons Glory</t>
+  </si>
+  <si>
+    <t>Create weapons even better then you were before.</t>
+  </si>
+  <si>
+    <t>Armour Smiths Hopes</t>
+  </si>
+  <si>
+    <t>The hopes of the Armour Smith flow through you into what you create.</t>
+  </si>
+  <si>
+    <t>Spell Crafters Blood</t>
+  </si>
+  <si>
+    <t>A spell crafter poured his blood into this enchantment, to help making crafting spells easier.</t>
+  </si>
+  <si>
+    <t>Astral Ring</t>
+  </si>
+  <si>
+    <t>Helps in crafting rings with the energies of the Astral plane.</t>
+  </si>
+  <si>
+    <t>Desert Winds</t>
+  </si>
+  <si>
+    <t>Helps in the crafting of affixes</t>
   </si>
   <si>
     <t>Artifact Crafting</t>
   </si>
   <si>
-    <t>Squires Hopes</t>
-  </si>
-  <si>
-    <t>Squires always have hopes of one day becoming a gallant knight. They train, and train and train and .... Does it ever get them what they truly want?</t>
-  </si>
-  <si>
-    <t>Dark Hopes</t>
-  </si>
-  <si>
-    <t>The darkest of dreams and hopes imbue this item for all shadows will hide deep in the hearts of men and women.</t>
-  </si>
-  <si>
-    <t>Festering Doubt</t>
-  </si>
-  <si>
-    <t>Let it fester, let the doubt take over and let it make you run from battle.</t>
-  </si>
-  <si>
-    <t>Treasures Winds</t>
-  </si>
-  <si>
-    <t>Follow the winds to the treasure.</t>
-  </si>
-  <si>
-    <t>Swfit Beat</t>
-  </si>
-  <si>
-    <t>The music is upbeat and the drums pound with the sounds of war. Move quickly my child.</t>
-  </si>
-  <si>
-    <t>Take Aim</t>
-  </si>
-  <si>
-    <t>Take aim at the enemy. Truly, they are vile. Never miss your mark, srtike em dead the first time. Right through the eyes.</t>
-  </si>
-  <si>
-    <t>Tears of Blood</t>
-  </si>
-  <si>
-    <t>Let the tears of blood rain down the necks of the innocent.</t>
-  </si>
-  <si>
-    <t>The Strength Of God</t>
-  </si>
-  <si>
-    <t>The Strength Of God imbues thee with great strength.</t>
-  </si>
-  <si>
-    <t>Mages Thoughts</t>
-  </si>
-  <si>
-    <t>The thoughts of the greatest mages of all time imbue this item.</t>
-  </si>
-  <si>
-    <t>Bulls Eye</t>
-  </si>
-  <si>
-    <t>Never miss the target. Not today!</t>
-  </si>
-  <si>
-    <t>Deaths Dance</t>
-  </si>
-  <si>
-    <t>The dance of death is an honor to preform. Let it's magic imbue this item of holy worth with that of sin and hatefulness.</t>
-  </si>
-  <si>
-    <t>Stomping Ground</t>
-  </si>
-  <si>
-    <t>The stomp upon the ground, the earth will tremble and shake. The stomp upon the ground is terrifying and haunting.</t>
-  </si>
-  <si>
-    <t>Alchemist Web</t>
-  </si>
-  <si>
-    <t>Made from the finest gold spun into a web, laced upon the item it adheres in place. Glowing faintly with the magic with in.</t>
-  </si>
-  <si>
-    <t>Umbering Cry</t>
-  </si>
-  <si>
-    <t>Deep in the bowls of the earth lies a creature unheard of before known as an Umbering Spirit Lord. He uses cry, his deathly cry, to haunt those that dare to venture to close to his home.</t>
-  </si>
-  <si>
-    <t>Lords Grace</t>
-  </si>
-  <si>
-    <t>Let the grace of the lord wash over your wounds child.</t>
-  </si>
-  <si>
-    <t>Banshee Wail</t>
-  </si>
-  <si>
-    <t>The witch who was burned turned into a banshee and now her scrams haunt the local villages.</t>
-  </si>
-  <si>
-    <t>Curse Of The Damned</t>
-  </si>
-  <si>
-    <t>Cast your look upon your enemies and watch them tremble on down.</t>
+    <t>Enchantress Luck</t>
+  </si>
+  <si>
+    <t>With the luck of the enchantress on your side, you'll be able to enchant items better.</t>
   </si>
 </sst>
 </file>
@@ -626,7 +614,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -634,8 +622,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="26.993408" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="220.517578" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="28.135986" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="180.384521" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="18.709717" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="19.995117" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="13.996582" bestFit="true" customWidth="true" style="0"/>
@@ -650,7 +638,7 @@
     <col min="14" max="14" width="21.137695" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="13.996582" bestFit="true" customWidth="true" style="0"/>
     <col min="16" max="16" width="24.708252" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="6.998291" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="18" max="18" width="8.140869" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
@@ -718,10 +706,28 @@
         <v>19</v>
       </c>
       <c r="C2">
-        <v>0.05</v>
+        <v>0.1</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2">
+        <v>0.1</v>
       </c>
       <c r="F2">
-        <v>0.05</v>
+        <v>0.1</v>
+      </c>
+      <c r="G2">
+        <v>0.1</v>
+      </c>
+      <c r="H2">
+        <v>0.1</v>
+      </c>
+      <c r="I2">
+        <v>0.1</v>
+      </c>
+      <c r="J2">
+        <v>0.1</v>
       </c>
       <c r="K2">
         <v>10</v>
@@ -746,11 +752,14 @@
       <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="C3">
-        <v>0.05</v>
-      </c>
-      <c r="J3">
-        <v>0.05</v>
+      <c r="F3">
+        <v>0.15</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
       </c>
       <c r="K3">
         <v>10</v>
@@ -775,11 +784,8 @@
       <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="C4">
-        <v>0.05</v>
-      </c>
       <c r="H4">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="K4">
         <v>10</v>
@@ -804,14 +810,8 @@
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5">
-        <v>0.05</v>
-      </c>
-      <c r="D5">
-        <v>0.05</v>
-      </c>
       <c r="G5">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="K5">
         <v>10</v>
@@ -836,14 +836,8 @@
       <c r="B6" t="s">
         <v>28</v>
       </c>
-      <c r="C6">
-        <v>0.05</v>
-      </c>
-      <c r="D6">
-        <v>0.05</v>
-      </c>
-      <c r="I6">
-        <v>0.05</v>
+      <c r="J6">
+        <v>0.15</v>
       </c>
       <c r="K6">
         <v>10</v>
@@ -868,320 +862,347 @@
       <c r="B7" t="s">
         <v>30</v>
       </c>
+      <c r="I7">
+        <v>0.15</v>
+      </c>
       <c r="K7">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="L7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M7">
-        <v>10</v>
-      </c>
-      <c r="N7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O7">
-        <v>0.1</v>
-      </c>
-      <c r="P7">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="Q7">
-        <v>750</v>
+        <v>500</v>
       </c>
       <c r="R7" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="H8">
+        <v>0.25</v>
       </c>
       <c r="K8">
         <v>15</v>
       </c>
       <c r="L8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M8">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="N8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O8">
         <v>0.1</v>
       </c>
       <c r="P8">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q8">
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="R8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" t="s">
-        <v>37</v>
+      <c r="H9">
+        <v>0.25</v>
       </c>
       <c r="K9">
         <v>15</v>
       </c>
       <c r="L9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M9">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="N9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O9">
         <v>0.1</v>
       </c>
       <c r="P9">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q9">
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="R9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>15</v>
+      </c>
+      <c r="L10">
+        <v>3</v>
+      </c>
+      <c r="M10">
+        <v>8</v>
+      </c>
+      <c r="N10" t="s">
         <v>40</v>
-      </c>
-      <c r="K10">
-        <v>16</v>
-      </c>
-      <c r="L10">
-        <v>6</v>
-      </c>
-      <c r="M10">
-        <v>20</v>
-      </c>
-      <c r="N10" t="s">
-        <v>41</v>
       </c>
       <c r="O10">
         <v>0.1</v>
       </c>
       <c r="P10">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q10">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="R10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
         <v>42</v>
       </c>
-      <c r="B11" t="s">
+      <c r="J11">
+        <v>0.15</v>
+      </c>
+      <c r="K11">
+        <v>20</v>
+      </c>
+      <c r="L11">
+        <v>6</v>
+      </c>
+      <c r="M11">
+        <v>12</v>
+      </c>
+      <c r="N11" t="s">
         <v>43</v>
       </c>
-      <c r="K11">
-        <v>16</v>
-      </c>
-      <c r="L11">
-        <v>7</v>
-      </c>
-      <c r="M11">
-        <v>25</v>
-      </c>
-      <c r="N11" t="s">
-        <v>44</v>
-      </c>
       <c r="O11">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="P11">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="Q11">
-        <v>800</v>
+        <v>5000</v>
       </c>
       <c r="R11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
         <v>45</v>
       </c>
-      <c r="B12" t="s">
+      <c r="J12">
+        <v>0.15</v>
+      </c>
+      <c r="K12">
+        <v>20</v>
+      </c>
+      <c r="L12">
+        <v>6</v>
+      </c>
+      <c r="M12">
+        <v>12</v>
+      </c>
+      <c r="N12" t="s">
         <v>46</v>
       </c>
-      <c r="K12">
-        <v>20</v>
-      </c>
-      <c r="L12">
-        <v>10</v>
-      </c>
-      <c r="M12">
-        <v>30</v>
-      </c>
-      <c r="N12" t="s">
-        <v>47</v>
-      </c>
       <c r="O12">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="P12">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="Q12">
-        <v>900</v>
+        <v>5000</v>
       </c>
       <c r="R12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
         <v>48</v>
       </c>
-      <c r="B13" t="s">
+      <c r="J13">
+        <v>0.15</v>
+      </c>
+      <c r="K13">
+        <v>20</v>
+      </c>
+      <c r="L13">
+        <v>6</v>
+      </c>
+      <c r="M13">
+        <v>12</v>
+      </c>
+      <c r="N13" t="s">
         <v>49</v>
       </c>
-      <c r="K13">
-        <v>22</v>
-      </c>
-      <c r="L13">
-        <v>10</v>
-      </c>
-      <c r="M13">
-        <v>35</v>
-      </c>
-      <c r="N13" t="s">
-        <v>50</v>
-      </c>
       <c r="O13">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="P13">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="Q13">
-        <v>800</v>
+        <v>5000</v>
       </c>
       <c r="R13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
         <v>51</v>
       </c>
-      <c r="B14" t="s">
+      <c r="J14">
+        <v>0.15</v>
+      </c>
+      <c r="K14">
+        <v>20</v>
+      </c>
+      <c r="L14">
+        <v>6</v>
+      </c>
+      <c r="M14">
+        <v>12</v>
+      </c>
+      <c r="N14" t="s">
         <v>52</v>
       </c>
-      <c r="K14">
-        <v>22</v>
-      </c>
-      <c r="L14">
-        <v>10</v>
-      </c>
-      <c r="M14">
-        <v>40</v>
-      </c>
-      <c r="N14" t="s">
-        <v>53</v>
-      </c>
       <c r="O14">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="P14">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="Q14">
-        <v>850</v>
+        <v>5000</v>
       </c>
       <c r="R14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
         <v>54</v>
       </c>
-      <c r="B15" t="s">
+      <c r="J15">
+        <v>0.15</v>
+      </c>
+      <c r="K15">
+        <v>20</v>
+      </c>
+      <c r="L15">
+        <v>6</v>
+      </c>
+      <c r="M15">
+        <v>12</v>
+      </c>
+      <c r="N15" t="s">
         <v>55</v>
       </c>
-      <c r="K15">
-        <v>22</v>
-      </c>
-      <c r="L15">
-        <v>10</v>
-      </c>
-      <c r="M15">
-        <v>40</v>
-      </c>
-      <c r="N15" t="s">
-        <v>56</v>
-      </c>
       <c r="O15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="P15">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="Q15">
-        <v>850</v>
+        <v>5000</v>
       </c>
       <c r="R15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
         <v>57</v>
       </c>
-      <c r="B16" t="s">
-        <v>58</v>
+      <c r="C16">
+        <v>0.22</v>
+      </c>
+      <c r="D16">
+        <v>0.22</v>
+      </c>
+      <c r="E16">
+        <v>0.22</v>
       </c>
       <c r="F16">
-        <v>0.1</v>
+        <v>0.22</v>
       </c>
       <c r="G16">
-        <v>0.1</v>
+        <v>0.22</v>
       </c>
       <c r="H16">
-        <v>0.1</v>
+        <v>0.22</v>
       </c>
       <c r="I16">
-        <v>0.1</v>
+        <v>0.22</v>
       </c>
       <c r="J16">
-        <v>0.1</v>
+        <v>0.22</v>
       </c>
       <c r="K16">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="L16">
         <v>10</v>
       </c>
       <c r="M16">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="Q16">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="R16" t="s">
         <v>20</v>
@@ -1189,46 +1210,37 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
         <v>59</v>
       </c>
-      <c r="B17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17">
-        <v>0.15</v>
-      </c>
-      <c r="D17">
-        <v>0.15</v>
-      </c>
-      <c r="E17">
-        <v>0.15</v>
-      </c>
       <c r="F17">
-        <v>0.13</v>
+        <v>0.3</v>
       </c>
       <c r="G17">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="L17">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M17">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="Q17">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="R17" t="s">
         <v>20</v>
@@ -1236,101 +1248,77 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
         <v>61</v>
-      </c>
-      <c r="B18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18">
-        <v>0.05</v>
-      </c>
-      <c r="D18">
-        <v>0.05</v>
-      </c>
-      <c r="E18">
-        <v>0.05</v>
-      </c>
-      <c r="G18">
-        <v>0.3</v>
       </c>
       <c r="H18">
         <v>0.3</v>
       </c>
       <c r="K18">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="L18">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="M18">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="Q18">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="R18" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
         <v>63</v>
       </c>
-      <c r="B19" t="s">
-        <v>64</v>
+      <c r="G19">
+        <v>0.3</v>
       </c>
       <c r="K19">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L19">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="M19">
-        <v>40</v>
-      </c>
-      <c r="N19" t="s">
-        <v>31</v>
-      </c>
-      <c r="O19">
-        <v>0.15</v>
-      </c>
-      <c r="P19">
-        <v>0.05</v>
+        <v>20</v>
       </c>
       <c r="Q19">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="R19" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
         <v>65</v>
       </c>
-      <c r="B20" t="s">
-        <v>66</v>
+      <c r="J20">
+        <v>0.3</v>
       </c>
       <c r="K20">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L20">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="M20">
-        <v>40</v>
-      </c>
-      <c r="N20" t="s">
-        <v>38</v>
-      </c>
-      <c r="O20">
-        <v>0.15</v>
-      </c>
-      <c r="P20">
-        <v>0.05</v>
+        <v>20</v>
       </c>
       <c r="Q20">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="R20" t="s">
         <v>20</v>
@@ -1338,225 +1326,243 @@
     </row>
     <row r="21" spans="1:18">
       <c r="A21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" t="s">
         <v>67</v>
       </c>
-      <c r="B21" t="s">
-        <v>68</v>
+      <c r="I21">
+        <v>0.3</v>
       </c>
       <c r="K21">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L21">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="M21">
-        <v>40</v>
-      </c>
-      <c r="N21" t="s">
-        <v>35</v>
-      </c>
-      <c r="O21">
-        <v>0.15</v>
-      </c>
-      <c r="P21">
-        <v>0.05</v>
+        <v>20</v>
       </c>
       <c r="Q21">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="R21" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
         <v>69</v>
       </c>
-      <c r="B22" t="s">
-        <v>70</v>
-      </c>
-      <c r="G22">
+      <c r="H22">
         <v>0.35</v>
       </c>
       <c r="K22">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="L22">
+        <v>18</v>
+      </c>
+      <c r="M22">
+        <v>36</v>
+      </c>
+      <c r="N22" t="s">
         <v>33</v>
       </c>
-      <c r="M22">
-        <v>50</v>
+      <c r="O22">
+        <v>0.25</v>
+      </c>
+      <c r="P22">
+        <v>0.35</v>
       </c>
       <c r="Q22">
-        <v>10000</v>
+        <v>50000</v>
       </c>
       <c r="R22" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:18">
       <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" t="s">
         <v>71</v>
       </c>
-      <c r="B23" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23">
+      <c r="H23">
         <v>0.35</v>
       </c>
       <c r="K23">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="L23">
+        <v>18</v>
+      </c>
+      <c r="M23">
         <v>36</v>
       </c>
-      <c r="M23">
-        <v>50</v>
+      <c r="N23" t="s">
+        <v>37</v>
+      </c>
+      <c r="O23">
+        <v>0.25</v>
+      </c>
+      <c r="P23">
+        <v>0.35</v>
       </c>
       <c r="Q23">
-        <v>10000</v>
+        <v>50000</v>
       </c>
       <c r="R23" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:18">
       <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" t="s">
         <v>73</v>
       </c>
-      <c r="B24" t="s">
-        <v>74</v>
-      </c>
-      <c r="J24">
+      <c r="K24">
+        <v>50</v>
+      </c>
+      <c r="L24">
+        <v>18</v>
+      </c>
+      <c r="M24">
+        <v>36</v>
+      </c>
+      <c r="N24" t="s">
+        <v>40</v>
+      </c>
+      <c r="O24">
+        <v>0.25</v>
+      </c>
+      <c r="P24">
         <v>0.35</v>
       </c>
-      <c r="K24">
-        <v>42</v>
-      </c>
-      <c r="L24">
-        <v>38</v>
-      </c>
-      <c r="M24">
-        <v>50</v>
-      </c>
       <c r="Q24">
-        <v>10000</v>
+        <v>50000</v>
       </c>
       <c r="R24" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" t="s">
         <v>75</v>
       </c>
-      <c r="B25" t="s">
-        <v>76</v>
-      </c>
-      <c r="H25">
+      <c r="J25">
+        <v>0.3</v>
+      </c>
+      <c r="K25">
+        <v>70</v>
+      </c>
+      <c r="L25">
+        <v>24</v>
+      </c>
+      <c r="M25">
+        <v>40</v>
+      </c>
+      <c r="N25" t="s">
+        <v>43</v>
+      </c>
+      <c r="O25">
+        <v>0.25</v>
+      </c>
+      <c r="P25">
         <v>0.35</v>
       </c>
-      <c r="K25">
-        <v>45</v>
-      </c>
-      <c r="L25">
-        <v>43</v>
-      </c>
-      <c r="M25">
-        <v>50</v>
-      </c>
       <c r="Q25">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="R25" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:18">
       <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" t="s">
         <v>77</v>
       </c>
-      <c r="B26" t="s">
-        <v>78</v>
-      </c>
-      <c r="H26">
+      <c r="J26">
         <v>0.3</v>
       </c>
       <c r="K26">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="L26">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="M26">
-        <v>60</v>
+        <v>40</v>
+      </c>
+      <c r="N26" t="s">
+        <v>46</v>
+      </c>
+      <c r="O26">
+        <v>0.25</v>
+      </c>
+      <c r="P26">
+        <v>0.35</v>
       </c>
       <c r="Q26">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="R26" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:18">
       <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
         <v>79</v>
       </c>
-      <c r="B27" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27">
-        <v>0.55</v>
-      </c>
-      <c r="D27">
-        <v>0.2</v>
-      </c>
-      <c r="E27">
+      <c r="J27">
+        <v>0.3</v>
+      </c>
+      <c r="K27">
+        <v>70</v>
+      </c>
+      <c r="L27">
+        <v>24</v>
+      </c>
+      <c r="M27">
+        <v>40</v>
+      </c>
+      <c r="N27" t="s">
+        <v>49</v>
+      </c>
+      <c r="O27">
+        <v>0.25</v>
+      </c>
+      <c r="P27">
         <v>0.35</v>
       </c>
-      <c r="F27">
-        <v>0.2</v>
-      </c>
-      <c r="G27">
-        <v>0.16</v>
-      </c>
-      <c r="H27">
-        <v>0.11</v>
-      </c>
-      <c r="K27">
-        <v>55</v>
-      </c>
-      <c r="L27">
-        <v>53</v>
-      </c>
-      <c r="M27">
-        <v>75</v>
-      </c>
       <c r="Q27">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="R27" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:18">
       <c r="A28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" t="s">
         <v>81</v>
-      </c>
-      <c r="B28" t="s">
-        <v>82</v>
-      </c>
-      <c r="F28">
-        <v>0.3</v>
-      </c>
-      <c r="G28">
-        <v>0.3</v>
-      </c>
-      <c r="H28">
-        <v>0.3</v>
-      </c>
-      <c r="I28">
-        <v>0.3</v>
       </c>
       <c r="J28">
         <v>0.3</v>
@@ -1565,81 +1571,60 @@
         <v>70</v>
       </c>
       <c r="L28">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="M28">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="N28" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="O28">
-        <v>0.18</v>
+        <v>0.25</v>
       </c>
       <c r="P28">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="Q28">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="R28" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:18">
       <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
         <v>83</v>
       </c>
-      <c r="B29" t="s">
+      <c r="J29">
+        <v>0.3</v>
+      </c>
+      <c r="K29">
+        <v>70</v>
+      </c>
+      <c r="L29">
+        <v>24</v>
+      </c>
+      <c r="M29">
+        <v>40</v>
+      </c>
+      <c r="N29" t="s">
         <v>84</v>
       </c>
-      <c r="C29">
-        <v>0.4</v>
-      </c>
-      <c r="D29">
+      <c r="O29">
         <v>0.25</v>
       </c>
-      <c r="E29">
-        <v>0.28</v>
-      </c>
-      <c r="F29">
-        <v>0.48</v>
-      </c>
-      <c r="G29">
-        <v>0.18</v>
-      </c>
-      <c r="H29">
-        <v>0.28</v>
-      </c>
-      <c r="I29">
-        <v>0.09</v>
-      </c>
-      <c r="J29">
-        <v>0.08</v>
-      </c>
-      <c r="K29">
-        <v>100</v>
-      </c>
-      <c r="L29">
-        <v>75</v>
-      </c>
-      <c r="M29">
-        <v>120</v>
-      </c>
-      <c r="N29" t="s">
-        <v>50</v>
-      </c>
-      <c r="O29">
-        <v>0.26</v>
-      </c>
       <c r="P29">
-        <v>0.18</v>
+        <v>0.35</v>
       </c>
       <c r="Q29">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="R29" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -1649,96 +1634,32 @@
       <c r="B30" t="s">
         <v>86</v>
       </c>
-      <c r="D30">
+      <c r="J30">
+        <v>0.3</v>
+      </c>
+      <c r="K30">
+        <v>70</v>
+      </c>
+      <c r="L30">
+        <v>24</v>
+      </c>
+      <c r="M30">
+        <v>40</v>
+      </c>
+      <c r="N30" t="s">
+        <v>55</v>
+      </c>
+      <c r="O30">
+        <v>0.25</v>
+      </c>
+      <c r="P30">
         <v>0.35</v>
       </c>
-      <c r="E30">
-        <v>0.4</v>
-      </c>
-      <c r="I30">
-        <v>0.5</v>
-      </c>
-      <c r="K30">
-        <v>125</v>
-      </c>
-      <c r="L30">
-        <v>75</v>
-      </c>
-      <c r="M30">
-        <v>130</v>
-      </c>
       <c r="Q30">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="R30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18">
-      <c r="A31" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31">
-        <v>0.4</v>
-      </c>
-      <c r="J31">
-        <v>0.5</v>
-      </c>
-      <c r="K31">
-        <v>150</v>
-      </c>
-      <c r="L31">
-        <v>80</v>
-      </c>
-      <c r="M31">
-        <v>130</v>
-      </c>
-      <c r="N31" t="s">
-        <v>47</v>
-      </c>
-      <c r="O31">
-        <v>0.16</v>
-      </c>
-      <c r="P31">
-        <v>0.18</v>
-      </c>
-      <c r="Q31">
-        <v>50000</v>
-      </c>
-      <c r="R31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18">
-      <c r="A32" t="s">
-        <v>89</v>
-      </c>
-      <c r="B32" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32">
-        <v>0.4</v>
-      </c>
-      <c r="G32">
-        <v>0.5</v>
-      </c>
-      <c r="K32">
-        <v>175</v>
-      </c>
-      <c r="L32">
-        <v>84</v>
-      </c>
-      <c r="M32">
-        <v>140</v>
-      </c>
-      <c r="Q32">
-        <v>50000</v>
-      </c>
-      <c r="R32" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor fix, more items, monsters and affixes
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="147">
   <si>
     <t>name</t>
   </si>
@@ -366,6 +366,96 @@
   </si>
   <si>
     <t>She cast a spell over this item. She cast a spell that give you the ability to better enchant items.</t>
+  </si>
+  <si>
+    <t>Wishing Spell</t>
+  </si>
+  <si>
+    <t>Make a wish and it might come true. This spell is powerful on the right item.</t>
+  </si>
+  <si>
+    <t>Gladiators Win</t>
+  </si>
+  <si>
+    <t>Feel the strength given to you by the crowd as they cheer you on!</t>
+  </si>
+  <si>
+    <t>Faith In The Aim</t>
+  </si>
+  <si>
+    <t>Have some faith child.</t>
+  </si>
+  <si>
+    <t>Blood Fever</t>
+  </si>
+  <si>
+    <t>Smell blood do ya? let it drive you insane!</t>
+  </si>
+  <si>
+    <t>Arch Mages Wrath</t>
+  </si>
+  <si>
+    <t>Feel the rage and terror of the arch mages magics.</t>
+  </si>
+  <si>
+    <t>Lord Of Lights Faith</t>
+  </si>
+  <si>
+    <t>Have faith in the Lord of Light and you shall prevail</t>
+  </si>
+  <si>
+    <t>Deaths Laugh</t>
+  </si>
+  <si>
+    <t>Death is laughing as you constantly miss your enemy.</t>
+  </si>
+  <si>
+    <t>Fleeting Hopes</t>
+  </si>
+  <si>
+    <t>Run away child. Take your hopes with you and run away!</t>
+  </si>
+  <si>
+    <t>Eye For Treasure</t>
+  </si>
+  <si>
+    <t>See the treasure child! Se it in your minds eye.</t>
+  </si>
+  <si>
+    <t>Holy Weapons</t>
+  </si>
+  <si>
+    <t>Let all your weapons that you craft be made of the holiest of metals.</t>
+  </si>
+  <si>
+    <t>Demonic Armour</t>
+  </si>
+  <si>
+    <t>When you create armour it will be with the fires of hell them selves.</t>
+  </si>
+  <si>
+    <t>Dragons Tongue</t>
+  </si>
+  <si>
+    <t>Engraved on the items is the language of the dragons.</t>
+  </si>
+  <si>
+    <t>Celestial Rings</t>
+  </si>
+  <si>
+    <t>Celestial rings surround this item making it easier to craft rings.</t>
+  </si>
+  <si>
+    <t>Astral Relics</t>
+  </si>
+  <si>
+    <t>Enchanted on the item are astral runes that lead you to better artifacts.</t>
+  </si>
+  <si>
+    <t>Demonic Enchantments</t>
+  </si>
+  <si>
+    <t>Use the powers of hell to enchant better items.</t>
   </si>
 </sst>
 </file>
@@ -704,7 +794,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:R45"/>
+  <dimension ref="A1:R60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -728,7 +818,7 @@
     <col min="14" max="14" width="21" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="13" bestFit="true" customWidth="true" style="0"/>
     <col min="16" max="16" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="10" bestFit="true" customWidth="true" style="0"/>
     <col min="18" max="18" width="8" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
@@ -2220,6 +2310,486 @@
         <v>2500000</v>
       </c>
       <c r="R45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
+      <c r="A46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46">
+        <v>0.28</v>
+      </c>
+      <c r="D46">
+        <v>0.28</v>
+      </c>
+      <c r="E46">
+        <v>0.28</v>
+      </c>
+      <c r="F46">
+        <v>0.28</v>
+      </c>
+      <c r="G46">
+        <v>0.28</v>
+      </c>
+      <c r="H46">
+        <v>0.28</v>
+      </c>
+      <c r="I46">
+        <v>0.28</v>
+      </c>
+      <c r="J46">
+        <v>0.28</v>
+      </c>
+      <c r="K46">
+        <v>170</v>
+      </c>
+      <c r="L46">
+        <v>55</v>
+      </c>
+      <c r="M46">
+        <v>150</v>
+      </c>
+      <c r="Q46">
+        <v>5000000</v>
+      </c>
+      <c r="R46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="A47" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47" t="s">
+        <v>120</v>
+      </c>
+      <c r="F47">
+        <v>0.38</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>200</v>
+      </c>
+      <c r="L47">
+        <v>60</v>
+      </c>
+      <c r="M47">
+        <v>160</v>
+      </c>
+      <c r="Q47">
+        <v>10500000</v>
+      </c>
+      <c r="R47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="A48" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" t="s">
+        <v>122</v>
+      </c>
+      <c r="H48">
+        <v>0.38</v>
+      </c>
+      <c r="K48">
+        <v>200</v>
+      </c>
+      <c r="L48">
+        <v>60</v>
+      </c>
+      <c r="M48">
+        <v>160</v>
+      </c>
+      <c r="Q48">
+        <v>10500000</v>
+      </c>
+      <c r="R48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18">
+      <c r="A49" t="s">
+        <v>123</v>
+      </c>
+      <c r="B49" t="s">
+        <v>124</v>
+      </c>
+      <c r="G49">
+        <v>0.38</v>
+      </c>
+      <c r="K49">
+        <v>200</v>
+      </c>
+      <c r="L49">
+        <v>60</v>
+      </c>
+      <c r="M49">
+        <v>160</v>
+      </c>
+      <c r="Q49">
+        <v>10500000</v>
+      </c>
+      <c r="R49" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18">
+      <c r="A50" t="s">
+        <v>125</v>
+      </c>
+      <c r="B50" t="s">
+        <v>126</v>
+      </c>
+      <c r="J50">
+        <v>0.38</v>
+      </c>
+      <c r="K50">
+        <v>200</v>
+      </c>
+      <c r="L50">
+        <v>60</v>
+      </c>
+      <c r="M50">
+        <v>160</v>
+      </c>
+      <c r="Q50">
+        <v>10500000</v>
+      </c>
+      <c r="R50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18">
+      <c r="A51" t="s">
+        <v>127</v>
+      </c>
+      <c r="B51" t="s">
+        <v>128</v>
+      </c>
+      <c r="I51">
+        <v>0.38</v>
+      </c>
+      <c r="K51">
+        <v>200</v>
+      </c>
+      <c r="L51">
+        <v>60</v>
+      </c>
+      <c r="M51">
+        <v>160</v>
+      </c>
+      <c r="Q51">
+        <v>10500000</v>
+      </c>
+      <c r="R51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18">
+      <c r="A52" t="s">
+        <v>129</v>
+      </c>
+      <c r="B52" t="s">
+        <v>130</v>
+      </c>
+      <c r="H52">
+        <v>0.42</v>
+      </c>
+      <c r="K52">
+        <v>240</v>
+      </c>
+      <c r="L52">
+        <v>65</v>
+      </c>
+      <c r="M52">
+        <v>170</v>
+      </c>
+      <c r="N52" t="s">
+        <v>33</v>
+      </c>
+      <c r="O52">
+        <v>0.3</v>
+      </c>
+      <c r="P52">
+        <v>0.4</v>
+      </c>
+      <c r="Q52">
+        <v>25000000</v>
+      </c>
+      <c r="R52" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18">
+      <c r="A53" t="s">
+        <v>131</v>
+      </c>
+      <c r="B53" t="s">
+        <v>132</v>
+      </c>
+      <c r="H53">
+        <v>0.42</v>
+      </c>
+      <c r="K53">
+        <v>240</v>
+      </c>
+      <c r="L53">
+        <v>65</v>
+      </c>
+      <c r="M53">
+        <v>170</v>
+      </c>
+      <c r="N53" t="s">
+        <v>37</v>
+      </c>
+      <c r="O53">
+        <v>0.3</v>
+      </c>
+      <c r="P53">
+        <v>0.4</v>
+      </c>
+      <c r="Q53">
+        <v>25000000</v>
+      </c>
+      <c r="R53" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18">
+      <c r="A54" t="s">
+        <v>133</v>
+      </c>
+      <c r="B54" t="s">
+        <v>134</v>
+      </c>
+      <c r="K54">
+        <v>240</v>
+      </c>
+      <c r="L54">
+        <v>65</v>
+      </c>
+      <c r="M54">
+        <v>170</v>
+      </c>
+      <c r="N54" t="s">
+        <v>40</v>
+      </c>
+      <c r="O54">
+        <v>0.3</v>
+      </c>
+      <c r="P54">
+        <v>0.4</v>
+      </c>
+      <c r="Q54">
+        <v>25000000</v>
+      </c>
+      <c r="R54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18">
+      <c r="A55" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" t="s">
+        <v>136</v>
+      </c>
+      <c r="K55">
+        <v>270</v>
+      </c>
+      <c r="L55">
+        <v>70</v>
+      </c>
+      <c r="M55">
+        <v>200</v>
+      </c>
+      <c r="N55" t="s">
+        <v>43</v>
+      </c>
+      <c r="O55">
+        <v>0.3</v>
+      </c>
+      <c r="P55">
+        <v>0.4</v>
+      </c>
+      <c r="Q55">
+        <v>55000000</v>
+      </c>
+      <c r="R55" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18">
+      <c r="A56" t="s">
+        <v>137</v>
+      </c>
+      <c r="B56" t="s">
+        <v>138</v>
+      </c>
+      <c r="K56">
+        <v>270</v>
+      </c>
+      <c r="L56">
+        <v>70</v>
+      </c>
+      <c r="M56">
+        <v>200</v>
+      </c>
+      <c r="N56" t="s">
+        <v>46</v>
+      </c>
+      <c r="O56">
+        <v>0.3</v>
+      </c>
+      <c r="P56">
+        <v>0.4</v>
+      </c>
+      <c r="Q56">
+        <v>55000000</v>
+      </c>
+      <c r="R56" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18">
+      <c r="A57" t="s">
+        <v>139</v>
+      </c>
+      <c r="B57" t="s">
+        <v>140</v>
+      </c>
+      <c r="K57">
+        <v>240</v>
+      </c>
+      <c r="L57">
+        <v>70</v>
+      </c>
+      <c r="M57">
+        <v>200</v>
+      </c>
+      <c r="N57" t="s">
+        <v>49</v>
+      </c>
+      <c r="O57">
+        <v>0.3</v>
+      </c>
+      <c r="P57">
+        <v>0.4</v>
+      </c>
+      <c r="Q57">
+        <v>55000000</v>
+      </c>
+      <c r="R57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18">
+      <c r="A58" t="s">
+        <v>141</v>
+      </c>
+      <c r="B58" t="s">
+        <v>142</v>
+      </c>
+      <c r="K58">
+        <v>270</v>
+      </c>
+      <c r="L58">
+        <v>70</v>
+      </c>
+      <c r="M58">
+        <v>200</v>
+      </c>
+      <c r="N58" t="s">
+        <v>52</v>
+      </c>
+      <c r="O58">
+        <v>0.3</v>
+      </c>
+      <c r="P58">
+        <v>0.4</v>
+      </c>
+      <c r="Q58">
+        <v>55000000</v>
+      </c>
+      <c r="R58" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18">
+      <c r="A59" t="s">
+        <v>143</v>
+      </c>
+      <c r="B59" t="s">
+        <v>144</v>
+      </c>
+      <c r="K59">
+        <v>270</v>
+      </c>
+      <c r="L59">
+        <v>70</v>
+      </c>
+      <c r="M59">
+        <v>200</v>
+      </c>
+      <c r="N59" t="s">
+        <v>84</v>
+      </c>
+      <c r="O59">
+        <v>0.3</v>
+      </c>
+      <c r="P59">
+        <v>0.4</v>
+      </c>
+      <c r="Q59">
+        <v>55000000</v>
+      </c>
+      <c r="R59" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18">
+      <c r="A60" t="s">
+        <v>145</v>
+      </c>
+      <c r="B60" t="s">
+        <v>146</v>
+      </c>
+      <c r="K60">
+        <v>270</v>
+      </c>
+      <c r="L60">
+        <v>70</v>
+      </c>
+      <c r="M60">
+        <v>200</v>
+      </c>
+      <c r="N60" t="s">
+        <v>55</v>
+      </c>
+      <c r="O60">
+        <v>0.3</v>
+      </c>
+      <c r="P60">
+        <v>0.4</v>
+      </c>
+      <c r="Q60">
+        <v>55000000</v>
+      </c>
+      <c r="R60" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed the integer on cost for affixes. Updated Items and affixes
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="207">
   <si>
     <t>name</t>
   </si>
@@ -546,6 +546,96 @@
   </si>
   <si>
     <t>The ice that flows through the veins of this item radiates an enchanted magic one cannot define.</t>
+  </si>
+  <si>
+    <t>Earth Tuned</t>
+  </si>
+  <si>
+    <t>Be tuned into the earth and its balancing energy</t>
+  </si>
+  <si>
+    <t>Strength of Courage</t>
+  </si>
+  <si>
+    <t>Give your self the belief in strength and courage to survive whats to come.</t>
+  </si>
+  <si>
+    <t>See All</t>
+  </si>
+  <si>
+    <t>Missing never was the option. Damage and accuracy was.</t>
+  </si>
+  <si>
+    <t>Reapers Kiss</t>
+  </si>
+  <si>
+    <t>Thirst for souls, thirst for death.</t>
+  </si>
+  <si>
+    <t>Scholars Research</t>
+  </si>
+  <si>
+    <t>All the research in the world that has been done so far on the study of magic, is yours.</t>
+  </si>
+  <si>
+    <t>Prayer Of Hope</t>
+  </si>
+  <si>
+    <t>If you pray, I shall give you hope. If you listen, I shall guide you.</t>
+  </si>
+  <si>
+    <t>Rangers Luck</t>
+  </si>
+  <si>
+    <t>With the luck of a well trained ranger you might be able to finally hit that bear.</t>
+  </si>
+  <si>
+    <t>Rumor's Movement</t>
+  </si>
+  <si>
+    <t>Move like a Rumor. Impossible o see, hit or know is coming.</t>
+  </si>
+  <si>
+    <t>Smell of Gold</t>
+  </si>
+  <si>
+    <t>The smell of gold can drag one deep into the lust for treasure.</t>
+  </si>
+  <si>
+    <t>Godly Weapon Crafting</t>
+  </si>
+  <si>
+    <t>You'll probably never fail to craft again.</t>
+  </si>
+  <si>
+    <t>Angelic Armour Smithing</t>
+  </si>
+  <si>
+    <t>Craft amour with the help of the angels.</t>
+  </si>
+  <si>
+    <t>Divine Magic Crafting</t>
+  </si>
+  <si>
+    <t>Use divine help to craft magical spells.</t>
+  </si>
+  <si>
+    <t>Devilish Ring Crafting</t>
+  </si>
+  <si>
+    <t>Let the thoughts and the inspiration from the devil inspire you.</t>
+  </si>
+  <si>
+    <t>Enchanted Labyrinth</t>
+  </si>
+  <si>
+    <t>Get lost in a labyrinth of all the enchantments you can create.</t>
+  </si>
+  <si>
+    <t>Dark Pact</t>
+  </si>
+  <si>
+    <t>Make a dark pact when creating artifacts.</t>
   </si>
 </sst>
 </file>
@@ -884,7 +974,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:R75"/>
+  <dimension ref="A1:R90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -908,7 +998,7 @@
     <col min="14" max="14" width="21" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="13" bestFit="true" customWidth="true" style="0"/>
     <col min="16" max="16" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="13" bestFit="true" customWidth="true" style="0"/>
     <col min="18" max="18" width="8" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
@@ -2890,6 +2980,15 @@
       <c r="B61" t="s">
         <v>148</v>
       </c>
+      <c r="C61">
+        <v>0.34</v>
+      </c>
+      <c r="D61">
+        <v>0.34</v>
+      </c>
+      <c r="E61">
+        <v>0.34</v>
+      </c>
       <c r="F61">
         <v>0.34</v>
       </c>
@@ -3342,6 +3441,489 @@
         <v>1340500000</v>
       </c>
       <c r="R75" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18">
+      <c r="A76" t="s">
+        <v>177</v>
+      </c>
+      <c r="B76" t="s">
+        <v>178</v>
+      </c>
+      <c r="C76">
+        <v>0.38</v>
+      </c>
+      <c r="D76">
+        <v>0.38</v>
+      </c>
+      <c r="E76">
+        <v>0.38</v>
+      </c>
+      <c r="F76">
+        <v>0.38</v>
+      </c>
+      <c r="G76">
+        <v>0.38</v>
+      </c>
+      <c r="H76">
+        <v>0.38</v>
+      </c>
+      <c r="I76">
+        <v>0.38</v>
+      </c>
+      <c r="J76">
+        <v>0.38</v>
+      </c>
+      <c r="K76">
+        <v>500</v>
+      </c>
+      <c r="L76">
+        <v>110</v>
+      </c>
+      <c r="M76">
+        <v>200</v>
+      </c>
+      <c r="Q76">
+        <v>2600980000</v>
+      </c>
+      <c r="R76" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18">
+      <c r="A77" t="s">
+        <v>179</v>
+      </c>
+      <c r="B77" t="s">
+        <v>180</v>
+      </c>
+      <c r="F77">
+        <v>0.48</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+      <c r="K77">
+        <v>530</v>
+      </c>
+      <c r="L77">
+        <v>120</v>
+      </c>
+      <c r="M77">
+        <v>200</v>
+      </c>
+      <c r="Q77">
+        <v>5670200000</v>
+      </c>
+      <c r="R77" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18">
+      <c r="A78" t="s">
+        <v>181</v>
+      </c>
+      <c r="B78" t="s">
+        <v>182</v>
+      </c>
+      <c r="H78">
+        <v>0.48</v>
+      </c>
+      <c r="K78">
+        <v>500</v>
+      </c>
+      <c r="L78">
+        <v>120</v>
+      </c>
+      <c r="M78">
+        <v>200</v>
+      </c>
+      <c r="Q78">
+        <v>5670200000</v>
+      </c>
+      <c r="R78" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18">
+      <c r="A79" t="s">
+        <v>183</v>
+      </c>
+      <c r="B79" t="s">
+        <v>184</v>
+      </c>
+      <c r="G79">
+        <v>0.48</v>
+      </c>
+      <c r="K79">
+        <v>500</v>
+      </c>
+      <c r="L79">
+        <v>120</v>
+      </c>
+      <c r="M79">
+        <v>200</v>
+      </c>
+      <c r="Q79">
+        <v>5670200000</v>
+      </c>
+      <c r="R79" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18">
+      <c r="A80" t="s">
+        <v>185</v>
+      </c>
+      <c r="B80" t="s">
+        <v>186</v>
+      </c>
+      <c r="J80">
+        <v>0.48</v>
+      </c>
+      <c r="K80">
+        <v>500</v>
+      </c>
+      <c r="L80">
+        <v>120</v>
+      </c>
+      <c r="M80">
+        <v>200</v>
+      </c>
+      <c r="Q80">
+        <v>5670200000</v>
+      </c>
+      <c r="R80" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18">
+      <c r="A81" t="s">
+        <v>187</v>
+      </c>
+      <c r="B81" t="s">
+        <v>188</v>
+      </c>
+      <c r="I81">
+        <v>0.48</v>
+      </c>
+      <c r="K81">
+        <v>500</v>
+      </c>
+      <c r="L81">
+        <v>120</v>
+      </c>
+      <c r="M81">
+        <v>200</v>
+      </c>
+      <c r="Q81">
+        <v>5670200000</v>
+      </c>
+      <c r="R81" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18">
+      <c r="A82" t="s">
+        <v>189</v>
+      </c>
+      <c r="B82" t="s">
+        <v>190</v>
+      </c>
+      <c r="H82">
+        <v>0.28</v>
+      </c>
+      <c r="K82">
+        <v>600</v>
+      </c>
+      <c r="L82">
+        <v>130</v>
+      </c>
+      <c r="M82">
+        <v>200</v>
+      </c>
+      <c r="N82" t="s">
+        <v>33</v>
+      </c>
+      <c r="O82">
+        <v>0.15</v>
+      </c>
+      <c r="P82">
+        <v>0.18</v>
+      </c>
+      <c r="Q82">
+        <v>7568900000</v>
+      </c>
+      <c r="R82" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18">
+      <c r="A83" t="s">
+        <v>191</v>
+      </c>
+      <c r="B83" t="s">
+        <v>192</v>
+      </c>
+      <c r="H83">
+        <v>0.28</v>
+      </c>
+      <c r="K83">
+        <v>600</v>
+      </c>
+      <c r="L83">
+        <v>130</v>
+      </c>
+      <c r="M83">
+        <v>200</v>
+      </c>
+      <c r="N83" t="s">
+        <v>37</v>
+      </c>
+      <c r="O83">
+        <v>0.15</v>
+      </c>
+      <c r="P83">
+        <v>0.18</v>
+      </c>
+      <c r="Q83">
+        <v>7568900000</v>
+      </c>
+      <c r="R83" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18">
+      <c r="A84" t="s">
+        <v>193</v>
+      </c>
+      <c r="B84" t="s">
+        <v>194</v>
+      </c>
+      <c r="K84">
+        <v>600</v>
+      </c>
+      <c r="L84">
+        <v>130</v>
+      </c>
+      <c r="M84">
+        <v>200</v>
+      </c>
+      <c r="N84" t="s">
+        <v>40</v>
+      </c>
+      <c r="O84">
+        <v>0.15</v>
+      </c>
+      <c r="P84">
+        <v>0.18</v>
+      </c>
+      <c r="Q84">
+        <v>7568900000</v>
+      </c>
+      <c r="R84" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18">
+      <c r="A85" t="s">
+        <v>195</v>
+      </c>
+      <c r="B85" t="s">
+        <v>196</v>
+      </c>
+      <c r="K85">
+        <v>700</v>
+      </c>
+      <c r="L85">
+        <v>140</v>
+      </c>
+      <c r="M85">
+        <v>200</v>
+      </c>
+      <c r="N85" t="s">
+        <v>43</v>
+      </c>
+      <c r="O85">
+        <v>0.4</v>
+      </c>
+      <c r="P85">
+        <v>0.45</v>
+      </c>
+      <c r="Q85">
+        <v>10670900000</v>
+      </c>
+      <c r="R85" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18">
+      <c r="A86" t="s">
+        <v>197</v>
+      </c>
+      <c r="B86" t="s">
+        <v>198</v>
+      </c>
+      <c r="K86">
+        <v>700</v>
+      </c>
+      <c r="L86">
+        <v>140</v>
+      </c>
+      <c r="M86">
+        <v>200</v>
+      </c>
+      <c r="N86" t="s">
+        <v>46</v>
+      </c>
+      <c r="O86">
+        <v>0.4</v>
+      </c>
+      <c r="P86">
+        <v>0.45</v>
+      </c>
+      <c r="Q86">
+        <v>10670900000</v>
+      </c>
+      <c r="R86" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18">
+      <c r="A87" t="s">
+        <v>199</v>
+      </c>
+      <c r="B87" t="s">
+        <v>200</v>
+      </c>
+      <c r="K87">
+        <v>700</v>
+      </c>
+      <c r="L87">
+        <v>140</v>
+      </c>
+      <c r="M87">
+        <v>200</v>
+      </c>
+      <c r="N87" t="s">
+        <v>49</v>
+      </c>
+      <c r="O87">
+        <v>0.4</v>
+      </c>
+      <c r="P87">
+        <v>0.45</v>
+      </c>
+      <c r="Q87">
+        <v>10670900000</v>
+      </c>
+      <c r="R87" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18">
+      <c r="A88" t="s">
+        <v>201</v>
+      </c>
+      <c r="B88" t="s">
+        <v>202</v>
+      </c>
+      <c r="K88">
+        <v>700</v>
+      </c>
+      <c r="L88">
+        <v>140</v>
+      </c>
+      <c r="M88">
+        <v>200</v>
+      </c>
+      <c r="N88" t="s">
+        <v>52</v>
+      </c>
+      <c r="O88">
+        <v>0.4</v>
+      </c>
+      <c r="P88">
+        <v>0.45</v>
+      </c>
+      <c r="Q88">
+        <v>10670900000</v>
+      </c>
+      <c r="R88" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18">
+      <c r="A89" t="s">
+        <v>203</v>
+      </c>
+      <c r="B89" t="s">
+        <v>204</v>
+      </c>
+      <c r="K89">
+        <v>700</v>
+      </c>
+      <c r="L89">
+        <v>120</v>
+      </c>
+      <c r="M89">
+        <v>200</v>
+      </c>
+      <c r="N89" t="s">
+        <v>55</v>
+      </c>
+      <c r="O89">
+        <v>0.4</v>
+      </c>
+      <c r="P89">
+        <v>0.45</v>
+      </c>
+      <c r="Q89">
+        <v>10670900000</v>
+      </c>
+      <c r="R89" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18">
+      <c r="A90" t="s">
+        <v>205</v>
+      </c>
+      <c r="B90" t="s">
+        <v>206</v>
+      </c>
+      <c r="K90">
+        <v>700</v>
+      </c>
+      <c r="L90">
+        <v>120</v>
+      </c>
+      <c r="M90">
+        <v>200</v>
+      </c>
+      <c r="N90" t="s">
+        <v>84</v>
+      </c>
+      <c r="O90">
+        <v>0.4</v>
+      </c>
+      <c r="P90">
+        <v>0.45</v>
+      </c>
+      <c r="Q90">
+        <v>10670900000</v>
+      </c>
+      <c r="R90" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nerfing how drops work. Nerfed items and enchantements.
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -1,21 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE68D5E4-B8DA-D14E-A3FF-974756940182}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Affixes" sheetId="1" r:id="rId4"/>
+    <sheet name="Affixes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="207">
   <si>
     <t>name</t>
   </si>
@@ -641,14 +657,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -659,28 +670,37 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -970,39 +990,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="I58" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N85" sqref="N85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="180" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="15" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="21" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="8" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="180" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1058,7 +1071,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1105,7 +1118,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1137,7 +1150,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1163,7 +1176,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1189,7 +1202,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1215,7 +1228,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1241,7 +1254,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1264,10 +1277,10 @@
         <v>33</v>
       </c>
       <c r="O8">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="P8">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="Q8">
         <v>1000</v>
@@ -1276,7 +1289,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1299,10 +1312,10 @@
         <v>37</v>
       </c>
       <c r="O9">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="P9">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="Q9">
         <v>1000</v>
@@ -1311,7 +1324,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1334,10 +1347,10 @@
         <v>40</v>
       </c>
       <c r="O10">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="P10">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="Q10">
         <v>1000</v>
@@ -1346,7 +1359,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1369,10 +1382,10 @@
         <v>43</v>
       </c>
       <c r="O11">
-        <v>0.2</v>
+        <v>0.03</v>
       </c>
       <c r="P11">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="Q11">
         <v>5000</v>
@@ -1381,7 +1394,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1404,10 +1417,10 @@
         <v>46</v>
       </c>
       <c r="O12">
-        <v>0.2</v>
+        <v>0.03</v>
       </c>
       <c r="P12">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="Q12">
         <v>5000</v>
@@ -1416,7 +1429,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -1439,10 +1452,10 @@
         <v>49</v>
       </c>
       <c r="O13">
-        <v>0.2</v>
+        <v>0.03</v>
       </c>
       <c r="P13">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="Q13">
         <v>5000</v>
@@ -1451,7 +1464,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1474,10 +1487,10 @@
         <v>52</v>
       </c>
       <c r="O14">
-        <v>0.2</v>
+        <v>0.03</v>
       </c>
       <c r="P14">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="Q14">
         <v>5000</v>
@@ -1486,7 +1499,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1509,10 +1522,10 @@
         <v>55</v>
       </c>
       <c r="O15">
-        <v>0.2</v>
+        <v>0.03</v>
       </c>
       <c r="P15">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="Q15">
         <v>5000</v>
@@ -1521,7 +1534,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -1568,7 +1581,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -1606,7 +1619,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -1632,7 +1645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -1658,7 +1671,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -1684,7 +1697,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -1710,7 +1723,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -1733,10 +1746,10 @@
         <v>33</v>
       </c>
       <c r="O22">
-        <v>0.25</v>
+        <v>0.08</v>
       </c>
       <c r="P22">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="Q22">
         <v>50000</v>
@@ -1745,7 +1758,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>70</v>
       </c>
@@ -1768,10 +1781,10 @@
         <v>37</v>
       </c>
       <c r="O23">
-        <v>0.25</v>
+        <v>0.08</v>
       </c>
       <c r="P23">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="Q23">
         <v>50000</v>
@@ -1780,7 +1793,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -1800,10 +1813,10 @@
         <v>40</v>
       </c>
       <c r="O24">
-        <v>0.25</v>
+        <v>0.08</v>
       </c>
       <c r="P24">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="Q24">
         <v>50000</v>
@@ -1812,7 +1825,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -1835,10 +1848,10 @@
         <v>43</v>
       </c>
       <c r="O25">
-        <v>0.25</v>
+        <v>0.08</v>
       </c>
       <c r="P25">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="Q25">
         <v>100000</v>
@@ -1847,7 +1860,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -1870,10 +1883,10 @@
         <v>46</v>
       </c>
       <c r="O26">
-        <v>0.25</v>
+        <v>0.08</v>
       </c>
       <c r="P26">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="Q26">
         <v>100000</v>
@@ -1882,7 +1895,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -1905,10 +1918,10 @@
         <v>49</v>
       </c>
       <c r="O27">
-        <v>0.25</v>
+        <v>0.08</v>
       </c>
       <c r="P27">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="Q27">
         <v>100000</v>
@@ -1917,7 +1930,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -1940,10 +1953,10 @@
         <v>52</v>
       </c>
       <c r="O28">
-        <v>0.25</v>
+        <v>0.08</v>
       </c>
       <c r="P28">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="Q28">
         <v>100000</v>
@@ -1952,7 +1965,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -1975,10 +1988,10 @@
         <v>84</v>
       </c>
       <c r="O29">
-        <v>0.25</v>
+        <v>0.08</v>
       </c>
       <c r="P29">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="Q29">
         <v>100000</v>
@@ -1987,7 +2000,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -2010,10 +2023,10 @@
         <v>55</v>
       </c>
       <c r="O30">
-        <v>0.25</v>
+        <v>0.08</v>
       </c>
       <c r="P30">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="Q30">
         <v>100000</v>
@@ -2022,7 +2035,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>87</v>
       </c>
@@ -2069,7 +2082,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -2095,7 +2108,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>91</v>
       </c>
@@ -2121,7 +2134,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>93</v>
       </c>
@@ -2147,7 +2160,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>95</v>
       </c>
@@ -2173,7 +2186,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>97</v>
       </c>
@@ -2199,7 +2212,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>99</v>
       </c>
@@ -2222,10 +2235,10 @@
         <v>33</v>
       </c>
       <c r="O37">
-        <v>0.28</v>
+        <v>0.12</v>
       </c>
       <c r="P37">
-        <v>0.38</v>
+        <v>0.18</v>
       </c>
       <c r="Q37">
         <v>1230000</v>
@@ -2234,7 +2247,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>101</v>
       </c>
@@ -2257,10 +2270,10 @@
         <v>37</v>
       </c>
       <c r="O38">
-        <v>0.28</v>
+        <v>0.12</v>
       </c>
       <c r="P38">
-        <v>0.38</v>
+        <v>0.18</v>
       </c>
       <c r="Q38">
         <v>1230000</v>
@@ -2269,7 +2282,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>103</v>
       </c>
@@ -2289,10 +2302,10 @@
         <v>40</v>
       </c>
       <c r="O39">
-        <v>0.28</v>
+        <v>0.12</v>
       </c>
       <c r="P39">
-        <v>0.38</v>
+        <v>0.18</v>
       </c>
       <c r="Q39">
         <v>1230000</v>
@@ -2301,7 +2314,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>105</v>
       </c>
@@ -2321,10 +2334,10 @@
         <v>43</v>
       </c>
       <c r="O40">
-        <v>0.28</v>
+        <v>0.12</v>
       </c>
       <c r="P40">
-        <v>0.38</v>
+        <v>0.18</v>
       </c>
       <c r="Q40">
         <v>2500000</v>
@@ -2333,7 +2346,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>107</v>
       </c>
@@ -2353,10 +2366,10 @@
         <v>46</v>
       </c>
       <c r="O41">
-        <v>0.28</v>
+        <v>0.12</v>
       </c>
       <c r="P41">
-        <v>0.38</v>
+        <v>0.18</v>
       </c>
       <c r="Q41">
         <v>2500000</v>
@@ -2365,7 +2378,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>109</v>
       </c>
@@ -2385,10 +2398,10 @@
         <v>49</v>
       </c>
       <c r="O42">
-        <v>0.28</v>
+        <v>0.12</v>
       </c>
       <c r="P42">
-        <v>0.38</v>
+        <v>0.18</v>
       </c>
       <c r="Q42">
         <v>2500000</v>
@@ -2397,7 +2410,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>111</v>
       </c>
@@ -2417,10 +2430,10 @@
         <v>52</v>
       </c>
       <c r="O43">
-        <v>0.28</v>
+        <v>0.12</v>
       </c>
       <c r="P43">
-        <v>0.38</v>
+        <v>0.18</v>
       </c>
       <c r="Q43">
         <v>2500000</v>
@@ -2429,7 +2442,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>113</v>
       </c>
@@ -2449,10 +2462,10 @@
         <v>84</v>
       </c>
       <c r="O44">
-        <v>0.28</v>
+        <v>0.12</v>
       </c>
       <c r="P44">
-        <v>0.38</v>
+        <v>0.18</v>
       </c>
       <c r="Q44">
         <v>2500000</v>
@@ -2461,7 +2474,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>115</v>
       </c>
@@ -2481,10 +2494,10 @@
         <v>55</v>
       </c>
       <c r="O45">
-        <v>0.28</v>
+        <v>0.12</v>
       </c>
       <c r="P45">
-        <v>0.38</v>
+        <v>0.18</v>
       </c>
       <c r="Q45">
         <v>2500000</v>
@@ -2493,7 +2506,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>117</v>
       </c>
@@ -2501,28 +2514,28 @@
         <v>118</v>
       </c>
       <c r="C46">
-        <v>0.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D46">
-        <v>0.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E46">
-        <v>0.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F46">
-        <v>0.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="G46">
-        <v>0.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H46">
-        <v>0.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="I46">
-        <v>0.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="J46">
-        <v>0.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="K46">
         <v>170</v>
@@ -2540,7 +2553,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>119</v>
       </c>
@@ -2575,7 +2588,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>121</v>
       </c>
@@ -2601,7 +2614,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>123</v>
       </c>
@@ -2627,7 +2640,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:18">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>125</v>
       </c>
@@ -2653,7 +2666,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>127</v>
       </c>
@@ -2679,7 +2692,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:18">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>129</v>
       </c>
@@ -2702,10 +2715,10 @@
         <v>33</v>
       </c>
       <c r="O52">
-        <v>0.3</v>
+        <v>0.18</v>
       </c>
       <c r="P52">
-        <v>0.4</v>
+        <v>0.22</v>
       </c>
       <c r="Q52">
         <v>25000000</v>
@@ -2714,7 +2727,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>131</v>
       </c>
@@ -2737,10 +2750,10 @@
         <v>37</v>
       </c>
       <c r="O53">
-        <v>0.3</v>
+        <v>0.18</v>
       </c>
       <c r="P53">
-        <v>0.4</v>
+        <v>0.22</v>
       </c>
       <c r="Q53">
         <v>25000000</v>
@@ -2749,7 +2762,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>133</v>
       </c>
@@ -2769,10 +2782,10 @@
         <v>40</v>
       </c>
       <c r="O54">
-        <v>0.3</v>
+        <v>0.18</v>
       </c>
       <c r="P54">
-        <v>0.4</v>
+        <v>0.22</v>
       </c>
       <c r="Q54">
         <v>25000000</v>
@@ -2781,7 +2794,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>135</v>
       </c>
@@ -2801,10 +2814,10 @@
         <v>43</v>
       </c>
       <c r="O55">
-        <v>0.3</v>
+        <v>0.18</v>
       </c>
       <c r="P55">
-        <v>0.4</v>
+        <v>0.22</v>
       </c>
       <c r="Q55">
         <v>55000000</v>
@@ -2813,7 +2826,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:18">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>137</v>
       </c>
@@ -2833,10 +2846,10 @@
         <v>46</v>
       </c>
       <c r="O56">
-        <v>0.3</v>
+        <v>0.18</v>
       </c>
       <c r="P56">
-        <v>0.4</v>
+        <v>0.22</v>
       </c>
       <c r="Q56">
         <v>55000000</v>
@@ -2845,7 +2858,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:18">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>139</v>
       </c>
@@ -2865,10 +2878,10 @@
         <v>49</v>
       </c>
       <c r="O57">
-        <v>0.3</v>
+        <v>0.18</v>
       </c>
       <c r="P57">
-        <v>0.4</v>
+        <v>0.22</v>
       </c>
       <c r="Q57">
         <v>55000000</v>
@@ -2877,7 +2890,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>141</v>
       </c>
@@ -2897,10 +2910,10 @@
         <v>52</v>
       </c>
       <c r="O58">
-        <v>0.3</v>
+        <v>0.18</v>
       </c>
       <c r="P58">
-        <v>0.4</v>
+        <v>0.22</v>
       </c>
       <c r="Q58">
         <v>55000000</v>
@@ -2909,7 +2922,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:18">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>143</v>
       </c>
@@ -2929,10 +2942,10 @@
         <v>84</v>
       </c>
       <c r="O59">
-        <v>0.3</v>
+        <v>0.18</v>
       </c>
       <c r="P59">
-        <v>0.4</v>
+        <v>0.22</v>
       </c>
       <c r="Q59">
         <v>55000000</v>
@@ -2941,7 +2954,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="60" spans="1:18">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>145</v>
       </c>
@@ -2961,10 +2974,10 @@
         <v>55</v>
       </c>
       <c r="O60">
-        <v>0.3</v>
+        <v>0.18</v>
       </c>
       <c r="P60">
-        <v>0.4</v>
+        <v>0.22</v>
       </c>
       <c r="Q60">
         <v>55000000</v>
@@ -2973,7 +2986,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="1:18">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>147</v>
       </c>
@@ -3020,7 +3033,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:18">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>149</v>
       </c>
@@ -3046,7 +3059,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:18">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>151</v>
       </c>
@@ -3072,7 +3085,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:18">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>153</v>
       </c>
@@ -3098,7 +3111,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:18">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>155</v>
       </c>
@@ -3124,7 +3137,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:18">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>157</v>
       </c>
@@ -3150,7 +3163,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:18">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>159</v>
       </c>
@@ -3173,10 +3186,10 @@
         <v>33</v>
       </c>
       <c r="O67">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="P67">
-        <v>0.43</v>
+        <v>0.25</v>
       </c>
       <c r="Q67">
         <v>560800000</v>
@@ -3185,7 +3198,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="68" spans="1:18">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>161</v>
       </c>
@@ -3208,10 +3221,10 @@
         <v>37</v>
       </c>
       <c r="O68">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="P68">
-        <v>0.43</v>
+        <v>0.25</v>
       </c>
       <c r="Q68">
         <v>560800000</v>
@@ -3220,7 +3233,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="1:18">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>163</v>
       </c>
@@ -3240,10 +3253,10 @@
         <v>40</v>
       </c>
       <c r="O69">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="P69">
-        <v>0.43</v>
+        <v>0.25</v>
       </c>
       <c r="Q69">
         <v>560800000</v>
@@ -3252,7 +3265,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="70" spans="1:18">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>165</v>
       </c>
@@ -3272,10 +3285,10 @@
         <v>43</v>
       </c>
       <c r="O70">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="P70">
-        <v>0.43</v>
+        <v>0.25</v>
       </c>
       <c r="Q70">
         <v>1340500000</v>
@@ -3284,7 +3297,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:18">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>167</v>
       </c>
@@ -3304,10 +3317,10 @@
         <v>46</v>
       </c>
       <c r="O71">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="P71">
-        <v>0.43</v>
+        <v>0.25</v>
       </c>
       <c r="Q71">
         <v>1340500000</v>
@@ -3316,7 +3329,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>169</v>
       </c>
@@ -3336,10 +3349,10 @@
         <v>49</v>
       </c>
       <c r="O72">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="P72">
-        <v>0.43</v>
+        <v>0.25</v>
       </c>
       <c r="Q72">
         <v>1340500000</v>
@@ -3348,7 +3361,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="1:18">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>171</v>
       </c>
@@ -3368,10 +3381,10 @@
         <v>52</v>
       </c>
       <c r="O73">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="P73">
-        <v>0.43</v>
+        <v>0.25</v>
       </c>
       <c r="Q73">
         <v>1340500000</v>
@@ -3380,7 +3393,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="74" spans="1:18">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>173</v>
       </c>
@@ -3400,10 +3413,10 @@
         <v>84</v>
       </c>
       <c r="O74">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="P74">
-        <v>0.43</v>
+        <v>0.25</v>
       </c>
       <c r="Q74">
         <v>1340500000</v>
@@ -3412,7 +3425,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:18">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>175</v>
       </c>
@@ -3432,10 +3445,10 @@
         <v>55</v>
       </c>
       <c r="O75">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="P75">
-        <v>0.43</v>
+        <v>0.25</v>
       </c>
       <c r="Q75">
         <v>1340500000</v>
@@ -3444,7 +3457,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="1:18">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>177</v>
       </c>
@@ -3491,30 +3504,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:18">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
       <c r="B77" t="s">
-        <v>180</v>
-      </c>
-      <c r="F77">
-        <v>0.48</v>
-      </c>
-      <c r="G77">
-        <v>0</v>
-      </c>
-      <c r="H77">
-        <v>0</v>
-      </c>
-      <c r="I77">
-        <v>0</v>
-      </c>
-      <c r="J77">
-        <v>0</v>
+        <v>204</v>
       </c>
       <c r="K77">
-        <v>530</v>
+        <v>700</v>
       </c>
       <c r="L77">
         <v>120</v>
@@ -3522,25 +3520,31 @@
       <c r="M77">
         <v>200</v>
       </c>
+      <c r="N77" t="s">
+        <v>55</v>
+      </c>
+      <c r="O77">
+        <v>0.23</v>
+      </c>
+      <c r="P77">
+        <v>0.28000000000000003</v>
+      </c>
       <c r="Q77">
-        <v>5670200000</v>
+        <v>10670900000</v>
       </c>
       <c r="R77" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="B78" t="s">
-        <v>182</v>
-      </c>
-      <c r="H78">
-        <v>0.48</v>
+        <v>206</v>
       </c>
       <c r="K78">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="L78">
         <v>120</v>
@@ -3548,25 +3552,46 @@
       <c r="M78">
         <v>200</v>
       </c>
+      <c r="N78" t="s">
+        <v>84</v>
+      </c>
+      <c r="O78">
+        <v>0.23</v>
+      </c>
+      <c r="P78">
+        <v>0.28000000000000003</v>
+      </c>
       <c r="Q78">
-        <v>5670200000</v>
+        <v>10670900000</v>
       </c>
       <c r="R78" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B79" t="s">
-        <v>184</v>
+        <v>180</v>
+      </c>
+      <c r="F79">
+        <v>0.48</v>
       </c>
       <c r="G79">
-        <v>0.48</v>
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
       </c>
       <c r="K79">
-        <v>500</v>
+        <v>530</v>
       </c>
       <c r="L79">
         <v>120</v>
@@ -3581,14 +3606,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:18">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B80" t="s">
-        <v>186</v>
-      </c>
-      <c r="J80">
+        <v>182</v>
+      </c>
+      <c r="H80">
         <v>0.48</v>
       </c>
       <c r="K80">
@@ -3607,14 +3632,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:18">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B81" t="s">
-        <v>188</v>
-      </c>
-      <c r="I81">
+        <v>184</v>
+      </c>
+      <c r="G81">
         <v>0.48</v>
       </c>
       <c r="K81">
@@ -3633,82 +3658,67 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:18">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B82" t="s">
-        <v>190</v>
-      </c>
-      <c r="H82">
-        <v>0.28</v>
+        <v>186</v>
+      </c>
+      <c r="J82">
+        <v>0.48</v>
       </c>
       <c r="K82">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="L82">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="M82">
         <v>200</v>
       </c>
-      <c r="N82" t="s">
-        <v>33</v>
-      </c>
-      <c r="O82">
-        <v>0.15</v>
-      </c>
-      <c r="P82">
-        <v>0.18</v>
-      </c>
       <c r="Q82">
-        <v>7568900000</v>
+        <v>5670200000</v>
       </c>
       <c r="R82" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="83" spans="1:18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B83" t="s">
-        <v>192</v>
-      </c>
-      <c r="H83">
-        <v>0.28</v>
+        <v>188</v>
+      </c>
+      <c r="I83">
+        <v>0.48</v>
       </c>
       <c r="K83">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="L83">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="M83">
         <v>200</v>
       </c>
-      <c r="N83" t="s">
-        <v>37</v>
-      </c>
-      <c r="O83">
-        <v>0.15</v>
-      </c>
-      <c r="P83">
-        <v>0.18</v>
-      </c>
       <c r="Q83">
-        <v>7568900000</v>
+        <v>5670200000</v>
       </c>
       <c r="R83" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="84" spans="1:18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B84" t="s">
-        <v>194</v>
+        <v>190</v>
+      </c>
+      <c r="H84">
+        <v>0.28000000000000003</v>
       </c>
       <c r="K84">
         <v>600</v>
@@ -3720,7 +3730,7 @@
         <v>200</v>
       </c>
       <c r="N84" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="O84">
         <v>0.15</v>
@@ -3735,76 +3745,79 @@
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="1:18">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B85" t="s">
-        <v>196</v>
+        <v>192</v>
+      </c>
+      <c r="H85">
+        <v>0.28000000000000003</v>
       </c>
       <c r="K85">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="L85">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="M85">
         <v>200</v>
       </c>
       <c r="N85" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="O85">
-        <v>0.4</v>
+        <v>0.15</v>
       </c>
       <c r="P85">
-        <v>0.45</v>
+        <v>0.18</v>
       </c>
       <c r="Q85">
-        <v>10670900000</v>
+        <v>7568900000</v>
       </c>
       <c r="R85" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="86" spans="1:18">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B86" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="K86">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="L86">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="M86">
         <v>200</v>
       </c>
       <c r="N86" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="O86">
-        <v>0.4</v>
+        <v>0.15</v>
       </c>
       <c r="P86">
-        <v>0.45</v>
+        <v>0.18</v>
       </c>
       <c r="Q86">
-        <v>10670900000</v>
+        <v>7568900000</v>
       </c>
       <c r="R86" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="87" spans="1:18">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B87" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="K87">
         <v>700</v>
@@ -3816,13 +3829,13 @@
         <v>200</v>
       </c>
       <c r="N87" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="O87">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="P87">
-        <v>0.45</v>
+        <v>0.3</v>
       </c>
       <c r="Q87">
         <v>10670900000</v>
@@ -3831,12 +3844,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="88" spans="1:18">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B88" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="K88">
         <v>700</v>
@@ -3848,13 +3861,13 @@
         <v>200</v>
       </c>
       <c r="N88" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="O88">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="P88">
-        <v>0.45</v>
+        <v>0.3</v>
       </c>
       <c r="Q88">
         <v>10670900000</v>
@@ -3863,30 +3876,30 @@
         <v>34</v>
       </c>
     </row>
-    <row r="89" spans="1:18">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B89" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="K89">
         <v>700</v>
       </c>
       <c r="L89">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="M89">
         <v>200</v>
       </c>
       <c r="N89" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="O89">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="P89">
-        <v>0.45</v>
+        <v>0.3</v>
       </c>
       <c r="Q89">
         <v>10670900000</v>
@@ -3895,30 +3908,30 @@
         <v>34</v>
       </c>
     </row>
-    <row r="90" spans="1:18">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B90" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="K90">
         <v>700</v>
       </c>
       <c r="L90">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="M90">
         <v>200</v>
       </c>
       <c r="N90" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="O90">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="P90">
-        <v>0.45</v>
+        <v>0.3</v>
       </c>
       <c r="Q90">
         <v>10670900000</v>
@@ -3928,17 +3941,11 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R90">
+    <sortCondition ref="L2:L90"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated items and prefixes
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -1,37 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE68D5E4-B8DA-D14E-A3FF-974756940182}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Affixes" sheetId="1" r:id="rId1"/>
+    <sheet name="Affixes" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" forceFullCalc="1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="207">
   <si>
     <t>name</t>
   </si>
@@ -570,6 +554,18 @@
     <t>Be tuned into the earth and its balancing energy</t>
   </si>
   <si>
+    <t>Enchanted Labyrinth</t>
+  </si>
+  <si>
+    <t>Get lost in a labyrinth of all the enchantments you can create.</t>
+  </si>
+  <si>
+    <t>Dark Pact</t>
+  </si>
+  <si>
+    <t>Make a dark pact when creating artifacts.</t>
+  </si>
+  <si>
     <t>Strength of Courage</t>
   </si>
   <si>
@@ -640,26 +636,19 @@
   </si>
   <si>
     <t>Let the thoughts and the inspiration from the devil inspire you.</t>
-  </si>
-  <si>
-    <t>Enchanted Labyrinth</t>
-  </si>
-  <si>
-    <t>Get lost in a labyrinth of all the enchantments you can create.</t>
-  </si>
-  <si>
-    <t>Dark Pact</t>
-  </si>
-  <si>
-    <t>Make a dark pact when creating artifacts.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -670,37 +659,28 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -990,32 +970,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:R90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I58" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N85" sqref="N85"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="180" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="180" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="18" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="19" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="15" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="23" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="21" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="8" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1071,7 +1058,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1118,7 +1105,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1150,7 +1137,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1176,7 +1163,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1202,7 +1189,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1228,7 +1215,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1254,7 +1241,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1289,7 +1276,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1324,7 +1311,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1359,7 +1346,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1394,7 +1381,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1429,7 +1416,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -1464,7 +1451,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1499,7 +1486,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1534,7 +1521,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -1581,7 +1568,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -1619,7 +1606,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -1645,7 +1632,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -1671,7 +1658,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -1697,7 +1684,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -1723,7 +1710,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -1758,7 +1745,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18">
       <c r="A23" t="s">
         <v>70</v>
       </c>
@@ -1793,7 +1780,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -1825,7 +1812,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -1860,7 +1847,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -1895,7 +1882,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -1930,7 +1917,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -1965,7 +1952,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -2000,7 +1987,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -2035,7 +2022,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18">
       <c r="A31" t="s">
         <v>87</v>
       </c>
@@ -2082,7 +2069,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -2108,7 +2095,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18">
       <c r="A33" t="s">
         <v>91</v>
       </c>
@@ -2134,7 +2121,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18">
       <c r="A34" t="s">
         <v>93</v>
       </c>
@@ -2160,7 +2147,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18">
       <c r="A35" t="s">
         <v>95</v>
       </c>
@@ -2186,7 +2173,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18">
       <c r="A36" t="s">
         <v>97</v>
       </c>
@@ -2212,7 +2199,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18">
       <c r="A37" t="s">
         <v>99</v>
       </c>
@@ -2247,7 +2234,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18">
       <c r="A38" t="s">
         <v>101</v>
       </c>
@@ -2282,7 +2269,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18">
       <c r="A39" t="s">
         <v>103</v>
       </c>
@@ -2314,7 +2301,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18">
       <c r="A40" t="s">
         <v>105</v>
       </c>
@@ -2346,7 +2333,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18">
       <c r="A41" t="s">
         <v>107</v>
       </c>
@@ -2378,7 +2365,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18">
       <c r="A42" t="s">
         <v>109</v>
       </c>
@@ -2410,7 +2397,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18">
       <c r="A43" t="s">
         <v>111</v>
       </c>
@@ -2442,7 +2429,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18">
       <c r="A44" t="s">
         <v>113</v>
       </c>
@@ -2474,7 +2461,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18">
       <c r="A45" t="s">
         <v>115</v>
       </c>
@@ -2506,7 +2493,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18">
       <c r="A46" t="s">
         <v>117</v>
       </c>
@@ -2514,28 +2501,28 @@
         <v>118</v>
       </c>
       <c r="C46">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="D46">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="E46">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="F46">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="G46">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="H46">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="I46">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="J46">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="K46">
         <v>170</v>
@@ -2553,7 +2540,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18">
       <c r="A47" t="s">
         <v>119</v>
       </c>
@@ -2588,7 +2575,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18">
       <c r="A48" t="s">
         <v>121</v>
       </c>
@@ -2614,7 +2601,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18">
       <c r="A49" t="s">
         <v>123</v>
       </c>
@@ -2640,7 +2627,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18">
       <c r="A50" t="s">
         <v>125</v>
       </c>
@@ -2666,7 +2653,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18">
       <c r="A51" t="s">
         <v>127</v>
       </c>
@@ -2692,7 +2679,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18">
       <c r="A52" t="s">
         <v>129</v>
       </c>
@@ -2727,7 +2714,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18">
       <c r="A53" t="s">
         <v>131</v>
       </c>
@@ -2762,7 +2749,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18">
       <c r="A54" t="s">
         <v>133</v>
       </c>
@@ -2794,7 +2781,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18">
       <c r="A55" t="s">
         <v>135</v>
       </c>
@@ -2826,7 +2813,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18">
       <c r="A56" t="s">
         <v>137</v>
       </c>
@@ -2858,7 +2845,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18">
       <c r="A57" t="s">
         <v>139</v>
       </c>
@@ -2890,7 +2877,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18">
       <c r="A58" t="s">
         <v>141</v>
       </c>
@@ -2922,7 +2909,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18">
       <c r="A59" t="s">
         <v>143</v>
       </c>
@@ -2954,7 +2941,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18">
       <c r="A60" t="s">
         <v>145</v>
       </c>
@@ -2986,7 +2973,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18">
       <c r="A61" t="s">
         <v>147</v>
       </c>
@@ -3033,7 +3020,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:18">
       <c r="A62" t="s">
         <v>149</v>
       </c>
@@ -3059,7 +3046,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18">
       <c r="A63" t="s">
         <v>151</v>
       </c>
@@ -3085,7 +3072,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:18">
       <c r="A64" t="s">
         <v>153</v>
       </c>
@@ -3111,7 +3098,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:18">
       <c r="A65" t="s">
         <v>155</v>
       </c>
@@ -3137,7 +3124,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:18">
       <c r="A66" t="s">
         <v>157</v>
       </c>
@@ -3163,7 +3150,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:18">
       <c r="A67" t="s">
         <v>159</v>
       </c>
@@ -3198,7 +3185,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:18">
       <c r="A68" t="s">
         <v>161</v>
       </c>
@@ -3233,7 +3220,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:18">
       <c r="A69" t="s">
         <v>163</v>
       </c>
@@ -3265,7 +3252,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:18">
       <c r="A70" t="s">
         <v>165</v>
       </c>
@@ -3297,7 +3284,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18">
       <c r="A71" t="s">
         <v>167</v>
       </c>
@@ -3329,7 +3316,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:18">
       <c r="A72" t="s">
         <v>169</v>
       </c>
@@ -3361,7 +3348,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:18">
       <c r="A73" t="s">
         <v>171</v>
       </c>
@@ -3393,7 +3380,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:18">
       <c r="A74" t="s">
         <v>173</v>
       </c>
@@ -3425,7 +3412,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:18">
       <c r="A75" t="s">
         <v>175</v>
       </c>
@@ -3457,7 +3444,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:18">
       <c r="A76" t="s">
         <v>177</v>
       </c>
@@ -3504,12 +3491,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:18">
       <c r="A77" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="B77" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="K77">
         <v>700</v>
@@ -3527,7 +3514,7 @@
         <v>0.23</v>
       </c>
       <c r="P77">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="Q77">
         <v>10670900000</v>
@@ -3536,12 +3523,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:18">
       <c r="A78" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="B78" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="K78">
         <v>700</v>
@@ -3559,7 +3546,7 @@
         <v>0.23</v>
       </c>
       <c r="P78">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="Q78">
         <v>10670900000</v>
@@ -3568,12 +3555,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:18">
       <c r="A79" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B79" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="F79">
         <v>0.48</v>
@@ -3606,12 +3593,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:18">
       <c r="A80" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B80" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="H80">
         <v>0.48</v>
@@ -3632,12 +3619,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:18">
       <c r="A81" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B81" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="G81">
         <v>0.48</v>
@@ -3658,12 +3645,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:18">
       <c r="A82" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B82" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="J82">
         <v>0.48</v>
@@ -3684,12 +3671,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:18">
       <c r="A83" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B83" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="I83">
         <v>0.48</v>
@@ -3710,15 +3697,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:18">
       <c r="A84" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B84" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="H84">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="K84">
         <v>600</v>
@@ -3745,15 +3732,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:18">
       <c r="A85" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B85" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="H85">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="K85">
         <v>600</v>
@@ -3780,12 +3767,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:18">
       <c r="A86" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B86" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="K86">
         <v>600</v>
@@ -3812,12 +3799,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:18">
       <c r="A87" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B87" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="K87">
         <v>700</v>
@@ -3844,12 +3831,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:18">
       <c r="A88" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B88" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="K88">
         <v>700</v>
@@ -3876,12 +3863,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:18">
       <c r="A89" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B89" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="K89">
         <v>700</v>
@@ -3908,12 +3895,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:18">
       <c r="A90" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B90" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="K90">
         <v>700</v>
@@ -3941,11 +3928,17 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R90">
-    <sortCondition ref="L2:L90"/>
-  </sortState>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All the prod items, monsters and affixes
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -554,6 +554,78 @@
     <t>Be tuned into the earth and its balancing energy</t>
   </si>
   <si>
+    <t>Strength of Courage</t>
+  </si>
+  <si>
+    <t>Give your self the belief in strength and courage to survive whats to come.</t>
+  </si>
+  <si>
+    <t>See All</t>
+  </si>
+  <si>
+    <t>Missing never was the option. Damage and accuracy was.</t>
+  </si>
+  <si>
+    <t>Reapers Kiss</t>
+  </si>
+  <si>
+    <t>Thirst for souls, thirst for death.</t>
+  </si>
+  <si>
+    <t>Scholars Research</t>
+  </si>
+  <si>
+    <t>All the research in the world that has been done so far on the study of magic, is yours.</t>
+  </si>
+  <si>
+    <t>Prayer Of Hope</t>
+  </si>
+  <si>
+    <t>If you pray, I shall give you hope. If you listen, I shall guide you.</t>
+  </si>
+  <si>
+    <t>Rangers Luck</t>
+  </si>
+  <si>
+    <t>With the luck of a well trained ranger you might be able to finally hit that bear.</t>
+  </si>
+  <si>
+    <t>Rumor's Movement</t>
+  </si>
+  <si>
+    <t>Move like a Rumor. Impossible o see, hit or know is coming.</t>
+  </si>
+  <si>
+    <t>Smell of Gold</t>
+  </si>
+  <si>
+    <t>The smell of gold can drag one deep into the lust for treasure.</t>
+  </si>
+  <si>
+    <t>Godly Weapon Crafting</t>
+  </si>
+  <si>
+    <t>You'll probably never fail to craft again.</t>
+  </si>
+  <si>
+    <t>Angelic Armour Smithing</t>
+  </si>
+  <si>
+    <t>Craft amour with the help of the angels.</t>
+  </si>
+  <si>
+    <t>Divine Magic Crafting</t>
+  </si>
+  <si>
+    <t>Use divine help to craft magical spells.</t>
+  </si>
+  <si>
+    <t>Devilish Ring Crafting</t>
+  </si>
+  <si>
+    <t>Let the thoughts and the inspiration from the devil inspire you.</t>
+  </si>
+  <si>
     <t>Enchanted Labyrinth</t>
   </si>
   <si>
@@ -564,78 +636,6 @@
   </si>
   <si>
     <t>Make a dark pact when creating artifacts.</t>
-  </si>
-  <si>
-    <t>Strength of Courage</t>
-  </si>
-  <si>
-    <t>Give your self the belief in strength and courage to survive whats to come.</t>
-  </si>
-  <si>
-    <t>See All</t>
-  </si>
-  <si>
-    <t>Missing never was the option. Damage and accuracy was.</t>
-  </si>
-  <si>
-    <t>Reapers Kiss</t>
-  </si>
-  <si>
-    <t>Thirst for souls, thirst for death.</t>
-  </si>
-  <si>
-    <t>Scholars Research</t>
-  </si>
-  <si>
-    <t>All the research in the world that has been done so far on the study of magic, is yours.</t>
-  </si>
-  <si>
-    <t>Prayer Of Hope</t>
-  </si>
-  <si>
-    <t>If you pray, I shall give you hope. If you listen, I shall guide you.</t>
-  </si>
-  <si>
-    <t>Rangers Luck</t>
-  </si>
-  <si>
-    <t>With the luck of a well trained ranger you might be able to finally hit that bear.</t>
-  </si>
-  <si>
-    <t>Rumor's Movement</t>
-  </si>
-  <si>
-    <t>Move like a Rumor. Impossible o see, hit or know is coming.</t>
-  </si>
-  <si>
-    <t>Smell of Gold</t>
-  </si>
-  <si>
-    <t>The smell of gold can drag one deep into the lust for treasure.</t>
-  </si>
-  <si>
-    <t>Godly Weapon Crafting</t>
-  </si>
-  <si>
-    <t>You'll probably never fail to craft again.</t>
-  </si>
-  <si>
-    <t>Angelic Armour Smithing</t>
-  </si>
-  <si>
-    <t>Craft amour with the help of the angels.</t>
-  </si>
-  <si>
-    <t>Divine Magic Crafting</t>
-  </si>
-  <si>
-    <t>Use divine help to craft magical spells.</t>
-  </si>
-  <si>
-    <t>Devilish Ring Crafting</t>
-  </si>
-  <si>
-    <t>Let the thoughts and the inspiration from the devil inspire you.</t>
   </si>
 </sst>
 </file>
@@ -3498,8 +3498,23 @@
       <c r="B77" t="s">
         <v>180</v>
       </c>
+      <c r="F77">
+        <v>0.48</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
       <c r="K77">
-        <v>700</v>
+        <v>530</v>
       </c>
       <c r="L77">
         <v>120</v>
@@ -3507,20 +3522,11 @@
       <c r="M77">
         <v>200</v>
       </c>
-      <c r="N77" t="s">
-        <v>55</v>
-      </c>
-      <c r="O77">
-        <v>0.23</v>
-      </c>
-      <c r="P77">
-        <v>0.28</v>
-      </c>
       <c r="Q77">
-        <v>10670900000</v>
+        <v>5670200000</v>
       </c>
       <c r="R77" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="78" spans="1:18">
@@ -3530,8 +3536,11 @@
       <c r="B78" t="s">
         <v>182</v>
       </c>
+      <c r="H78">
+        <v>0.48</v>
+      </c>
       <c r="K78">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="L78">
         <v>120</v>
@@ -3539,20 +3548,11 @@
       <c r="M78">
         <v>200</v>
       </c>
-      <c r="N78" t="s">
-        <v>84</v>
-      </c>
-      <c r="O78">
-        <v>0.23</v>
-      </c>
-      <c r="P78">
-        <v>0.28</v>
-      </c>
       <c r="Q78">
-        <v>10670900000</v>
+        <v>5670200000</v>
       </c>
       <c r="R78" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:18">
@@ -3562,23 +3562,11 @@
       <c r="B79" t="s">
         <v>184</v>
       </c>
-      <c r="F79">
+      <c r="G79">
         <v>0.48</v>
       </c>
-      <c r="G79">
-        <v>0</v>
-      </c>
-      <c r="H79">
-        <v>0</v>
-      </c>
-      <c r="I79">
-        <v>0</v>
-      </c>
-      <c r="J79">
-        <v>0</v>
-      </c>
       <c r="K79">
-        <v>530</v>
+        <v>500</v>
       </c>
       <c r="L79">
         <v>120</v>
@@ -3600,7 +3588,7 @@
       <c r="B80" t="s">
         <v>186</v>
       </c>
-      <c r="H80">
+      <c r="J80">
         <v>0.48</v>
       </c>
       <c r="K80">
@@ -3626,7 +3614,7 @@
       <c r="B81" t="s">
         <v>188</v>
       </c>
-      <c r="G81">
+      <c r="I81">
         <v>0.48</v>
       </c>
       <c r="K81">
@@ -3652,23 +3640,32 @@
       <c r="B82" t="s">
         <v>190</v>
       </c>
-      <c r="J82">
-        <v>0.48</v>
+      <c r="H82">
+        <v>0.28</v>
       </c>
       <c r="K82">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="L82">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="M82">
         <v>200</v>
       </c>
+      <c r="N82" t="s">
+        <v>33</v>
+      </c>
+      <c r="O82">
+        <v>0.15</v>
+      </c>
+      <c r="P82">
+        <v>0.18</v>
+      </c>
       <c r="Q82">
-        <v>5670200000</v>
+        <v>7568900000</v>
       </c>
       <c r="R82" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="83" spans="1:18">
@@ -3678,23 +3675,32 @@
       <c r="B83" t="s">
         <v>192</v>
       </c>
-      <c r="I83">
-        <v>0.48</v>
+      <c r="H83">
+        <v>0.28</v>
       </c>
       <c r="K83">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="L83">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="M83">
         <v>200</v>
       </c>
+      <c r="N83" t="s">
+        <v>37</v>
+      </c>
+      <c r="O83">
+        <v>0.15</v>
+      </c>
+      <c r="P83">
+        <v>0.18</v>
+      </c>
       <c r="Q83">
-        <v>5670200000</v>
+        <v>7568900000</v>
       </c>
       <c r="R83" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="84" spans="1:18">
@@ -3704,9 +3710,6 @@
       <c r="B84" t="s">
         <v>194</v>
       </c>
-      <c r="H84">
-        <v>0.28</v>
-      </c>
       <c r="K84">
         <v>600</v>
       </c>
@@ -3717,7 +3720,7 @@
         <v>200</v>
       </c>
       <c r="N84" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="O84">
         <v>0.15</v>
@@ -3739,29 +3742,26 @@
       <c r="B85" t="s">
         <v>196</v>
       </c>
-      <c r="H85">
-        <v>0.28</v>
-      </c>
       <c r="K85">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="L85">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="M85">
         <v>200</v>
       </c>
       <c r="N85" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="O85">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="P85">
-        <v>0.18</v>
+        <v>0.3</v>
       </c>
       <c r="Q85">
-        <v>7568900000</v>
+        <v>10670900000</v>
       </c>
       <c r="R85" t="s">
         <v>34</v>
@@ -3775,25 +3775,25 @@
         <v>198</v>
       </c>
       <c r="K86">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="L86">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="M86">
         <v>200</v>
       </c>
       <c r="N86" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="O86">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="P86">
-        <v>0.18</v>
+        <v>0.3</v>
       </c>
       <c r="Q86">
-        <v>7568900000</v>
+        <v>10670900000</v>
       </c>
       <c r="R86" t="s">
         <v>34</v>
@@ -3816,7 +3816,7 @@
         <v>200</v>
       </c>
       <c r="N87" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="O87">
         <v>0.25</v>
@@ -3848,7 +3848,7 @@
         <v>200</v>
       </c>
       <c r="N88" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="O88">
         <v>0.25</v>
@@ -3874,19 +3874,19 @@
         <v>700</v>
       </c>
       <c r="L89">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="M89">
         <v>200</v>
       </c>
       <c r="N89" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="O89">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="P89">
-        <v>0.3</v>
+        <v>0.28</v>
       </c>
       <c r="Q89">
         <v>10670900000</v>
@@ -3906,19 +3906,19 @@
         <v>700</v>
       </c>
       <c r="L90">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="M90">
         <v>200</v>
       </c>
       <c r="N90" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="O90">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="P90">
-        <v>0.3</v>
+        <v>0.28</v>
       </c>
       <c r="Q90">
         <v>10670900000</v>

</xml_diff>

<commit_message>
Updated items, fixed a few last minute bugs
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -1,37 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1C4729-DA4D-BF44-8B1B-16B363A3E263}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Affixes" sheetId="1" r:id="rId1"/>
+    <sheet name="Affixes" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" forceFullCalc="1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="93">
   <si>
     <t>name</t>
   </si>
@@ -96,15 +80,18 @@
     <t>Balance your energies and feel on top of the world.</t>
   </si>
   <si>
+    <t>prefix</t>
+  </si>
+  <si>
+    <t>Fighters Strength</t>
+  </si>
+  <si>
+    <t>Sometimes all you need is a little extra strength</t>
+  </si>
+  <si>
     <t>suffix</t>
   </si>
   <si>
-    <t>Fighters Strength</t>
-  </si>
-  <si>
-    <t>Sometimes all you need is a little extra strength</t>
-  </si>
-  <si>
     <t>Archers Bane</t>
   </si>
   <si>
@@ -307,17 +294,19 @@
   </si>
   <si>
     <t>If you pray, I shall give you hope. If you listen, I shall guide you.</t>
-  </si>
-  <si>
-    <t>prefix</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -328,37 +317,28 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -648,33 +628,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="180" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="180" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="18" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="19" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="15" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="23" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="8" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -733,7 +720,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -741,25 +728,25 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="D2">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="E2">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="F2">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="G2">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="H2">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="I2">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="J2">
         <v>0.1</v>
@@ -780,10 +767,10 @@
         <v>500</v>
       </c>
       <c r="S2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -791,7 +778,7 @@
         <v>23</v>
       </c>
       <c r="F3">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -815,18 +802,18 @@
         <v>500</v>
       </c>
       <c r="S3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H4">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="K4">
         <v>10</v>
@@ -844,18 +831,18 @@
         <v>500</v>
       </c>
       <c r="S4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="K5">
         <v>10</v>
@@ -873,18 +860,18 @@
         <v>500</v>
       </c>
       <c r="S5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J6">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="K6">
         <v>10</v>
@@ -902,18 +889,18 @@
         <v>500</v>
       </c>
       <c r="S6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I7">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="K7">
         <v>10</v>
@@ -931,39 +918,39 @@
         <v>500</v>
       </c>
       <c r="S7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8">
-        <v>0.22</v>
+        <v>0.05</v>
       </c>
       <c r="D8">
-        <v>0.22</v>
+        <v>0.05</v>
       </c>
       <c r="E8">
-        <v>0.22</v>
+        <v>0.05</v>
       </c>
       <c r="F8">
-        <v>0.22</v>
+        <v>0.05</v>
       </c>
       <c r="G8">
-        <v>0.22</v>
+        <v>0.05</v>
       </c>
       <c r="H8">
-        <v>0.22</v>
+        <v>0.05</v>
       </c>
       <c r="I8">
-        <v>0.22</v>
+        <v>0.05</v>
       </c>
       <c r="J8">
-        <v>0.22</v>
+        <v>0.05</v>
       </c>
       <c r="K8">
         <v>30</v>
@@ -974,25 +961,22 @@
       <c r="M8">
         <v>20</v>
       </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
       <c r="R8">
         <v>10000</v>
       </c>
       <c r="S8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F9">
-        <v>0.3</v>
+        <v>0.07</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1015,25 +999,22 @@
       <c r="M9">
         <v>20</v>
       </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
       <c r="R9">
         <v>10000</v>
       </c>
       <c r="S9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H10">
-        <v>0.3</v>
+        <v>0.07</v>
       </c>
       <c r="K10">
         <v>30</v>
@@ -1044,25 +1025,22 @@
       <c r="M10">
         <v>20</v>
       </c>
-      <c r="Q10">
-        <v>1</v>
-      </c>
       <c r="R10">
         <v>10000</v>
       </c>
       <c r="S10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G11">
-        <v>0.3</v>
+        <v>0.07</v>
       </c>
       <c r="K11">
         <v>30</v>
@@ -1073,25 +1051,22 @@
       <c r="M11">
         <v>20</v>
       </c>
-      <c r="Q11">
-        <v>1</v>
-      </c>
       <c r="R11">
         <v>10000</v>
       </c>
       <c r="S11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J12">
-        <v>0.3</v>
+        <v>0.07</v>
       </c>
       <c r="K12">
         <v>30</v>
@@ -1102,25 +1077,22 @@
       <c r="M12">
         <v>20</v>
       </c>
-      <c r="Q12">
-        <v>1</v>
-      </c>
       <c r="R12">
         <v>10000</v>
       </c>
       <c r="S12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I13">
-        <v>0.3</v>
+        <v>0.07</v>
       </c>
       <c r="K13">
         <v>30</v>
@@ -1131,46 +1103,43 @@
       <c r="M13">
         <v>20</v>
       </c>
-      <c r="Q13">
-        <v>1</v>
-      </c>
       <c r="R13">
         <v>10000</v>
       </c>
       <c r="S13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14">
-        <v>0.24</v>
+        <v>0.08</v>
       </c>
       <c r="D14">
-        <v>0.24</v>
+        <v>0.08</v>
       </c>
       <c r="E14">
-        <v>0.24</v>
+        <v>0.08</v>
       </c>
       <c r="F14">
-        <v>0.24</v>
+        <v>0.08</v>
       </c>
       <c r="G14">
-        <v>0.24</v>
+        <v>0.08</v>
       </c>
       <c r="H14">
-        <v>0.24</v>
+        <v>0.08</v>
       </c>
       <c r="I14">
-        <v>0.24</v>
+        <v>0.08</v>
       </c>
       <c r="J14">
-        <v>0.24</v>
+        <v>0.08</v>
       </c>
       <c r="K14">
         <v>80</v>
@@ -1181,25 +1150,22 @@
       <c r="M14">
         <v>60</v>
       </c>
-      <c r="Q14">
-        <v>1</v>
-      </c>
       <c r="R14">
         <v>500000</v>
       </c>
       <c r="S14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F15">
-        <v>0.35</v>
+        <v>0.1</v>
       </c>
       <c r="K15">
         <v>90</v>
@@ -1210,25 +1176,22 @@
       <c r="M15">
         <v>70</v>
       </c>
-      <c r="Q15">
-        <v>1</v>
-      </c>
       <c r="R15">
         <v>700000</v>
       </c>
       <c r="S15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H16">
-        <v>0.35</v>
+        <v>0.1</v>
       </c>
       <c r="K16">
         <v>90</v>
@@ -1239,25 +1202,22 @@
       <c r="M16">
         <v>70</v>
       </c>
-      <c r="Q16">
-        <v>1</v>
-      </c>
       <c r="R16">
         <v>700000</v>
       </c>
       <c r="S16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G17">
-        <v>0.35</v>
+        <v>0.1</v>
       </c>
       <c r="K17">
         <v>90</v>
@@ -1268,25 +1228,22 @@
       <c r="M17">
         <v>70</v>
       </c>
-      <c r="Q17">
-        <v>1</v>
-      </c>
       <c r="R17">
         <v>700000</v>
       </c>
       <c r="S17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J18">
-        <v>0.35</v>
+        <v>0.1</v>
       </c>
       <c r="K18">
         <v>90</v>
@@ -1297,25 +1254,22 @@
       <c r="M18">
         <v>70</v>
       </c>
-      <c r="Q18">
-        <v>1</v>
-      </c>
       <c r="R18">
         <v>700000</v>
       </c>
       <c r="S18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I19">
-        <v>0.35</v>
+        <v>0.1</v>
       </c>
       <c r="K19">
         <v>90</v>
@@ -1326,46 +1280,43 @@
       <c r="M19">
         <v>70</v>
       </c>
-      <c r="Q19">
-        <v>1</v>
-      </c>
       <c r="R19">
         <v>700000</v>
       </c>
       <c r="S19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20">
-        <v>0.28000000000000003</v>
+        <v>0.1</v>
       </c>
       <c r="D20">
-        <v>0.28000000000000003</v>
+        <v>0.1</v>
       </c>
       <c r="E20">
-        <v>0.28000000000000003</v>
+        <v>0.1</v>
       </c>
       <c r="F20">
-        <v>0.28000000000000003</v>
+        <v>0.1</v>
       </c>
       <c r="G20">
-        <v>0.28000000000000003</v>
+        <v>0.1</v>
       </c>
       <c r="H20">
-        <v>0.28000000000000003</v>
+        <v>0.1</v>
       </c>
       <c r="I20">
-        <v>0.28000000000000003</v>
+        <v>0.1</v>
       </c>
       <c r="J20">
-        <v>0.28000000000000003</v>
+        <v>0.1</v>
       </c>
       <c r="K20">
         <v>170</v>
@@ -1380,18 +1331,18 @@
         <v>5000000</v>
       </c>
       <c r="S20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F21">
-        <v>0.38</v>
+        <v>0.11</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -1415,18 +1366,18 @@
         <v>10500000</v>
       </c>
       <c r="S21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H22">
-        <v>0.38</v>
+        <v>0.11</v>
       </c>
       <c r="K22">
         <v>200</v>
@@ -1441,18 +1392,18 @@
         <v>10500000</v>
       </c>
       <c r="S22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G23">
-        <v>0.38</v>
+        <v>0.11</v>
       </c>
       <c r="K23">
         <v>200</v>
@@ -1467,18 +1418,18 @@
         <v>10500000</v>
       </c>
       <c r="S23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J24">
-        <v>0.38</v>
+        <v>0.11</v>
       </c>
       <c r="K24">
         <v>200</v>
@@ -1493,18 +1444,18 @@
         <v>10500000</v>
       </c>
       <c r="S24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I25">
-        <v>0.38</v>
+        <v>0.11</v>
       </c>
       <c r="K25">
         <v>200</v>
@@ -1519,39 +1470,39 @@
         <v>10500000</v>
       </c>
       <c r="S25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C26">
-        <v>0.34</v>
+        <v>0.12</v>
       </c>
       <c r="D26">
-        <v>0.34</v>
+        <v>0.12</v>
       </c>
       <c r="E26">
-        <v>0.34</v>
+        <v>0.12</v>
       </c>
       <c r="F26">
-        <v>0.34</v>
+        <v>0.12</v>
       </c>
       <c r="G26">
-        <v>0.34</v>
+        <v>0.12</v>
       </c>
       <c r="H26">
-        <v>0.34</v>
+        <v>0.12</v>
       </c>
       <c r="I26">
-        <v>0.34</v>
+        <v>0.12</v>
       </c>
       <c r="J26">
-        <v>0.34</v>
+        <v>0.12</v>
       </c>
       <c r="K26">
         <v>300</v>
@@ -1566,18 +1517,18 @@
         <v>125400000</v>
       </c>
       <c r="S26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F27">
-        <v>0.44</v>
+        <v>0.15</v>
       </c>
       <c r="K27">
         <v>350</v>
@@ -1592,18 +1543,18 @@
         <v>340600000</v>
       </c>
       <c r="S27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H28">
-        <v>0.44</v>
+        <v>0.15</v>
       </c>
       <c r="K28">
         <v>350</v>
@@ -1618,18 +1569,18 @@
         <v>340600000</v>
       </c>
       <c r="S28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G29">
-        <v>0.44</v>
+        <v>0.15</v>
       </c>
       <c r="K29">
         <v>350</v>
@@ -1644,18 +1595,18 @@
         <v>340600000</v>
       </c>
       <c r="S29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J30">
-        <v>0.44</v>
+        <v>0.15</v>
       </c>
       <c r="K30">
         <v>350</v>
@@ -1670,18 +1621,18 @@
         <v>340600000</v>
       </c>
       <c r="S30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I31">
-        <v>0.44</v>
+        <v>0.15</v>
       </c>
       <c r="K31">
         <v>350</v>
@@ -1696,39 +1647,39 @@
         <v>340600000</v>
       </c>
       <c r="S31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C32">
-        <v>0.38</v>
+        <v>0.15</v>
       </c>
       <c r="D32">
-        <v>0.38</v>
+        <v>0.15</v>
       </c>
       <c r="E32">
-        <v>0.38</v>
+        <v>0.15</v>
       </c>
       <c r="F32">
-        <v>0.38</v>
+        <v>0.15</v>
       </c>
       <c r="G32">
-        <v>0.38</v>
+        <v>0.15</v>
       </c>
       <c r="H32">
-        <v>0.38</v>
+        <v>0.15</v>
       </c>
       <c r="I32">
-        <v>0.38</v>
+        <v>0.15</v>
       </c>
       <c r="J32">
-        <v>0.38</v>
+        <v>0.15</v>
       </c>
       <c r="K32">
         <v>500</v>
@@ -1743,18 +1694,18 @@
         <v>2600980000</v>
       </c>
       <c r="S32" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F33">
-        <v>0.48</v>
+        <v>0.17</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1781,18 +1732,18 @@
         <v>5670200000</v>
       </c>
       <c r="S33" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B34" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H34">
-        <v>0.48</v>
+        <v>0.17</v>
       </c>
       <c r="K34">
         <v>500</v>
@@ -1807,18 +1758,18 @@
         <v>5670200000</v>
       </c>
       <c r="S34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G35">
-        <v>0.48</v>
+        <v>0.17</v>
       </c>
       <c r="K35">
         <v>500</v>
@@ -1833,18 +1784,18 @@
         <v>5670200000</v>
       </c>
       <c r="S35" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J36">
-        <v>0.48</v>
+        <v>0.17</v>
       </c>
       <c r="K36">
         <v>500</v>
@@ -1859,18 +1810,18 @@
         <v>5670200000</v>
       </c>
       <c r="S36" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I37">
-        <v>0.48</v>
+        <v>0.17</v>
       </c>
       <c r="K37">
         <v>500</v>
@@ -1885,12 +1836,21 @@
         <v>5670200000</v>
       </c>
       <c r="S37" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed market issues, added a couple new affixes
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="103">
   <si>
     <t>name</t>
   </si>
@@ -294,6 +294,36 @@
   </si>
   <si>
     <t>If you pray, I shall give you hope. If you listen, I shall guide you.</t>
+  </si>
+  <si>
+    <t>Shadow Fiend Lover</t>
+  </si>
+  <si>
+    <t>Feel the strength of a shadow fiend crawling through the veins of your body.</t>
+  </si>
+  <si>
+    <t>Dark Thoughts</t>
+  </si>
+  <si>
+    <t>These thoughts are drifting through your head all the time. What can you do about it?</t>
+  </si>
+  <si>
+    <t>Fiathless Hate</t>
+  </si>
+  <si>
+    <t>There is nothing worse then the hatefilled vengance of the faithless.</t>
+  </si>
+  <si>
+    <t>Demonic Pact</t>
+  </si>
+  <si>
+    <t>Make a demonic pact for the stats you want. Trust, it always works.</t>
+  </si>
+  <si>
+    <t>Shadow Sands Dust</t>
+  </si>
+  <si>
+    <t>The curse of the shadow suns is one far too long to tell child, alas it will fill you with the magic you need.</t>
   </si>
 </sst>
 </file>
@@ -632,7 +662,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1511,7 +1541,7 @@
         <v>75</v>
       </c>
       <c r="M26">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="R26">
         <v>125400000</v>
@@ -1837,6 +1867,172 @@
       </c>
       <c r="S37" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
+      <c r="A38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38">
+        <v>0.05</v>
+      </c>
+      <c r="D38">
+        <v>0.05</v>
+      </c>
+      <c r="E38">
+        <v>0.05</v>
+      </c>
+      <c r="K38">
+        <v>15</v>
+      </c>
+      <c r="L38">
+        <v>3</v>
+      </c>
+      <c r="M38">
+        <v>8</v>
+      </c>
+      <c r="Q38">
+        <v>1</v>
+      </c>
+      <c r="R38">
+        <v>750</v>
+      </c>
+      <c r="S38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
+      <c r="A39" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39">
+        <v>0.08</v>
+      </c>
+      <c r="D39">
+        <v>0.08</v>
+      </c>
+      <c r="E39">
+        <v>0.08</v>
+      </c>
+      <c r="K39">
+        <v>35</v>
+      </c>
+      <c r="L39">
+        <v>15</v>
+      </c>
+      <c r="M39">
+        <v>30</v>
+      </c>
+      <c r="Q39">
+        <v>1</v>
+      </c>
+      <c r="R39">
+        <v>7000</v>
+      </c>
+      <c r="S39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
+      <c r="A40" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40">
+        <v>0.1</v>
+      </c>
+      <c r="D40">
+        <v>0.1</v>
+      </c>
+      <c r="E40">
+        <v>0.1</v>
+      </c>
+      <c r="K40">
+        <v>38</v>
+      </c>
+      <c r="L40">
+        <v>15</v>
+      </c>
+      <c r="M40">
+        <v>30</v>
+      </c>
+      <c r="R40">
+        <v>100000</v>
+      </c>
+      <c r="S40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
+      <c r="A41" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41">
+        <v>0.15</v>
+      </c>
+      <c r="D41">
+        <v>0.15</v>
+      </c>
+      <c r="E41">
+        <v>0.15</v>
+      </c>
+      <c r="K41">
+        <v>250</v>
+      </c>
+      <c r="L41">
+        <v>65</v>
+      </c>
+      <c r="M41">
+        <v>165</v>
+      </c>
+      <c r="R41">
+        <v>20300000</v>
+      </c>
+      <c r="S41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19">
+      <c r="A42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42">
+        <v>0.18</v>
+      </c>
+      <c r="D42">
+        <v>0.18</v>
+      </c>
+      <c r="E42">
+        <v>0.18</v>
+      </c>
+      <c r="K42">
+        <v>400</v>
+      </c>
+      <c r="L42">
+        <v>90</v>
+      </c>
+      <c r="M42">
+        <v>200</v>
+      </c>
+      <c r="R42">
+        <v>440500000</v>
+      </c>
+      <c r="S42" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
We can now export and import skills.
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -1,37 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A63D53-00EE-5F4A-8095-6938D55C22C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Affixes" sheetId="1" r:id="rId1"/>
+    <sheet name="Affixes" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" forceFullCalc="1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="147">
   <si>
     <t>name</t>
   </si>
@@ -171,7 +155,19 @@
     <t>Do you have the courage to keep fighting? Time is running out child.</t>
   </si>
   <si>
-    <t>Fighters Courage</t>
+    <t>Fighters Resilience</t>
+  </si>
+  <si>
+    <t>Archbishops Prayer</t>
+  </si>
+  <si>
+    <t>The Archbishop once prayed for the end to a nasty plague. His prayer was answered when they stopped dying. But they're was a side effect, they all rose.</t>
+  </si>
+  <si>
+    <t>Life Stealer</t>
+  </si>
+  <si>
+    <t>Steal the soul and life right out of your enemy.</t>
   </si>
   <si>
     <t>Natures Balancing Bliss</t>
@@ -180,34 +176,46 @@
     <t>Nature has a way of balancing it's self out, and those around it.</t>
   </si>
   <si>
-    <t>Archbishops Prayer</t>
-  </si>
-  <si>
-    <t>The Archbishop once prayed for the end to a nasty plague. His prayer was answered when they stopped dying. But they're was a side effect, they all rose.</t>
-  </si>
-  <si>
     <t>Sorcerers Magic</t>
   </si>
   <si>
     <t>Sorcerers are strange beings, wickedly intelligent and born of dragon magic, they're intelligence will inspire you.</t>
   </si>
   <si>
+    <t>Soldiers Resilance</t>
+  </si>
+  <si>
+    <t>Let the strength of a soldier, seasoned with war, flow through you.</t>
+  </si>
+  <si>
     <t>Hawk Eye</t>
   </si>
   <si>
     <t>See the enemy from miles away, see them better then they see them selves.</t>
   </si>
   <si>
-    <t>Life Stealer</t>
-  </si>
-  <si>
-    <t>Steal the soul and life right out of your enemy.</t>
-  </si>
-  <si>
-    <t>Soldiers Resilance</t>
-  </si>
-  <si>
-    <t>Let the strength of a soldier, seasoned with war, flow through you.</t>
+    <t>Dark Thoughts</t>
+  </si>
+  <si>
+    <t>These thoughts are drifting through your head all the time. What can you do about it?</t>
+  </si>
+  <si>
+    <t>Winds Movement</t>
+  </si>
+  <si>
+    <t>Let the winds move you out of the way child.</t>
+  </si>
+  <si>
+    <t>Devils Deliverence</t>
+  </si>
+  <si>
+    <t>Let the devil deliver this aim child!</t>
+  </si>
+  <si>
+    <t>Shadow Soldier</t>
+  </si>
+  <si>
+    <t>The time to die is not now. Fight faster child! Fight harder!</t>
   </si>
   <si>
     <t>Blessed Treasures</t>
@@ -216,82 +224,64 @@
     <t>Want more loot child? Time to get your self one of these bad boys!</t>
   </si>
   <si>
-    <t>Winds Movement</t>
-  </si>
-  <si>
-    <t>Let the winds move you out of the way child.</t>
-  </si>
-  <si>
-    <t>Devils Deliverence</t>
-  </si>
-  <si>
-    <t>Let the devil deliver this aim child!</t>
-  </si>
-  <si>
-    <t>Shadow Soldier</t>
-  </si>
-  <si>
-    <t>The time to die is not now. Fight faster child! Fight harder!</t>
-  </si>
-  <si>
-    <t>Dark Thoughts</t>
-  </si>
-  <si>
-    <t>These thoughts are drifting through your head all the time. What can you do about it?</t>
-  </si>
-  <si>
     <t>Fiathless Hate</t>
   </si>
   <si>
     <t>There is nothing worse then the hatefilled vengance of the faithless.</t>
   </si>
   <si>
+    <t>Devli's Stance</t>
+  </si>
+  <si>
+    <t>Take a stance before the devil! Ask for less time!</t>
+  </si>
+  <si>
+    <t>Angelic Arrow</t>
+  </si>
+  <si>
+    <t>Never let the enemy see you fail. Failing is missing. never miss.</t>
+  </si>
+  <si>
+    <t>Bards Dance</t>
+  </si>
+  <si>
+    <t>Dance your way out of this situation child!</t>
+  </si>
+  <si>
     <t>Thieves Eyes</t>
   </si>
   <si>
     <t>See gold do you? Smell it can you?</t>
   </si>
   <si>
-    <t>Bards Dance</t>
-  </si>
-  <si>
-    <t>Dance your way out of this situation child!</t>
-  </si>
-  <si>
-    <t>Angelic Arrow</t>
-  </si>
-  <si>
-    <t>Never let the enemy see you fail. Failing is missing. never miss.</t>
-  </si>
-  <si>
-    <t>Devli's Stance</t>
-  </si>
-  <si>
-    <t>Take a stance before the devil! Ask for less time!</t>
-  </si>
-  <si>
     <t>Queens Blessing</t>
   </si>
   <si>
     <t>The Queen Has given her blessing child, the blessing of hope.</t>
   </si>
   <si>
+    <t>Priests Vow</t>
+  </si>
+  <si>
+    <t>Take the vow and let the lord be the one true light.</t>
+  </si>
+  <si>
+    <t>Deaths Magic Spell</t>
+  </si>
+  <si>
+    <t>Gives more and more every time you use it. But takes more and more too.</t>
+  </si>
+  <si>
     <t>Vampires Hope</t>
   </si>
   <si>
     <t>Give hope to the creatures of death. Give hope to them.</t>
   </si>
   <si>
-    <t>Deaths Magic Spell</t>
-  </si>
-  <si>
-    <t>Gives more and more every time you use it. But takes more and more too.</t>
-  </si>
-  <si>
-    <t>Priests Vow</t>
-  </si>
-  <si>
-    <t>Take the vow and let the lord be the one true light.</t>
+    <t>Rangers Sight</t>
+  </si>
+  <si>
+    <t>With the rangers sight you will never forget, not will you lose your way.</t>
   </si>
   <si>
     <t>Knights Blessing</t>
@@ -300,12 +290,6 @@
     <t>The blessing of strength and courage lie upon this item.</t>
   </si>
   <si>
-    <t>Rangers Sight</t>
-  </si>
-  <si>
-    <t>With the rangers sight you will never forget, not will you lose your way.</t>
-  </si>
-  <si>
     <t>Dragons Treasure</t>
   </si>
   <si>
@@ -336,12 +320,42 @@
     <t>Make a wish and it might come true. This spell is powerful on the right item.</t>
   </si>
   <si>
+    <t>Fates Blessing</t>
+  </si>
+  <si>
+    <t>fate be with you child. Let the hands of time move faster.</t>
+  </si>
+  <si>
+    <t>Shattered Illusions</t>
+  </si>
+  <si>
+    <t>To get better at accuracy, you must train child. Do you hear? Train.</t>
+  </si>
+  <si>
+    <t>Lifes Dance</t>
+  </si>
+  <si>
+    <t>Dance to the song of life child.</t>
+  </si>
+  <si>
+    <t>Lost and Found</t>
+  </si>
+  <si>
+    <t>What was once lost is now found.</t>
+  </si>
+  <si>
     <t>Gladiators Win</t>
   </si>
   <si>
     <t>Feel the strength given to you by the crowd as they cheer you on!</t>
   </si>
   <si>
+    <t>Faith In The Aim</t>
+  </si>
+  <si>
+    <t>Have some faith child.</t>
+  </si>
+  <si>
     <t>Blood Fever</t>
   </si>
   <si>
@@ -358,36 +372,6 @@
   </si>
   <si>
     <t>Have faith in the Lord of Light and you shall prevail</t>
-  </si>
-  <si>
-    <t>Faith In The Aim</t>
-  </si>
-  <si>
-    <t>Have some faith child.</t>
-  </si>
-  <si>
-    <t>Fates Blessing</t>
-  </si>
-  <si>
-    <t>fate be with you child. Let the hands of time move faster.</t>
-  </si>
-  <si>
-    <t>Shattered Illusions</t>
-  </si>
-  <si>
-    <t>To get better at accuracy, you must train child. Do you hear? Train.</t>
-  </si>
-  <si>
-    <t>Lifes Dance</t>
-  </si>
-  <si>
-    <t>Dance to the song of life child.</t>
-  </si>
-  <si>
-    <t>Lost and Found</t>
-  </si>
-  <si>
-    <t>What was once lost is now found.</t>
   </si>
   <si>
     <t>Demonic Pact</t>
@@ -477,9 +461,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -490,37 +479,28 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -810,33 +790,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="180" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="180" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="18" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="19" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="15" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="23" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="23" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="8" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -895,7 +882,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -905,6 +892,12 @@
       <c r="F2">
         <v>0.05</v>
       </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
       <c r="K2">
         <v>10</v>
       </c>
@@ -924,7 +917,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -953,7 +946,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -982,7 +975,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1011,7 +1004,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1040,7 +1033,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1090,7 +1083,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1125,7 +1118,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1157,7 +1150,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1189,7 +1182,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1221,7 +1214,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1253,36 +1246,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
         <v>47</v>
       </c>
       <c r="B13" t="s">
         <v>48</v>
       </c>
-      <c r="C13">
-        <v>0.05</v>
-      </c>
-      <c r="D13">
-        <v>0.05</v>
-      </c>
-      <c r="E13">
-        <v>0.05</v>
-      </c>
-      <c r="F13">
-        <v>0.05</v>
-      </c>
-      <c r="G13">
-        <v>0.05</v>
-      </c>
-      <c r="H13">
-        <v>0.05</v>
-      </c>
       <c r="I13">
-        <v>0.05</v>
-      </c>
-      <c r="J13">
-        <v>0.05</v>
+        <v>0.07</v>
       </c>
       <c r="K13">
         <v>30</v>
@@ -1297,18 +1269,18 @@
         <v>10000</v>
       </c>
       <c r="S13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>49</v>
       </c>
       <c r="B14" t="s">
         <v>50</v>
       </c>
-      <c r="I14">
-        <v>7.0000000000000007E-2</v>
+      <c r="G14">
+        <v>0.07</v>
       </c>
       <c r="K14">
         <v>30</v>
@@ -1326,15 +1298,36 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
         <v>51</v>
       </c>
       <c r="B15" t="s">
         <v>52</v>
       </c>
+      <c r="C15">
+        <v>0.05</v>
+      </c>
+      <c r="D15">
+        <v>0.05</v>
+      </c>
+      <c r="E15">
+        <v>0.05</v>
+      </c>
+      <c r="F15">
+        <v>0.05</v>
+      </c>
+      <c r="G15">
+        <v>0.05</v>
+      </c>
+      <c r="H15">
+        <v>0.05</v>
+      </c>
+      <c r="I15">
+        <v>0.05</v>
+      </c>
       <c r="J15">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="K15">
         <v>30</v>
@@ -1349,18 +1342,18 @@
         <v>10000</v>
       </c>
       <c r="S15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
         <v>53</v>
       </c>
       <c r="B16" t="s">
         <v>54</v>
       </c>
-      <c r="H16">
-        <v>7.0000000000000007E-2</v>
+      <c r="J16">
+        <v>0.07</v>
       </c>
       <c r="K16">
         <v>30</v>
@@ -1378,15 +1371,27 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19">
       <c r="A17" t="s">
         <v>55</v>
       </c>
       <c r="B17" t="s">
         <v>56</v>
       </c>
+      <c r="F17">
+        <v>0.07</v>
+      </c>
       <c r="G17">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
       </c>
       <c r="K17">
         <v>30</v>
@@ -1404,27 +1409,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19">
       <c r="A18" t="s">
         <v>57</v>
       </c>
       <c r="B18" t="s">
         <v>58</v>
       </c>
-      <c r="F18">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
       <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
+        <v>0.07</v>
       </c>
       <c r="K18">
         <v>30</v>
@@ -1442,39 +1435,42 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19">
       <c r="A19" t="s">
         <v>59</v>
       </c>
       <c r="B19" t="s">
         <v>60</v>
       </c>
+      <c r="C19">
+        <v>0.08</v>
+      </c>
+      <c r="D19">
+        <v>0.08</v>
+      </c>
+      <c r="E19">
+        <v>0.08</v>
+      </c>
       <c r="K19">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="L19">
         <v>15</v>
       </c>
       <c r="M19">
-        <v>45</v>
-      </c>
-      <c r="N19" t="s">
-        <v>37</v>
-      </c>
-      <c r="O19">
-        <v>2E-3</v>
-      </c>
-      <c r="P19">
-        <v>0.08</v>
+        <v>30</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
       </c>
       <c r="R19">
-        <v>1500</v>
+        <v>7000</v>
       </c>
       <c r="S19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -1494,7 +1490,7 @@
         <v>40</v>
       </c>
       <c r="O20">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="P20">
         <v>0.08</v>
@@ -1506,7 +1502,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -1526,7 +1522,7 @@
         <v>43</v>
       </c>
       <c r="O21">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="P21">
         <v>0.08</v>
@@ -1538,7 +1534,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -1558,7 +1554,7 @@
         <v>46</v>
       </c>
       <c r="O22">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="P22">
         <v>0.08</v>
@@ -1570,42 +1566,39 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19">
       <c r="A23" t="s">
         <v>67</v>
       </c>
       <c r="B23" t="s">
         <v>68</v>
       </c>
-      <c r="C23">
-        <v>0.08</v>
-      </c>
-      <c r="D23">
-        <v>0.08</v>
-      </c>
-      <c r="E23">
-        <v>0.08</v>
-      </c>
       <c r="K23">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="L23">
         <v>15</v>
       </c>
       <c r="M23">
-        <v>30</v>
-      </c>
-      <c r="Q23">
-        <v>1</v>
+        <v>45</v>
+      </c>
+      <c r="N23" t="s">
+        <v>37</v>
+      </c>
+      <c r="O23">
+        <v>0.002</v>
+      </c>
+      <c r="P23">
+        <v>0.08</v>
       </c>
       <c r="R23">
-        <v>7000</v>
+        <v>1500</v>
       </c>
       <c r="S23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1637,7 +1630,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1654,10 +1647,10 @@
         <v>60</v>
       </c>
       <c r="N25" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="O25">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="P25">
         <v>0.1</v>
@@ -1669,7 +1662,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -1686,10 +1679,10 @@
         <v>60</v>
       </c>
       <c r="N26" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="O26">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="P26">
         <v>0.1</v>
@@ -1701,7 +1694,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19">
       <c r="A27" t="s">
         <v>75</v>
       </c>
@@ -1718,10 +1711,10 @@
         <v>60</v>
       </c>
       <c r="N27" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="O27">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="P27">
         <v>0.1</v>
@@ -1733,7 +1726,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -1750,10 +1743,10 @@
         <v>60</v>
       </c>
       <c r="N28" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="O28">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="P28">
         <v>0.1</v>
@@ -1765,7 +1758,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19">
       <c r="A29" t="s">
         <v>79</v>
       </c>
@@ -1812,14 +1805,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19">
       <c r="A30" t="s">
         <v>81</v>
       </c>
       <c r="B30" t="s">
         <v>82</v>
       </c>
-      <c r="G30">
+      <c r="I30">
         <v>0.1</v>
       </c>
       <c r="K30">
@@ -1838,7 +1831,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19">
       <c r="A31" t="s">
         <v>83</v>
       </c>
@@ -1864,14 +1857,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19">
       <c r="A32" t="s">
         <v>85</v>
       </c>
       <c r="B32" t="s">
         <v>86</v>
       </c>
-      <c r="I32">
+      <c r="G32">
         <v>0.1</v>
       </c>
       <c r="K32">
@@ -1890,14 +1883,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19">
       <c r="A33" t="s">
         <v>87</v>
       </c>
       <c r="B33" t="s">
         <v>88</v>
       </c>
-      <c r="F33">
+      <c r="H33">
         <v>0.1</v>
       </c>
       <c r="K33">
@@ -1916,14 +1909,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19">
       <c r="A34" t="s">
         <v>89</v>
       </c>
       <c r="B34" t="s">
         <v>90</v>
       </c>
-      <c r="H34">
+      <c r="F34">
         <v>0.1</v>
       </c>
       <c r="K34">
@@ -1942,7 +1935,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -1962,7 +1955,7 @@
         <v>37</v>
       </c>
       <c r="O35">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="P35">
         <v>0.12</v>
@@ -1974,7 +1967,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19">
       <c r="A36" t="s">
         <v>93</v>
       </c>
@@ -1994,7 +1987,7 @@
         <v>40</v>
       </c>
       <c r="O36">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="P36">
         <v>0.12</v>
@@ -2006,7 +1999,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19">
       <c r="A37" t="s">
         <v>95</v>
       </c>
@@ -2026,7 +2019,7 @@
         <v>43</v>
       </c>
       <c r="O37">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="P37">
         <v>0.12</v>
@@ -2038,7 +2031,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -2058,7 +2051,7 @@
         <v>46</v>
       </c>
       <c r="O38">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="P38">
         <v>0.12</v>
@@ -2070,7 +2063,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19">
       <c r="A39" t="s">
         <v>99</v>
       </c>
@@ -2117,128 +2110,152 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19">
       <c r="A40" t="s">
         <v>101</v>
       </c>
       <c r="B40" t="s">
         <v>102</v>
       </c>
-      <c r="F40">
-        <v>0.11</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
       <c r="K40">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="L40">
         <v>60</v>
       </c>
       <c r="M40">
-        <v>160</v>
+        <v>100</v>
+      </c>
+      <c r="N40" t="s">
+        <v>46</v>
+      </c>
+      <c r="O40">
+        <v>0.01</v>
+      </c>
+      <c r="P40">
+        <v>0.14</v>
       </c>
       <c r="R40">
-        <v>10500000</v>
+        <v>2600000</v>
       </c>
       <c r="S40" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
       <c r="A41" t="s">
         <v>103</v>
       </c>
       <c r="B41" t="s">
         <v>104</v>
       </c>
-      <c r="G41">
-        <v>0.11</v>
-      </c>
       <c r="K41">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="L41">
         <v>60</v>
       </c>
       <c r="M41">
-        <v>160</v>
+        <v>100</v>
+      </c>
+      <c r="N41" t="s">
+        <v>43</v>
+      </c>
+      <c r="O41">
+        <v>0.01</v>
+      </c>
+      <c r="P41">
+        <v>0.14</v>
       </c>
       <c r="R41">
-        <v>10500000</v>
+        <v>2600000</v>
       </c>
       <c r="S41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19">
       <c r="A42" t="s">
         <v>105</v>
       </c>
       <c r="B42" t="s">
         <v>106</v>
       </c>
-      <c r="J42">
-        <v>0.11</v>
-      </c>
       <c r="K42">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="L42">
         <v>60</v>
       </c>
       <c r="M42">
-        <v>160</v>
+        <v>100</v>
+      </c>
+      <c r="N42" t="s">
+        <v>40</v>
+      </c>
+      <c r="O42">
+        <v>0.01</v>
+      </c>
+      <c r="P42">
+        <v>0.14</v>
       </c>
       <c r="R42">
-        <v>10500000</v>
+        <v>2600000</v>
       </c>
       <c r="S42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19">
       <c r="A43" t="s">
         <v>107</v>
       </c>
       <c r="B43" t="s">
         <v>108</v>
       </c>
-      <c r="I43">
-        <v>0.11</v>
-      </c>
       <c r="K43">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="L43">
         <v>60</v>
       </c>
       <c r="M43">
-        <v>160</v>
+        <v>100</v>
+      </c>
+      <c r="N43" t="s">
+        <v>37</v>
+      </c>
+      <c r="O43">
+        <v>0.01</v>
+      </c>
+      <c r="P43">
+        <v>0.14</v>
       </c>
       <c r="R43">
-        <v>10500000</v>
+        <v>2600000</v>
       </c>
       <c r="S43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
       <c r="A44" t="s">
         <v>109</v>
       </c>
       <c r="B44" t="s">
         <v>110</v>
       </c>
+      <c r="F44">
+        <v>0.11</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
       <c r="H44">
-        <v>0.11</v>
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
       </c>
       <c r="K44">
         <v>200</v>
@@ -2256,135 +2273,111 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19">
       <c r="A45" t="s">
         <v>111</v>
       </c>
       <c r="B45" t="s">
         <v>112</v>
       </c>
+      <c r="H45">
+        <v>0.11</v>
+      </c>
       <c r="K45">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="L45">
         <v>60</v>
       </c>
       <c r="M45">
-        <v>100</v>
-      </c>
-      <c r="N45" t="s">
-        <v>46</v>
-      </c>
-      <c r="O45">
-        <v>0.01</v>
-      </c>
-      <c r="P45">
-        <v>0.14000000000000001</v>
+        <v>160</v>
       </c>
       <c r="R45">
-        <v>2600000</v>
+        <v>10500000</v>
       </c>
       <c r="S45" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19">
       <c r="A46" t="s">
         <v>113</v>
       </c>
       <c r="B46" t="s">
         <v>114</v>
       </c>
+      <c r="G46">
+        <v>0.11</v>
+      </c>
       <c r="K46">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="L46">
         <v>60</v>
       </c>
       <c r="M46">
-        <v>100</v>
-      </c>
-      <c r="N46" t="s">
-        <v>43</v>
-      </c>
-      <c r="O46">
-        <v>0.01</v>
-      </c>
-      <c r="P46">
-        <v>0.14000000000000001</v>
+        <v>160</v>
       </c>
       <c r="R46">
-        <v>2600000</v>
+        <v>10500000</v>
       </c>
       <c r="S46" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47" t="s">
         <v>115</v>
       </c>
       <c r="B47" t="s">
         <v>116</v>
       </c>
+      <c r="J47">
+        <v>0.11</v>
+      </c>
       <c r="K47">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="L47">
         <v>60</v>
       </c>
       <c r="M47">
-        <v>100</v>
-      </c>
-      <c r="N47" t="s">
-        <v>40</v>
-      </c>
-      <c r="O47">
-        <v>0.01</v>
-      </c>
-      <c r="P47">
-        <v>0.14000000000000001</v>
+        <v>160</v>
       </c>
       <c r="R47">
-        <v>2600000</v>
+        <v>10500000</v>
       </c>
       <c r="S47" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19">
       <c r="A48" t="s">
         <v>117</v>
       </c>
       <c r="B48" t="s">
         <v>118</v>
       </c>
+      <c r="I48">
+        <v>0.11</v>
+      </c>
       <c r="K48">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="L48">
         <v>60</v>
       </c>
       <c r="M48">
-        <v>100</v>
-      </c>
-      <c r="N48" t="s">
-        <v>37</v>
-      </c>
-      <c r="O48">
-        <v>0.01</v>
-      </c>
-      <c r="P48">
-        <v>0.14000000000000001</v>
+        <v>160</v>
       </c>
       <c r="R48">
-        <v>2600000</v>
+        <v>10500000</v>
       </c>
       <c r="S48" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19">
       <c r="A49" t="s">
         <v>119</v>
       </c>
@@ -2416,7 +2409,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19">
       <c r="A50" t="s">
         <v>121</v>
       </c>
@@ -2463,7 +2456,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:19">
       <c r="A51" t="s">
         <v>123</v>
       </c>
@@ -2489,7 +2482,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:19">
       <c r="A52" t="s">
         <v>125</v>
       </c>
@@ -2515,7 +2508,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:19">
       <c r="A53" t="s">
         <v>127</v>
       </c>
@@ -2541,7 +2534,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:19">
       <c r="A54" t="s">
         <v>129</v>
       </c>
@@ -2567,7 +2560,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:19">
       <c r="A55" t="s">
         <v>131</v>
       </c>
@@ -2593,7 +2586,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:19">
       <c r="A56" t="s">
         <v>133</v>
       </c>
@@ -2625,7 +2618,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:19">
       <c r="A57" t="s">
         <v>135</v>
       </c>
@@ -2672,7 +2665,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:19">
       <c r="A58" t="s">
         <v>137</v>
       </c>
@@ -2710,7 +2703,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:19">
       <c r="A59" t="s">
         <v>139</v>
       </c>
@@ -2736,7 +2729,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:19">
       <c r="A60" t="s">
         <v>141</v>
       </c>
@@ -2762,7 +2755,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:19">
       <c r="A61" t="s">
         <v>143</v>
       </c>
@@ -2788,7 +2781,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:19">
       <c r="A62" t="s">
         <v>145</v>
       </c>
@@ -2815,8 +2808,17 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pulled down the latest versions of the exports.
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -1202,7 +1202,7 @@
         <v>43</v>
       </c>
       <c r="P11">
-        <v>0.3</v>
+        <v>0.03</v>
       </c>
       <c r="Q11">
         <v>1</v>
@@ -1459,9 +1459,6 @@
       </c>
       <c r="M19">
         <v>30</v>
-      </c>
-      <c r="Q19">
-        <v>1</v>
       </c>
       <c r="R19">
         <v>7000</v>

</xml_diff>

<commit_message>
Started working on price and monster adjustments.
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -1,21 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7423937A-942D-4049-9724-14BEC182C504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Affixes" sheetId="1" r:id="rId4"/>
+    <sheet name="Affixes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="147">
   <si>
     <t>name</t>
   </si>
@@ -158,70 +174,118 @@
     <t>Fighters Resilience</t>
   </si>
   <si>
+    <t>Blessed Treasures</t>
+  </si>
+  <si>
+    <t>Want more loot child? Time to get your self one of these bad boys!</t>
+  </si>
+  <si>
+    <t>Shadow Soldier</t>
+  </si>
+  <si>
+    <t>The time to die is not now. Fight faster child! Fight harder!</t>
+  </si>
+  <si>
+    <t>Devils Deliverence</t>
+  </si>
+  <si>
+    <t>Let the devil deliver this aim child!</t>
+  </si>
+  <si>
+    <t>Winds Movement</t>
+  </si>
+  <si>
+    <t>Let the winds move you out of the way child.</t>
+  </si>
+  <si>
+    <t>Dark Thoughts</t>
+  </si>
+  <si>
+    <t>These thoughts are drifting through your head all the time. What can you do about it?</t>
+  </si>
+  <si>
+    <t>Hawk Eye</t>
+  </si>
+  <si>
+    <t>See the enemy from miles away, see them better then they see them selves.</t>
+  </si>
+  <si>
+    <t>Soldiers Resilance</t>
+  </si>
+  <si>
+    <t>Let the strength of a soldier, seasoned with war, flow through you.</t>
+  </si>
+  <si>
+    <t>Sorcerers Magic</t>
+  </si>
+  <si>
+    <t>Sorcerers are strange beings, wickedly intelligent and born of dragon magic, they're intelligence will inspire you.</t>
+  </si>
+  <si>
+    <t>Natures Balancing Bliss</t>
+  </si>
+  <si>
+    <t>Nature has a way of balancing it's self out, and those around it.</t>
+  </si>
+  <si>
+    <t>Life Stealer</t>
+  </si>
+  <si>
+    <t>Steal the soul and life right out of your enemy.</t>
+  </si>
+  <si>
     <t>Archbishops Prayer</t>
   </si>
   <si>
     <t>The Archbishop once prayed for the end to a nasty plague. His prayer was answered when they stopped dying. But they're was a side effect, they all rose.</t>
   </si>
   <si>
-    <t>Life Stealer</t>
-  </si>
-  <si>
-    <t>Steal the soul and life right out of your enemy.</t>
-  </si>
-  <si>
-    <t>Natures Balancing Bliss</t>
-  </si>
-  <si>
-    <t>Nature has a way of balancing it's self out, and those around it.</t>
-  </si>
-  <si>
-    <t>Sorcerers Magic</t>
-  </si>
-  <si>
-    <t>Sorcerers are strange beings, wickedly intelligent and born of dragon magic, they're intelligence will inspire you.</t>
-  </si>
-  <si>
-    <t>Soldiers Resilance</t>
-  </si>
-  <si>
-    <t>Let the strength of a soldier, seasoned with war, flow through you.</t>
-  </si>
-  <si>
-    <t>Hawk Eye</t>
-  </si>
-  <si>
-    <t>See the enemy from miles away, see them better then they see them selves.</t>
-  </si>
-  <si>
-    <t>Dark Thoughts</t>
-  </si>
-  <si>
-    <t>These thoughts are drifting through your head all the time. What can you do about it?</t>
-  </si>
-  <si>
-    <t>Winds Movement</t>
-  </si>
-  <si>
-    <t>Let the winds move you out of the way child.</t>
-  </si>
-  <si>
-    <t>Devils Deliverence</t>
-  </si>
-  <si>
-    <t>Let the devil deliver this aim child!</t>
-  </si>
-  <si>
-    <t>Shadow Soldier</t>
-  </si>
-  <si>
-    <t>The time to die is not now. Fight faster child! Fight harder!</t>
-  </si>
-  <si>
-    <t>Blessed Treasures</t>
-  </si>
-  <si>
-    <t>Want more loot child? Time to get your self one of these bad boys!</t>
+    <t>Devli's Stance</t>
+  </si>
+  <si>
+    <t>Take a stance before the devil! Ask for less time!</t>
+  </si>
+  <si>
+    <t>Angelic Arrow</t>
+  </si>
+  <si>
+    <t>Never let the enemy see you fail. Failing is missing. never miss.</t>
+  </si>
+  <si>
+    <t>Bards Dance</t>
+  </si>
+  <si>
+    <t>Dance your way out of this situation child!</t>
+  </si>
+  <si>
+    <t>Thieves Eyes</t>
+  </si>
+  <si>
+    <t>See gold do you? Smell it can you?</t>
+  </si>
+  <si>
+    <t>Time Mages Blessing</t>
+  </si>
+  <si>
+    <t>Let time be on your side child.</t>
+  </si>
+  <si>
+    <t>Astral Dexterity</t>
+  </si>
+  <si>
+    <t>See.....Hear ..... Feel .... Believe.</t>
+  </si>
+  <si>
+    <t>Dancers Moves</t>
+  </si>
+  <si>
+    <t>Are you a fan of dancing child? I hope so.</t>
+  </si>
+  <si>
+    <t>Dragons Treasure</t>
+  </si>
+  <si>
+    <t>Never miss an opportunity for treasure.</t>
   </si>
   <si>
     <t>Fiathless Hate</t>
@@ -230,118 +294,70 @@
     <t>There is nothing worse then the hatefilled vengance of the faithless.</t>
   </si>
   <si>
-    <t>Devli's Stance</t>
-  </si>
-  <si>
-    <t>Take a stance before the devil! Ask for less time!</t>
-  </si>
-  <si>
-    <t>Angelic Arrow</t>
-  </si>
-  <si>
-    <t>Never let the enemy see you fail. Failing is missing. never miss.</t>
-  </si>
-  <si>
-    <t>Bards Dance</t>
-  </si>
-  <si>
-    <t>Dance your way out of this situation child!</t>
-  </si>
-  <si>
-    <t>Thieves Eyes</t>
-  </si>
-  <si>
-    <t>See gold do you? Smell it can you?</t>
-  </si>
-  <si>
     <t>Queens Blessing</t>
   </si>
   <si>
     <t>The Queen Has given her blessing child, the blessing of hope.</t>
   </si>
   <si>
+    <t>Knights Blessing</t>
+  </si>
+  <si>
+    <t>The blessing of strength and courage lie upon this item.</t>
+  </si>
+  <si>
+    <t>Rangers Sight</t>
+  </si>
+  <si>
+    <t>With the rangers sight you will never forget, not will you lose your way.</t>
+  </si>
+  <si>
+    <t>Vampires Hope</t>
+  </si>
+  <si>
+    <t>Give hope to the creatures of death. Give hope to them.</t>
+  </si>
+  <si>
+    <t>Deaths Magic Spell</t>
+  </si>
+  <si>
+    <t>Gives more and more every time you use it. But takes more and more too.</t>
+  </si>
+  <si>
     <t>Priests Vow</t>
   </si>
   <si>
     <t>Take the vow and let the lord be the one true light.</t>
   </si>
   <si>
-    <t>Deaths Magic Spell</t>
-  </si>
-  <si>
-    <t>Gives more and more every time you use it. But takes more and more too.</t>
-  </si>
-  <si>
-    <t>Vampires Hope</t>
-  </si>
-  <si>
-    <t>Give hope to the creatures of death. Give hope to them.</t>
-  </si>
-  <si>
-    <t>Rangers Sight</t>
-  </si>
-  <si>
-    <t>With the rangers sight you will never forget, not will you lose your way.</t>
-  </si>
-  <si>
-    <t>Knights Blessing</t>
-  </si>
-  <si>
-    <t>The blessing of strength and courage lie upon this item.</t>
-  </si>
-  <si>
-    <t>Dragons Treasure</t>
-  </si>
-  <si>
-    <t>Never miss an opportunity for treasure.</t>
-  </si>
-  <si>
-    <t>Dancers Moves</t>
-  </si>
-  <si>
-    <t>Are you a fan of dancing child? I hope so.</t>
-  </si>
-  <si>
-    <t>Astral Dexterity</t>
-  </si>
-  <si>
-    <t>See.....Hear ..... Feel .... Believe.</t>
-  </si>
-  <si>
-    <t>Time Mages Blessing</t>
-  </si>
-  <si>
-    <t>Let time be on your side child.</t>
+    <t>Fates Blessing</t>
+  </si>
+  <si>
+    <t>fate be with you child. Let the hands of time move faster.</t>
+  </si>
+  <si>
+    <t>Shattered Illusions</t>
+  </si>
+  <si>
+    <t>To get better at accuracy, you must train child. Do you hear? Train.</t>
+  </si>
+  <si>
+    <t>Lifes Dance</t>
+  </si>
+  <si>
+    <t>Dance to the song of life child.</t>
+  </si>
+  <si>
+    <t>Lost and Found</t>
+  </si>
+  <si>
+    <t>What was once lost is now found.</t>
   </si>
   <si>
     <t>Wishing Spell</t>
   </si>
   <si>
     <t>Make a wish and it might come true. This spell is powerful on the right item.</t>
-  </si>
-  <si>
-    <t>Fates Blessing</t>
-  </si>
-  <si>
-    <t>fate be with you child. Let the hands of time move faster.</t>
-  </si>
-  <si>
-    <t>Shattered Illusions</t>
-  </si>
-  <si>
-    <t>To get better at accuracy, you must train child. Do you hear? Train.</t>
-  </si>
-  <si>
-    <t>Lifes Dance</t>
-  </si>
-  <si>
-    <t>Dance to the song of life child.</t>
-  </si>
-  <si>
-    <t>Lost and Found</t>
-  </si>
-  <si>
-    <t>What was once lost is now found.</t>
   </si>
   <si>
     <t>Gladiators Win</t>
@@ -461,14 +477,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -479,28 +490,37 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -790,40 +810,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="180" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="15" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="10" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="12" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="8" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="180" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -882,7 +894,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -911,13 +923,13 @@
         <v>1</v>
       </c>
       <c r="R2">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="S2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -940,13 +952,13 @@
         <v>1</v>
       </c>
       <c r="R3">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="S3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -969,13 +981,13 @@
         <v>1</v>
       </c>
       <c r="R4">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="S4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -998,13 +1010,13 @@
         <v>1</v>
       </c>
       <c r="R5">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="S5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1027,13 +1039,13 @@
         <v>1</v>
       </c>
       <c r="R6">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="S6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1077,13 +1089,13 @@
         <v>1</v>
       </c>
       <c r="R7">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="S7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1112,13 +1124,13 @@
         <v>1</v>
       </c>
       <c r="R8">
-        <v>750</v>
+        <v>350</v>
       </c>
       <c r="S8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1144,13 +1156,13 @@
         <v>1</v>
       </c>
       <c r="R9">
-        <v>780</v>
+        <v>400</v>
       </c>
       <c r="S9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1176,13 +1188,13 @@
         <v>1</v>
       </c>
       <c r="R10">
-        <v>780</v>
+        <v>400</v>
       </c>
       <c r="S10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1202,19 +1214,19 @@
         <v>43</v>
       </c>
       <c r="P11">
-        <v>0.3</v>
+        <v>0.03</v>
       </c>
       <c r="Q11">
         <v>1</v>
       </c>
       <c r="R11">
-        <v>780</v>
+        <v>400</v>
       </c>
       <c r="S11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1240,176 +1252,188 @@
         <v>1</v>
       </c>
       <c r="R12">
-        <v>780</v>
+        <v>400</v>
       </c>
       <c r="S12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>47</v>
       </c>
       <c r="B13" t="s">
         <v>48</v>
       </c>
-      <c r="I13">
-        <v>0.07</v>
-      </c>
       <c r="K13">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="L13">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="M13">
-        <v>20</v>
+        <v>45</v>
+      </c>
+      <c r="N13" t="s">
+        <v>37</v>
+      </c>
+      <c r="O13">
+        <v>2E-3</v>
+      </c>
+      <c r="P13">
+        <v>0.08</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
       </c>
       <c r="R13">
-        <v>10000</v>
+        <v>800</v>
       </c>
       <c r="S13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>49</v>
       </c>
       <c r="B14" t="s">
         <v>50</v>
       </c>
-      <c r="G14">
-        <v>0.07</v>
-      </c>
       <c r="K14">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="L14">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="M14">
-        <v>20</v>
+        <v>45</v>
+      </c>
+      <c r="N14" t="s">
+        <v>46</v>
+      </c>
+      <c r="O14">
+        <v>2E-3</v>
+      </c>
+      <c r="P14">
+        <v>0.08</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
       </c>
       <c r="R14">
-        <v>10000</v>
+        <v>800</v>
       </c>
       <c r="S14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>51</v>
       </c>
       <c r="B15" t="s">
         <v>52</v>
       </c>
-      <c r="C15">
-        <v>0.05</v>
-      </c>
-      <c r="D15">
-        <v>0.05</v>
-      </c>
-      <c r="E15">
-        <v>0.05</v>
-      </c>
-      <c r="F15">
-        <v>0.05</v>
-      </c>
-      <c r="G15">
-        <v>0.05</v>
-      </c>
-      <c r="H15">
-        <v>0.05</v>
-      </c>
-      <c r="I15">
-        <v>0.05</v>
-      </c>
-      <c r="J15">
-        <v>0.05</v>
-      </c>
       <c r="K15">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="L15">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="M15">
-        <v>20</v>
+        <v>45</v>
+      </c>
+      <c r="N15" t="s">
+        <v>43</v>
+      </c>
+      <c r="O15">
+        <v>2E-3</v>
+      </c>
+      <c r="P15">
+        <v>0.08</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
       </c>
       <c r="R15">
-        <v>10000</v>
+        <v>800</v>
       </c>
       <c r="S15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>53</v>
       </c>
       <c r="B16" t="s">
         <v>54</v>
       </c>
-      <c r="J16">
-        <v>0.07</v>
-      </c>
       <c r="K16">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="L16">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="M16">
-        <v>20</v>
+        <v>45</v>
+      </c>
+      <c r="N16" t="s">
+        <v>40</v>
+      </c>
+      <c r="O16">
+        <v>2E-3</v>
+      </c>
+      <c r="P16">
+        <v>0.08</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
       </c>
       <c r="R16">
-        <v>10000</v>
+        <v>800</v>
       </c>
       <c r="S16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>55</v>
       </c>
       <c r="B17" t="s">
         <v>56</v>
       </c>
-      <c r="F17">
-        <v>0.07</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
+      <c r="C17">
+        <v>0.08</v>
+      </c>
+      <c r="D17">
+        <v>0.08</v>
+      </c>
+      <c r="E17">
+        <v>0.08</v>
       </c>
       <c r="K17">
+        <v>35</v>
+      </c>
+      <c r="L17">
+        <v>15</v>
+      </c>
+      <c r="M17">
         <v>30</v>
       </c>
-      <c r="L17">
-        <v>10</v>
-      </c>
-      <c r="M17">
-        <v>20</v>
+      <c r="Q17">
+        <v>1</v>
       </c>
       <c r="R17">
-        <v>10000</v>
+        <v>975</v>
       </c>
       <c r="S17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -1417,7 +1441,7 @@
         <v>58</v>
       </c>
       <c r="H18">
-        <v>0.07</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K18">
         <v>30</v>
@@ -1429,208 +1453,208 @@
         <v>20</v>
       </c>
       <c r="R18">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="S18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>59</v>
       </c>
       <c r="B19" t="s">
         <v>60</v>
       </c>
-      <c r="C19">
-        <v>0.08</v>
-      </c>
-      <c r="D19">
-        <v>0.08</v>
-      </c>
-      <c r="E19">
-        <v>0.08</v>
+      <c r="F19">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
       </c>
       <c r="K19">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="L19">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="M19">
-        <v>30</v>
-      </c>
-      <c r="Q19">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="R19">
-        <v>7000</v>
+        <v>1000</v>
       </c>
       <c r="S19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>61</v>
       </c>
       <c r="B20" t="s">
         <v>62</v>
       </c>
+      <c r="J20">
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="K20">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="L20">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="M20">
-        <v>45</v>
-      </c>
-      <c r="N20" t="s">
-        <v>40</v>
-      </c>
-      <c r="O20">
-        <v>0.002</v>
-      </c>
-      <c r="P20">
-        <v>0.08</v>
+        <v>20</v>
       </c>
       <c r="R20">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="S20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>63</v>
       </c>
       <c r="B21" t="s">
         <v>64</v>
       </c>
+      <c r="C21">
+        <v>0.05</v>
+      </c>
+      <c r="D21">
+        <v>0.05</v>
+      </c>
+      <c r="E21">
+        <v>0.05</v>
+      </c>
+      <c r="F21">
+        <v>0.05</v>
+      </c>
+      <c r="G21">
+        <v>0.05</v>
+      </c>
+      <c r="H21">
+        <v>0.05</v>
+      </c>
+      <c r="I21">
+        <v>0.05</v>
+      </c>
+      <c r="J21">
+        <v>0.05</v>
+      </c>
       <c r="K21">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="L21">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="M21">
-        <v>45</v>
-      </c>
-      <c r="N21" t="s">
-        <v>43</v>
-      </c>
-      <c r="O21">
-        <v>0.002</v>
-      </c>
-      <c r="P21">
-        <v>0.08</v>
+        <v>20</v>
       </c>
       <c r="R21">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="S21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>65</v>
       </c>
       <c r="B22" t="s">
         <v>66</v>
       </c>
+      <c r="G22">
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="K22">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="L22">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="M22">
-        <v>45</v>
-      </c>
-      <c r="N22" t="s">
-        <v>46</v>
-      </c>
-      <c r="O22">
-        <v>0.002</v>
-      </c>
-      <c r="P22">
-        <v>0.08</v>
+        <v>20</v>
       </c>
       <c r="R22">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="S22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>67</v>
       </c>
       <c r="B23" t="s">
         <v>68</v>
       </c>
+      <c r="I23">
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="K23">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="L23">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="M23">
-        <v>45</v>
-      </c>
-      <c r="N23" t="s">
-        <v>37</v>
-      </c>
-      <c r="O23">
-        <v>0.002</v>
-      </c>
-      <c r="P23">
-        <v>0.08</v>
+        <v>20</v>
       </c>
       <c r="R23">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="S23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>69</v>
       </c>
       <c r="B24" t="s">
         <v>70</v>
       </c>
-      <c r="C24">
+      <c r="K24">
+        <v>150</v>
+      </c>
+      <c r="L24">
+        <v>25</v>
+      </c>
+      <c r="M24">
+        <v>60</v>
+      </c>
+      <c r="N24" t="s">
+        <v>46</v>
+      </c>
+      <c r="O24">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="P24">
         <v>0.1</v>
       </c>
-      <c r="D24">
-        <v>0.1</v>
-      </c>
-      <c r="E24">
-        <v>0.1</v>
-      </c>
-      <c r="K24">
-        <v>38</v>
-      </c>
-      <c r="L24">
-        <v>15</v>
-      </c>
-      <c r="M24">
-        <v>30</v>
-      </c>
       <c r="R24">
-        <v>100000</v>
+        <v>2500</v>
       </c>
       <c r="S24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1647,22 +1671,22 @@
         <v>60</v>
       </c>
       <c r="N25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="O25">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="P25">
         <v>0.1</v>
       </c>
       <c r="R25">
-        <v>35000</v>
+        <v>2500</v>
       </c>
       <c r="S25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -1679,22 +1703,22 @@
         <v>60</v>
       </c>
       <c r="N26" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="O26">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="P26">
         <v>0.1</v>
       </c>
       <c r="R26">
-        <v>35000</v>
+        <v>2500</v>
       </c>
       <c r="S26" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>75</v>
       </c>
@@ -1711,22 +1735,22 @@
         <v>60</v>
       </c>
       <c r="N27" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="O27">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="P27">
         <v>0.1</v>
       </c>
       <c r="R27">
-        <v>35000</v>
+        <v>2500</v>
       </c>
       <c r="S27" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -1734,182 +1758,206 @@
         <v>78</v>
       </c>
       <c r="K28">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="L28">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="M28">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="N28" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="O28">
-        <v>0.005</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="P28">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="R28">
-        <v>35000</v>
+        <v>3800</v>
       </c>
       <c r="S28" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>79</v>
       </c>
       <c r="B29" t="s">
         <v>80</v>
       </c>
-      <c r="C29">
-        <v>0.08</v>
-      </c>
-      <c r="D29">
-        <v>0.08</v>
-      </c>
-      <c r="E29">
-        <v>0.08</v>
-      </c>
-      <c r="F29">
-        <v>0.08</v>
-      </c>
-      <c r="G29">
-        <v>0.08</v>
-      </c>
-      <c r="H29">
-        <v>0.08</v>
-      </c>
-      <c r="I29">
-        <v>0.08</v>
-      </c>
-      <c r="J29">
-        <v>0.08</v>
-      </c>
       <c r="K29">
+        <v>300</v>
+      </c>
+      <c r="L29">
+        <v>45</v>
+      </c>
+      <c r="M29">
         <v>80</v>
       </c>
-      <c r="L29">
-        <v>30</v>
-      </c>
-      <c r="M29">
-        <v>60</v>
+      <c r="N29" t="s">
+        <v>43</v>
+      </c>
+      <c r="O29">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="P29">
+        <v>0.12</v>
       </c>
       <c r="R29">
-        <v>500000</v>
+        <v>3800</v>
       </c>
       <c r="S29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>81</v>
       </c>
       <c r="B30" t="s">
         <v>82</v>
       </c>
-      <c r="I30">
-        <v>0.1</v>
-      </c>
       <c r="K30">
-        <v>90</v>
+        <v>300</v>
       </c>
       <c r="L30">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="M30">
-        <v>70</v>
+        <v>80</v>
+      </c>
+      <c r="N30" t="s">
+        <v>40</v>
+      </c>
+      <c r="O30">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="P30">
+        <v>0.12</v>
       </c>
       <c r="R30">
-        <v>700000</v>
+        <v>3800</v>
       </c>
       <c r="S30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>83</v>
       </c>
       <c r="B31" t="s">
         <v>84</v>
       </c>
-      <c r="J31">
-        <v>0.1</v>
-      </c>
       <c r="K31">
-        <v>90</v>
+        <v>300</v>
       </c>
       <c r="L31">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="M31">
-        <v>70</v>
+        <v>80</v>
+      </c>
+      <c r="N31" t="s">
+        <v>37</v>
+      </c>
+      <c r="O31">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="P31">
+        <v>0.12</v>
       </c>
       <c r="R31">
-        <v>700000</v>
+        <v>3800</v>
       </c>
       <c r="S31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>85</v>
       </c>
       <c r="B32" t="s">
         <v>86</v>
       </c>
-      <c r="G32">
+      <c r="C32">
         <v>0.1</v>
       </c>
+      <c r="D32">
+        <v>0.1</v>
+      </c>
+      <c r="E32">
+        <v>0.1</v>
+      </c>
       <c r="K32">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="L32">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="M32">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="R32">
-        <v>700000</v>
+        <v>5000</v>
       </c>
       <c r="S32" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>87</v>
       </c>
       <c r="B33" t="s">
         <v>88</v>
       </c>
+      <c r="C33">
+        <v>0.08</v>
+      </c>
+      <c r="D33">
+        <v>0.08</v>
+      </c>
+      <c r="E33">
+        <v>0.08</v>
+      </c>
+      <c r="F33">
+        <v>0.08</v>
+      </c>
+      <c r="G33">
+        <v>0.08</v>
+      </c>
       <c r="H33">
-        <v>0.1</v>
+        <v>0.08</v>
+      </c>
+      <c r="I33">
+        <v>0.08</v>
+      </c>
+      <c r="J33">
+        <v>0.08</v>
       </c>
       <c r="K33">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="L33">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="M33">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="R33">
-        <v>700000</v>
+        <v>5000</v>
       </c>
       <c r="S33" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>89</v>
       </c>
@@ -1929,188 +1977,149 @@
         <v>70</v>
       </c>
       <c r="R34">
-        <v>700000</v>
+        <v>6000</v>
       </c>
       <c r="S34" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:19">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>91</v>
       </c>
       <c r="B35" t="s">
         <v>92</v>
       </c>
+      <c r="H35">
+        <v>0.1</v>
+      </c>
       <c r="K35">
-        <v>300</v>
+        <v>90</v>
       </c>
       <c r="L35">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="M35">
-        <v>80</v>
-      </c>
-      <c r="N35" t="s">
-        <v>37</v>
-      </c>
-      <c r="O35">
-        <v>0.008</v>
-      </c>
-      <c r="P35">
-        <v>0.12</v>
+        <v>70</v>
       </c>
       <c r="R35">
-        <v>58000</v>
+        <v>6000</v>
       </c>
       <c r="S35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>93</v>
       </c>
       <c r="B36" t="s">
         <v>94</v>
       </c>
+      <c r="G36">
+        <v>0.1</v>
+      </c>
       <c r="K36">
-        <v>300</v>
+        <v>90</v>
       </c>
       <c r="L36">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="M36">
-        <v>80</v>
-      </c>
-      <c r="N36" t="s">
-        <v>40</v>
-      </c>
-      <c r="O36">
-        <v>0.008</v>
-      </c>
-      <c r="P36">
-        <v>0.12</v>
+        <v>70</v>
       </c>
       <c r="R36">
-        <v>58000</v>
+        <v>6000</v>
       </c>
       <c r="S36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>95</v>
       </c>
       <c r="B37" t="s">
         <v>96</v>
       </c>
+      <c r="J37">
+        <v>0.1</v>
+      </c>
       <c r="K37">
-        <v>300</v>
+        <v>90</v>
       </c>
       <c r="L37">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="M37">
-        <v>80</v>
-      </c>
-      <c r="N37" t="s">
-        <v>43</v>
-      </c>
-      <c r="O37">
-        <v>0.008</v>
-      </c>
-      <c r="P37">
-        <v>0.12</v>
+        <v>70</v>
       </c>
       <c r="R37">
-        <v>58000</v>
+        <v>6000</v>
       </c>
       <c r="S37" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>97</v>
       </c>
       <c r="B38" t="s">
         <v>98</v>
       </c>
+      <c r="I38">
+        <v>0.1</v>
+      </c>
       <c r="K38">
-        <v>300</v>
+        <v>90</v>
       </c>
       <c r="L38">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="M38">
-        <v>80</v>
-      </c>
-      <c r="N38" t="s">
-        <v>46</v>
-      </c>
-      <c r="O38">
-        <v>0.008</v>
-      </c>
-      <c r="P38">
-        <v>0.12</v>
+        <v>70</v>
       </c>
       <c r="R38">
-        <v>58000</v>
+        <v>6000</v>
       </c>
       <c r="S38" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>99</v>
       </c>
       <c r="B39" t="s">
         <v>100</v>
       </c>
-      <c r="C39">
-        <v>0.1</v>
-      </c>
-      <c r="D39">
-        <v>0.1</v>
-      </c>
-      <c r="E39">
-        <v>0.1</v>
-      </c>
-      <c r="F39">
-        <v>0.1</v>
-      </c>
-      <c r="G39">
-        <v>0.1</v>
-      </c>
-      <c r="H39">
-        <v>0.1</v>
-      </c>
-      <c r="I39">
-        <v>0.1</v>
-      </c>
-      <c r="J39">
-        <v>0.1</v>
-      </c>
       <c r="K39">
-        <v>170</v>
+        <v>500</v>
       </c>
       <c r="L39">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="M39">
-        <v>150</v>
+        <v>100</v>
+      </c>
+      <c r="N39" t="s">
+        <v>46</v>
+      </c>
+      <c r="O39">
+        <v>0.01</v>
+      </c>
+      <c r="P39">
+        <v>0.14000000000000001</v>
       </c>
       <c r="R39">
-        <v>5000000</v>
+        <v>8000</v>
       </c>
       <c r="S39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:19">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>101</v>
       </c>
@@ -2127,22 +2136,22 @@
         <v>100</v>
       </c>
       <c r="N40" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="O40">
         <v>0.01</v>
       </c>
       <c r="P40">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="R40">
-        <v>2600000</v>
+        <v>8000</v>
       </c>
       <c r="S40" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:19">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>103</v>
       </c>
@@ -2159,22 +2168,22 @@
         <v>100</v>
       </c>
       <c r="N41" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="O41">
         <v>0.01</v>
       </c>
       <c r="P41">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="R41">
-        <v>2600000</v>
+        <v>8000</v>
       </c>
       <c r="S41" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:19">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>105</v>
       </c>
@@ -2191,54 +2200,69 @@
         <v>100</v>
       </c>
       <c r="N42" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="O42">
         <v>0.01</v>
       </c>
       <c r="P42">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="R42">
-        <v>2600000</v>
+        <v>8000</v>
       </c>
       <c r="S42" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:19">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>107</v>
       </c>
       <c r="B43" t="s">
         <v>108</v>
       </c>
+      <c r="C43">
+        <v>0.1</v>
+      </c>
+      <c r="D43">
+        <v>0.1</v>
+      </c>
+      <c r="E43">
+        <v>0.1</v>
+      </c>
+      <c r="F43">
+        <v>0.1</v>
+      </c>
+      <c r="G43">
+        <v>0.1</v>
+      </c>
+      <c r="H43">
+        <v>0.1</v>
+      </c>
+      <c r="I43">
+        <v>0.1</v>
+      </c>
+      <c r="J43">
+        <v>0.1</v>
+      </c>
       <c r="K43">
-        <v>500</v>
+        <v>170</v>
       </c>
       <c r="L43">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="M43">
-        <v>100</v>
-      </c>
-      <c r="N43" t="s">
-        <v>37</v>
-      </c>
-      <c r="O43">
-        <v>0.01</v>
-      </c>
-      <c r="P43">
-        <v>0.14</v>
+        <v>150</v>
       </c>
       <c r="R43">
-        <v>2600000</v>
+        <v>10000</v>
       </c>
       <c r="S43" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:19">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>109</v>
       </c>
@@ -2267,13 +2291,13 @@
         <v>160</v>
       </c>
       <c r="R44">
-        <v>10500000</v>
+        <v>10000</v>
       </c>
       <c r="S44" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:19">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>111</v>
       </c>
@@ -2293,13 +2317,13 @@
         <v>160</v>
       </c>
       <c r="R45">
-        <v>10500000</v>
+        <v>10000</v>
       </c>
       <c r="S45" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:19">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>113</v>
       </c>
@@ -2319,13 +2343,13 @@
         <v>160</v>
       </c>
       <c r="R46">
-        <v>10500000</v>
+        <v>10000</v>
       </c>
       <c r="S46" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:19">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>115</v>
       </c>
@@ -2345,13 +2369,13 @@
         <v>160</v>
       </c>
       <c r="R47">
-        <v>10500000</v>
+        <v>10000</v>
       </c>
       <c r="S47" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:19">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>117</v>
       </c>
@@ -2371,13 +2395,13 @@
         <v>160</v>
       </c>
       <c r="R48">
-        <v>10500000</v>
+        <v>10000</v>
       </c>
       <c r="S48" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:19">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>119</v>
       </c>
@@ -2403,13 +2427,13 @@
         <v>165</v>
       </c>
       <c r="R49">
-        <v>20300000</v>
+        <v>15000</v>
       </c>
       <c r="S49" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:19">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>121</v>
       </c>
@@ -2450,13 +2474,13 @@
         <v>180</v>
       </c>
       <c r="R50">
-        <v>125400000</v>
+        <v>18000</v>
       </c>
       <c r="S50" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:19">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>123</v>
       </c>
@@ -2476,13 +2500,13 @@
         <v>200</v>
       </c>
       <c r="R51">
-        <v>340600000</v>
+        <v>18000</v>
       </c>
       <c r="S51" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:19">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>125</v>
       </c>
@@ -2502,13 +2526,13 @@
         <v>100</v>
       </c>
       <c r="R52">
-        <v>340600000</v>
+        <v>18000</v>
       </c>
       <c r="S52" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:19">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>127</v>
       </c>
@@ -2528,13 +2552,13 @@
         <v>200</v>
       </c>
       <c r="R53">
-        <v>340600000</v>
+        <v>18000</v>
       </c>
       <c r="S53" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:19">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>129</v>
       </c>
@@ -2554,13 +2578,13 @@
         <v>200</v>
       </c>
       <c r="R54">
-        <v>340600000</v>
+        <v>18000</v>
       </c>
       <c r="S54" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:19">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>131</v>
       </c>
@@ -2580,13 +2604,13 @@
         <v>200</v>
       </c>
       <c r="R55">
-        <v>340600000</v>
+        <v>18000</v>
       </c>
       <c r="S55" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:19">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>133</v>
       </c>
@@ -2612,13 +2636,13 @@
         <v>200</v>
       </c>
       <c r="R56">
-        <v>440500000</v>
+        <v>25000</v>
       </c>
       <c r="S56" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:19">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>135</v>
       </c>
@@ -2659,13 +2683,13 @@
         <v>200</v>
       </c>
       <c r="R57">
-        <v>2600980000</v>
+        <v>30000</v>
       </c>
       <c r="S57" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:19">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>137</v>
       </c>
@@ -2697,13 +2721,13 @@
         <v>200</v>
       </c>
       <c r="R58">
-        <v>5670200000</v>
+        <v>30000</v>
       </c>
       <c r="S58" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:19">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>139</v>
       </c>
@@ -2723,13 +2747,13 @@
         <v>200</v>
       </c>
       <c r="R59">
-        <v>5670200000</v>
+        <v>30000</v>
       </c>
       <c r="S59" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:19">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>141</v>
       </c>
@@ -2749,13 +2773,13 @@
         <v>200</v>
       </c>
       <c r="R60">
-        <v>5670200000</v>
+        <v>30000</v>
       </c>
       <c r="S60" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:19">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>143</v>
       </c>
@@ -2775,13 +2799,13 @@
         <v>200</v>
       </c>
       <c r="R61">
-        <v>5670200000</v>
+        <v>30000</v>
       </c>
       <c r="S61" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:19">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>145</v>
       </c>
@@ -2801,24 +2825,15 @@
         <v>200</v>
       </c>
       <c r="R62">
-        <v>5670200000</v>
+        <v>30000</v>
       </c>
       <c r="S62" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated items, affixes and monsters.
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7423937A-942D-4049-9724-14BEC182C504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B7A2A9-49A3-424C-BD28-579AF9E54F16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="Y60" sqref="Y60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -923,7 +923,7 @@
         <v>1</v>
       </c>
       <c r="R2">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="S2" t="s">
         <v>21</v>
@@ -952,7 +952,7 @@
         <v>1</v>
       </c>
       <c r="R3">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="S3" t="s">
         <v>21</v>
@@ -981,7 +981,7 @@
         <v>1</v>
       </c>
       <c r="R4">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="S4" t="s">
         <v>21</v>
@@ -1010,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="R5">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="S5" t="s">
         <v>21</v>
@@ -1039,7 +1039,7 @@
         <v>1</v>
       </c>
       <c r="R6">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="S6" t="s">
         <v>21</v>
@@ -1089,7 +1089,7 @@
         <v>1</v>
       </c>
       <c r="R7">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="S7" t="s">
         <v>32</v>
@@ -1124,7 +1124,7 @@
         <v>1</v>
       </c>
       <c r="R8">
-        <v>350</v>
+        <v>750</v>
       </c>
       <c r="S8" t="s">
         <v>32</v>
@@ -1156,7 +1156,7 @@
         <v>1</v>
       </c>
       <c r="R9">
-        <v>400</v>
+        <v>1500</v>
       </c>
       <c r="S9" t="s">
         <v>32</v>
@@ -1188,7 +1188,7 @@
         <v>1</v>
       </c>
       <c r="R10">
-        <v>400</v>
+        <v>1500</v>
       </c>
       <c r="S10" t="s">
         <v>32</v>
@@ -1220,7 +1220,7 @@
         <v>1</v>
       </c>
       <c r="R11">
-        <v>400</v>
+        <v>1500</v>
       </c>
       <c r="S11" t="s">
         <v>32</v>
@@ -1252,7 +1252,7 @@
         <v>1</v>
       </c>
       <c r="R12">
-        <v>400</v>
+        <v>1500</v>
       </c>
       <c r="S12" t="s">
         <v>32</v>
@@ -1287,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="R13">
-        <v>800</v>
+        <v>3000</v>
       </c>
       <c r="S13" t="s">
         <v>32</v>
@@ -1322,7 +1322,7 @@
         <v>1</v>
       </c>
       <c r="R14">
-        <v>800</v>
+        <v>3000</v>
       </c>
       <c r="S14" t="s">
         <v>32</v>
@@ -1357,7 +1357,7 @@
         <v>1</v>
       </c>
       <c r="R15">
-        <v>800</v>
+        <v>3000</v>
       </c>
       <c r="S15" t="s">
         <v>32</v>
@@ -1392,7 +1392,7 @@
         <v>1</v>
       </c>
       <c r="R16">
-        <v>800</v>
+        <v>3000</v>
       </c>
       <c r="S16" t="s">
         <v>32</v>
@@ -1427,7 +1427,7 @@
         <v>1</v>
       </c>
       <c r="R17">
-        <v>975</v>
+        <v>5000</v>
       </c>
       <c r="S17" t="s">
         <v>32</v>
@@ -1453,7 +1453,7 @@
         <v>20</v>
       </c>
       <c r="R18">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="S18" t="s">
         <v>21</v>
@@ -1491,7 +1491,7 @@
         <v>20</v>
       </c>
       <c r="R19">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="S19" t="s">
         <v>21</v>
@@ -1517,7 +1517,7 @@
         <v>20</v>
       </c>
       <c r="R20">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="S20" t="s">
         <v>21</v>
@@ -1564,7 +1564,7 @@
         <v>20</v>
       </c>
       <c r="R21">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="S21" t="s">
         <v>32</v>
@@ -1590,7 +1590,7 @@
         <v>20</v>
       </c>
       <c r="R22">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="S22" t="s">
         <v>21</v>
@@ -1616,7 +1616,7 @@
         <v>20</v>
       </c>
       <c r="R23">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="S23" t="s">
         <v>21</v>
@@ -1648,7 +1648,7 @@
         <v>0.1</v>
       </c>
       <c r="R24">
-        <v>2500</v>
+        <v>25000</v>
       </c>
       <c r="S24" t="s">
         <v>32</v>
@@ -1680,7 +1680,7 @@
         <v>0.1</v>
       </c>
       <c r="R25">
-        <v>2500</v>
+        <v>25000</v>
       </c>
       <c r="S25" t="s">
         <v>32</v>
@@ -1712,7 +1712,7 @@
         <v>0.1</v>
       </c>
       <c r="R26">
-        <v>2500</v>
+        <v>25000</v>
       </c>
       <c r="S26" t="s">
         <v>32</v>
@@ -1744,7 +1744,7 @@
         <v>0.1</v>
       </c>
       <c r="R27">
-        <v>2500</v>
+        <v>25000</v>
       </c>
       <c r="S27" t="s">
         <v>32</v>
@@ -1776,7 +1776,7 @@
         <v>0.12</v>
       </c>
       <c r="R28">
-        <v>3800</v>
+        <v>50000</v>
       </c>
       <c r="S28" t="s">
         <v>32</v>
@@ -1808,7 +1808,7 @@
         <v>0.12</v>
       </c>
       <c r="R29">
-        <v>3800</v>
+        <v>50000</v>
       </c>
       <c r="S29" t="s">
         <v>32</v>
@@ -1840,7 +1840,7 @@
         <v>0.12</v>
       </c>
       <c r="R30">
-        <v>3800</v>
+        <v>50000</v>
       </c>
       <c r="S30" t="s">
         <v>32</v>
@@ -1872,7 +1872,7 @@
         <v>0.12</v>
       </c>
       <c r="R31">
-        <v>3800</v>
+        <v>50000</v>
       </c>
       <c r="S31" t="s">
         <v>32</v>
@@ -1904,7 +1904,7 @@
         <v>30</v>
       </c>
       <c r="R32">
-        <v>5000</v>
+        <v>100000</v>
       </c>
       <c r="S32" t="s">
         <v>32</v>
@@ -1951,7 +1951,7 @@
         <v>60</v>
       </c>
       <c r="R33">
-        <v>5000</v>
+        <v>100000</v>
       </c>
       <c r="S33" t="s">
         <v>32</v>
@@ -1977,7 +1977,7 @@
         <v>70</v>
       </c>
       <c r="R34">
-        <v>6000</v>
+        <v>150000</v>
       </c>
       <c r="S34" t="s">
         <v>21</v>
@@ -2003,7 +2003,7 @@
         <v>70</v>
       </c>
       <c r="R35">
-        <v>6000</v>
+        <v>150000</v>
       </c>
       <c r="S35" t="s">
         <v>21</v>
@@ -2029,7 +2029,7 @@
         <v>70</v>
       </c>
       <c r="R36">
-        <v>6000</v>
+        <v>150000</v>
       </c>
       <c r="S36" t="s">
         <v>21</v>
@@ -2055,7 +2055,7 @@
         <v>70</v>
       </c>
       <c r="R37">
-        <v>6000</v>
+        <v>150000</v>
       </c>
       <c r="S37" t="s">
         <v>21</v>
@@ -2081,7 +2081,7 @@
         <v>70</v>
       </c>
       <c r="R38">
-        <v>6000</v>
+        <v>150000</v>
       </c>
       <c r="S38" t="s">
         <v>21</v>
@@ -2113,7 +2113,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="R39">
-        <v>8000</v>
+        <v>300000</v>
       </c>
       <c r="S39" t="s">
         <v>32</v>
@@ -2145,7 +2145,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="R40">
-        <v>8000</v>
+        <v>300000</v>
       </c>
       <c r="S40" t="s">
         <v>32</v>
@@ -2177,7 +2177,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="R41">
-        <v>8000</v>
+        <v>300000</v>
       </c>
       <c r="S41" t="s">
         <v>32</v>
@@ -2209,7 +2209,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="R42">
-        <v>8000</v>
+        <v>300000</v>
       </c>
       <c r="S42" t="s">
         <v>32</v>
@@ -2256,7 +2256,7 @@
         <v>150</v>
       </c>
       <c r="R43">
-        <v>10000</v>
+        <v>500000</v>
       </c>
       <c r="S43" t="s">
         <v>32</v>
@@ -2291,7 +2291,7 @@
         <v>160</v>
       </c>
       <c r="R44">
-        <v>10000</v>
+        <v>500000</v>
       </c>
       <c r="S44" t="s">
         <v>21</v>
@@ -2317,7 +2317,7 @@
         <v>160</v>
       </c>
       <c r="R45">
-        <v>10000</v>
+        <v>500000</v>
       </c>
       <c r="S45" t="s">
         <v>21</v>
@@ -2343,7 +2343,7 @@
         <v>160</v>
       </c>
       <c r="R46">
-        <v>10000</v>
+        <v>500000</v>
       </c>
       <c r="S46" t="s">
         <v>21</v>
@@ -2369,7 +2369,7 @@
         <v>160</v>
       </c>
       <c r="R47">
-        <v>10000</v>
+        <v>500000</v>
       </c>
       <c r="S47" t="s">
         <v>21</v>
@@ -2395,7 +2395,7 @@
         <v>160</v>
       </c>
       <c r="R48">
-        <v>10000</v>
+        <v>500000</v>
       </c>
       <c r="S48" t="s">
         <v>21</v>
@@ -2427,7 +2427,7 @@
         <v>165</v>
       </c>
       <c r="R49">
-        <v>15000</v>
+        <v>750000</v>
       </c>
       <c r="S49" t="s">
         <v>32</v>
@@ -2474,7 +2474,7 @@
         <v>180</v>
       </c>
       <c r="R50">
-        <v>18000</v>
+        <v>750000</v>
       </c>
       <c r="S50" t="s">
         <v>32</v>
@@ -2500,7 +2500,7 @@
         <v>200</v>
       </c>
       <c r="R51">
-        <v>18000</v>
+        <v>750000</v>
       </c>
       <c r="S51" t="s">
         <v>21</v>
@@ -2526,7 +2526,7 @@
         <v>100</v>
       </c>
       <c r="R52">
-        <v>18000</v>
+        <v>750000</v>
       </c>
       <c r="S52" t="s">
         <v>21</v>
@@ -2552,7 +2552,7 @@
         <v>200</v>
       </c>
       <c r="R53">
-        <v>18000</v>
+        <v>750000</v>
       </c>
       <c r="S53" t="s">
         <v>21</v>
@@ -2578,7 +2578,7 @@
         <v>200</v>
       </c>
       <c r="R54">
-        <v>18000</v>
+        <v>750000</v>
       </c>
       <c r="S54" t="s">
         <v>21</v>
@@ -2604,7 +2604,7 @@
         <v>200</v>
       </c>
       <c r="R55">
-        <v>18000</v>
+        <v>750000</v>
       </c>
       <c r="S55" t="s">
         <v>21</v>
@@ -2636,7 +2636,7 @@
         <v>200</v>
       </c>
       <c r="R56">
-        <v>25000</v>
+        <v>1000000</v>
       </c>
       <c r="S56" t="s">
         <v>32</v>
@@ -2683,7 +2683,7 @@
         <v>200</v>
       </c>
       <c r="R57">
-        <v>30000</v>
+        <v>5000000</v>
       </c>
       <c r="S57" t="s">
         <v>32</v>
@@ -2721,7 +2721,7 @@
         <v>200</v>
       </c>
       <c r="R58">
-        <v>30000</v>
+        <v>5000000</v>
       </c>
       <c r="S58" t="s">
         <v>21</v>
@@ -2747,7 +2747,7 @@
         <v>200</v>
       </c>
       <c r="R59">
-        <v>30000</v>
+        <v>5000000</v>
       </c>
       <c r="S59" t="s">
         <v>21</v>
@@ -2773,7 +2773,7 @@
         <v>200</v>
       </c>
       <c r="R60">
-        <v>30000</v>
+        <v>5000000</v>
       </c>
       <c r="S60" t="s">
         <v>21</v>
@@ -2799,7 +2799,7 @@
         <v>200</v>
       </c>
       <c r="R61">
-        <v>30000</v>
+        <v>5000000</v>
       </c>
       <c r="S61" t="s">
         <v>21</v>
@@ -2825,7 +2825,7 @@
         <v>200</v>
       </c>
       <c r="R62">
-        <v>30000</v>
+        <v>5000000</v>
       </c>
       <c r="S62" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Minor fix and data import updates
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -1,37 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/1.1.0/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6316F594-923E-3E49-8AEE-C289DE8499CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Affixes" sheetId="1" r:id="rId1"/>
+    <sheet name="Affixes" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" forceFullCalc="1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="384">
   <si>
     <t>name</t>
   </si>
@@ -1188,9 +1172,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1201,37 +1190,28 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -1521,38 +1501,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:AA171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="R45" sqref="R45"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="225" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="23" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="29" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="28" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="225" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="18" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="19" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="15" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="23" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="23" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="22" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="25" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="26" bestFit="true" customWidth="true" style="0"/>
+    <col min="22" max="22" width="21" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="29" bestFit="true" customWidth="true" style="0"/>
+    <col min="24" max="24" width="28" bestFit="true" customWidth="true" style="0"/>
+    <col min="25" max="25" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="26" max="26" width="8" bestFit="true" customWidth="true" style="0"/>
+    <col min="27" max="27" width="8" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1635,7 +1625,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1685,7 +1675,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1729,7 +1719,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1773,7 +1763,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1817,7 +1807,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1861,7 +1851,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -1926,7 +1916,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -1979,7 +1969,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -2029,7 +2019,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -2082,7 +2072,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -2120,7 +2110,7 @@
         <v>0</v>
       </c>
       <c r="W11">
-        <v>5.0000000000000001E-4</v>
+        <v>0.0005</v>
       </c>
       <c r="X11">
         <v>0</v>
@@ -2135,7 +2125,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -2173,7 +2163,7 @@
         <v>0</v>
       </c>
       <c r="W12">
-        <v>5.0000000000000001E-4</v>
+        <v>0.0005</v>
       </c>
       <c r="X12">
         <v>0</v>
@@ -2188,7 +2178,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -2241,7 +2231,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -2291,7 +2281,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -2335,7 +2325,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -2372,9 +2362,6 @@
       <c r="X16">
         <v>0</v>
       </c>
-      <c r="Y16">
-        <v>1</v>
-      </c>
       <c r="Z16">
         <v>1500</v>
       </c>
@@ -2382,7 +2369,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -2419,9 +2406,6 @@
       <c r="X17">
         <v>0</v>
       </c>
-      <c r="Y17">
-        <v>1</v>
-      </c>
       <c r="Z17">
         <v>1500</v>
       </c>
@@ -2429,7 +2413,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -2482,7 +2466,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -2532,7 +2516,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -2582,7 +2566,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -2629,7 +2613,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -2667,7 +2651,7 @@
         <v>0</v>
       </c>
       <c r="W22">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="X22">
         <v>0</v>
@@ -2679,7 +2663,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -2717,7 +2701,7 @@
         <v>0</v>
       </c>
       <c r="W23">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="X23">
         <v>0</v>
@@ -2729,7 +2713,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -2769,9 +2753,6 @@
       <c r="X24">
         <v>0</v>
       </c>
-      <c r="Y24">
-        <v>1</v>
-      </c>
       <c r="Z24">
         <v>2000</v>
       </c>
@@ -2779,7 +2760,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27">
       <c r="A25" t="s">
         <v>84</v>
       </c>
@@ -2819,9 +2800,6 @@
       <c r="X25">
         <v>0</v>
       </c>
-      <c r="Y25">
-        <v>1</v>
-      </c>
       <c r="Z25">
         <v>2000</v>
       </c>
@@ -2829,7 +2807,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -2869,9 +2847,6 @@
       <c r="X26">
         <v>0</v>
       </c>
-      <c r="Y26">
-        <v>1</v>
-      </c>
       <c r="Z26">
         <v>2000</v>
       </c>
@@ -2879,7 +2854,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -2919,9 +2894,6 @@
       <c r="X27">
         <v>0</v>
       </c>
-      <c r="Y27">
-        <v>1</v>
-      </c>
       <c r="Z27">
         <v>2000</v>
       </c>
@@ -2929,7 +2901,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -2969,9 +2941,6 @@
       <c r="X28">
         <v>0</v>
       </c>
-      <c r="Y28">
-        <v>1</v>
-      </c>
       <c r="Z28">
         <v>2000</v>
       </c>
@@ -2979,7 +2948,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27">
       <c r="A29" t="s">
         <v>96</v>
       </c>
@@ -3019,9 +2988,6 @@
       <c r="X29">
         <v>0</v>
       </c>
-      <c r="Y29">
-        <v>1</v>
-      </c>
       <c r="Z29">
         <v>2000</v>
       </c>
@@ -3029,7 +2995,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27">
       <c r="A30" t="s">
         <v>99</v>
       </c>
@@ -3037,7 +3003,7 @@
         <v>100</v>
       </c>
       <c r="I30">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="M30">
         <v>30</v>
@@ -3070,7 +3036,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27">
       <c r="A31" t="s">
         <v>101</v>
       </c>
@@ -3078,7 +3044,7 @@
         <v>102</v>
       </c>
       <c r="J31">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="M31">
         <v>30</v>
@@ -3111,7 +3077,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27">
       <c r="A32" t="s">
         <v>103</v>
       </c>
@@ -3119,7 +3085,7 @@
         <v>104</v>
       </c>
       <c r="G32">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="M32">
         <v>30</v>
@@ -3152,7 +3118,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27">
       <c r="A33" t="s">
         <v>105</v>
       </c>
@@ -3160,7 +3126,7 @@
         <v>106</v>
       </c>
       <c r="H33">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="M33">
         <v>30</v>
@@ -3193,7 +3159,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27">
       <c r="A34" t="s">
         <v>107</v>
       </c>
@@ -3201,7 +3167,7 @@
         <v>108</v>
       </c>
       <c r="F34">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -3246,7 +3212,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27">
       <c r="A35" t="s">
         <v>109</v>
       </c>
@@ -3308,7 +3274,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27">
       <c r="A36" t="s">
         <v>111</v>
       </c>
@@ -3358,7 +3324,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27">
       <c r="A37" t="s">
         <v>113</v>
       </c>
@@ -3411,7 +3377,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27">
       <c r="A38" t="s">
         <v>115</v>
       </c>
@@ -3461,7 +3427,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27">
       <c r="A39" t="s">
         <v>117</v>
       </c>
@@ -3499,7 +3465,7 @@
         <v>0</v>
       </c>
       <c r="W39">
-        <v>1.5E-3</v>
+        <v>0.0015</v>
       </c>
       <c r="X39">
         <v>0</v>
@@ -3511,7 +3477,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27">
       <c r="A40" t="s">
         <v>119</v>
       </c>
@@ -3558,7 +3524,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27">
       <c r="A41" t="s">
         <v>121</v>
       </c>
@@ -3596,7 +3562,7 @@
         <v>0</v>
       </c>
       <c r="W41">
-        <v>1.5E-3</v>
+        <v>0.0015</v>
       </c>
       <c r="X41">
         <v>0</v>
@@ -3608,7 +3574,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27">
       <c r="A42" t="s">
         <v>123</v>
       </c>
@@ -3628,7 +3594,7 @@
         <v>68</v>
       </c>
       <c r="R42">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="S42">
         <v>0.05</v>
@@ -3648,9 +3614,6 @@
       <c r="X42">
         <v>0</v>
       </c>
-      <c r="Y42">
-        <v>1</v>
-      </c>
       <c r="Z42">
         <v>3000</v>
       </c>
@@ -3658,7 +3621,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27">
       <c r="A43" t="s">
         <v>125</v>
       </c>
@@ -3678,7 +3641,7 @@
         <v>127</v>
       </c>
       <c r="R43">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="S43">
         <v>0.05</v>
@@ -3698,9 +3661,6 @@
       <c r="X43">
         <v>0</v>
       </c>
-      <c r="Y43">
-        <v>1</v>
-      </c>
       <c r="Z43">
         <v>3000</v>
       </c>
@@ -3708,7 +3668,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27">
       <c r="A44" t="s">
         <v>128</v>
       </c>
@@ -3728,7 +3688,7 @@
         <v>65</v>
       </c>
       <c r="R44">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="S44">
         <v>0.05</v>
@@ -3748,9 +3708,6 @@
       <c r="X44">
         <v>0</v>
       </c>
-      <c r="Y44">
-        <v>1</v>
-      </c>
       <c r="Z44">
         <v>3000</v>
       </c>
@@ -3758,7 +3715,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:27">
       <c r="A45" t="s">
         <v>130</v>
       </c>
@@ -3790,7 +3747,7 @@
         <v>0</v>
       </c>
       <c r="W45">
-        <v>2.0000000000000001E-4</v>
+        <v>0.0002</v>
       </c>
       <c r="X45">
         <v>0</v>
@@ -3802,7 +3759,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:27">
       <c r="A46" t="s">
         <v>132</v>
       </c>
@@ -3849,7 +3806,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:27">
       <c r="A47" t="s">
         <v>134</v>
       </c>
@@ -3896,7 +3853,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:27">
       <c r="A48" t="s">
         <v>136</v>
       </c>
@@ -3946,7 +3903,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27">
       <c r="A49" t="s">
         <v>138</v>
       </c>
@@ -3996,7 +3953,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:27">
       <c r="A50" t="s">
         <v>140</v>
       </c>
@@ -4046,7 +4003,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:27">
       <c r="A51" t="s">
         <v>142</v>
       </c>
@@ -4084,7 +4041,7 @@
         <v>0</v>
       </c>
       <c r="W51">
-        <v>1.8E-3</v>
+        <v>0.0018</v>
       </c>
       <c r="X51">
         <v>0</v>
@@ -4096,7 +4053,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:27">
       <c r="A52" t="s">
         <v>144</v>
       </c>
@@ -4143,7 +4100,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27">
       <c r="A53" t="s">
         <v>146</v>
       </c>
@@ -4181,7 +4138,7 @@
         <v>0</v>
       </c>
       <c r="W53">
-        <v>1.8E-3</v>
+        <v>0.0018</v>
       </c>
       <c r="X53">
         <v>0</v>
@@ -4193,7 +4150,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:27">
       <c r="A54" t="s">
         <v>148</v>
       </c>
@@ -4240,7 +4197,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:27">
       <c r="A55" t="s">
         <v>150</v>
       </c>
@@ -4287,7 +4244,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:27">
       <c r="A56" t="s">
         <v>152</v>
       </c>
@@ -4334,7 +4291,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:27">
       <c r="A57" t="s">
         <v>154</v>
       </c>
@@ -4381,7 +4338,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:27">
       <c r="A58" t="s">
         <v>156</v>
       </c>
@@ -4428,7 +4385,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:27">
       <c r="A59" t="s">
         <v>158</v>
       </c>
@@ -4475,7 +4432,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:27">
       <c r="A60" t="s">
         <v>160</v>
       </c>
@@ -4507,7 +4464,7 @@
         <v>0</v>
       </c>
       <c r="W60">
-        <v>5.0000000000000001E-4</v>
+        <v>0.0005</v>
       </c>
       <c r="X60">
         <v>0</v>
@@ -4519,7 +4476,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:27">
       <c r="A61" t="s">
         <v>162</v>
       </c>
@@ -4539,7 +4496,7 @@
         <v>65</v>
       </c>
       <c r="R61">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="S61">
         <v>0.1</v>
@@ -4566,7 +4523,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:27">
       <c r="A62" t="s">
         <v>164</v>
       </c>
@@ -4586,7 +4543,7 @@
         <v>127</v>
       </c>
       <c r="R62">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="S62">
         <v>0.1</v>
@@ -4613,7 +4570,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:27">
       <c r="A63" t="s">
         <v>166</v>
       </c>
@@ -4633,7 +4590,7 @@
         <v>68</v>
       </c>
       <c r="R63">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="S63">
         <v>0.1</v>
@@ -4660,7 +4617,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:27">
       <c r="A64" t="s">
         <v>168</v>
       </c>
@@ -4707,7 +4664,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:27">
       <c r="A65" t="s">
         <v>170</v>
       </c>
@@ -4754,7 +4711,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:27">
       <c r="A66" t="s">
         <v>172</v>
       </c>
@@ -4801,7 +4758,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:27">
       <c r="A67" t="s">
         <v>174</v>
       </c>
@@ -4848,7 +4805,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:27">
       <c r="A68" t="s">
         <v>176</v>
       </c>
@@ -4895,7 +4852,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:27">
       <c r="A69" t="s">
         <v>178</v>
       </c>
@@ -4942,7 +4899,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:27">
       <c r="A70" t="s">
         <v>180</v>
       </c>
@@ -5004,7 +4961,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:27">
       <c r="A71" t="s">
         <v>182</v>
       </c>
@@ -5054,7 +5011,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:27">
       <c r="A72" t="s">
         <v>184</v>
       </c>
@@ -5104,7 +5061,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:27">
       <c r="A73" t="s">
         <v>186</v>
       </c>
@@ -5154,7 +5111,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:27">
       <c r="A74" t="s">
         <v>188</v>
       </c>
@@ -5192,7 +5149,7 @@
         <v>0</v>
       </c>
       <c r="W74">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="X74">
         <v>0</v>
@@ -5204,7 +5161,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:27">
       <c r="A75" t="s">
         <v>190</v>
       </c>
@@ -5251,7 +5208,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:27">
       <c r="A76" t="s">
         <v>192</v>
       </c>
@@ -5289,7 +5246,7 @@
         <v>0</v>
       </c>
       <c r="W76">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="X76">
         <v>0</v>
@@ -5301,7 +5258,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:27">
       <c r="A77" t="s">
         <v>194</v>
       </c>
@@ -5342,7 +5299,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:27">
       <c r="A78" t="s">
         <v>196</v>
       </c>
@@ -5383,7 +5340,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:27">
       <c r="A79" t="s">
         <v>198</v>
       </c>
@@ -5424,7 +5381,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:27">
       <c r="A80" t="s">
         <v>200</v>
       </c>
@@ -5465,7 +5422,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:27">
       <c r="A81" t="s">
         <v>202</v>
       </c>
@@ -5506,7 +5463,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:27">
       <c r="A82" t="s">
         <v>204</v>
       </c>
@@ -5553,7 +5510,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:27">
       <c r="A83" t="s">
         <v>206</v>
       </c>
@@ -5600,7 +5557,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:27">
       <c r="A84" t="s">
         <v>208</v>
       </c>
@@ -5647,7 +5604,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:27">
       <c r="A85" t="s">
         <v>210</v>
       </c>
@@ -5694,7 +5651,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:27">
       <c r="A86" t="s">
         <v>212</v>
       </c>
@@ -5741,7 +5698,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:27">
       <c r="A87" t="s">
         <v>214</v>
       </c>
@@ -5788,7 +5745,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:27">
       <c r="A88" t="s">
         <v>216</v>
       </c>
@@ -5838,7 +5795,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:27">
       <c r="A89" t="s">
         <v>218</v>
       </c>
@@ -5888,7 +5845,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:27">
       <c r="A90" t="s">
         <v>220</v>
       </c>
@@ -5938,7 +5895,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:27">
       <c r="A91" t="s">
         <v>222</v>
       </c>
@@ -5976,7 +5933,7 @@
         <v>0</v>
       </c>
       <c r="W91">
-        <v>2.3999999999999998E-3</v>
+        <v>0.0024</v>
       </c>
       <c r="X91">
         <v>0</v>
@@ -5988,7 +5945,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:27">
       <c r="A92" t="s">
         <v>224</v>
       </c>
@@ -6035,7 +5992,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:27">
       <c r="A93" t="s">
         <v>226</v>
       </c>
@@ -6073,7 +6030,7 @@
         <v>0</v>
       </c>
       <c r="W93">
-        <v>2.3999999999999998E-3</v>
+        <v>0.0024</v>
       </c>
       <c r="X93">
         <v>0</v>
@@ -6085,7 +6042,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:27">
       <c r="A94" t="s">
         <v>228</v>
       </c>
@@ -6105,7 +6062,7 @@
         <v>127</v>
       </c>
       <c r="R94">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="S94">
         <v>0.12</v>
@@ -6132,7 +6089,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:27">
       <c r="A95" t="s">
         <v>230</v>
       </c>
@@ -6152,7 +6109,7 @@
         <v>68</v>
       </c>
       <c r="R95">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="S95">
         <v>0.12</v>
@@ -6179,7 +6136,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:27">
       <c r="A96" t="s">
         <v>232</v>
       </c>
@@ -6199,7 +6156,7 @@
         <v>65</v>
       </c>
       <c r="R96">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="S96">
         <v>0.12</v>
@@ -6226,7 +6183,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:27">
       <c r="A97" t="s">
         <v>234</v>
       </c>
@@ -6258,7 +6215,7 @@
         <v>0</v>
       </c>
       <c r="W97">
-        <v>8.0000000000000004E-4</v>
+        <v>0.0008</v>
       </c>
       <c r="X97">
         <v>0</v>
@@ -6270,7 +6227,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:27">
       <c r="A98" t="s">
         <v>236</v>
       </c>
@@ -6332,7 +6289,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:27">
       <c r="A99" t="s">
         <v>238</v>
       </c>
@@ -6340,10 +6297,10 @@
         <v>239</v>
       </c>
       <c r="J99">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="L99">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="M99">
         <v>500</v>
@@ -6361,7 +6318,7 @@
         <v>0.24</v>
       </c>
       <c r="T99">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="U99">
         <v>0</v>
@@ -6382,7 +6339,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:27">
       <c r="A100" t="s">
         <v>240</v>
       </c>
@@ -6390,10 +6347,10 @@
         <v>241</v>
       </c>
       <c r="J100">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="L100">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="M100">
         <v>500</v>
@@ -6411,10 +6368,10 @@
         <v>0.24</v>
       </c>
       <c r="T100">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="U100">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="V100">
         <v>0</v>
@@ -6432,7 +6389,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:27">
       <c r="A101" t="s">
         <v>242</v>
       </c>
@@ -6440,10 +6397,10 @@
         <v>243</v>
       </c>
       <c r="F101">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="H101">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="M101">
         <v>500</v>
@@ -6461,13 +6418,13 @@
         <v>0.24</v>
       </c>
       <c r="T101">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="U101">
         <v>0</v>
       </c>
       <c r="V101">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="W101">
         <v>0</v>
@@ -6482,7 +6439,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:27">
       <c r="A102" t="s">
         <v>244</v>
       </c>
@@ -6490,10 +6447,10 @@
         <v>245</v>
       </c>
       <c r="H102">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="K102">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="M102">
         <v>500</v>
@@ -6511,7 +6468,7 @@
         <v>0.24</v>
       </c>
       <c r="T102">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="U102">
         <v>0</v>
@@ -6520,7 +6477,7 @@
         <v>0</v>
       </c>
       <c r="W102">
-        <v>2.8E-3</v>
+        <v>0.0028</v>
       </c>
       <c r="X102">
         <v>0</v>
@@ -6532,7 +6489,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:27">
       <c r="A103" t="s">
         <v>246</v>
       </c>
@@ -6540,7 +6497,7 @@
         <v>247</v>
       </c>
       <c r="G103">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="M103">
         <v>500</v>
@@ -6558,10 +6515,10 @@
         <v>0.24</v>
       </c>
       <c r="T103">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="U103">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="V103">
         <v>0</v>
@@ -6579,7 +6536,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:27">
       <c r="A104" t="s">
         <v>248</v>
       </c>
@@ -6587,10 +6544,10 @@
         <v>249</v>
       </c>
       <c r="H104">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="K104">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="M104">
         <v>500</v>
@@ -6608,7 +6565,7 @@
         <v>0.24</v>
       </c>
       <c r="T104">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="U104">
         <v>0</v>
@@ -6617,7 +6574,7 @@
         <v>0</v>
       </c>
       <c r="W104">
-        <v>2.8E-3</v>
+        <v>0.0028</v>
       </c>
       <c r="X104">
         <v>0</v>
@@ -6629,7 +6586,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:27">
       <c r="A105" t="s">
         <v>250</v>
       </c>
@@ -6649,7 +6606,7 @@
         <v>62</v>
       </c>
       <c r="S105">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="T105">
         <v>0</v>
@@ -6661,7 +6618,7 @@
         <v>0</v>
       </c>
       <c r="W105">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="X105">
         <v>0</v>
@@ -6673,7 +6630,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:27">
       <c r="A106" t="s">
         <v>252</v>
       </c>
@@ -6693,10 +6650,10 @@
         <v>65</v>
       </c>
       <c r="R106">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="S106">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="T106">
         <v>0</v>
@@ -6720,7 +6677,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:27">
       <c r="A107" t="s">
         <v>254</v>
       </c>
@@ -6740,10 +6697,10 @@
         <v>127</v>
       </c>
       <c r="R107">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="S107">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="T107">
         <v>0</v>
@@ -6767,7 +6724,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:27">
       <c r="A108" t="s">
         <v>256</v>
       </c>
@@ -6787,10 +6744,10 @@
         <v>68</v>
       </c>
       <c r="R108">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="S108">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="T108">
         <v>0</v>
@@ -6814,7 +6771,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:27">
       <c r="A109" t="s">
         <v>258</v>
       </c>
@@ -6855,7 +6812,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:27">
       <c r="A110" t="s">
         <v>260</v>
       </c>
@@ -6902,7 +6859,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:27">
       <c r="A111" t="s">
         <v>262</v>
       </c>
@@ -6949,7 +6906,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:27">
       <c r="A112" t="s">
         <v>264</v>
       </c>
@@ -6996,7 +6953,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="113" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:27">
       <c r="A113" t="s">
         <v>266</v>
       </c>
@@ -7043,7 +7000,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="114" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:27">
       <c r="A114" t="s">
         <v>268</v>
       </c>
@@ -7090,7 +7047,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="115" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:27">
       <c r="A115" t="s">
         <v>270</v>
       </c>
@@ -7137,7 +7094,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="116" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:27">
       <c r="A116" t="s">
         <v>272</v>
       </c>
@@ -7187,7 +7144,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="117" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:27">
       <c r="A117" t="s">
         <v>274</v>
       </c>
@@ -7228,7 +7185,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="118" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:27">
       <c r="A118" t="s">
         <v>276</v>
       </c>
@@ -7269,7 +7226,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:27">
       <c r="A119" t="s">
         <v>278</v>
       </c>
@@ -7310,7 +7267,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="120" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:27">
       <c r="A120" t="s">
         <v>280</v>
       </c>
@@ -7336,7 +7293,7 @@
         <v>54</v>
       </c>
       <c r="S120">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="T120">
         <v>0.3</v>
@@ -7348,7 +7305,7 @@
         <v>0</v>
       </c>
       <c r="W120">
-        <v>3.0000000000000001E-3</v>
+        <v>0.003</v>
       </c>
       <c r="X120">
         <v>0</v>
@@ -7360,7 +7317,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="121" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:27">
       <c r="A121" t="s">
         <v>282</v>
       </c>
@@ -7386,7 +7343,7 @@
         <v>43</v>
       </c>
       <c r="S121">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="T121">
         <v>0.3</v>
@@ -7410,7 +7367,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="122" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:27">
       <c r="A122" t="s">
         <v>284</v>
       </c>
@@ -7436,7 +7393,7 @@
         <v>48</v>
       </c>
       <c r="S122">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="T122">
         <v>0.3</v>
@@ -7460,7 +7417,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="123" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:27">
       <c r="A123" t="s">
         <v>286</v>
       </c>
@@ -7486,7 +7443,7 @@
         <v>57</v>
       </c>
       <c r="S123">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="T123">
         <v>0.3</v>
@@ -7510,7 +7467,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="124" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:27">
       <c r="A124" t="s">
         <v>288</v>
       </c>
@@ -7533,7 +7490,7 @@
         <v>32</v>
       </c>
       <c r="S124">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="T124">
         <v>0.3</v>
@@ -7557,7 +7514,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="125" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:27">
       <c r="A125" t="s">
         <v>290</v>
       </c>
@@ -7583,7 +7540,7 @@
         <v>51</v>
       </c>
       <c r="S125">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="T125">
         <v>0.3</v>
@@ -7595,7 +7552,7 @@
         <v>0</v>
       </c>
       <c r="W125">
-        <v>3.0000000000000001E-3</v>
+        <v>0.003</v>
       </c>
       <c r="X125">
         <v>0</v>
@@ -7607,7 +7564,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="126" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:27">
       <c r="A126" t="s">
         <v>292</v>
       </c>
@@ -7639,7 +7596,7 @@
         <v>0</v>
       </c>
       <c r="W126">
-        <v>1.8E-3</v>
+        <v>0.0018</v>
       </c>
       <c r="X126">
         <v>0</v>
@@ -7651,7 +7608,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="127" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:27">
       <c r="A127" t="s">
         <v>294</v>
       </c>
@@ -7698,7 +7655,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="128" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:27">
       <c r="A128" t="s">
         <v>296</v>
       </c>
@@ -7718,7 +7675,7 @@
         <v>65</v>
       </c>
       <c r="R128">
-        <v>1.7999999999999999E-2</v>
+        <v>0.018</v>
       </c>
       <c r="S128">
         <v>0.15</v>
@@ -7745,7 +7702,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="129" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:27">
       <c r="A129" t="s">
         <v>298</v>
       </c>
@@ -7765,7 +7722,7 @@
         <v>127</v>
       </c>
       <c r="R129">
-        <v>1.7999999999999999E-2</v>
+        <v>0.018</v>
       </c>
       <c r="S129">
         <v>0.15</v>
@@ -7792,7 +7749,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="130" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:27">
       <c r="A130" t="s">
         <v>300</v>
       </c>
@@ -7812,7 +7769,7 @@
         <v>68</v>
       </c>
       <c r="R130">
-        <v>1.7999999999999999E-2</v>
+        <v>0.018</v>
       </c>
       <c r="S130">
         <v>0.15</v>
@@ -7839,7 +7796,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="131" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:27">
       <c r="A131" t="s">
         <v>302</v>
       </c>
@@ -7886,7 +7843,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="132" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:27">
       <c r="A132" t="s">
         <v>304</v>
       </c>
@@ -7933,7 +7890,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="133" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:27">
       <c r="A133" t="s">
         <v>306</v>
       </c>
@@ -7980,7 +7937,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="134" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:27">
       <c r="A134" t="s">
         <v>308</v>
       </c>
@@ -8027,7 +7984,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="135" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:27">
       <c r="A135" t="s">
         <v>310</v>
       </c>
@@ -8074,7 +8031,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="136" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:27">
       <c r="A136" t="s">
         <v>312</v>
       </c>
@@ -8121,7 +8078,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="137" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:27">
       <c r="A137" t="s">
         <v>314</v>
       </c>
@@ -8183,7 +8140,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="138" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:27">
       <c r="A138" t="s">
         <v>316</v>
       </c>
@@ -8215,7 +8172,7 @@
         <v>0</v>
       </c>
       <c r="W138">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="X138">
         <v>0</v>
@@ -8227,7 +8184,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="139" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:27">
       <c r="A139" t="s">
         <v>318</v>
       </c>
@@ -8268,7 +8225,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="140" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:27">
       <c r="A140" t="s">
         <v>320</v>
       </c>
@@ -8309,7 +8266,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="141" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:27">
       <c r="A141" t="s">
         <v>322</v>
       </c>
@@ -8350,7 +8307,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="142" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:27">
       <c r="A142" t="s">
         <v>324</v>
       </c>
@@ -8391,7 +8348,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="143" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:27">
       <c r="A143" t="s">
         <v>326</v>
       </c>
@@ -8432,7 +8389,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="144" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:27">
       <c r="A144" t="s">
         <v>328</v>
       </c>
@@ -8464,7 +8421,7 @@
         <v>0</v>
       </c>
       <c r="W144">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="X144">
         <v>0</v>
@@ -8476,7 +8433,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="145" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:27">
       <c r="A145" t="s">
         <v>330</v>
       </c>
@@ -8499,7 +8456,7 @@
         <v>0.25</v>
       </c>
       <c r="S145">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="T145">
         <v>0</v>
@@ -8523,7 +8480,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="146" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:27">
       <c r="A146" t="s">
         <v>332</v>
       </c>
@@ -8546,7 +8503,7 @@
         <v>0.25</v>
       </c>
       <c r="S146">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="T146">
         <v>0</v>
@@ -8570,7 +8527,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="147" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:27">
       <c r="A147" t="s">
         <v>334</v>
       </c>
@@ -8593,7 +8550,7 @@
         <v>0.25</v>
       </c>
       <c r="S147">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="T147">
         <v>0</v>
@@ -8617,7 +8574,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="148" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:27">
       <c r="A148" t="s">
         <v>336</v>
       </c>
@@ -8640,7 +8597,7 @@
         <v>0.25</v>
       </c>
       <c r="S148">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="T148">
         <v>0</v>
@@ -8664,7 +8621,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="149" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:27">
       <c r="A149" t="s">
         <v>338</v>
       </c>
@@ -8687,7 +8644,7 @@
         <v>0.25</v>
       </c>
       <c r="S149">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="T149">
         <v>0</v>
@@ -8711,7 +8668,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="150" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:27">
       <c r="A150" t="s">
         <v>340</v>
       </c>
@@ -8734,7 +8691,7 @@
         <v>0.25</v>
       </c>
       <c r="S150">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="T150">
         <v>0</v>
@@ -8758,7 +8715,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="151" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:27">
       <c r="A151" t="s">
         <v>342</v>
       </c>
@@ -8805,7 +8762,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="152" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:27">
       <c r="A152" t="s">
         <v>344</v>
       </c>
@@ -8867,7 +8824,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="153" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:27">
       <c r="A153" t="s">
         <v>346</v>
       </c>
@@ -8899,7 +8856,7 @@
         <v>0</v>
       </c>
       <c r="W153">
-        <v>3.0000000000000001E-3</v>
+        <v>0.003</v>
       </c>
       <c r="X153">
         <v>0</v>
@@ -8911,7 +8868,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="154" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:27">
       <c r="A154" t="s">
         <v>348</v>
       </c>
@@ -8958,7 +8915,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="155" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:27">
       <c r="A155" t="s">
         <v>350</v>
       </c>
@@ -9005,7 +8962,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="156" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:27">
       <c r="A156" t="s">
         <v>352</v>
       </c>
@@ -9052,7 +9009,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="157" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:27">
       <c r="A157" t="s">
         <v>354</v>
       </c>
@@ -9105,7 +9062,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="158" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:27">
       <c r="A158" t="s">
         <v>356</v>
       </c>
@@ -9146,7 +9103,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="159" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:27">
       <c r="A159" t="s">
         <v>358</v>
       </c>
@@ -9187,7 +9144,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="160" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:27">
       <c r="A160" t="s">
         <v>360</v>
       </c>
@@ -9228,7 +9185,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="161" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:27">
       <c r="A161" t="s">
         <v>362</v>
       </c>
@@ -9269,7 +9226,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="162" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:27">
       <c r="A162" t="s">
         <v>364</v>
       </c>
@@ -9289,7 +9246,7 @@
         <v>65</v>
       </c>
       <c r="R162">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="S162">
         <v>0.22</v>
@@ -9316,7 +9273,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="163" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:27">
       <c r="A163" t="s">
         <v>366</v>
       </c>
@@ -9336,7 +9293,7 @@
         <v>127</v>
       </c>
       <c r="R163">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="S163">
         <v>0.22</v>
@@ -9363,7 +9320,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="164" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:27">
       <c r="A164" t="s">
         <v>368</v>
       </c>
@@ -9383,7 +9340,7 @@
         <v>68</v>
       </c>
       <c r="R164">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="S164">
         <v>0.22</v>
@@ -9410,7 +9367,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="165" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:27">
       <c r="A165" t="s">
         <v>370</v>
       </c>
@@ -9442,7 +9399,7 @@
         <v>0</v>
       </c>
       <c r="W165">
-        <v>4.0000000000000002E-4</v>
+        <v>0.0004</v>
       </c>
       <c r="X165">
         <v>0</v>
@@ -9454,7 +9411,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="166" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:27">
       <c r="A166" t="s">
         <v>372</v>
       </c>
@@ -9501,7 +9458,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="167" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:27">
       <c r="A167" t="s">
         <v>374</v>
       </c>
@@ -9548,7 +9505,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="168" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:27">
       <c r="A168" t="s">
         <v>376</v>
       </c>
@@ -9595,7 +9552,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="169" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:27">
       <c r="A169" t="s">
         <v>378</v>
       </c>
@@ -9642,7 +9599,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="170" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:27">
       <c r="A170" t="s">
         <v>380</v>
       </c>
@@ -9689,7 +9646,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="171" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:27">
       <c r="A171" t="s">
         <v>382</v>
       </c>
@@ -9737,8 +9694,17 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lots of little fixes.
- Kingdom fixes - specifically around the map updating when one is taken.
- Attack Log fixes, make sure the bomb drop goes to the right character.
- Various other fixes.
- items and affixes droppability updated
- monsters updated - alas the final critter for surface is too strong.
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -197,6 +197,24 @@
     <t>Feel the strength of a shadow fiend crawling through the veins of your body.</t>
   </si>
   <si>
+    <t>Defiant Aim</t>
+  </si>
+  <si>
+    <t>Are you tired of missing child? You'll never miss again, I promise.</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Treasure Goblin Luck</t>
+  </si>
+  <si>
+    <t>Luck of the treasure goblin I tell ya!</t>
+  </si>
+  <si>
+    <t>Looting</t>
+  </si>
+  <si>
     <t>Courage</t>
   </si>
   <si>
@@ -206,24 +224,6 @@
     <t>Fighters Resilience</t>
   </si>
   <si>
-    <t>Defiant Aim</t>
-  </si>
-  <si>
-    <t>Are you tired of missing child? You'll never miss again, I promise.</t>
-  </si>
-  <si>
-    <t>Accuracy</t>
-  </si>
-  <si>
-    <t>Treasure Goblin Luck</t>
-  </si>
-  <si>
-    <t>Luck of the treasure goblin I tell ya!</t>
-  </si>
-  <si>
-    <t>Looting</t>
-  </si>
-  <si>
     <t>Heretics Infusions</t>
   </si>
   <si>
@@ -407,24 +407,24 @@
     <t>Let the devil deliver this aim child!</t>
   </si>
   <si>
+    <t>Dark Thoughts</t>
+  </si>
+  <si>
+    <t>These thoughts are drifting through your head all the time. What can you do about it?</t>
+  </si>
+  <si>
+    <t>Faithless Hate</t>
+  </si>
+  <si>
+    <t>There is nothing worse then the hatefilled vengance of the faithless.</t>
+  </si>
+  <si>
     <t>Shadow Soldier</t>
   </si>
   <si>
     <t>The time to die is not now. Fight faster child! Fight harder!</t>
   </si>
   <si>
-    <t>Dark Thoughts</t>
-  </si>
-  <si>
-    <t>These thoughts are drifting through your head all the time. What can you do about it?</t>
-  </si>
-  <si>
-    <t>Faithless Hate</t>
-  </si>
-  <si>
-    <t>There is nothing worse then the hatefilled vengance of the faithless.</t>
-  </si>
-  <si>
     <t>Celestial Mages Blood</t>
   </si>
   <si>
@@ -497,30 +497,30 @@
     <t>The legacy of these affixes and enchantments goes back thousands of years. Learn what you can child. Learn what you can.</t>
   </si>
   <si>
+    <t>Angelic Arrow</t>
+  </si>
+  <si>
+    <t>Never let the enemy see you fail. Failing is missing. never miss.</t>
+  </si>
+  <si>
+    <t>Bards Dance</t>
+  </si>
+  <si>
+    <t>Dance your way out of this situation child!</t>
+  </si>
+  <si>
+    <t>Thieves Eyes</t>
+  </si>
+  <si>
+    <t>See gold do you? Smell it can you?</t>
+  </si>
+  <si>
     <t>Devli's Stance</t>
   </si>
   <si>
     <t>Take a stance before the devil! Ask for less time!</t>
   </si>
   <si>
-    <t>Angelic Arrow</t>
-  </si>
-  <si>
-    <t>Never let the enemy see you fail. Failing is missing. never miss.</t>
-  </si>
-  <si>
-    <t>Bards Dance</t>
-  </si>
-  <si>
-    <t>Dance your way out of this situation child!</t>
-  </si>
-  <si>
-    <t>Thieves Eyes</t>
-  </si>
-  <si>
-    <t>See gold do you? Smell it can you?</t>
-  </si>
-  <si>
     <t>Ring Crafters Enchanted Thought</t>
   </si>
   <si>
@@ -767,34 +767,34 @@
     <t>Nature is a fickle beast, but she can help you if you turn to her in your most dire of need.</t>
   </si>
   <si>
+    <t>Shattered Illusions</t>
+  </si>
+  <si>
+    <t>To get better at accuracy, you must train child. Do you hear? Train.</t>
+  </si>
+  <si>
+    <t>Lifes Dance</t>
+  </si>
+  <si>
+    <t>Dance to the song of life child.</t>
+  </si>
+  <si>
+    <t>Lost and Found</t>
+  </si>
+  <si>
+    <t>What was once lost is now found.</t>
+  </si>
+  <si>
+    <t>Blood Fever</t>
+  </si>
+  <si>
+    <t>Smell blood do ya? let it drive you insane!</t>
+  </si>
+  <si>
     <t>Fates Blessing</t>
   </si>
   <si>
     <t>fate be with you child. Let the hands of time move faster.</t>
-  </si>
-  <si>
-    <t>Shattered Illusions</t>
-  </si>
-  <si>
-    <t>To get better at accuracy, you must train child. Do you hear? Train.</t>
-  </si>
-  <si>
-    <t>Lifes Dance</t>
-  </si>
-  <si>
-    <t>Dance to the song of life child.</t>
-  </si>
-  <si>
-    <t>Lost and Found</t>
-  </si>
-  <si>
-    <t>What was once lost is now found.</t>
-  </si>
-  <si>
-    <t>Blood Fever</t>
-  </si>
-  <si>
-    <t>Smell blood do ya? let it drive you insane!</t>
   </si>
   <si>
     <t>Inspiring Weapons</t>
@@ -2295,13 +2295,13 @@
         <v>5</v>
       </c>
       <c r="O15">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="P15" t="s">
         <v>62</v>
       </c>
       <c r="S15">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="T15">
         <v>0</v>
@@ -2333,7 +2333,7 @@
         <v>64</v>
       </c>
       <c r="M16">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="N16">
         <v>5</v>
@@ -2377,19 +2377,19 @@
         <v>67</v>
       </c>
       <c r="M17">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="N17">
         <v>5</v>
       </c>
       <c r="O17">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="P17" t="s">
         <v>68</v>
       </c>
       <c r="S17">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="T17">
         <v>0</v>
@@ -3591,7 +3591,7 @@
         <v>45</v>
       </c>
       <c r="P42" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R42">
         <v>0.002</v>
@@ -3685,7 +3685,7 @@
         <v>45</v>
       </c>
       <c r="P44" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="R44">
         <v>0.002</v>
@@ -3722,20 +3722,23 @@
       <c r="B45" t="s">
         <v>131</v>
       </c>
+      <c r="C45">
+        <v>0.08</v>
+      </c>
+      <c r="D45">
+        <v>0.08</v>
+      </c>
+      <c r="E45">
+        <v>0.08</v>
+      </c>
       <c r="M45">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="N45">
         <v>15</v>
       </c>
       <c r="O45">
-        <v>45</v>
-      </c>
-      <c r="P45" t="s">
-        <v>62</v>
-      </c>
-      <c r="S45">
-        <v>0.05</v>
+        <v>30</v>
       </c>
       <c r="T45">
         <v>0</v>
@@ -3747,13 +3750,13 @@
         <v>0</v>
       </c>
       <c r="W45">
-        <v>0.0002</v>
+        <v>0</v>
       </c>
       <c r="X45">
         <v>0</v>
       </c>
       <c r="Z45">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="AA45" t="s">
         <v>40</v>
@@ -3767,16 +3770,16 @@
         <v>133</v>
       </c>
       <c r="C46">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="D46">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="E46">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="M46">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="N46">
         <v>15</v>
@@ -3800,7 +3803,7 @@
         <v>0</v>
       </c>
       <c r="Z46">
-        <v>5000</v>
+        <v>8000</v>
       </c>
       <c r="AA46" t="s">
         <v>40</v>
@@ -3813,23 +3816,20 @@
       <c r="B47" t="s">
         <v>135</v>
       </c>
-      <c r="C47">
-        <v>0.1</v>
-      </c>
-      <c r="D47">
-        <v>0.1</v>
-      </c>
-      <c r="E47">
-        <v>0.1</v>
-      </c>
       <c r="M47">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="N47">
         <v>15</v>
       </c>
       <c r="O47">
-        <v>30</v>
+        <v>45</v>
+      </c>
+      <c r="P47" t="s">
+        <v>68</v>
+      </c>
+      <c r="S47">
+        <v>0.05</v>
       </c>
       <c r="T47">
         <v>0</v>
@@ -3841,13 +3841,13 @@
         <v>0</v>
       </c>
       <c r="W47">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="X47">
         <v>0</v>
       </c>
       <c r="Z47">
-        <v>8000</v>
+        <v>3000</v>
       </c>
       <c r="AA47" t="s">
         <v>40</v>
@@ -4451,6 +4451,9 @@
       <c r="P60" t="s">
         <v>62</v>
       </c>
+      <c r="R60">
+        <v>0.005</v>
+      </c>
       <c r="S60">
         <v>0.1</v>
       </c>
@@ -4464,7 +4467,7 @@
         <v>0</v>
       </c>
       <c r="W60">
-        <v>0.0005</v>
+        <v>0</v>
       </c>
       <c r="X60">
         <v>0</v>
@@ -4493,7 +4496,7 @@
         <v>60</v>
       </c>
       <c r="P61" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="R61">
         <v>0.005</v>
@@ -4540,7 +4543,7 @@
         <v>60</v>
       </c>
       <c r="P62" t="s">
-        <v>127</v>
+        <v>65</v>
       </c>
       <c r="R62">
         <v>0.005</v>
@@ -4589,9 +4592,6 @@
       <c r="P63" t="s">
         <v>68</v>
       </c>
-      <c r="R63">
-        <v>0.005</v>
-      </c>
       <c r="S63">
         <v>0.1</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>0</v>
       </c>
       <c r="W63">
-        <v>0</v>
+        <v>0.0005</v>
       </c>
       <c r="X63">
         <v>0</v>
@@ -6106,7 +6106,7 @@
         <v>80</v>
       </c>
       <c r="P95" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R95">
         <v>0.008</v>
@@ -6153,7 +6153,7 @@
         <v>80</v>
       </c>
       <c r="P96" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="R96">
         <v>0.008</v>
@@ -6200,7 +6200,7 @@
         <v>80</v>
       </c>
       <c r="P97" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="S97">
         <v>0.12</v>
@@ -6605,6 +6605,9 @@
       <c r="P105" t="s">
         <v>62</v>
       </c>
+      <c r="R105">
+        <v>0.015</v>
+      </c>
       <c r="S105">
         <v>0.14</v>
       </c>
@@ -6618,7 +6621,7 @@
         <v>0</v>
       </c>
       <c r="W105">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="X105">
         <v>0</v>
@@ -6647,7 +6650,7 @@
         <v>100</v>
       </c>
       <c r="P106" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="R106">
         <v>0.015</v>
@@ -6694,7 +6697,7 @@
         <v>100</v>
       </c>
       <c r="P107" t="s">
-        <v>127</v>
+        <v>65</v>
       </c>
       <c r="R107">
         <v>0.015</v>
@@ -6731,23 +6734,17 @@
       <c r="B108" t="s">
         <v>257</v>
       </c>
+      <c r="G108">
+        <v>0.11</v>
+      </c>
       <c r="M108">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="N108">
         <v>45</v>
       </c>
       <c r="O108">
-        <v>100</v>
-      </c>
-      <c r="P108" t="s">
-        <v>68</v>
-      </c>
-      <c r="R108">
-        <v>0.015</v>
-      </c>
-      <c r="S108">
-        <v>0.14</v>
+        <v>160</v>
       </c>
       <c r="T108">
         <v>0</v>
@@ -6765,10 +6762,10 @@
         <v>0</v>
       </c>
       <c r="Z108">
-        <v>100000</v>
+        <v>120000</v>
       </c>
       <c r="AA108" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="109" spans="1:27">
@@ -6778,17 +6775,20 @@
       <c r="B109" t="s">
         <v>259</v>
       </c>
-      <c r="G109">
-        <v>0.11</v>
-      </c>
       <c r="M109">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="N109">
         <v>45</v>
       </c>
       <c r="O109">
-        <v>160</v>
+        <v>100</v>
+      </c>
+      <c r="P109" t="s">
+        <v>68</v>
+      </c>
+      <c r="S109">
+        <v>0.14</v>
       </c>
       <c r="T109">
         <v>0</v>
@@ -6800,16 +6800,16 @@
         <v>0</v>
       </c>
       <c r="W109">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="X109">
         <v>0</v>
       </c>
       <c r="Z109">
-        <v>120000</v>
+        <v>100000</v>
       </c>
       <c r="AA109" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="110" spans="1:27">
@@ -7581,7 +7581,7 @@
         <v>200</v>
       </c>
       <c r="P126" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="S126">
         <v>0.15</v>
@@ -7672,7 +7672,7 @@
         <v>200</v>
       </c>
       <c r="P128" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="R128">
         <v>0.018</v>
@@ -7766,7 +7766,7 @@
         <v>200</v>
       </c>
       <c r="P130" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R130">
         <v>0.018</v>
@@ -8157,7 +8157,7 @@
         <v>200</v>
       </c>
       <c r="P138" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="S138">
         <v>0.18</v>
@@ -8406,7 +8406,7 @@
         <v>200</v>
       </c>
       <c r="P144" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="S144">
         <v>0.2</v>
@@ -8841,7 +8841,7 @@
         <v>200</v>
       </c>
       <c r="P153" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="S153">
         <v>0.22</v>
@@ -8885,7 +8885,7 @@
         <v>200</v>
       </c>
       <c r="P154" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="R154">
         <v>0.02</v>
@@ -8979,7 +8979,7 @@
         <v>200</v>
       </c>
       <c r="P156" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R156">
         <v>0.02</v>
@@ -9243,7 +9243,7 @@
         <v>200</v>
       </c>
       <c r="P162" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="R162">
         <v>0.025</v>
@@ -9337,7 +9337,7 @@
         <v>200</v>
       </c>
       <c r="P164" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R164">
         <v>0.025</v>
@@ -9384,7 +9384,7 @@
         <v>200</v>
       </c>
       <c r="P165" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="S165">
         <v>0.24</v>

</xml_diff>

<commit_message>
Added a way to filter out duplicate items.
- These items cannot have affixes attached.
- Added new monsters, affixes and items - but no new artifacts.
- Fixed kingdom API Limit.
- Allow admin to select Alchemy and Quest items from the drop down.
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="789">
   <si>
     <t>name</t>
   </si>
@@ -2271,6 +2271,117 @@
   </si>
   <si>
     <t>The faithless scream so loud, your enemies ears bleed.</t>
+  </si>
+  <si>
+    <t>Fighters Scorn</t>
+  </si>
+  <si>
+    <t>This enchantment is best suited for a Fighter as it increases their stats and class bonuses as well as gives other Fighter specific enhancements</t>
+  </si>
+  <si>
+    <t>Heretics Flaming Hands</t>
+  </si>
+  <si>
+    <t>This relic is best suited for a Heretic as it increases their stats and class bonuses as well as gives other Heretic specific enhancements</t>
+  </si>
+  <si>
+    <t>Prophets Curse</t>
+  </si>
+  <si>
+    <t>This enchantment is best suited for a Prophet as it increases their stats and class bonuses as well as gives other Prophet specific enhancements</t>
+  </si>
+  <si>
+    <t>Rangers Prayer</t>
+  </si>
+  <si>
+    <t>This enchantment is best suited for a Ranger as it increases their stats and class bonuses as well as gives other Ranger specific enhancements</t>
+  </si>
+  <si>
+    <t>Thieves Double Dance</t>
+  </si>
+  <si>
+    <t>This enchantment is best suited for a Thief as it increases their stats and class bonuses as well as gives other Thief specific enhancements</t>
+  </si>
+  <si>
+    <t>Vampires Deliverance</t>
+  </si>
+  <si>
+    <t>This relic is best suited for a Vampire as it increases their stats and class bonuses as well as gives other Vampire specific enhancements. This is known as a kill enchantment. That is the damage on it will kill in conjunction with the life stealing.</t>
+  </si>
+  <si>
+    <t>Fighters Raging Despair</t>
+  </si>
+  <si>
+    <t>This enchantment is best suited for a Fighter as it increases their stats and class bonuses as well as gives other Fighter specific enhancements.</t>
+  </si>
+  <si>
+    <t>Heretics Maddness</t>
+  </si>
+  <si>
+    <t>This enchantment is best suited for a Heretic as it increases their stats and class bonuses as well as gives other Heretic specific enhancements.</t>
+  </si>
+  <si>
+    <t>Prophets Faith</t>
+  </si>
+  <si>
+    <t>This enchantment is best suited for a Prophet as it increases their stats and class bonuses as well as gives other Prophet specific enhancements.</t>
+  </si>
+  <si>
+    <t>Rangers Guidance</t>
+  </si>
+  <si>
+    <t>Thieves Decadence</t>
+  </si>
+  <si>
+    <t>This enchantment is best suited for a Thief as it increases their stats and class bonuses as well as gives other Thief specific enhancements.</t>
+  </si>
+  <si>
+    <t>Vampires Unquenchable Thirst</t>
+  </si>
+  <si>
+    <t>This enchantment is best suited for a Vampire as it increases their stats and class bonuses as well as gives other Vampire specific enhancements. This is considered a kill enchantment. That is, with the damage from life stealing and the damage from the enchantment its self, is enough to kill (in most cases)</t>
+  </si>
+  <si>
+    <t>Satans Delicious Flesh Ripper</t>
+  </si>
+  <si>
+    <t>The enemy screams as you rip the flesh from their bones and lay it upon the ground.</t>
+  </si>
+  <si>
+    <t>Deaths War</t>
+  </si>
+  <si>
+    <t>The enemy cannot contain their fear as the horse of death appears from the fog that surrounds them.</t>
+  </si>
+  <si>
+    <t>Egregious Assault</t>
+  </si>
+  <si>
+    <t>The enemy cannot stand any-longer, the assault on their soul is too much. They slump into a depression of regret.</t>
+  </si>
+  <si>
+    <t>Gods Tear</t>
+  </si>
+  <si>
+    <t>The enemy feels the weight of the world.....Crush them to death.</t>
+  </si>
+  <si>
+    <t>Demonic Adoration of Hope</t>
+  </si>
+  <si>
+    <t>The enemies eyes explodes and they rip their lungs out infront of you.</t>
+  </si>
+  <si>
+    <t>Astral Invocation</t>
+  </si>
+  <si>
+    <t>The enemy watches as you rip a portal to the Astral plane and suck them in to a land of death and despair!</t>
+  </si>
+  <si>
+    <t>Soul Craving Flesh Wound</t>
+  </si>
+  <si>
+    <t>The enemies flesh opens and their soul starts to rip through the wounds.</t>
   </si>
 </sst>
 </file>
@@ -2609,7 +2720,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AR369"/>
+  <dimension ref="A1:AR388"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -8760,6 +8871,9 @@
       <c r="AO67">
         <v>0</v>
       </c>
+      <c r="AP67">
+        <v>0</v>
+      </c>
       <c r="AQ67">
         <v>0.1</v>
       </c>
@@ -8843,6 +8957,9 @@
       <c r="AO68">
         <v>0</v>
       </c>
+      <c r="AP68">
+        <v>0</v>
+      </c>
       <c r="AQ68">
         <v>0</v>
       </c>
@@ -12086,6 +12203,9 @@
       <c r="AO104">
         <v>0</v>
       </c>
+      <c r="AP104">
+        <v>0</v>
+      </c>
       <c r="AQ104">
         <v>0.15</v>
       </c>
@@ -12169,6 +12289,9 @@
       <c r="AO105">
         <v>0</v>
       </c>
+      <c r="AP105">
+        <v>0</v>
+      </c>
       <c r="AQ105">
         <v>0</v>
       </c>
@@ -14795,6 +14918,9 @@
       <c r="AO134">
         <v>0</v>
       </c>
+      <c r="AP134">
+        <v>0</v>
+      </c>
       <c r="AQ134">
         <v>0.2</v>
       </c>
@@ -14878,6 +15004,9 @@
       <c r="AO135">
         <v>0</v>
       </c>
+      <c r="AP135">
+        <v>0</v>
+      </c>
       <c r="AQ135">
         <v>0</v>
       </c>
@@ -17773,6 +17902,9 @@
       <c r="AO168">
         <v>0</v>
       </c>
+      <c r="AP168">
+        <v>0</v>
+      </c>
       <c r="AQ168">
         <v>0.25</v>
       </c>
@@ -17856,6 +17988,9 @@
       <c r="AO169">
         <v>0</v>
       </c>
+      <c r="AP169">
+        <v>0</v>
+      </c>
       <c r="AQ169">
         <v>0</v>
       </c>
@@ -21369,6 +21504,9 @@
       <c r="AO208">
         <v>0</v>
       </c>
+      <c r="AP208">
+        <v>0</v>
+      </c>
       <c r="AQ208">
         <v>0.3</v>
       </c>
@@ -21452,6 +21590,9 @@
       <c r="AO209">
         <v>0</v>
       </c>
+      <c r="AP209">
+        <v>0</v>
+      </c>
       <c r="AQ209">
         <v>0</v>
       </c>
@@ -23689,6 +23830,9 @@
       <c r="AO234">
         <v>0</v>
       </c>
+      <c r="AP234">
+        <v>0</v>
+      </c>
       <c r="AQ234">
         <v>0.35</v>
       </c>
@@ -23772,6 +23916,9 @@
       <c r="AO235">
         <v>0</v>
       </c>
+      <c r="AP235">
+        <v>0</v>
+      </c>
       <c r="AQ235">
         <v>0</v>
       </c>
@@ -26222,6 +26369,9 @@
       <c r="AO263">
         <v>0</v>
       </c>
+      <c r="AP263">
+        <v>0</v>
+      </c>
       <c r="AQ263">
         <v>0.4</v>
       </c>
@@ -26305,6 +26455,9 @@
       <c r="AO264">
         <v>0</v>
       </c>
+      <c r="AP264">
+        <v>0</v>
+      </c>
       <c r="AQ264">
         <v>0</v>
       </c>
@@ -29776,6 +29929,9 @@
       <c r="AO303">
         <v>0</v>
       </c>
+      <c r="AP303">
+        <v>0</v>
+      </c>
       <c r="AQ303">
         <v>0.45</v>
       </c>
@@ -29859,6 +30015,9 @@
       <c r="AO304">
         <v>0</v>
       </c>
+      <c r="AP304">
+        <v>0</v>
+      </c>
       <c r="AQ304">
         <v>0</v>
       </c>
@@ -31286,6 +31445,9 @@
       <c r="AO320">
         <v>0</v>
       </c>
+      <c r="AP320">
+        <v>0</v>
+      </c>
       <c r="AQ320">
         <v>0.5</v>
       </c>
@@ -31369,6 +31531,9 @@
       <c r="AO321">
         <v>0</v>
       </c>
+      <c r="AP321">
+        <v>0</v>
+      </c>
       <c r="AQ321">
         <v>0</v>
       </c>
@@ -34603,13 +34768,13 @@
         <v>0</v>
       </c>
       <c r="U358">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="V358">
         <v>0</v>
       </c>
       <c r="W358">
-        <v>500000</v>
+        <v>800</v>
       </c>
       <c r="X358">
         <v>10000</v>
@@ -34645,7 +34810,7 @@
         <v>49</v>
       </c>
       <c r="AO358">
-        <v>0.35</v>
+        <v>0.05</v>
       </c>
       <c r="AP358">
         <v>0.05</v>
@@ -34668,7 +34833,7 @@
         <v>0.1</v>
       </c>
       <c r="G359">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H359">
         <v>0.2</v>
@@ -34680,7 +34845,7 @@
         <v>0.15</v>
       </c>
       <c r="K359">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="L359">
         <v>0.15</v>
@@ -34710,7 +34875,7 @@
         <v>0</v>
       </c>
       <c r="V359">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="W359">
         <v>1500</v>
@@ -34734,10 +34899,10 @@
         <v>0</v>
       </c>
       <c r="AH359">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="AI359">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="AK359">
         <v>1</v>
@@ -34775,10 +34940,13 @@
         <v>0.75</v>
       </c>
       <c r="F360">
-        <v>2</v>
+        <v>0.85</v>
       </c>
       <c r="G360">
-        <v>1</v>
+        <v>0.45</v>
+      </c>
+      <c r="H360">
+        <v>0.05</v>
       </c>
       <c r="K360">
         <v>0</v>
@@ -34817,7 +34985,7 @@
         <v>0</v>
       </c>
       <c r="W360">
-        <v>1000000</v>
+        <v>5000</v>
       </c>
       <c r="X360">
         <v>18000</v>
@@ -34829,19 +34997,25 @@
         <v>260</v>
       </c>
       <c r="AE360">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="AF360">
         <v>0</v>
       </c>
       <c r="AG360">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AH360">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AI360">
         <v>0</v>
+      </c>
+      <c r="AK360">
+        <v>1</v>
+      </c>
+      <c r="AL360">
+        <v>1</v>
       </c>
       <c r="AM360">
         <v>1000000000</v>
@@ -34870,20 +35044,20 @@
         <v>735</v>
       </c>
       <c r="C361">
-        <v>0.75</v>
+        <v>0.35</v>
       </c>
       <c r="G361">
+        <v>0.25</v>
+      </c>
+      <c r="J361">
+        <v>1</v>
+      </c>
+      <c r="K361">
+        <v>0</v>
+      </c>
+      <c r="L361">
         <v>0.5</v>
       </c>
-      <c r="J361">
-        <v>2</v>
-      </c>
-      <c r="K361">
-        <v>0</v>
-      </c>
-      <c r="L361">
-        <v>1</v>
-      </c>
       <c r="M361">
         <v>0</v>
       </c>
@@ -34909,13 +35083,13 @@
         <v>0</v>
       </c>
       <c r="U361">
-        <v>0.58</v>
+        <v>0.25</v>
       </c>
       <c r="V361">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="W361">
-        <v>1000000</v>
+        <v>10000</v>
       </c>
       <c r="X361">
         <v>20000</v>
@@ -34927,7 +35101,7 @@
         <v>260</v>
       </c>
       <c r="AE361">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AF361">
         <v>0</v>
@@ -34936,7 +35110,7 @@
         <v>0</v>
       </c>
       <c r="AH361">
-        <v>0.45</v>
+        <v>0.05</v>
       </c>
       <c r="AI361">
         <v>0</v>
@@ -34971,19 +35145,19 @@
         <v>737</v>
       </c>
       <c r="C362">
+        <v>0</v>
+      </c>
+      <c r="D362">
+        <v>0</v>
+      </c>
+      <c r="E362">
+        <v>0.0</v>
+      </c>
+      <c r="H362">
         <v>1</v>
       </c>
-      <c r="D362">
-        <v>1</v>
-      </c>
-      <c r="E362">
-        <v>0.75</v>
-      </c>
-      <c r="H362">
-        <v>2</v>
-      </c>
       <c r="K362">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L362">
         <v>0</v>
@@ -35013,13 +35187,13 @@
         <v>0</v>
       </c>
       <c r="U362">
-        <v>0.58</v>
+        <v>0</v>
       </c>
       <c r="V362">
         <v>0</v>
       </c>
       <c r="W362">
-        <v>1500000</v>
+        <v>15000</v>
       </c>
       <c r="X362">
         <v>25000</v>
@@ -35031,19 +35205,19 @@
         <v>250</v>
       </c>
       <c r="AE362">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="AF362">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="AG362">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AH362">
-        <v>0.2</v>
+        <v>0.13</v>
       </c>
       <c r="AI362">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="AL362">
         <v>1</v>
@@ -35055,7 +35229,7 @@
         <v>46</v>
       </c>
       <c r="AO362">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="AP362">
         <v>0</v>
@@ -35105,7 +35279,7 @@
         <v>0</v>
       </c>
       <c r="U363">
-        <v>0.7</v>
+        <v>0.35</v>
       </c>
       <c r="V363">
         <v>0</v>
@@ -35123,16 +35297,16 @@
         <v>260</v>
       </c>
       <c r="AE363">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AF363">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG363">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH363">
-        <v>0.02</v>
+        <v>0.14</v>
       </c>
       <c r="AI363">
         <v>0</v>
@@ -35200,7 +35374,7 @@
         <v>0</v>
       </c>
       <c r="U364">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="V364">
         <v>0</v>
@@ -35239,10 +35413,13 @@
         <v>49</v>
       </c>
       <c r="AO364">
-        <v>0.7</v>
+        <v>0.35</v>
+      </c>
+      <c r="AP364">
+        <v>0</v>
       </c>
       <c r="AQ364">
-        <v>0.68</v>
+        <v>0.18</v>
       </c>
       <c r="AR364">
         <v>0.05</v>
@@ -35256,7 +35433,7 @@
         <v>743</v>
       </c>
       <c r="J365">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K365">
         <v>0</v>
@@ -35277,7 +35454,7 @@
         <v>0</v>
       </c>
       <c r="Q365">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R365">
         <v>0</v>
@@ -35289,13 +35466,13 @@
         <v>1</v>
       </c>
       <c r="U365">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="V365">
         <v>0</v>
       </c>
       <c r="W365">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="X365">
         <v>5000</v>
@@ -35307,19 +35484,19 @@
         <v>260</v>
       </c>
       <c r="AE365">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="AF365">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG365">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="AH365">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="AI365">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AK365">
         <v>1</v>
@@ -35334,7 +35511,7 @@
         <v>46</v>
       </c>
       <c r="AO365">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
       <c r="AP365">
         <v>0.1</v>
@@ -35343,7 +35520,7 @@
         <v>0</v>
       </c>
       <c r="AR365">
-        <v>0.68</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="366" spans="1:44">
@@ -35390,13 +35567,13 @@
         <v>0</v>
       </c>
       <c r="U366">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="V366">
         <v>0</v>
       </c>
       <c r="W366">
-        <v>3000</v>
+        <v>25000</v>
       </c>
       <c r="X366">
         <v>8000</v>
@@ -35408,19 +35585,19 @@
         <v>260</v>
       </c>
       <c r="AE366">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="AF366">
         <v>0</v>
       </c>
       <c r="AG366">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="AH366">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AI366">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AK366">
         <v>1</v>
@@ -35438,13 +35615,13 @@
         <v>0</v>
       </c>
       <c r="AP366">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AQ366">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="AR366">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="367" spans="1:44">
@@ -35455,13 +35632,13 @@
         <v>747</v>
       </c>
       <c r="I367">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="K367">
         <v>0</v>
       </c>
       <c r="L367">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="M367">
         <v>0</v>
@@ -35488,13 +35665,13 @@
         <v>0</v>
       </c>
       <c r="U367">
-        <v>0.6</v>
+        <v>0.25</v>
       </c>
       <c r="V367">
         <v>0</v>
       </c>
       <c r="W367">
-        <v>4000000</v>
+        <v>50000</v>
       </c>
       <c r="X367">
         <v>8000</v>
@@ -35509,7 +35686,7 @@
         <v>0</v>
       </c>
       <c r="AF367">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="AG367">
         <v>0</v>
@@ -35530,7 +35707,7 @@
         <v>46</v>
       </c>
       <c r="AO367">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="AP367">
         <v>0.15</v>
@@ -35539,7 +35716,7 @@
         <v>0</v>
       </c>
       <c r="AR367">
-        <v>0.85</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="368" spans="1:44">
@@ -35550,22 +35727,22 @@
         <v>749</v>
       </c>
       <c r="C368">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="D368">
-        <v>3</v>
+        <v>0.1</v>
       </c>
       <c r="E368">
-        <v>3.0</v>
+        <v>0.75</v>
       </c>
       <c r="J368">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K368">
         <v>0</v>
       </c>
       <c r="L368">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M368">
         <v>0</v>
@@ -35592,10 +35769,10 @@
         <v>0</v>
       </c>
       <c r="V368">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="W368">
-        <v>2000000</v>
+        <v>100000</v>
       </c>
       <c r="X368">
         <v>12000</v>
@@ -35607,7 +35784,7 @@
         <v>260</v>
       </c>
       <c r="AE368">
-        <v>500</v>
+        <v>1.5</v>
       </c>
       <c r="AF368">
         <v>0</v>
@@ -35616,7 +35793,7 @@
         <v>0</v>
       </c>
       <c r="AH368">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="AI368">
         <v>0</v>
@@ -35631,13 +35808,16 @@
         <v>49</v>
       </c>
       <c r="AO368">
-        <v>0.8</v>
+        <v>0.45</v>
+      </c>
+      <c r="AP368">
+        <v>0</v>
       </c>
       <c r="AQ368">
-        <v>0.99</v>
+        <v>0.2</v>
       </c>
       <c r="AR368">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="369" spans="1:44">
@@ -35654,25 +35834,25 @@
         <v>0</v>
       </c>
       <c r="M369">
-        <v>0.7</v>
+        <v>0.35</v>
       </c>
       <c r="N369">
-        <v>0.7</v>
+        <v>0.35</v>
       </c>
       <c r="O369">
-        <v>0.7</v>
+        <v>0.35</v>
       </c>
       <c r="P369">
-        <v>0.7</v>
+        <v>0.35</v>
       </c>
       <c r="Q369">
-        <v>0.7</v>
+        <v>0.35</v>
       </c>
       <c r="R369">
-        <v>0.7</v>
+        <v>0.35</v>
       </c>
       <c r="S369">
-        <v>0.7</v>
+        <v>0.35</v>
       </c>
       <c r="T369">
         <v>1</v>
@@ -35681,7 +35861,7 @@
         <v>0</v>
       </c>
       <c r="W369">
-        <v>5000</v>
+        <v>110000</v>
       </c>
       <c r="X369">
         <v>12000</v>
@@ -35693,7 +35873,7 @@
         <v>260</v>
       </c>
       <c r="AE369">
-        <v>3</v>
+        <v>1.8</v>
       </c>
       <c r="AF369">
         <v>0</v>
@@ -35706,9 +35886,6 @@
       </c>
       <c r="AI369">
         <v>0</v>
-      </c>
-      <c r="AK369">
-        <v>1</v>
       </c>
       <c r="AL369">
         <v>1</v>
@@ -35720,13 +35897,1923 @@
         <v>46</v>
       </c>
       <c r="AO369">
+        <v>0.15</v>
+      </c>
+      <c r="AP369">
+        <v>0</v>
+      </c>
+      <c r="AQ369">
+        <v>0.15</v>
+      </c>
+      <c r="AR369">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="370" spans="1:44">
+      <c r="A370" t="s">
+        <v>752</v>
+      </c>
+      <c r="B370" t="s">
+        <v>753</v>
+      </c>
+      <c r="C370">
+        <v>1.5</v>
+      </c>
+      <c r="E370">
+        <v>1.5</v>
+      </c>
+      <c r="F370">
+        <v>2</v>
+      </c>
+      <c r="G370">
+        <v>0.5</v>
+      </c>
+      <c r="H370">
+        <v>1.8</v>
+      </c>
+      <c r="K370">
+        <v>0</v>
+      </c>
+      <c r="L370">
+        <v>0</v>
+      </c>
+      <c r="M370">
+        <v>0</v>
+      </c>
+      <c r="N370">
+        <v>0</v>
+      </c>
+      <c r="O370">
+        <v>0</v>
+      </c>
+      <c r="P370">
+        <v>0</v>
+      </c>
+      <c r="Q370">
+        <v>0</v>
+      </c>
+      <c r="R370">
+        <v>0</v>
+      </c>
+      <c r="S370">
+        <v>0</v>
+      </c>
+      <c r="T370">
+        <v>0</v>
+      </c>
+      <c r="V370">
+        <v>0.3</v>
+      </c>
+      <c r="W370">
+        <v>500000</v>
+      </c>
+      <c r="X370">
+        <v>15000</v>
+      </c>
+      <c r="Y370">
+        <v>173</v>
+      </c>
+      <c r="Z370">
+        <v>280</v>
+      </c>
+      <c r="AE370">
+        <v>1.8</v>
+      </c>
+      <c r="AF370">
+        <v>0</v>
+      </c>
+      <c r="AG370">
+        <v>1.5</v>
+      </c>
+      <c r="AH370">
+        <v>0.3</v>
+      </c>
+      <c r="AI370">
+        <v>0</v>
+      </c>
+      <c r="AL370">
+        <v>1</v>
+      </c>
+      <c r="AM370">
+        <v>3500000000</v>
+      </c>
+      <c r="AN370" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO370">
+        <v>0</v>
+      </c>
+      <c r="AQ370">
+        <v>0</v>
+      </c>
+      <c r="AR370">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371" spans="1:44">
+      <c r="A371" t="s">
+        <v>754</v>
+      </c>
+      <c r="B371" t="s">
+        <v>755</v>
+      </c>
+      <c r="C371">
+        <v>1.5</v>
+      </c>
+      <c r="G371">
+        <v>0.75</v>
+      </c>
+      <c r="J371">
+        <v>2</v>
+      </c>
+      <c r="K371">
+        <v>0</v>
+      </c>
+      <c r="L371">
+        <v>1.8</v>
+      </c>
+      <c r="M371">
+        <v>0</v>
+      </c>
+      <c r="N371">
+        <v>0</v>
+      </c>
+      <c r="O371">
+        <v>0</v>
+      </c>
+      <c r="P371">
+        <v>0</v>
+      </c>
+      <c r="Q371">
+        <v>0</v>
+      </c>
+      <c r="R371">
+        <v>0</v>
+      </c>
+      <c r="S371">
+        <v>0</v>
+      </c>
+      <c r="T371">
+        <v>0</v>
+      </c>
+      <c r="V371">
+        <v>0.3</v>
+      </c>
+      <c r="W371">
+        <v>500000</v>
+      </c>
+      <c r="X371">
+        <v>15000</v>
+      </c>
+      <c r="Y371">
+        <v>173</v>
+      </c>
+      <c r="Z371">
+        <v>280</v>
+      </c>
+      <c r="AE371">
+        <v>1.3</v>
+      </c>
+      <c r="AF371">
+        <v>0</v>
+      </c>
+      <c r="AG371">
+        <v>0</v>
+      </c>
+      <c r="AH371">
+        <v>0.3</v>
+      </c>
+      <c r="AI371">
+        <v>0</v>
+      </c>
+      <c r="AL371">
+        <v>1</v>
+      </c>
+      <c r="AM371">
+        <v>3500000000</v>
+      </c>
+      <c r="AN371" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO371">
+        <v>0.15</v>
+      </c>
+      <c r="AQ371">
+        <v>0</v>
+      </c>
+      <c r="AR371">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="372" spans="1:44">
+      <c r="A372" t="s">
+        <v>756</v>
+      </c>
+      <c r="B372" t="s">
+        <v>757</v>
+      </c>
+      <c r="D372">
+        <v>1.5</v>
+      </c>
+      <c r="I372">
+        <v>2</v>
+      </c>
+      <c r="K372">
+        <v>0</v>
+      </c>
+      <c r="L372">
+        <v>1.8</v>
+      </c>
+      <c r="M372">
+        <v>0</v>
+      </c>
+      <c r="N372">
+        <v>0</v>
+      </c>
+      <c r="O372">
+        <v>0</v>
+      </c>
+      <c r="P372">
+        <v>0</v>
+      </c>
+      <c r="Q372">
+        <v>0</v>
+      </c>
+      <c r="R372">
+        <v>0</v>
+      </c>
+      <c r="S372">
+        <v>0</v>
+      </c>
+      <c r="T372">
+        <v>0</v>
+      </c>
+      <c r="V372">
+        <v>0.3</v>
+      </c>
+      <c r="W372">
+        <v>500000</v>
+      </c>
+      <c r="X372">
+        <v>15000</v>
+      </c>
+      <c r="Y372">
+        <v>173</v>
+      </c>
+      <c r="Z372">
+        <v>280</v>
+      </c>
+      <c r="AE372">
+        <v>0</v>
+      </c>
+      <c r="AF372">
+        <v>1.5</v>
+      </c>
+      <c r="AG372">
+        <v>0</v>
+      </c>
+      <c r="AH372">
+        <v>0.3</v>
+      </c>
+      <c r="AI372">
+        <v>0</v>
+      </c>
+      <c r="AL372">
+        <v>1</v>
+      </c>
+      <c r="AM372">
+        <v>3500000000</v>
+      </c>
+      <c r="AN372" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO372">
+        <v>0</v>
+      </c>
+      <c r="AQ372">
+        <v>0</v>
+      </c>
+      <c r="AR372">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="373" spans="1:44">
+      <c r="A373" t="s">
+        <v>758</v>
+      </c>
+      <c r="B373" t="s">
+        <v>759</v>
+      </c>
+      <c r="C373">
+        <v>1.5</v>
+      </c>
+      <c r="D373">
+        <v>1</v>
+      </c>
+      <c r="H373">
+        <v>2</v>
+      </c>
+      <c r="K373">
+        <v>1.8</v>
+      </c>
+      <c r="L373">
+        <v>0</v>
+      </c>
+      <c r="M373">
+        <v>0</v>
+      </c>
+      <c r="N373">
+        <v>0</v>
+      </c>
+      <c r="O373">
+        <v>0</v>
+      </c>
+      <c r="P373">
+        <v>0</v>
+      </c>
+      <c r="Q373">
+        <v>0</v>
+      </c>
+      <c r="R373">
+        <v>0</v>
+      </c>
+      <c r="S373">
+        <v>0</v>
+      </c>
+      <c r="T373">
+        <v>0</v>
+      </c>
+      <c r="V373">
+        <v>0.3</v>
+      </c>
+      <c r="W373">
+        <v>500000</v>
+      </c>
+      <c r="X373">
+        <v>15000</v>
+      </c>
+      <c r="Y373">
+        <v>173</v>
+      </c>
+      <c r="Z373">
+        <v>280</v>
+      </c>
+      <c r="AE373">
+        <v>1.5</v>
+      </c>
+      <c r="AF373">
+        <v>0.5</v>
+      </c>
+      <c r="AG373">
+        <v>0.1</v>
+      </c>
+      <c r="AH373">
+        <v>0.3</v>
+      </c>
+      <c r="AI373">
+        <v>0</v>
+      </c>
+      <c r="AL373">
+        <v>1</v>
+      </c>
+      <c r="AM373">
+        <v>3500000000</v>
+      </c>
+      <c r="AN373" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO373">
+        <v>0</v>
+      </c>
+      <c r="AQ373">
+        <v>0</v>
+      </c>
+      <c r="AR373">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374" spans="1:44">
+      <c r="A374" t="s">
+        <v>760</v>
+      </c>
+      <c r="B374" t="s">
+        <v>761</v>
+      </c>
+      <c r="C374">
+        <v>1</v>
+      </c>
+      <c r="H374">
+        <v>2</v>
+      </c>
+      <c r="K374">
+        <v>1.9</v>
+      </c>
+      <c r="L374">
+        <v>0</v>
+      </c>
+      <c r="M374">
+        <v>0</v>
+      </c>
+      <c r="N374">
+        <v>0</v>
+      </c>
+      <c r="O374">
+        <v>0</v>
+      </c>
+      <c r="P374">
+        <v>0</v>
+      </c>
+      <c r="Q374">
+        <v>0</v>
+      </c>
+      <c r="R374">
+        <v>0</v>
+      </c>
+      <c r="S374">
+        <v>0</v>
+      </c>
+      <c r="T374">
+        <v>0</v>
+      </c>
+      <c r="V374">
+        <v>0.3</v>
+      </c>
+      <c r="W374">
+        <v>500000</v>
+      </c>
+      <c r="X374">
+        <v>15000</v>
+      </c>
+      <c r="Y374">
+        <v>173</v>
+      </c>
+      <c r="Z374">
+        <v>280</v>
+      </c>
+      <c r="AA374" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC374">
+        <v>0.75</v>
+      </c>
+      <c r="AD374">
+        <v>0.25</v>
+      </c>
+      <c r="AE374">
+        <v>0.8</v>
+      </c>
+      <c r="AF374">
+        <v>0</v>
+      </c>
+      <c r="AG374">
+        <v>0</v>
+      </c>
+      <c r="AH374">
+        <v>0.3</v>
+      </c>
+      <c r="AI374">
+        <v>0</v>
+      </c>
+      <c r="AL374">
+        <v>1</v>
+      </c>
+      <c r="AM374">
+        <v>3500000000</v>
+      </c>
+      <c r="AN374" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO374">
+        <v>0</v>
+      </c>
+      <c r="AQ374">
+        <v>0</v>
+      </c>
+      <c r="AR374">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="375" spans="1:44">
+      <c r="A375" t="s">
+        <v>762</v>
+      </c>
+      <c r="B375" t="s">
+        <v>763</v>
+      </c>
+      <c r="C375">
+        <v>0.5</v>
+      </c>
+      <c r="D375">
+        <v>0.1</v>
+      </c>
+      <c r="G375">
+        <v>2</v>
+      </c>
+      <c r="K375">
+        <v>0</v>
+      </c>
+      <c r="L375">
+        <v>0</v>
+      </c>
+      <c r="M375">
+        <v>0</v>
+      </c>
+      <c r="N375">
+        <v>0</v>
+      </c>
+      <c r="O375">
+        <v>0</v>
+      </c>
+      <c r="P375">
+        <v>0</v>
+      </c>
+      <c r="Q375">
+        <v>0</v>
+      </c>
+      <c r="R375">
+        <v>0</v>
+      </c>
+      <c r="S375">
+        <v>0</v>
+      </c>
+      <c r="T375">
+        <v>0</v>
+      </c>
+      <c r="U375">
+        <v>0.5</v>
+      </c>
+      <c r="V375">
+        <v>0.3</v>
+      </c>
+      <c r="W375">
+        <v>500000</v>
+      </c>
+      <c r="X375">
+        <v>15000</v>
+      </c>
+      <c r="Y375">
+        <v>173</v>
+      </c>
+      <c r="Z375">
+        <v>280</v>
+      </c>
+      <c r="AE375">
+        <v>0.1</v>
+      </c>
+      <c r="AF375">
+        <v>0</v>
+      </c>
+      <c r="AG375">
+        <v>0</v>
+      </c>
+      <c r="AH375">
+        <v>0.3</v>
+      </c>
+      <c r="AI375">
+        <v>0</v>
+      </c>
+      <c r="AL375">
+        <v>1</v>
+      </c>
+      <c r="AM375">
+        <v>3500000000</v>
+      </c>
+      <c r="AN375" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO375">
+        <v>0</v>
+      </c>
+      <c r="AQ375">
+        <v>0</v>
+      </c>
+      <c r="AR375">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="376" spans="1:44">
+      <c r="A376" t="s">
+        <v>764</v>
+      </c>
+      <c r="B376" t="s">
+        <v>765</v>
+      </c>
+      <c r="C376">
+        <v>1.8</v>
+      </c>
+      <c r="E376">
+        <v>1.8</v>
+      </c>
+      <c r="F376">
+        <v>2.5</v>
+      </c>
+      <c r="G376">
+        <v>1.5</v>
+      </c>
+      <c r="H376">
+        <v>2</v>
+      </c>
+      <c r="K376">
+        <v>0</v>
+      </c>
+      <c r="L376">
+        <v>0</v>
+      </c>
+      <c r="M376">
+        <v>1.5</v>
+      </c>
+      <c r="N376">
+        <v>1.5</v>
+      </c>
+      <c r="O376">
+        <v>1.5</v>
+      </c>
+      <c r="P376">
+        <v>0</v>
+      </c>
+      <c r="Q376">
+        <v>0</v>
+      </c>
+      <c r="R376">
+        <v>0</v>
+      </c>
+      <c r="S376">
+        <v>0</v>
+      </c>
+      <c r="T376">
+        <v>1</v>
+      </c>
+      <c r="V376">
+        <v>0</v>
+      </c>
+      <c r="W376">
+        <v>1000000</v>
+      </c>
+      <c r="X376">
+        <v>30000</v>
+      </c>
+      <c r="Y376">
+        <v>178</v>
+      </c>
+      <c r="Z376">
+        <v>290</v>
+      </c>
+      <c r="AE376">
+        <v>1.5</v>
+      </c>
+      <c r="AF376">
+        <v>0</v>
+      </c>
+      <c r="AG376">
+        <v>0.45</v>
+      </c>
+      <c r="AH376">
+        <v>0.5</v>
+      </c>
+      <c r="AI376">
+        <v>0</v>
+      </c>
+      <c r="AL376">
+        <v>1</v>
+      </c>
+      <c r="AM376">
+        <v>4200000000</v>
+      </c>
+      <c r="AN376" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO376">
+        <v>0</v>
+      </c>
+      <c r="AP376">
+        <v>0.1</v>
+      </c>
+      <c r="AQ376">
+        <v>0</v>
+      </c>
+      <c r="AR376">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="377" spans="1:44">
+      <c r="A377" t="s">
+        <v>766</v>
+      </c>
+      <c r="B377" t="s">
+        <v>767</v>
+      </c>
+      <c r="C377">
+        <v>1.8</v>
+      </c>
+      <c r="J377">
+        <v>2.5</v>
+      </c>
+      <c r="K377">
+        <v>0</v>
+      </c>
+      <c r="L377">
+        <v>2.3</v>
+      </c>
+      <c r="M377">
+        <v>0</v>
+      </c>
+      <c r="N377">
+        <v>0</v>
+      </c>
+      <c r="O377">
+        <v>0</v>
+      </c>
+      <c r="P377">
+        <v>0</v>
+      </c>
+      <c r="Q377">
+        <v>1.5</v>
+      </c>
+      <c r="R377">
+        <v>0</v>
+      </c>
+      <c r="S377">
+        <v>1.8</v>
+      </c>
+      <c r="T377">
+        <v>1</v>
+      </c>
+      <c r="V377">
+        <v>0.5</v>
+      </c>
+      <c r="W377">
+        <v>1000000</v>
+      </c>
+      <c r="X377">
+        <v>30000</v>
+      </c>
+      <c r="Y377">
+        <v>178</v>
+      </c>
+      <c r="Z377">
+        <v>290</v>
+      </c>
+      <c r="AE377">
+        <v>2</v>
+      </c>
+      <c r="AF377">
+        <v>0</v>
+      </c>
+      <c r="AG377">
+        <v>0</v>
+      </c>
+      <c r="AH377">
+        <v>0.5</v>
+      </c>
+      <c r="AI377">
+        <v>0</v>
+      </c>
+      <c r="AL377">
+        <v>1</v>
+      </c>
+      <c r="AM377">
+        <v>4200000000</v>
+      </c>
+      <c r="AN377" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO377">
+        <v>0.3</v>
+      </c>
+      <c r="AP377">
+        <v>0.1</v>
+      </c>
+      <c r="AQ377">
+        <v>0</v>
+      </c>
+      <c r="AR377">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="378" spans="1:44">
+      <c r="A378" t="s">
+        <v>768</v>
+      </c>
+      <c r="B378" t="s">
+        <v>769</v>
+      </c>
+      <c r="D378">
+        <v>2</v>
+      </c>
+      <c r="I378">
+        <v>2.5</v>
+      </c>
+      <c r="K378">
+        <v>0</v>
+      </c>
+      <c r="L378">
+        <v>2.3</v>
+      </c>
+      <c r="M378">
+        <v>0</v>
+      </c>
+      <c r="N378">
+        <v>0</v>
+      </c>
+      <c r="O378">
+        <v>0</v>
+      </c>
+      <c r="P378">
+        <v>1.8</v>
+      </c>
+      <c r="Q378">
+        <v>0</v>
+      </c>
+      <c r="R378">
+        <v>0</v>
+      </c>
+      <c r="S378">
+        <v>1.3</v>
+      </c>
+      <c r="T378">
+        <v>1</v>
+      </c>
+      <c r="V378">
+        <v>0.5</v>
+      </c>
+      <c r="W378">
+        <v>1000000</v>
+      </c>
+      <c r="X378">
+        <v>30000</v>
+      </c>
+      <c r="Y378">
+        <v>178</v>
+      </c>
+      <c r="Z378">
+        <v>290</v>
+      </c>
+      <c r="AE378">
+        <v>0</v>
+      </c>
+      <c r="AF378">
+        <v>0.55</v>
+      </c>
+      <c r="AG378">
+        <v>0</v>
+      </c>
+      <c r="AH378">
+        <v>0.5</v>
+      </c>
+      <c r="AI378">
+        <v>0</v>
+      </c>
+      <c r="AL378">
+        <v>1</v>
+      </c>
+      <c r="AM378">
+        <v>4200000000</v>
+      </c>
+      <c r="AN378" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO378">
+        <v>0</v>
+      </c>
+      <c r="AP378">
+        <v>0.1</v>
+      </c>
+      <c r="AQ378">
+        <v>0</v>
+      </c>
+      <c r="AR378">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="379" spans="1:44">
+      <c r="A379" t="s">
+        <v>770</v>
+      </c>
+      <c r="B379" t="s">
+        <v>767</v>
+      </c>
+      <c r="C379">
+        <v>1.9</v>
+      </c>
+      <c r="D379">
+        <v>0.8</v>
+      </c>
+      <c r="H379">
+        <v>2.5</v>
+      </c>
+      <c r="K379">
+        <v>2.1</v>
+      </c>
+      <c r="L379">
+        <v>0</v>
+      </c>
+      <c r="M379">
+        <v>0</v>
+      </c>
+      <c r="N379">
+        <v>0</v>
+      </c>
+      <c r="O379">
+        <v>1.5</v>
+      </c>
+      <c r="P379">
+        <v>0</v>
+      </c>
+      <c r="Q379">
+        <v>0</v>
+      </c>
+      <c r="R379">
+        <v>1.3</v>
+      </c>
+      <c r="S379">
+        <v>0</v>
+      </c>
+      <c r="T379">
+        <v>1</v>
+      </c>
+      <c r="V379">
+        <v>0.5</v>
+      </c>
+      <c r="W379">
+        <v>1000000</v>
+      </c>
+      <c r="X379">
+        <v>30000</v>
+      </c>
+      <c r="Y379">
+        <v>178</v>
+      </c>
+      <c r="Z379">
+        <v>290</v>
+      </c>
+      <c r="AE379">
+        <v>1.5</v>
+      </c>
+      <c r="AF379">
+        <v>0.5</v>
+      </c>
+      <c r="AG379">
+        <v>0</v>
+      </c>
+      <c r="AH379">
+        <v>0.5</v>
+      </c>
+      <c r="AI379">
+        <v>0.25</v>
+      </c>
+      <c r="AL379">
+        <v>1</v>
+      </c>
+      <c r="AM379">
+        <v>4200000000</v>
+      </c>
+      <c r="AN379" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO379">
+        <v>0</v>
+      </c>
+      <c r="AP379">
+        <v>0.1</v>
+      </c>
+      <c r="AQ379">
+        <v>0</v>
+      </c>
+      <c r="AR379">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="380" spans="1:44">
+      <c r="A380" t="s">
+        <v>771</v>
+      </c>
+      <c r="B380" t="s">
+        <v>772</v>
+      </c>
+      <c r="C380">
+        <v>1.7</v>
+      </c>
+      <c r="H380">
+        <v>2.5</v>
+      </c>
+      <c r="K380">
+        <v>2.3</v>
+      </c>
+      <c r="L380">
+        <v>0</v>
+      </c>
+      <c r="M380">
+        <v>0</v>
+      </c>
+      <c r="N380">
+        <v>0</v>
+      </c>
+      <c r="O380">
+        <v>1.8</v>
+      </c>
+      <c r="P380">
+        <v>0</v>
+      </c>
+      <c r="Q380">
+        <v>0</v>
+      </c>
+      <c r="R380">
+        <v>1.5</v>
+      </c>
+      <c r="S380">
+        <v>0</v>
+      </c>
+      <c r="T380">
+        <v>1</v>
+      </c>
+      <c r="V380">
+        <v>0.5</v>
+      </c>
+      <c r="W380">
+        <v>1000000</v>
+      </c>
+      <c r="X380">
+        <v>30000</v>
+      </c>
+      <c r="Y380">
+        <v>178</v>
+      </c>
+      <c r="Z380">
+        <v>290</v>
+      </c>
+      <c r="AA380" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC380">
+        <v>1</v>
+      </c>
+      <c r="AD380">
+        <v>0.5</v>
+      </c>
+      <c r="AE380">
+        <v>1</v>
+      </c>
+      <c r="AF380">
+        <v>0</v>
+      </c>
+      <c r="AG380">
+        <v>0</v>
+      </c>
+      <c r="AH380">
+        <v>0.55</v>
+      </c>
+      <c r="AI380">
+        <v>0.3</v>
+      </c>
+      <c r="AL380">
+        <v>1</v>
+      </c>
+      <c r="AM380">
+        <v>4200000000</v>
+      </c>
+      <c r="AN380" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO380">
+        <v>0.1</v>
+      </c>
+      <c r="AP380">
+        <v>0.1</v>
+      </c>
+      <c r="AQ380">
+        <v>0.35</v>
+      </c>
+      <c r="AR380">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="381" spans="1:44">
+      <c r="A381" t="s">
+        <v>773</v>
+      </c>
+      <c r="B381" t="s">
+        <v>774</v>
+      </c>
+      <c r="C381">
+        <v>1.5</v>
+      </c>
+      <c r="D381">
+        <v>0.8</v>
+      </c>
+      <c r="G381">
+        <v>2.5</v>
+      </c>
+      <c r="K381">
+        <v>0</v>
+      </c>
+      <c r="L381">
+        <v>0</v>
+      </c>
+      <c r="M381">
+        <v>0</v>
+      </c>
+      <c r="N381">
+        <v>2</v>
+      </c>
+      <c r="O381">
+        <v>0</v>
+      </c>
+      <c r="P381">
+        <v>0</v>
+      </c>
+      <c r="Q381">
+        <v>0</v>
+      </c>
+      <c r="R381">
+        <v>0</v>
+      </c>
+      <c r="S381">
+        <v>0</v>
+      </c>
+      <c r="T381">
+        <v>1</v>
+      </c>
+      <c r="U381">
+        <v>0.75</v>
+      </c>
+      <c r="V381">
+        <v>0</v>
+      </c>
+      <c r="W381">
+        <v>1000000</v>
+      </c>
+      <c r="X381">
+        <v>30000</v>
+      </c>
+      <c r="Y381">
+        <v>178</v>
+      </c>
+      <c r="Z381">
+        <v>290</v>
+      </c>
+      <c r="AE381">
+        <v>1.5</v>
+      </c>
+      <c r="AF381">
+        <v>0.55</v>
+      </c>
+      <c r="AG381">
+        <v>0</v>
+      </c>
+      <c r="AH381">
+        <v>0.5</v>
+      </c>
+      <c r="AI381">
+        <v>0</v>
+      </c>
+      <c r="AL381">
+        <v>1</v>
+      </c>
+      <c r="AM381">
+        <v>4200000000</v>
+      </c>
+      <c r="AN381" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO381">
+        <v>0</v>
+      </c>
+      <c r="AP381">
+        <v>0.1</v>
+      </c>
+      <c r="AQ381">
+        <v>0</v>
+      </c>
+      <c r="AR381">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="382" spans="1:44">
+      <c r="A382" t="s">
+        <v>775</v>
+      </c>
+      <c r="B382" t="s">
+        <v>776</v>
+      </c>
+      <c r="C382">
+        <v>2.5</v>
+      </c>
+      <c r="D382">
+        <v>0.55</v>
+      </c>
+      <c r="E382">
+        <v>1.0</v>
+      </c>
+      <c r="F382">
+        <v>1</v>
+      </c>
+      <c r="G382">
+        <v>1.5</v>
+      </c>
+      <c r="H382">
+        <v>1</v>
+      </c>
+      <c r="I382">
+        <v>1.3</v>
+      </c>
+      <c r="J382">
+        <v>1.3</v>
+      </c>
+      <c r="K382">
+        <v>1</v>
+      </c>
+      <c r="L382">
+        <v>1.1</v>
+      </c>
+      <c r="M382">
+        <v>0.5</v>
+      </c>
+      <c r="N382">
         <v>0.6</v>
       </c>
-      <c r="AQ369">
-        <v>0</v>
-      </c>
-      <c r="AR369">
+      <c r="O382">
+        <v>0.6</v>
+      </c>
+      <c r="P382">
+        <v>0.5</v>
+      </c>
+      <c r="Q382">
+        <v>0.5</v>
+      </c>
+      <c r="R382">
+        <v>0.6</v>
+      </c>
+      <c r="S382">
+        <v>0.6</v>
+      </c>
+      <c r="T382">
+        <v>1</v>
+      </c>
+      <c r="U382">
+        <v>0.3</v>
+      </c>
+      <c r="V382">
+        <v>0.45</v>
+      </c>
+      <c r="W382">
+        <v>1500000</v>
+      </c>
+      <c r="X382">
+        <v>50000</v>
+      </c>
+      <c r="Y382">
+        <v>183</v>
+      </c>
+      <c r="Z382">
+        <v>295</v>
+      </c>
+      <c r="AE382">
+        <v>0.55</v>
+      </c>
+      <c r="AF382">
+        <v>0.25</v>
+      </c>
+      <c r="AG382">
+        <v>0.15</v>
+      </c>
+      <c r="AH382">
+        <v>0</v>
+      </c>
+      <c r="AI382">
+        <v>0</v>
+      </c>
+      <c r="AK382">
+        <v>1</v>
+      </c>
+      <c r="AL382">
+        <v>1</v>
+      </c>
+      <c r="AM382">
+        <v>4800000000</v>
+      </c>
+      <c r="AN382" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO382">
+        <v>0.35</v>
+      </c>
+      <c r="AP382">
+        <v>0.15</v>
+      </c>
+      <c r="AQ382">
+        <v>0</v>
+      </c>
+      <c r="AR382">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="383" spans="1:44">
+      <c r="A383" t="s">
+        <v>777</v>
+      </c>
+      <c r="B383" t="s">
+        <v>778</v>
+      </c>
+      <c r="F383">
+        <v>2</v>
+      </c>
+      <c r="G383">
+        <v>2</v>
+      </c>
+      <c r="H383">
+        <v>2</v>
+      </c>
+      <c r="I383">
+        <v>2</v>
+      </c>
+      <c r="J383">
+        <v>2</v>
+      </c>
+      <c r="K383">
+        <v>2</v>
+      </c>
+      <c r="L383">
+        <v>2</v>
+      </c>
+      <c r="M383">
+        <v>0.8</v>
+      </c>
+      <c r="N383">
+        <v>0.8</v>
+      </c>
+      <c r="O383">
+        <v>0.8</v>
+      </c>
+      <c r="P383">
+        <v>0.8</v>
+      </c>
+      <c r="Q383">
+        <v>0.8</v>
+      </c>
+      <c r="R383">
+        <v>0.8</v>
+      </c>
+      <c r="S383">
+        <v>0.8</v>
+      </c>
+      <c r="T383">
+        <v>1</v>
+      </c>
+      <c r="U383">
+        <v>0.5</v>
+      </c>
+      <c r="V383">
+        <v>1</v>
+      </c>
+      <c r="W383">
+        <v>1800000</v>
+      </c>
+      <c r="X383">
+        <v>55000</v>
+      </c>
+      <c r="Y383">
+        <v>188</v>
+      </c>
+      <c r="Z383">
+        <v>300</v>
+      </c>
+      <c r="AE383">
+        <v>0.25</v>
+      </c>
+      <c r="AF383">
+        <v>0.25</v>
+      </c>
+      <c r="AG383">
+        <v>0.15</v>
+      </c>
+      <c r="AH383">
+        <v>0</v>
+      </c>
+      <c r="AI383">
+        <v>0</v>
+      </c>
+      <c r="AK383">
+        <v>1</v>
+      </c>
+      <c r="AL383">
+        <v>1</v>
+      </c>
+      <c r="AM383">
+        <v>5000000000</v>
+      </c>
+      <c r="AN383" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO383">
+        <v>0.25</v>
+      </c>
+      <c r="AP383">
+        <v>0</v>
+      </c>
+      <c r="AQ383">
+        <v>0</v>
+      </c>
+      <c r="AR383">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="384" spans="1:44">
+      <c r="A384" t="s">
+        <v>779</v>
+      </c>
+      <c r="B384" t="s">
+        <v>780</v>
+      </c>
+      <c r="K384">
+        <v>0</v>
+      </c>
+      <c r="L384">
+        <v>0</v>
+      </c>
+      <c r="M384">
+        <v>0.85</v>
+      </c>
+      <c r="N384">
+        <v>0.85</v>
+      </c>
+      <c r="O384">
+        <v>0.85</v>
+      </c>
+      <c r="P384">
+        <v>0.85</v>
+      </c>
+      <c r="Q384">
+        <v>0.85</v>
+      </c>
+      <c r="R384">
+        <v>0.85</v>
+      </c>
+      <c r="S384">
+        <v>0.85</v>
+      </c>
+      <c r="T384">
+        <v>1</v>
+      </c>
+      <c r="V384">
+        <v>0</v>
+      </c>
+      <c r="W384">
+        <v>1800000</v>
+      </c>
+      <c r="X384">
+        <v>55000</v>
+      </c>
+      <c r="Y384">
+        <v>193</v>
+      </c>
+      <c r="Z384">
+        <v>300</v>
+      </c>
+      <c r="AE384">
+        <v>1</v>
+      </c>
+      <c r="AF384">
+        <v>1</v>
+      </c>
+      <c r="AG384">
+        <v>1</v>
+      </c>
+      <c r="AH384">
+        <v>0</v>
+      </c>
+      <c r="AI384">
+        <v>0</v>
+      </c>
+      <c r="AK384">
+        <v>1</v>
+      </c>
+      <c r="AL384">
+        <v>1</v>
+      </c>
+      <c r="AM384">
+        <v>5200000000</v>
+      </c>
+      <c r="AN384" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO384">
+        <v>0.5</v>
+      </c>
+      <c r="AQ384">
+        <v>0.6</v>
+      </c>
+      <c r="AR384">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="385" spans="1:44">
+      <c r="A385" t="s">
+        <v>781</v>
+      </c>
+      <c r="B385" t="s">
+        <v>782</v>
+      </c>
+      <c r="C385">
+        <v>1.8</v>
+      </c>
+      <c r="D385">
+        <v>0.6</v>
+      </c>
+      <c r="E385">
+        <v>0.5</v>
+      </c>
+      <c r="K385">
+        <v>0</v>
+      </c>
+      <c r="L385">
+        <v>0</v>
+      </c>
+      <c r="M385">
+        <v>1</v>
+      </c>
+      <c r="N385">
+        <v>1</v>
+      </c>
+      <c r="O385">
+        <v>1</v>
+      </c>
+      <c r="P385">
+        <v>1</v>
+      </c>
+      <c r="Q385">
+        <v>1</v>
+      </c>
+      <c r="R385">
+        <v>1</v>
+      </c>
+      <c r="S385">
+        <v>1</v>
+      </c>
+      <c r="T385">
+        <v>1</v>
+      </c>
+      <c r="U385">
+        <v>0.5</v>
+      </c>
+      <c r="V385">
+        <v>0</v>
+      </c>
+      <c r="W385">
+        <v>2000000</v>
+      </c>
+      <c r="X385">
+        <v>60000</v>
+      </c>
+      <c r="Y385">
+        <v>200</v>
+      </c>
+      <c r="Z385">
+        <v>310</v>
+      </c>
+      <c r="AE385">
+        <v>0</v>
+      </c>
+      <c r="AF385">
+        <v>0</v>
+      </c>
+      <c r="AG385">
+        <v>0</v>
+      </c>
+      <c r="AH385">
+        <v>0</v>
+      </c>
+      <c r="AI385">
+        <v>0</v>
+      </c>
+      <c r="AL385">
+        <v>1</v>
+      </c>
+      <c r="AM385">
+        <v>5500000000</v>
+      </c>
+      <c r="AN385" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO385">
+        <v>0.5</v>
+      </c>
+      <c r="AQ385">
+        <v>0.75</v>
+      </c>
+      <c r="AR385">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="386" spans="1:44">
+      <c r="A386" t="s">
+        <v>783</v>
+      </c>
+      <c r="B386" t="s">
+        <v>784</v>
+      </c>
+      <c r="C386">
+        <v>2</v>
+      </c>
+      <c r="D386">
+        <v>2</v>
+      </c>
+      <c r="E386">
+        <v>2.0</v>
+      </c>
+      <c r="F386">
+        <v>0</v>
+      </c>
+      <c r="G386">
+        <v>0.6</v>
+      </c>
+      <c r="K386">
+        <v>0</v>
+      </c>
+      <c r="L386">
+        <v>0</v>
+      </c>
+      <c r="M386">
+        <v>0</v>
+      </c>
+      <c r="N386">
+        <v>0</v>
+      </c>
+      <c r="O386">
+        <v>0</v>
+      </c>
+      <c r="P386">
+        <v>0</v>
+      </c>
+      <c r="Q386">
+        <v>0</v>
+      </c>
+      <c r="R386">
+        <v>0</v>
+      </c>
+      <c r="S386">
+        <v>0</v>
+      </c>
+      <c r="T386">
+        <v>0</v>
+      </c>
+      <c r="U386">
+        <v>0.8</v>
+      </c>
+      <c r="V386">
+        <v>0</v>
+      </c>
+      <c r="W386">
+        <v>4000000</v>
+      </c>
+      <c r="X386">
+        <v>68000</v>
+      </c>
+      <c r="Y386">
+        <v>208</v>
+      </c>
+      <c r="Z386">
+        <v>310</v>
+      </c>
+      <c r="AE386">
+        <v>0</v>
+      </c>
+      <c r="AF386">
+        <v>0</v>
+      </c>
+      <c r="AG386">
+        <v>0</v>
+      </c>
+      <c r="AH386">
+        <v>0.3</v>
+      </c>
+      <c r="AI386">
+        <v>0</v>
+      </c>
+      <c r="AL386">
+        <v>1</v>
+      </c>
+      <c r="AM386">
+        <v>5800000000</v>
+      </c>
+      <c r="AN386" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO386">
+        <v>0.6</v>
+      </c>
+      <c r="AQ386">
+        <v>0.95</v>
+      </c>
+      <c r="AR386">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387" spans="1:44">
+      <c r="A387" t="s">
+        <v>785</v>
+      </c>
+      <c r="B387" t="s">
+        <v>786</v>
+      </c>
+      <c r="C387">
+        <v>3</v>
+      </c>
+      <c r="D387">
+        <v>1</v>
+      </c>
+      <c r="E387">
+        <v>2.0</v>
+      </c>
+      <c r="K387">
+        <v>0</v>
+      </c>
+      <c r="L387">
+        <v>0</v>
+      </c>
+      <c r="M387">
+        <v>0.9</v>
+      </c>
+      <c r="N387">
+        <v>0.9</v>
+      </c>
+      <c r="O387">
+        <v>0.9</v>
+      </c>
+      <c r="P387">
+        <v>0.9</v>
+      </c>
+      <c r="Q387">
+        <v>0.9</v>
+      </c>
+      <c r="R387">
+        <v>0.9</v>
+      </c>
+      <c r="S387">
+        <v>0.9</v>
+      </c>
+      <c r="T387">
+        <v>1</v>
+      </c>
+      <c r="U387">
+        <v>0</v>
+      </c>
+      <c r="V387">
+        <v>0</v>
+      </c>
+      <c r="W387">
+        <v>4000000</v>
+      </c>
+      <c r="X387">
+        <v>73000</v>
+      </c>
+      <c r="Y387">
+        <v>212</v>
+      </c>
+      <c r="Z387">
+        <v>316</v>
+      </c>
+      <c r="AE387">
+        <v>0</v>
+      </c>
+      <c r="AF387">
+        <v>0</v>
+      </c>
+      <c r="AG387">
+        <v>0</v>
+      </c>
+      <c r="AH387">
+        <v>0</v>
+      </c>
+      <c r="AI387">
+        <v>0</v>
+      </c>
+      <c r="AK387">
+        <v>1</v>
+      </c>
+      <c r="AL387">
+        <v>1</v>
+      </c>
+      <c r="AM387">
+        <v>6000000000</v>
+      </c>
+      <c r="AN387" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO387">
+        <v>0</v>
+      </c>
+      <c r="AQ387">
+        <v>1.1</v>
+      </c>
+      <c r="AR387">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="388" spans="1:44">
+      <c r="A388" t="s">
+        <v>787</v>
+      </c>
+      <c r="B388" t="s">
+        <v>788</v>
+      </c>
+      <c r="F388">
+        <v>2</v>
+      </c>
+      <c r="G388">
+        <v>2</v>
+      </c>
+      <c r="H388">
+        <v>2</v>
+      </c>
+      <c r="I388">
+        <v>2</v>
+      </c>
+      <c r="J388">
+        <v>2</v>
+      </c>
+      <c r="K388">
+        <v>2</v>
+      </c>
+      <c r="L388">
+        <v>2</v>
+      </c>
+      <c r="M388">
+        <v>0</v>
+      </c>
+      <c r="N388">
+        <v>0</v>
+      </c>
+      <c r="O388">
+        <v>0</v>
+      </c>
+      <c r="P388">
+        <v>0</v>
+      </c>
+      <c r="Q388">
+        <v>0</v>
+      </c>
+      <c r="R388">
+        <v>0</v>
+      </c>
+      <c r="S388">
+        <v>0</v>
+      </c>
+      <c r="T388">
+        <v>0</v>
+      </c>
+      <c r="U388">
         <v>0.99</v>
+      </c>
+      <c r="V388">
+        <v>2</v>
+      </c>
+      <c r="W388">
+        <v>4500000</v>
+      </c>
+      <c r="X388">
+        <v>75000</v>
+      </c>
+      <c r="Y388">
+        <v>216</v>
+      </c>
+      <c r="Z388">
+        <v>316</v>
+      </c>
+      <c r="AE388">
+        <v>1.5</v>
+      </c>
+      <c r="AF388">
+        <v>1.5</v>
+      </c>
+      <c r="AG388">
+        <v>1.5</v>
+      </c>
+      <c r="AH388">
+        <v>0</v>
+      </c>
+      <c r="AI388">
+        <v>0</v>
+      </c>
+      <c r="AK388">
+        <v>1</v>
+      </c>
+      <c r="AL388">
+        <v>1</v>
+      </c>
+      <c r="AM388">
+        <v>6500000000</v>
+      </c>
+      <c r="AN388" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO388">
+        <v>1</v>
+      </c>
+      <c r="AQ388">
+        <v>1.5</v>
+      </c>
+      <c r="AR388">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes to kingdom related features
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69171872-0285-CA4A-8E10-8F3DDA4F9D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6324C47-6C41-8B48-B502-B711265FEC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="830">
   <si>
     <t>name</t>
   </si>
@@ -2337,9 +2337,6 @@
     <t>Vampires Deliverance</t>
   </si>
   <si>
-    <t>This relic is best suited for a Vampire as it increases their stats and class bonuses as well as gives other Vampire specific enhancements. This is known as a kill enchantment. That is the damage on it will kill in conjunction with the life stealing.</t>
-  </si>
-  <si>
     <t>Prophets Curse</t>
   </si>
   <si>
@@ -2482,6 +2479,48 @@
   </si>
   <si>
     <t>Let The Creator intervene and smite the enemy for you!</t>
+  </si>
+  <si>
+    <t>This enchantment is best suited for a Heretic as it increases their stats and class bonuses as well as gives other Heretic specific enhancements</t>
+  </si>
+  <si>
+    <t>This enchantment is best suited for a Vampire as it increases their stats and class bonuses as well as gives other Vampire specific enhancements. This is known as a kill enchantment. That is the damage on it will kill in conjunction with the life stealing.</t>
+  </si>
+  <si>
+    <t>Heretics Insanity</t>
+  </si>
+  <si>
+    <t>Prophet's Raging Prayer</t>
+  </si>
+  <si>
+    <t>Earths Maddness</t>
+  </si>
+  <si>
+    <t>Assassins Lucid Dream</t>
+  </si>
+  <si>
+    <t>Vampiric Ascension</t>
+  </si>
+  <si>
+    <t>Prophets Deliverance</t>
+  </si>
+  <si>
+    <t>Soldiers Strike of Faith</t>
+  </si>
+  <si>
+    <t>Fanatics Rage</t>
+  </si>
+  <si>
+    <t>Clerics Heavenly Devotion</t>
+  </si>
+  <si>
+    <t>Natures Seeking Shadows</t>
+  </si>
+  <si>
+    <t>Thieves Courage</t>
+  </si>
+  <si>
+    <t>Vampires Imortal Blood Lust</t>
   </si>
 </sst>
 </file>
@@ -2821,10 +2860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR406"/>
+  <dimension ref="A1:AR418"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D386" workbookViewId="0">
-      <selection activeCell="L404" sqref="L404"/>
+    <sheetView tabSelected="1" topLeftCell="A347" workbookViewId="0">
+      <selection activeCell="A382" sqref="A382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -37051,7 +37090,7 @@
         <v>767</v>
       </c>
       <c r="B381" t="s">
-        <v>768</v>
+        <v>817</v>
       </c>
       <c r="C381">
         <v>0.5</v>
@@ -37149,7 +37188,7 @@
     </row>
     <row r="382" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B382" t="s">
         <v>762</v>
@@ -37244,10 +37283,10 @@
     </row>
     <row r="383" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
+        <v>769</v>
+      </c>
+      <c r="B383" t="s">
         <v>770</v>
-      </c>
-      <c r="B383" t="s">
-        <v>771</v>
       </c>
       <c r="C383">
         <v>0.9</v>
@@ -37348,10 +37387,10 @@
     </row>
     <row r="384" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
+        <v>771</v>
+      </c>
+      <c r="B384" t="s">
         <v>772</v>
-      </c>
-      <c r="B384" t="s">
-        <v>773</v>
       </c>
       <c r="C384">
         <v>0.9</v>
@@ -37443,10 +37482,10 @@
     </row>
     <row r="385" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
+        <v>773</v>
+      </c>
+      <c r="B385" t="s">
         <v>774</v>
-      </c>
-      <c r="B385" t="s">
-        <v>775</v>
       </c>
       <c r="D385">
         <v>1</v>
@@ -37538,10 +37577,10 @@
     </row>
     <row r="386" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B386" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C386">
         <v>0.95</v>
@@ -37636,10 +37675,10 @@
     </row>
     <row r="387" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
+        <v>776</v>
+      </c>
+      <c r="B387" t="s">
         <v>777</v>
-      </c>
-      <c r="B387" t="s">
-        <v>778</v>
       </c>
       <c r="C387">
         <v>0.85</v>
@@ -37740,10 +37779,10 @@
     </row>
     <row r="388" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
+        <v>778</v>
+      </c>
+      <c r="B388" t="s">
         <v>779</v>
-      </c>
-      <c r="B388" t="s">
-        <v>780</v>
       </c>
       <c r="C388">
         <v>0.9</v>
@@ -37841,10 +37880,10 @@
     </row>
     <row r="389" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
+        <v>780</v>
+      </c>
+      <c r="B389" t="s">
         <v>781</v>
-      </c>
-      <c r="B389" t="s">
-        <v>782</v>
       </c>
       <c r="C389">
         <v>2.5</v>
@@ -37960,10 +37999,10 @@
     </row>
     <row r="390" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
+        <v>782</v>
+      </c>
+      <c r="B390" t="s">
         <v>783</v>
-      </c>
-      <c r="B390" t="s">
-        <v>784</v>
       </c>
       <c r="F390">
         <v>0.95</v>
@@ -38070,10 +38109,10 @@
     </row>
     <row r="391" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
+        <v>784</v>
+      </c>
+      <c r="B391" t="s">
         <v>785</v>
-      </c>
-      <c r="B391" t="s">
-        <v>786</v>
       </c>
       <c r="K391">
         <v>0</v>
@@ -38162,10 +38201,10 @@
     </row>
     <row r="392" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
+        <v>786</v>
+      </c>
+      <c r="B392" t="s">
         <v>787</v>
-      </c>
-      <c r="B392" t="s">
-        <v>788</v>
       </c>
       <c r="C392">
         <v>0.9</v>
@@ -38263,10 +38302,10 @@
     </row>
     <row r="393" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
+        <v>788</v>
+      </c>
+      <c r="B393" t="s">
         <v>789</v>
-      </c>
-      <c r="B393" t="s">
-        <v>790</v>
       </c>
       <c r="C393">
         <v>0.95</v>
@@ -38370,10 +38409,10 @@
     </row>
     <row r="394" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
+        <v>790</v>
+      </c>
+      <c r="B394" t="s">
         <v>791</v>
-      </c>
-      <c r="B394" t="s">
-        <v>792</v>
       </c>
       <c r="C394">
         <v>0.95</v>
@@ -38474,10 +38513,10 @@
     </row>
     <row r="395" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
+        <v>792</v>
+      </c>
+      <c r="B395" t="s">
         <v>793</v>
-      </c>
-      <c r="B395" t="s">
-        <v>794</v>
       </c>
       <c r="F395">
         <v>0.95</v>
@@ -38584,10 +38623,10 @@
     </row>
     <row r="396" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
+        <v>794</v>
+      </c>
+      <c r="B396" t="s">
         <v>795</v>
-      </c>
-      <c r="B396" t="s">
-        <v>796</v>
       </c>
       <c r="E396">
         <v>1.5</v>
@@ -38656,7 +38695,7 @@
         <v>0</v>
       </c>
       <c r="AM396">
-        <v>7000000</v>
+        <v>7000000000</v>
       </c>
       <c r="AN396" t="s">
         <v>49</v>
@@ -38673,10 +38712,10 @@
     </row>
     <row r="397" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
+        <v>796</v>
+      </c>
+      <c r="B397" t="s">
         <v>797</v>
-      </c>
-      <c r="B397" t="s">
-        <v>798</v>
       </c>
       <c r="D397">
         <v>0.5</v>
@@ -38768,10 +38807,10 @@
     </row>
     <row r="398" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
+        <v>798</v>
+      </c>
+      <c r="B398" t="s">
         <v>799</v>
-      </c>
-      <c r="B398" t="s">
-        <v>800</v>
       </c>
       <c r="C398">
         <v>0.25</v>
@@ -38875,10 +38914,10 @@
     </row>
     <row r="399" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
+        <v>800</v>
+      </c>
+      <c r="B399" t="s">
         <v>801</v>
-      </c>
-      <c r="B399" t="s">
-        <v>802</v>
       </c>
       <c r="C399">
         <v>0</v>
@@ -38973,10 +39012,10 @@
     </row>
     <row r="400" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
+        <v>802</v>
+      </c>
+      <c r="B400" t="s">
         <v>803</v>
-      </c>
-      <c r="B400" t="s">
-        <v>804</v>
       </c>
       <c r="C400">
         <v>1.2</v>
@@ -39086,10 +39125,10 @@
     </row>
     <row r="401" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
+        <v>804</v>
+      </c>
+      <c r="B401" t="s">
         <v>805</v>
-      </c>
-      <c r="B401" t="s">
-        <v>806</v>
       </c>
       <c r="K401">
         <v>0</v>
@@ -39175,10 +39214,10 @@
     </row>
     <row r="402" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
+        <v>806</v>
+      </c>
+      <c r="B402" t="s">
         <v>807</v>
-      </c>
-      <c r="B402" t="s">
-        <v>808</v>
       </c>
       <c r="K402">
         <v>0</v>
@@ -39270,10 +39309,10 @@
     </row>
     <row r="403" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
+        <v>808</v>
+      </c>
+      <c r="B403" t="s">
         <v>809</v>
-      </c>
-      <c r="B403" t="s">
-        <v>810</v>
       </c>
       <c r="F403">
         <v>1.5</v>
@@ -39374,10 +39413,10 @@
     </row>
     <row r="404" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
+        <v>810</v>
+      </c>
+      <c r="B404" t="s">
         <v>811</v>
-      </c>
-      <c r="B404" t="s">
-        <v>812</v>
       </c>
       <c r="C404">
         <v>1.3</v>
@@ -39493,10 +39532,10 @@
     </row>
     <row r="405" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
+        <v>812</v>
+      </c>
+      <c r="B405" t="s">
         <v>813</v>
-      </c>
-      <c r="B405" t="s">
-        <v>814</v>
       </c>
       <c r="K405">
         <v>0</v>
@@ -39538,7 +39577,7 @@
         <v>5000000</v>
       </c>
       <c r="X405">
-        <v>150000000</v>
+        <v>150000</v>
       </c>
       <c r="Y405">
         <v>300</v>
@@ -39579,19 +39618,19 @@
     </row>
     <row r="406" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
+        <v>814</v>
+      </c>
+      <c r="B406" t="s">
         <v>815</v>
       </c>
-      <c r="B406" t="s">
-        <v>816</v>
-      </c>
       <c r="D406">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E406">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G406">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="K406">
         <v>0</v>
@@ -39676,6 +39715,1194 @@
       </c>
       <c r="AR406">
         <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="407" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A407" t="s">
+        <v>818</v>
+      </c>
+      <c r="B407" t="s">
+        <v>816</v>
+      </c>
+      <c r="C407">
+        <v>1.2</v>
+      </c>
+      <c r="G407">
+        <v>1</v>
+      </c>
+      <c r="J407">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K407">
+        <v>0</v>
+      </c>
+      <c r="L407">
+        <v>1.2</v>
+      </c>
+      <c r="M407">
+        <v>0</v>
+      </c>
+      <c r="N407">
+        <v>0</v>
+      </c>
+      <c r="O407">
+        <v>0</v>
+      </c>
+      <c r="P407">
+        <v>0</v>
+      </c>
+      <c r="Q407">
+        <v>0</v>
+      </c>
+      <c r="R407">
+        <v>0</v>
+      </c>
+      <c r="S407">
+        <v>0</v>
+      </c>
+      <c r="T407">
+        <v>0</v>
+      </c>
+      <c r="V407">
+        <v>0.3</v>
+      </c>
+      <c r="W407">
+        <v>1500000</v>
+      </c>
+      <c r="X407">
+        <v>170000</v>
+      </c>
+      <c r="Y407">
+        <v>320</v>
+      </c>
+      <c r="Z407">
+        <v>360</v>
+      </c>
+      <c r="AE407">
+        <v>1</v>
+      </c>
+      <c r="AF407">
+        <v>0</v>
+      </c>
+      <c r="AG407">
+        <v>0</v>
+      </c>
+      <c r="AH407">
+        <v>0.2</v>
+      </c>
+      <c r="AI407">
+        <v>0</v>
+      </c>
+      <c r="AL407">
+        <v>1</v>
+      </c>
+      <c r="AM407">
+        <v>17000000000</v>
+      </c>
+      <c r="AN407" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO407">
+        <v>0.15</v>
+      </c>
+      <c r="AP407">
+        <v>0</v>
+      </c>
+      <c r="AQ407">
+        <v>0</v>
+      </c>
+      <c r="AR407">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="408" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A408" t="s">
+        <v>819</v>
+      </c>
+      <c r="B408" t="s">
+        <v>762</v>
+      </c>
+      <c r="D408">
+        <v>1.5</v>
+      </c>
+      <c r="I408">
+        <v>2</v>
+      </c>
+      <c r="K408">
+        <v>0</v>
+      </c>
+      <c r="L408">
+        <v>2</v>
+      </c>
+      <c r="M408">
+        <v>0</v>
+      </c>
+      <c r="N408">
+        <v>0</v>
+      </c>
+      <c r="O408">
+        <v>0</v>
+      </c>
+      <c r="P408">
+        <v>0</v>
+      </c>
+      <c r="Q408">
+        <v>0</v>
+      </c>
+      <c r="R408">
+        <v>0</v>
+      </c>
+      <c r="S408">
+        <v>0</v>
+      </c>
+      <c r="T408">
+        <v>0</v>
+      </c>
+      <c r="V408">
+        <v>0.3</v>
+      </c>
+      <c r="W408">
+        <v>1500000</v>
+      </c>
+      <c r="X408">
+        <v>170000</v>
+      </c>
+      <c r="Y408">
+        <v>320</v>
+      </c>
+      <c r="Z408">
+        <v>360</v>
+      </c>
+      <c r="AE408">
+        <v>0</v>
+      </c>
+      <c r="AF408">
+        <v>1.6</v>
+      </c>
+      <c r="AG408">
+        <v>0</v>
+      </c>
+      <c r="AH408">
+        <v>0.6</v>
+      </c>
+      <c r="AI408">
+        <v>0</v>
+      </c>
+      <c r="AL408">
+        <v>1</v>
+      </c>
+      <c r="AM408">
+        <v>17000000000</v>
+      </c>
+      <c r="AN408" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO408">
+        <v>0</v>
+      </c>
+      <c r="AP408">
+        <v>0</v>
+      </c>
+      <c r="AQ408">
+        <v>0</v>
+      </c>
+      <c r="AR408">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="409" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A409" t="s">
+        <v>820</v>
+      </c>
+      <c r="B409" t="s">
+        <v>764</v>
+      </c>
+      <c r="C409">
+        <v>1.2</v>
+      </c>
+      <c r="D409">
+        <v>1.05</v>
+      </c>
+      <c r="H409">
+        <v>1</v>
+      </c>
+      <c r="K409">
+        <v>1.8</v>
+      </c>
+      <c r="L409">
+        <v>0</v>
+      </c>
+      <c r="M409">
+        <v>0</v>
+      </c>
+      <c r="N409">
+        <v>0</v>
+      </c>
+      <c r="O409">
+        <v>0</v>
+      </c>
+      <c r="P409">
+        <v>0</v>
+      </c>
+      <c r="Q409">
+        <v>0</v>
+      </c>
+      <c r="R409">
+        <v>0</v>
+      </c>
+      <c r="S409">
+        <v>0</v>
+      </c>
+      <c r="T409">
+        <v>0</v>
+      </c>
+      <c r="V409">
+        <v>0.3</v>
+      </c>
+      <c r="W409">
+        <v>1500000</v>
+      </c>
+      <c r="X409">
+        <v>170000</v>
+      </c>
+      <c r="Y409">
+        <v>320</v>
+      </c>
+      <c r="Z409">
+        <v>360</v>
+      </c>
+      <c r="AE409">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AF409">
+        <v>0.6</v>
+      </c>
+      <c r="AG409">
+        <v>0.1</v>
+      </c>
+      <c r="AH409">
+        <v>0.2</v>
+      </c>
+      <c r="AI409">
+        <v>0</v>
+      </c>
+      <c r="AL409">
+        <v>1</v>
+      </c>
+      <c r="AM409">
+        <v>17000000000</v>
+      </c>
+      <c r="AN409" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO409">
+        <v>0</v>
+      </c>
+      <c r="AP409">
+        <v>0</v>
+      </c>
+      <c r="AQ409">
+        <v>0</v>
+      </c>
+      <c r="AR409">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="410" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A410" t="s">
+        <v>821</v>
+      </c>
+      <c r="B410" t="s">
+        <v>766</v>
+      </c>
+      <c r="C410">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H410">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K410">
+        <v>1.9</v>
+      </c>
+      <c r="L410">
+        <v>0</v>
+      </c>
+      <c r="M410">
+        <v>0</v>
+      </c>
+      <c r="N410">
+        <v>0</v>
+      </c>
+      <c r="O410">
+        <v>0</v>
+      </c>
+      <c r="P410">
+        <v>0</v>
+      </c>
+      <c r="Q410">
+        <v>0</v>
+      </c>
+      <c r="R410">
+        <v>0</v>
+      </c>
+      <c r="S410">
+        <v>0</v>
+      </c>
+      <c r="T410">
+        <v>0</v>
+      </c>
+      <c r="V410">
+        <v>0.3</v>
+      </c>
+      <c r="W410">
+        <v>1500000</v>
+      </c>
+      <c r="X410">
+        <v>170000</v>
+      </c>
+      <c r="Y410">
+        <v>320</v>
+      </c>
+      <c r="Z410">
+        <v>360</v>
+      </c>
+      <c r="AA410" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC410">
+        <v>1</v>
+      </c>
+      <c r="AD410">
+        <v>0.5</v>
+      </c>
+      <c r="AE410">
+        <v>1</v>
+      </c>
+      <c r="AF410">
+        <v>0</v>
+      </c>
+      <c r="AG410">
+        <v>0</v>
+      </c>
+      <c r="AH410">
+        <v>0.2</v>
+      </c>
+      <c r="AI410">
+        <v>0</v>
+      </c>
+      <c r="AL410">
+        <v>1</v>
+      </c>
+      <c r="AM410">
+        <v>17000000000</v>
+      </c>
+      <c r="AN410" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO410">
+        <v>0</v>
+      </c>
+      <c r="AP410">
+        <v>0</v>
+      </c>
+      <c r="AQ410">
+        <v>0</v>
+      </c>
+      <c r="AR410">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="411" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A411" t="s">
+        <v>822</v>
+      </c>
+      <c r="B411" t="s">
+        <v>817</v>
+      </c>
+      <c r="C411">
+        <v>0.8</v>
+      </c>
+      <c r="D411">
+        <v>0.6</v>
+      </c>
+      <c r="G411">
+        <v>1.05</v>
+      </c>
+      <c r="K411">
+        <v>0</v>
+      </c>
+      <c r="L411">
+        <v>0</v>
+      </c>
+      <c r="M411">
+        <v>0</v>
+      </c>
+      <c r="N411">
+        <v>0</v>
+      </c>
+      <c r="O411">
+        <v>0</v>
+      </c>
+      <c r="P411">
+        <v>0</v>
+      </c>
+      <c r="Q411">
+        <v>0</v>
+      </c>
+      <c r="R411">
+        <v>0</v>
+      </c>
+      <c r="S411">
+        <v>0</v>
+      </c>
+      <c r="T411">
+        <v>0</v>
+      </c>
+      <c r="U411">
+        <v>0.7</v>
+      </c>
+      <c r="V411">
+        <v>0.3</v>
+      </c>
+      <c r="W411">
+        <v>1500000</v>
+      </c>
+      <c r="X411">
+        <v>170000</v>
+      </c>
+      <c r="Y411">
+        <v>320</v>
+      </c>
+      <c r="Z411">
+        <v>360</v>
+      </c>
+      <c r="AE411">
+        <v>0.2</v>
+      </c>
+      <c r="AF411">
+        <v>0</v>
+      </c>
+      <c r="AG411">
+        <v>0</v>
+      </c>
+      <c r="AH411">
+        <v>0.2</v>
+      </c>
+      <c r="AI411">
+        <v>0</v>
+      </c>
+      <c r="AL411">
+        <v>1</v>
+      </c>
+      <c r="AM411">
+        <v>17000000000</v>
+      </c>
+      <c r="AN411" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO411">
+        <v>0</v>
+      </c>
+      <c r="AP411">
+        <v>0</v>
+      </c>
+      <c r="AQ411">
+        <v>0</v>
+      </c>
+      <c r="AR411">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="412" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A412" t="s">
+        <v>823</v>
+      </c>
+      <c r="B412" t="s">
+        <v>762</v>
+      </c>
+      <c r="D412">
+        <v>1.2</v>
+      </c>
+      <c r="I412">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K412">
+        <v>0</v>
+      </c>
+      <c r="L412">
+        <v>1</v>
+      </c>
+      <c r="M412">
+        <v>0</v>
+      </c>
+      <c r="N412">
+        <v>0</v>
+      </c>
+      <c r="O412">
+        <v>0</v>
+      </c>
+      <c r="P412">
+        <v>0</v>
+      </c>
+      <c r="Q412">
+        <v>0</v>
+      </c>
+      <c r="R412">
+        <v>0</v>
+      </c>
+      <c r="S412">
+        <v>0</v>
+      </c>
+      <c r="T412">
+        <v>0</v>
+      </c>
+      <c r="V412">
+        <v>0.3</v>
+      </c>
+      <c r="W412">
+        <v>1500000</v>
+      </c>
+      <c r="X412">
+        <v>170000</v>
+      </c>
+      <c r="Y412">
+        <v>320</v>
+      </c>
+      <c r="Z412">
+        <v>360</v>
+      </c>
+      <c r="AE412">
+        <v>0</v>
+      </c>
+      <c r="AF412">
+        <v>1.6</v>
+      </c>
+      <c r="AG412">
+        <v>0</v>
+      </c>
+      <c r="AH412">
+        <v>0.2</v>
+      </c>
+      <c r="AI412">
+        <v>0</v>
+      </c>
+      <c r="AL412">
+        <v>1</v>
+      </c>
+      <c r="AM412">
+        <v>17000000000</v>
+      </c>
+      <c r="AN412" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO412">
+        <v>0</v>
+      </c>
+      <c r="AP412">
+        <v>0</v>
+      </c>
+      <c r="AQ412">
+        <v>0</v>
+      </c>
+      <c r="AR412">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="413" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A413" t="s">
+        <v>824</v>
+      </c>
+      <c r="B413" t="s">
+        <v>770</v>
+      </c>
+      <c r="C413">
+        <v>1.2</v>
+      </c>
+      <c r="E413">
+        <v>1.8</v>
+      </c>
+      <c r="F413">
+        <v>2.8</v>
+      </c>
+      <c r="G413">
+        <v>1.5</v>
+      </c>
+      <c r="H413">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K413">
+        <v>0</v>
+      </c>
+      <c r="L413">
+        <v>0</v>
+      </c>
+      <c r="M413">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N413">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O413">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P413">
+        <v>0</v>
+      </c>
+      <c r="Q413">
+        <v>0</v>
+      </c>
+      <c r="R413">
+        <v>0</v>
+      </c>
+      <c r="S413">
+        <v>0</v>
+      </c>
+      <c r="T413">
+        <v>1</v>
+      </c>
+      <c r="V413">
+        <v>0</v>
+      </c>
+      <c r="W413">
+        <v>2000000</v>
+      </c>
+      <c r="X413">
+        <v>180000</v>
+      </c>
+      <c r="Y413">
+        <v>330</v>
+      </c>
+      <c r="Z413">
+        <v>360</v>
+      </c>
+      <c r="AE413">
+        <v>1</v>
+      </c>
+      <c r="AF413">
+        <v>0</v>
+      </c>
+      <c r="AG413">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AH413">
+        <v>0.23</v>
+      </c>
+      <c r="AI413">
+        <v>0</v>
+      </c>
+      <c r="AL413">
+        <v>1</v>
+      </c>
+      <c r="AM413">
+        <v>18000000000</v>
+      </c>
+      <c r="AN413" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO413">
+        <v>0</v>
+      </c>
+      <c r="AP413">
+        <v>0.1</v>
+      </c>
+      <c r="AQ413">
+        <v>0</v>
+      </c>
+      <c r="AR413">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="414" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A414" t="s">
+        <v>825</v>
+      </c>
+      <c r="B414" t="s">
+        <v>772</v>
+      </c>
+      <c r="C414">
+        <v>1.2</v>
+      </c>
+      <c r="J414">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K414">
+        <v>0</v>
+      </c>
+      <c r="L414">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M414">
+        <v>0</v>
+      </c>
+      <c r="N414">
+        <v>0</v>
+      </c>
+      <c r="O414">
+        <v>0</v>
+      </c>
+      <c r="P414">
+        <v>0</v>
+      </c>
+      <c r="Q414">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R414">
+        <v>0</v>
+      </c>
+      <c r="S414">
+        <v>1</v>
+      </c>
+      <c r="T414">
+        <v>1</v>
+      </c>
+      <c r="V414">
+        <v>0.5</v>
+      </c>
+      <c r="W414">
+        <v>2000000</v>
+      </c>
+      <c r="X414">
+        <v>180000</v>
+      </c>
+      <c r="Y414">
+        <v>330</v>
+      </c>
+      <c r="Z414">
+        <v>360</v>
+      </c>
+      <c r="AE414">
+        <v>1</v>
+      </c>
+      <c r="AF414">
+        <v>0</v>
+      </c>
+      <c r="AG414">
+        <v>0</v>
+      </c>
+      <c r="AH414">
+        <v>0.23</v>
+      </c>
+      <c r="AI414">
+        <v>0</v>
+      </c>
+      <c r="AL414">
+        <v>1</v>
+      </c>
+      <c r="AM414">
+        <v>18000000000</v>
+      </c>
+      <c r="AN414" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO414">
+        <v>0.3</v>
+      </c>
+      <c r="AP414">
+        <v>0.1</v>
+      </c>
+      <c r="AQ414">
+        <v>0</v>
+      </c>
+      <c r="AR414">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="415" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A415" t="s">
+        <v>826</v>
+      </c>
+      <c r="B415" t="s">
+        <v>774</v>
+      </c>
+      <c r="D415">
+        <v>1</v>
+      </c>
+      <c r="I415">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K415">
+        <v>0</v>
+      </c>
+      <c r="L415">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M415">
+        <v>0</v>
+      </c>
+      <c r="N415">
+        <v>0</v>
+      </c>
+      <c r="O415">
+        <v>0</v>
+      </c>
+      <c r="P415">
+        <v>1</v>
+      </c>
+      <c r="Q415">
+        <v>0</v>
+      </c>
+      <c r="R415">
+        <v>0</v>
+      </c>
+      <c r="S415">
+        <v>0.95</v>
+      </c>
+      <c r="T415">
+        <v>1</v>
+      </c>
+      <c r="V415">
+        <v>0.5</v>
+      </c>
+      <c r="W415">
+        <v>2000000</v>
+      </c>
+      <c r="X415">
+        <v>180000</v>
+      </c>
+      <c r="Y415">
+        <v>330</v>
+      </c>
+      <c r="Z415">
+        <v>360</v>
+      </c>
+      <c r="AE415">
+        <v>0</v>
+      </c>
+      <c r="AF415">
+        <v>0.65</v>
+      </c>
+      <c r="AG415">
+        <v>0</v>
+      </c>
+      <c r="AH415">
+        <v>0.23</v>
+      </c>
+      <c r="AI415">
+        <v>0</v>
+      </c>
+      <c r="AL415">
+        <v>1</v>
+      </c>
+      <c r="AM415">
+        <v>18000000000</v>
+      </c>
+      <c r="AN415" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO415">
+        <v>0</v>
+      </c>
+      <c r="AP415">
+        <v>0.1</v>
+      </c>
+      <c r="AQ415">
+        <v>0</v>
+      </c>
+      <c r="AR415">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="416" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A416" t="s">
+        <v>827</v>
+      </c>
+      <c r="B416" t="s">
+        <v>772</v>
+      </c>
+      <c r="C416">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D416">
+        <v>1</v>
+      </c>
+      <c r="H416">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K416">
+        <v>0.8</v>
+      </c>
+      <c r="L416">
+        <v>0</v>
+      </c>
+      <c r="M416">
+        <v>0</v>
+      </c>
+      <c r="N416">
+        <v>0</v>
+      </c>
+      <c r="O416">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P416">
+        <v>0</v>
+      </c>
+      <c r="Q416">
+        <v>0</v>
+      </c>
+      <c r="R416">
+        <v>0.95</v>
+      </c>
+      <c r="S416">
+        <v>0</v>
+      </c>
+      <c r="T416">
+        <v>1</v>
+      </c>
+      <c r="V416">
+        <v>0.5</v>
+      </c>
+      <c r="W416">
+        <v>2000000</v>
+      </c>
+      <c r="X416">
+        <v>180000</v>
+      </c>
+      <c r="Y416">
+        <v>330</v>
+      </c>
+      <c r="Z416">
+        <v>360</v>
+      </c>
+      <c r="AE416">
+        <v>1.3</v>
+      </c>
+      <c r="AF416">
+        <v>0.6</v>
+      </c>
+      <c r="AG416">
+        <v>0</v>
+      </c>
+      <c r="AH416">
+        <v>0.23</v>
+      </c>
+      <c r="AI416">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AL416">
+        <v>1</v>
+      </c>
+      <c r="AM416">
+        <v>18000000000</v>
+      </c>
+      <c r="AN416" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO416">
+        <v>0</v>
+      </c>
+      <c r="AP416">
+        <v>0.1</v>
+      </c>
+      <c r="AQ416">
+        <v>0</v>
+      </c>
+      <c r="AR416">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="417" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A417" t="s">
+        <v>828</v>
+      </c>
+      <c r="B417" t="s">
+        <v>777</v>
+      </c>
+      <c r="C417">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H417">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K417">
+        <v>1</v>
+      </c>
+      <c r="L417">
+        <v>0</v>
+      </c>
+      <c r="M417">
+        <v>0</v>
+      </c>
+      <c r="N417">
+        <v>0</v>
+      </c>
+      <c r="O417">
+        <v>1</v>
+      </c>
+      <c r="P417">
+        <v>0</v>
+      </c>
+      <c r="Q417">
+        <v>0</v>
+      </c>
+      <c r="R417">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="S417">
+        <v>0</v>
+      </c>
+      <c r="T417">
+        <v>1</v>
+      </c>
+      <c r="V417">
+        <v>0.5</v>
+      </c>
+      <c r="W417">
+        <v>2000000</v>
+      </c>
+      <c r="X417">
+        <v>180000</v>
+      </c>
+      <c r="Y417">
+        <v>330</v>
+      </c>
+      <c r="Z417">
+        <v>360</v>
+      </c>
+      <c r="AA417" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC417">
+        <v>1</v>
+      </c>
+      <c r="AD417">
+        <v>0.75</v>
+      </c>
+      <c r="AE417">
+        <v>1.3</v>
+      </c>
+      <c r="AF417">
+        <v>0</v>
+      </c>
+      <c r="AG417">
+        <v>0</v>
+      </c>
+      <c r="AH417">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AI417">
+        <v>0.32</v>
+      </c>
+      <c r="AL417">
+        <v>1</v>
+      </c>
+      <c r="AM417">
+        <v>18000000000</v>
+      </c>
+      <c r="AN417" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO417">
+        <v>0.1</v>
+      </c>
+      <c r="AP417">
+        <v>0.1</v>
+      </c>
+      <c r="AQ417">
+        <v>0.35</v>
+      </c>
+      <c r="AR417">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="418" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A418" t="s">
+        <v>829</v>
+      </c>
+      <c r="B418" t="s">
+        <v>779</v>
+      </c>
+      <c r="C418">
+        <v>1.2</v>
+      </c>
+      <c r="D418">
+        <v>1</v>
+      </c>
+      <c r="G418">
+        <v>2.8</v>
+      </c>
+      <c r="K418">
+        <v>0</v>
+      </c>
+      <c r="L418">
+        <v>0</v>
+      </c>
+      <c r="M418">
+        <v>0</v>
+      </c>
+      <c r="N418">
+        <v>2.1</v>
+      </c>
+      <c r="O418">
+        <v>0</v>
+      </c>
+      <c r="P418">
+        <v>0</v>
+      </c>
+      <c r="Q418">
+        <v>0</v>
+      </c>
+      <c r="R418">
+        <v>0</v>
+      </c>
+      <c r="S418">
+        <v>0</v>
+      </c>
+      <c r="T418">
+        <v>1</v>
+      </c>
+      <c r="U418">
+        <v>0.95</v>
+      </c>
+      <c r="V418">
+        <v>0</v>
+      </c>
+      <c r="W418">
+        <v>2000000</v>
+      </c>
+      <c r="X418">
+        <v>180000</v>
+      </c>
+      <c r="Y418">
+        <v>330</v>
+      </c>
+      <c r="Z418">
+        <v>360</v>
+      </c>
+      <c r="AE418">
+        <v>1.3</v>
+      </c>
+      <c r="AF418">
+        <v>0.65</v>
+      </c>
+      <c r="AG418">
+        <v>0</v>
+      </c>
+      <c r="AH418">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AI418">
+        <v>0</v>
+      </c>
+      <c r="AL418">
+        <v>1</v>
+      </c>
+      <c r="AM418">
+        <v>18000000000</v>
+      </c>
+      <c r="AN418" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO418">
+        <v>0</v>
+      </c>
+      <c r="AP418">
+        <v>0.1</v>
+      </c>
+      <c r="AQ418">
+        <v>0</v>
+      </c>
+      <c r="AR418">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding more to the quest section.
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="835">
   <si>
     <t>name</t>
   </si>
@@ -2369,27 +2369,30 @@
     <t>This enchantment is best suited for a Heretic as it increases their stats and class bonuses as well as gives other Heretic specific enhancements.</t>
   </si>
   <si>
+    <t>Prophet's Faith</t>
+  </si>
+  <si>
+    <t>This enchantment is best suited for a Prophet as it increases their stats and class bonuses as well as gives other Prophet specific enhancements.</t>
+  </si>
+  <si>
+    <t>Rangers Guidance</t>
+  </si>
+  <si>
+    <t>Thieves Decadence</t>
+  </si>
+  <si>
+    <t>This enchantment is best suited for a Thief as it increases their stats and class bonuses as well as gives other Thief specific enhancements.</t>
+  </si>
+  <si>
+    <t>Vampires Unquenchable Thirst</t>
+  </si>
+  <si>
+    <t>This enchantment is best suited for a Vampire as it increases their stats and class bonuses as well as gives other Vampire specific enhancements. This is considered a kill enchantment. That is, with the damage from life stealing and the damage from the enchantment its self, is enough to kill (in most cases)</t>
+  </si>
+  <si>
     <t>Prophets Faith</t>
   </si>
   <si>
-    <t>This enchantment is best suited for a Prophet as it increases their stats and class bonuses as well as gives other Prophet specific enhancements.</t>
-  </si>
-  <si>
-    <t>Rangers Guidance</t>
-  </si>
-  <si>
-    <t>Thieves Decadence</t>
-  </si>
-  <si>
-    <t>This enchantment is best suited for a Thief as it increases their stats and class bonuses as well as gives other Thief specific enhancements.</t>
-  </si>
-  <si>
-    <t>Vampires Unquenchable Thirst</t>
-  </si>
-  <si>
-    <t>This enchantment is best suited for a Vampire as it increases their stats and class bonuses as well as gives other Vampire specific enhancements. This is considered a kill enchantment. That is, with the damage from life stealing and the damage from the enchantment its self, is enough to kill (in most cases)</t>
-  </si>
-  <si>
     <t>Satans Delicious Flesh Ripper</t>
   </si>
   <si>
@@ -2496,6 +2499,9 @@
   </si>
   <si>
     <t>Rangers Curse of Nature</t>
+  </si>
+  <si>
+    <t>This enchantment is best suited for a Rangers as it increases their stats and class bonuses as well as gives other Ranger specific enhancements.</t>
   </si>
   <si>
     <t>Thieves Eye of Treasure</t>
@@ -2852,7 +2858,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AR413"/>
+  <dimension ref="A1:AR414"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -37626,16 +37632,16 @@
         <v>785</v>
       </c>
       <c r="D386">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I386">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="K386">
         <v>0</v>
       </c>
       <c r="L386">
-        <v>0.98</v>
+        <v>2.3</v>
       </c>
       <c r="M386">
         <v>0</v>
@@ -37647,7 +37653,7 @@
         <v>0</v>
       </c>
       <c r="P386">
-        <v>1.2</v>
+        <v>1.8</v>
       </c>
       <c r="Q386">
         <v>0</v>
@@ -37656,16 +37662,13 @@
         <v>0</v>
       </c>
       <c r="S386">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="T386">
         <v>1</v>
       </c>
-      <c r="U386">
-        <v>0.25</v>
-      </c>
       <c r="V386">
-        <v>0.55</v>
+        <v>0.5</v>
       </c>
       <c r="W386">
         <v>1000000</v>
@@ -37683,28 +37686,25 @@
         <v>0</v>
       </c>
       <c r="AF386">
-        <v>0.85</v>
+        <v>0.55</v>
       </c>
       <c r="AG386">
         <v>0</v>
       </c>
       <c r="AH386">
-        <v>0.055</v>
+        <v>0.5</v>
       </c>
       <c r="AI386">
         <v>0</v>
-      </c>
-      <c r="AK386">
-        <v>1</v>
       </c>
       <c r="AL386">
         <v>1</v>
       </c>
       <c r="AM386">
-        <v>4800000000</v>
+        <v>4200000000</v>
       </c>
       <c r="AN386" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AO386">
         <v>0</v>
@@ -37716,7 +37716,7 @@
         <v>0</v>
       </c>
       <c r="AR386">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="387" spans="1:44">
@@ -38027,91 +38027,73 @@
         <v>791</v>
       </c>
       <c r="B390" t="s">
-        <v>792</v>
-      </c>
-      <c r="C390">
+        <v>785</v>
+      </c>
+      <c r="D390">
         <v>1</v>
       </c>
-      <c r="D390">
-        <v>0.55</v>
-      </c>
-      <c r="E390">
-        <v>1.0</v>
-      </c>
-      <c r="F390">
-        <v>0.85</v>
-      </c>
-      <c r="G390">
-        <v>0.9</v>
-      </c>
-      <c r="H390">
-        <v>0.85</v>
-      </c>
       <c r="I390">
-        <v>0.9</v>
-      </c>
-      <c r="J390">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="K390">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="L390">
-        <v>0.9</v>
+        <v>0.98</v>
       </c>
       <c r="M390">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="N390">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="O390">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="P390">
-        <v>0.65</v>
+        <v>1.2</v>
       </c>
       <c r="Q390">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="R390">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="S390">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="T390">
         <v>1</v>
       </c>
       <c r="U390">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="V390">
-        <v>0.25</v>
+        <v>0.55</v>
       </c>
       <c r="W390">
-        <v>500000</v>
+        <v>1000000</v>
       </c>
       <c r="X390">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="Y390">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="Z390">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="AE390">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AF390">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="AG390">
         <v>0</v>
       </c>
       <c r="AH390">
-        <v>0</v>
+        <v>0.055</v>
       </c>
       <c r="AI390">
         <v>0</v>
@@ -38119,40 +38101,52 @@
       <c r="AK390">
         <v>1</v>
       </c>
+      <c r="AL390">
+        <v>1</v>
+      </c>
       <c r="AM390">
-        <v>5800000000</v>
+        <v>4800000000</v>
       </c>
       <c r="AN390" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AO390">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="AP390">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AQ390">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR390">
-        <v>1.25</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="391" spans="1:44">
       <c r="A391" t="s">
+        <v>792</v>
+      </c>
+      <c r="B391" t="s">
         <v>793</v>
       </c>
-      <c r="B391" t="s">
-        <v>794</v>
+      <c r="C391">
+        <v>1</v>
+      </c>
+      <c r="D391">
+        <v>0.55</v>
+      </c>
+      <c r="E391">
+        <v>1.0</v>
       </c>
       <c r="F391">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="G391">
         <v>0.9</v>
       </c>
       <c r="H391">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="I391">
         <v>0.9</v>
@@ -38167,25 +38161,25 @@
         <v>0.9</v>
       </c>
       <c r="M391">
-        <v>0.95</v>
+        <v>0.75</v>
       </c>
       <c r="N391">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="O391">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="P391">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="Q391">
-        <v>0.95</v>
+        <v>0.75</v>
       </c>
       <c r="R391">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="S391">
-        <v>0.95</v>
+        <v>0.6</v>
       </c>
       <c r="T391">
         <v>1</v>
@@ -38194,28 +38188,28 @@
         <v>0</v>
       </c>
       <c r="V391">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="W391">
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="X391">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="Y391">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="Z391">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="AE391">
-        <v>0.15</v>
+        <v>0.65</v>
       </c>
       <c r="AF391">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="AG391">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AH391">
         <v>0</v>
@@ -38223,314 +38217,308 @@
       <c r="AI391">
         <v>0</v>
       </c>
-      <c r="AL391">
+      <c r="AK391">
         <v>1</v>
       </c>
       <c r="AM391">
-        <v>6000000000</v>
+        <v>5800000000</v>
       </c>
       <c r="AN391" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AO391">
-        <v>0.1</v>
+        <v>0.45</v>
       </c>
       <c r="AP391">
         <v>0</v>
       </c>
       <c r="AQ391">
-        <v>0.55</v>
+        <v>1</v>
       </c>
       <c r="AR391">
-        <v>1.2</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="392" spans="1:44">
       <c r="A392" t="s">
+        <v>794</v>
+      </c>
+      <c r="B392" t="s">
         <v>795</v>
       </c>
-      <c r="B392" t="s">
-        <v>796</v>
-      </c>
       <c r="F392">
-        <v>1.05</v>
+        <v>0.9</v>
       </c>
       <c r="G392">
-        <v>0.25</v>
+        <v>0.9</v>
       </c>
       <c r="H392">
-        <v>0.55</v>
+        <v>0.9</v>
+      </c>
+      <c r="I392">
+        <v>0.9</v>
+      </c>
+      <c r="J392">
+        <v>0.9</v>
       </c>
       <c r="K392">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="L392">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="M392">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="N392">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="O392">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="P392">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="Q392">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="R392">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="S392">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="T392">
         <v>1</v>
       </c>
+      <c r="U392">
+        <v>0</v>
+      </c>
       <c r="V392">
         <v>0</v>
       </c>
       <c r="W392">
-        <v>750000</v>
+        <v>0</v>
       </c>
       <c r="X392">
         <v>55000</v>
       </c>
       <c r="Y392">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="Z392">
         <v>300</v>
       </c>
       <c r="AE392">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="AF392">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="AG392">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AH392">
         <v>0</v>
       </c>
       <c r="AI392">
         <v>0</v>
-      </c>
-      <c r="AK392">
-        <v>1</v>
       </c>
       <c r="AL392">
         <v>1</v>
       </c>
       <c r="AM392">
-        <v>6500000000</v>
+        <v>6000000000</v>
       </c>
       <c r="AN392" t="s">
         <v>49</v>
       </c>
       <c r="AO392">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="AP392">
         <v>0</v>
       </c>
       <c r="AQ392">
-        <v>1.5</v>
+        <v>0.55</v>
       </c>
       <c r="AR392">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="393" spans="1:44">
       <c r="A393" t="s">
+        <v>796</v>
+      </c>
+      <c r="B393" t="s">
         <v>797</v>
       </c>
-      <c r="B393" t="s">
-        <v>798</v>
-      </c>
-      <c r="C393">
-        <v>1.5</v>
-      </c>
-      <c r="D393">
-        <v>0.6</v>
-      </c>
-      <c r="E393">
-        <v>0.5</v>
-      </c>
-      <c r="I393">
-        <v>0.5</v>
-      </c>
-      <c r="J393">
-        <v>0.5</v>
+      <c r="F393">
+        <v>1.05</v>
+      </c>
+      <c r="G393">
+        <v>0.25</v>
+      </c>
+      <c r="H393">
+        <v>0.55</v>
       </c>
       <c r="K393">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="L393">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="M393">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="N393">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="O393">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="P393">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="Q393">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="R393">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="S393">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="T393">
         <v>1</v>
       </c>
-      <c r="U393">
+      <c r="V393">
+        <v>0</v>
+      </c>
+      <c r="W393">
+        <v>750000</v>
+      </c>
+      <c r="X393">
+        <v>55000</v>
+      </c>
+      <c r="Y393">
+        <v>193</v>
+      </c>
+      <c r="Z393">
+        <v>300</v>
+      </c>
+      <c r="AE393">
+        <v>1</v>
+      </c>
+      <c r="AF393">
         <v>0.25</v>
       </c>
-      <c r="V393">
-        <v>0.25</v>
-      </c>
-      <c r="W393">
-        <v>250000</v>
-      </c>
-      <c r="X393">
-        <v>60000</v>
-      </c>
-      <c r="Y393">
-        <v>200</v>
-      </c>
-      <c r="Z393">
-        <v>310</v>
-      </c>
-      <c r="AE393">
-        <v>0.75</v>
-      </c>
-      <c r="AF393">
-        <v>0</v>
-      </c>
       <c r="AG393">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AH393">
         <v>0</v>
       </c>
       <c r="AI393">
         <v>0</v>
+      </c>
+      <c r="AK393">
+        <v>1</v>
       </c>
       <c r="AL393">
         <v>1</v>
       </c>
       <c r="AM393">
-        <v>6850000000</v>
+        <v>6500000000</v>
       </c>
       <c r="AN393" t="s">
         <v>49</v>
       </c>
       <c r="AO393">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP393">
         <v>0</v>
       </c>
       <c r="AQ393">
-        <v>0.15</v>
+        <v>1.5</v>
       </c>
       <c r="AR393">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="394" spans="1:44">
       <c r="A394" t="s">
+        <v>798</v>
+      </c>
+      <c r="B394" t="s">
         <v>799</v>
       </c>
-      <c r="B394" t="s">
-        <v>800</v>
-      </c>
       <c r="C394">
-        <v>1.1</v>
+        <v>1.5</v>
       </c>
       <c r="D394">
+        <v>0.6</v>
+      </c>
+      <c r="E394">
+        <v>0.5</v>
+      </c>
+      <c r="I394">
+        <v>0.5</v>
+      </c>
+      <c r="J394">
+        <v>0.5</v>
+      </c>
+      <c r="K394">
+        <v>0.25</v>
+      </c>
+      <c r="L394">
         <v>0.75</v>
       </c>
-      <c r="E394">
-        <v>0.95</v>
-      </c>
-      <c r="F394">
-        <v>1.2</v>
-      </c>
-      <c r="G394">
-        <v>0.65</v>
-      </c>
-      <c r="H394">
-        <v>1.2</v>
-      </c>
-      <c r="J394">
-        <v>0</v>
-      </c>
-      <c r="K394">
-        <v>0.45</v>
-      </c>
-      <c r="L394">
-        <v>0</v>
-      </c>
       <c r="M394">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N394">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O394">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P394">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q394">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R394">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S394">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T394">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U394">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="V394">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="W394">
-        <v>1500000</v>
+        <v>250000</v>
       </c>
       <c r="X394">
-        <v>68000</v>
+        <v>60000</v>
       </c>
       <c r="Y394">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="Z394">
         <v>310</v>
       </c>
       <c r="AE394">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AF394">
         <v>0</v>
@@ -38539,7 +38527,7 @@
         <v>0</v>
       </c>
       <c r="AH394">
-        <v>0.015</v>
+        <v>0</v>
       </c>
       <c r="AI394">
         <v>0</v>
@@ -38548,105 +38536,111 @@
         <v>1</v>
       </c>
       <c r="AM394">
-        <v>7200000000</v>
+        <v>6850000000</v>
       </c>
       <c r="AN394" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AO394">
+        <v>0</v>
+      </c>
+      <c r="AP394">
+        <v>0</v>
+      </c>
+      <c r="AQ394">
+        <v>0.15</v>
+      </c>
+      <c r="AR394">
         <v>0.5</v>
-      </c>
-      <c r="AP394">
-        <v>0.25</v>
-      </c>
-      <c r="AQ394">
-        <v>0</v>
-      </c>
-      <c r="AR394">
-        <v>1.4</v>
       </c>
     </row>
     <row r="395" spans="1:44">
       <c r="A395" t="s">
+        <v>800</v>
+      </c>
+      <c r="B395" t="s">
         <v>801</v>
       </c>
-      <c r="B395" t="s">
-        <v>802</v>
-      </c>
       <c r="C395">
-        <v>0</v>
+        <v>1.1</v>
       </c>
       <c r="D395">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E395">
-        <v>0.0</v>
-      </c>
-      <c r="I395">
-        <v>1</v>
+        <v>0.95</v>
+      </c>
+      <c r="F395">
+        <v>1.2</v>
+      </c>
+      <c r="G395">
+        <v>0.65</v>
+      </c>
+      <c r="H395">
+        <v>1.2</v>
       </c>
       <c r="J395">
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="K395">
-        <v>0.85</v>
+        <v>0.45</v>
       </c>
       <c r="L395">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="M395">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="N395">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="O395">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="P395">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="Q395">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="R395">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="S395">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="T395">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U395">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="V395">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="W395">
         <v>1500000</v>
       </c>
       <c r="X395">
-        <v>73000</v>
+        <v>68000</v>
       </c>
       <c r="Y395">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="Z395">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="AE395">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="AF395">
         <v>0</v>
       </c>
       <c r="AG395">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="AH395">
-        <v>0.028</v>
+        <v>0.015</v>
       </c>
       <c r="AI395">
         <v>0</v>
@@ -38655,149 +38649,158 @@
         <v>1</v>
       </c>
       <c r="AM395">
-        <v>7800000000</v>
+        <v>7200000000</v>
       </c>
       <c r="AN395" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AO395">
+        <v>0.5</v>
+      </c>
+      <c r="AP395">
         <v>0.25</v>
       </c>
-      <c r="AP395">
-        <v>0.2</v>
-      </c>
       <c r="AQ395">
         <v>0</v>
       </c>
       <c r="AR395">
-        <v>0</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="396" spans="1:44">
       <c r="A396" t="s">
+        <v>802</v>
+      </c>
+      <c r="B396" t="s">
         <v>803</v>
       </c>
-      <c r="B396" t="s">
-        <v>804</v>
-      </c>
-      <c r="F396">
-        <v>0.6</v>
-      </c>
-      <c r="G396">
-        <v>0.5</v>
-      </c>
-      <c r="H396">
+      <c r="C396">
+        <v>0</v>
+      </c>
+      <c r="D396">
+        <v>0</v>
+      </c>
+      <c r="E396">
+        <v>0.0</v>
+      </c>
+      <c r="I396">
+        <v>1</v>
+      </c>
+      <c r="J396">
+        <v>1.1</v>
+      </c>
+      <c r="K396">
+        <v>0.85</v>
+      </c>
+      <c r="L396">
+        <v>0.95</v>
+      </c>
+      <c r="M396">
+        <v>0.9</v>
+      </c>
+      <c r="N396">
+        <v>0.9</v>
+      </c>
+      <c r="O396">
+        <v>0.9</v>
+      </c>
+      <c r="P396">
+        <v>0.9</v>
+      </c>
+      <c r="Q396">
+        <v>0.9</v>
+      </c>
+      <c r="R396">
+        <v>0.9</v>
+      </c>
+      <c r="S396">
+        <v>0.9</v>
+      </c>
+      <c r="T396">
+        <v>1</v>
+      </c>
+      <c r="U396">
+        <v>0.1</v>
+      </c>
+      <c r="V396">
         <v>0.3</v>
       </c>
-      <c r="I396">
-        <v>0.55</v>
-      </c>
-      <c r="J396">
-        <v>0.7</v>
-      </c>
-      <c r="K396">
-        <v>0.35</v>
-      </c>
-      <c r="L396">
-        <v>0.5</v>
-      </c>
-      <c r="M396">
-        <v>0</v>
-      </c>
-      <c r="N396">
-        <v>0</v>
-      </c>
-      <c r="O396">
-        <v>0</v>
-      </c>
-      <c r="P396">
-        <v>0</v>
-      </c>
-      <c r="Q396">
-        <v>0</v>
-      </c>
-      <c r="R396">
-        <v>0</v>
-      </c>
-      <c r="S396">
-        <v>0</v>
-      </c>
-      <c r="T396">
-        <v>0</v>
-      </c>
-      <c r="U396">
-        <v>0.2</v>
-      </c>
-      <c r="V396">
-        <v>0.4</v>
-      </c>
       <c r="W396">
-        <v>750000</v>
+        <v>1500000</v>
       </c>
       <c r="X396">
-        <v>75000</v>
+        <v>73000</v>
       </c>
       <c r="Y396">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="Z396">
         <v>316</v>
       </c>
       <c r="AE396">
-        <v>1.5</v>
+        <v>0.3</v>
       </c>
       <c r="AF396">
         <v>0</v>
       </c>
       <c r="AG396">
-        <v>1.1</v>
+        <v>0.2</v>
       </c>
       <c r="AH396">
-        <v>0.15</v>
+        <v>0.028</v>
       </c>
       <c r="AI396">
         <v>0</v>
       </c>
-      <c r="AK396">
+      <c r="AL396">
         <v>1</v>
       </c>
       <c r="AM396">
-        <v>7900000000</v>
+        <v>7800000000</v>
       </c>
       <c r="AN396" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AO396">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AP396">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="AQ396">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="AR396">
-        <v>1.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="397" spans="1:44">
       <c r="A397" t="s">
+        <v>804</v>
+      </c>
+      <c r="B397" t="s">
         <v>805</v>
       </c>
-      <c r="B397" t="s">
-        <v>806</v>
+      <c r="F397">
+        <v>0.6</v>
       </c>
       <c r="G397">
-        <v>1.2</v>
+        <v>0.5</v>
+      </c>
+      <c r="H397">
+        <v>0.3</v>
       </c>
       <c r="I397">
-        <v>1.1</v>
+        <v>0.55</v>
+      </c>
+      <c r="J397">
+        <v>0.7</v>
       </c>
       <c r="K397">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="L397">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M397">
         <v>0</v>
@@ -38827,123 +38830,129 @@
         <v>0.2</v>
       </c>
       <c r="V397">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="W397">
-        <v>850000</v>
+        <v>750000</v>
       </c>
       <c r="X397">
-        <v>80000</v>
+        <v>75000</v>
       </c>
       <c r="Y397">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="Z397">
         <v>316</v>
       </c>
       <c r="AE397">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AF397">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="AG397">
-        <v>0</v>
+        <v>1.1</v>
       </c>
       <c r="AH397">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="AI397">
         <v>0</v>
       </c>
-      <c r="AL397">
+      <c r="AK397">
         <v>1</v>
       </c>
       <c r="AM397">
-        <v>8300000000</v>
+        <v>7900000000</v>
       </c>
       <c r="AN397" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AO397">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AP397">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AQ397">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="AR397">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="398" spans="1:44">
       <c r="A398" t="s">
+        <v>806</v>
+      </c>
+      <c r="B398" t="s">
         <v>807</v>
       </c>
-      <c r="B398" t="s">
-        <v>808</v>
+      <c r="G398">
+        <v>1.2</v>
+      </c>
+      <c r="I398">
+        <v>1.1</v>
       </c>
       <c r="K398">
         <v>0</v>
       </c>
       <c r="L398">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M398">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N398">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O398">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P398">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q398">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R398">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S398">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T398">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U398">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="V398">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="W398">
-        <v>1300000</v>
+        <v>850000</v>
       </c>
       <c r="X398">
-        <v>83000</v>
+        <v>80000</v>
       </c>
       <c r="Y398">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="Z398">
         <v>316</v>
       </c>
       <c r="AE398">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="AF398">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="AG398">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="AH398">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="AI398">
         <v>0</v>
@@ -38958,7 +38967,7 @@
         <v>49</v>
       </c>
       <c r="AO398">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AP398">
         <v>0.5</v>
@@ -38972,195 +38981,183 @@
     </row>
     <row r="399" spans="1:44">
       <c r="A399" t="s">
+        <v>808</v>
+      </c>
+      <c r="B399" t="s">
         <v>809</v>
       </c>
-      <c r="B399" t="s">
-        <v>810</v>
-      </c>
-      <c r="C399">
-        <v>0.5</v>
-      </c>
-      <c r="D399">
-        <v>0.5</v>
-      </c>
-      <c r="E399">
-        <v>0.5</v>
-      </c>
-      <c r="F399">
-        <v>1.18</v>
-      </c>
-      <c r="G399">
-        <v>1.18</v>
-      </c>
-      <c r="H399">
-        <v>1.18</v>
-      </c>
-      <c r="I399">
-        <v>1.18</v>
-      </c>
-      <c r="J399">
-        <v>1.18</v>
-      </c>
       <c r="K399">
-        <v>1.18</v>
+        <v>0</v>
       </c>
       <c r="L399">
-        <v>1.18</v>
+        <v>0</v>
       </c>
       <c r="M399">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N399">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O399">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P399">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q399">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R399">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S399">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T399">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U399">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="V399">
-        <v>1.18</v>
+        <v>0</v>
       </c>
       <c r="W399">
-        <v>3000000</v>
+        <v>1300000</v>
       </c>
       <c r="X399">
-        <v>85000</v>
+        <v>83000</v>
       </c>
       <c r="Y399">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="Z399">
         <v>316</v>
       </c>
       <c r="AE399">
-        <v>0.6</v>
+        <v>0.45</v>
       </c>
       <c r="AF399">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="AG399">
+        <v>0.15</v>
+      </c>
+      <c r="AH399">
+        <v>0.03</v>
+      </c>
+      <c r="AI399">
+        <v>0</v>
+      </c>
+      <c r="AL399">
+        <v>1</v>
+      </c>
+      <c r="AM399">
+        <v>8300000000</v>
+      </c>
+      <c r="AN399" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO399">
+        <v>0.1</v>
+      </c>
+      <c r="AP399">
         <v>0.5</v>
       </c>
-      <c r="AH399">
-        <v>0</v>
-      </c>
-      <c r="AI399">
-        <v>0</v>
-      </c>
-      <c r="AK399">
+      <c r="AQ399">
         <v>1</v>
       </c>
-      <c r="AM399">
-        <v>8800000000</v>
-      </c>
-      <c r="AN399" t="s">
-        <v>46</v>
-      </c>
-      <c r="AO399">
-        <v>0.5</v>
-      </c>
-      <c r="AP399">
-        <v>0</v>
-      </c>
-      <c r="AQ399">
-        <v>0.75</v>
-      </c>
       <c r="AR399">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="400" spans="1:44">
       <c r="A400" t="s">
+        <v>810</v>
+      </c>
+      <c r="B400" t="s">
         <v>811</v>
       </c>
-      <c r="B400" t="s">
-        <v>812</v>
+      <c r="C400">
+        <v>0.5</v>
+      </c>
+      <c r="D400">
+        <v>0.5</v>
+      </c>
+      <c r="E400">
+        <v>0.5</v>
       </c>
       <c r="F400">
-        <v>1.2</v>
+        <v>1.18</v>
       </c>
       <c r="G400">
-        <v>1.2</v>
+        <v>1.18</v>
       </c>
       <c r="H400">
-        <v>1.2</v>
+        <v>1.18</v>
       </c>
       <c r="I400">
-        <v>1.2</v>
+        <v>1.18</v>
       </c>
       <c r="J400">
-        <v>1.2</v>
+        <v>1.18</v>
       </c>
       <c r="K400">
-        <v>1.2</v>
+        <v>1.18</v>
       </c>
       <c r="L400">
-        <v>1.2</v>
+        <v>1.18</v>
       </c>
       <c r="M400">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="N400">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="O400">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="P400">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="Q400">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="R400">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="S400">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="T400">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="U400">
+        <v>0.25</v>
       </c>
       <c r="V400">
-        <v>1.2</v>
+        <v>1.18</v>
       </c>
       <c r="W400">
-        <v>3500000</v>
+        <v>3000000</v>
       </c>
       <c r="X400">
-        <v>90000</v>
+        <v>85000</v>
       </c>
       <c r="Y400">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="Z400">
         <v>316</v>
       </c>
       <c r="AE400">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="AF400">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AG400">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="AH400">
         <v>0</v>
@@ -39168,23 +39165,23 @@
       <c r="AI400">
         <v>0</v>
       </c>
-      <c r="AL400">
+      <c r="AK400">
         <v>1</v>
       </c>
       <c r="AM400">
-        <v>9000000000</v>
+        <v>8800000000</v>
       </c>
       <c r="AN400" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AO400">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="AP400">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="AQ400">
-        <v>0.65</v>
+        <v>0.75</v>
       </c>
       <c r="AR400">
         <v>1.5</v>
@@ -39192,124 +39189,124 @@
     </row>
     <row r="401" spans="1:44">
       <c r="A401" t="s">
+        <v>812</v>
+      </c>
+      <c r="B401" t="s">
         <v>813</v>
       </c>
-      <c r="B401" t="s">
-        <v>814</v>
-      </c>
-      <c r="C401">
+      <c r="F401">
+        <v>1.2</v>
+      </c>
+      <c r="G401">
+        <v>1.2</v>
+      </c>
+      <c r="H401">
+        <v>1.2</v>
+      </c>
+      <c r="I401">
+        <v>1.2</v>
+      </c>
+      <c r="J401">
+        <v>1.2</v>
+      </c>
+      <c r="K401">
+        <v>1.2</v>
+      </c>
+      <c r="L401">
+        <v>1.2</v>
+      </c>
+      <c r="M401">
+        <v>1.2</v>
+      </c>
+      <c r="N401">
+        <v>1.2</v>
+      </c>
+      <c r="O401">
+        <v>1.2</v>
+      </c>
+      <c r="P401">
+        <v>1.2</v>
+      </c>
+      <c r="Q401">
+        <v>1.2</v>
+      </c>
+      <c r="R401">
+        <v>1.2</v>
+      </c>
+      <c r="S401">
+        <v>1.2</v>
+      </c>
+      <c r="T401">
         <v>1</v>
       </c>
-      <c r="D401">
-        <v>1</v>
-      </c>
-      <c r="E401">
-        <v>1.0</v>
-      </c>
-      <c r="F401">
-        <v>1.28</v>
-      </c>
-      <c r="G401">
-        <v>1.28</v>
-      </c>
-      <c r="H401">
-        <v>1.28</v>
-      </c>
-      <c r="J401">
-        <v>1.28</v>
-      </c>
-      <c r="K401">
-        <v>0</v>
-      </c>
-      <c r="L401">
-        <v>1.28</v>
-      </c>
-      <c r="M401">
-        <v>0</v>
-      </c>
-      <c r="N401">
-        <v>0</v>
-      </c>
-      <c r="O401">
-        <v>0</v>
-      </c>
-      <c r="P401">
-        <v>0</v>
-      </c>
-      <c r="Q401">
-        <v>0</v>
-      </c>
-      <c r="R401">
-        <v>0</v>
-      </c>
-      <c r="S401">
-        <v>0</v>
-      </c>
-      <c r="T401">
-        <v>0</v>
-      </c>
       <c r="V401">
-        <v>0.2</v>
+        <v>1.2</v>
       </c>
       <c r="W401">
-        <v>4000000</v>
+        <v>3500000</v>
       </c>
       <c r="X401">
-        <v>95000</v>
+        <v>90000</v>
       </c>
       <c r="Y401">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="Z401">
         <v>316</v>
       </c>
       <c r="AE401">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="AF401">
         <v>0</v>
       </c>
       <c r="AG401">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="AH401">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AI401">
-        <v>0.15</v>
-      </c>
-      <c r="AK401">
+        <v>0</v>
+      </c>
+      <c r="AL401">
         <v>1</v>
       </c>
       <c r="AM401">
-        <v>9500000000</v>
+        <v>9000000000</v>
       </c>
       <c r="AN401" t="s">
         <v>49</v>
       </c>
       <c r="AO401">
-        <v>0.45</v>
+        <v>0.25</v>
       </c>
       <c r="AP401">
-        <v>0.55</v>
+        <v>0.3</v>
       </c>
       <c r="AQ401">
         <v>0.65</v>
       </c>
       <c r="AR401">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="402" spans="1:44">
       <c r="A402" t="s">
+        <v>814</v>
+      </c>
+      <c r="B402" t="s">
         <v>815</v>
       </c>
-      <c r="B402" t="s">
-        <v>816</v>
+      <c r="C402">
+        <v>1</v>
       </c>
       <c r="D402">
         <v>1</v>
       </c>
+      <c r="E402">
+        <v>1.0</v>
+      </c>
       <c r="F402">
         <v>1.28</v>
       </c>
@@ -39319,7 +39316,7 @@
       <c r="H402">
         <v>1.28</v>
       </c>
-      <c r="I402">
+      <c r="J402">
         <v>1.28</v>
       </c>
       <c r="K402">
@@ -39352,9 +39349,6 @@
       <c r="T402">
         <v>0</v>
       </c>
-      <c r="U402">
-        <v>0.55</v>
-      </c>
       <c r="V402">
         <v>0.2</v>
       </c>
@@ -39362,7 +39356,7 @@
         <v>4000000</v>
       </c>
       <c r="X402">
-        <v>98000</v>
+        <v>95000</v>
       </c>
       <c r="Y402">
         <v>260</v>
@@ -39374,7 +39368,7 @@
         <v>0</v>
       </c>
       <c r="AF402">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AG402">
         <v>0</v>
@@ -39385,103 +39379,94 @@
       <c r="AI402">
         <v>0.15</v>
       </c>
-      <c r="AL402">
+      <c r="AK402">
         <v>1</v>
       </c>
       <c r="AM402">
-        <v>10000000000</v>
+        <v>9500000000</v>
       </c>
       <c r="AN402" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AO402">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="AP402">
-        <v>0.2</v>
+        <v>0.55</v>
       </c>
       <c r="AQ402">
-        <v>0.3</v>
+        <v>0.65</v>
       </c>
       <c r="AR402">
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="403" spans="1:44">
       <c r="A403" t="s">
+        <v>816</v>
+      </c>
+      <c r="B403" t="s">
         <v>817</v>
       </c>
-      <c r="B403" t="s">
-        <v>818</v>
-      </c>
-      <c r="C403">
-        <v>0.75</v>
-      </c>
       <c r="D403">
-        <v>0.25</v>
-      </c>
-      <c r="E403">
-        <v>0.55</v>
+        <v>1</v>
       </c>
       <c r="F403">
-        <v>1.3</v>
+        <v>1.28</v>
       </c>
       <c r="G403">
-        <v>1.3</v>
+        <v>1.28</v>
       </c>
       <c r="H403">
-        <v>1.3</v>
+        <v>1.28</v>
       </c>
       <c r="I403">
-        <v>1.3</v>
-      </c>
-      <c r="J403">
-        <v>1.3</v>
+        <v>1.28</v>
       </c>
       <c r="K403">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="L403">
-        <v>1.3</v>
+        <v>1.28</v>
       </c>
       <c r="M403">
         <v>0</v>
       </c>
       <c r="N403">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="O403">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="P403">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="Q403">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R403">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="S403">
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="T403">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U403">
         <v>0.55</v>
       </c>
       <c r="V403">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="W403">
-        <v>5000000</v>
+        <v>4000000</v>
       </c>
       <c r="X403">
-        <v>110000</v>
+        <v>98000</v>
       </c>
       <c r="Y403">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="Z403">
         <v>316</v>
@@ -39490,16 +39475,16 @@
         <v>0</v>
       </c>
       <c r="AF403">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AG403">
         <v>0</v>
       </c>
       <c r="AH403">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AI403">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="AL403">
         <v>1</v>
@@ -39511,81 +39496,99 @@
         <v>46</v>
       </c>
       <c r="AO403">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="AP403">
         <v>0.2</v>
       </c>
       <c r="AQ403">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AR403">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="404" spans="1:44">
       <c r="A404" t="s">
+        <v>818</v>
+      </c>
+      <c r="B404" t="s">
         <v>819</v>
       </c>
-      <c r="B404" t="s">
-        <v>820</v>
-      </c>
       <c r="C404">
-        <v>0.9</v>
+        <v>0.75</v>
+      </c>
+      <c r="D404">
+        <v>0.25</v>
+      </c>
+      <c r="E404">
+        <v>0.55</v>
+      </c>
+      <c r="F404">
+        <v>1.3</v>
       </c>
       <c r="G404">
-        <v>1.35</v>
+        <v>1.3</v>
+      </c>
+      <c r="H404">
+        <v>1.3</v>
+      </c>
+      <c r="I404">
+        <v>1.3</v>
+      </c>
+      <c r="J404">
+        <v>1.3</v>
       </c>
       <c r="K404">
-        <v>1.35</v>
+        <v>1.3</v>
       </c>
       <c r="L404">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="M404">
         <v>0</v>
       </c>
       <c r="N404">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="O404">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="P404">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="Q404">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R404">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="S404">
-        <v>0</v>
+        <v>1.1</v>
       </c>
       <c r="T404">
         <v>1</v>
       </c>
       <c r="U404">
-        <v>0.75</v>
+        <v>0.55</v>
       </c>
       <c r="V404">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="W404">
-        <v>5500000</v>
+        <v>5000000</v>
       </c>
       <c r="X404">
-        <v>115000</v>
+        <v>110000</v>
       </c>
       <c r="Y404">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="Z404">
         <v>316</v>
       </c>
       <c r="AE404">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AF404">
         <v>0</v>
@@ -39594,7 +39597,7 @@
         <v>0</v>
       </c>
       <c r="AH404">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AI404">
         <v>0</v>
@@ -39609,13 +39612,13 @@
         <v>46</v>
       </c>
       <c r="AO404">
-        <v>0.28</v>
+        <v>0.6</v>
       </c>
       <c r="AP404">
         <v>0.2</v>
       </c>
       <c r="AQ404">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="AR404">
         <v>0.7</v>
@@ -39623,40 +39626,28 @@
     </row>
     <row r="405" spans="1:44">
       <c r="A405" t="s">
+        <v>820</v>
+      </c>
+      <c r="B405" t="s">
         <v>821</v>
       </c>
-      <c r="B405" t="s">
-        <v>822</v>
-      </c>
       <c r="C405">
-        <v>1.1</v>
-      </c>
-      <c r="D405">
-        <v>1.1</v>
-      </c>
-      <c r="E405">
-        <v>0.75</v>
+        <v>0.9</v>
       </c>
       <c r="G405">
         <v>1.35</v>
       </c>
-      <c r="I405">
-        <v>1.35</v>
-      </c>
-      <c r="J405">
-        <v>1.35</v>
-      </c>
       <c r="K405">
         <v>1.35</v>
       </c>
       <c r="L405">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="M405">
         <v>0</v>
       </c>
       <c r="N405">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O405">
         <v>0</v>
@@ -39674,28 +39665,28 @@
         <v>0</v>
       </c>
       <c r="T405">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U405">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="V405">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="W405">
         <v>5500000</v>
       </c>
       <c r="X405">
-        <v>120000</v>
+        <v>115000</v>
       </c>
       <c r="Y405">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="Z405">
         <v>316</v>
       </c>
       <c r="AE405">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AF405">
         <v>0</v>
@@ -39704,7 +39695,7 @@
         <v>0</v>
       </c>
       <c r="AH405">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AI405">
         <v>0</v>
@@ -39719,13 +39710,13 @@
         <v>46</v>
       </c>
       <c r="AO405">
-        <v>0</v>
+        <v>0.28</v>
       </c>
       <c r="AP405">
         <v>0.2</v>
       </c>
       <c r="AQ405">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="AR405">
         <v>0.7</v>
@@ -39733,40 +39724,43 @@
     </row>
     <row r="406" spans="1:44">
       <c r="A406" t="s">
+        <v>822</v>
+      </c>
+      <c r="B406" t="s">
         <v>823</v>
       </c>
-      <c r="B406" t="s">
-        <v>781</v>
-      </c>
       <c r="C406">
-        <v>1.4</v>
+        <v>1.1</v>
+      </c>
+      <c r="D406">
+        <v>1.1</v>
       </c>
       <c r="E406">
-        <v>1.4</v>
-      </c>
-      <c r="F406">
-        <v>1.4</v>
+        <v>0.75</v>
       </c>
       <c r="G406">
-        <v>1.4</v>
-      </c>
-      <c r="H406">
-        <v>1.4</v>
+        <v>1.35</v>
+      </c>
+      <c r="I406">
+        <v>1.35</v>
+      </c>
+      <c r="J406">
+        <v>1.35</v>
       </c>
       <c r="K406">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="L406">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="M406">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="N406">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="O406">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="P406">
         <v>0</v>
@@ -39781,34 +39775,37 @@
         <v>0</v>
       </c>
       <c r="T406">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="U406">
+        <v>0</v>
       </c>
       <c r="V406">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="W406">
-        <v>1500000</v>
+        <v>5500000</v>
       </c>
       <c r="X406">
-        <v>125000</v>
+        <v>120000</v>
       </c>
       <c r="Y406">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="Z406">
         <v>316</v>
       </c>
       <c r="AE406">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="AF406">
         <v>0</v>
       </c>
       <c r="AG406">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH406">
-        <v>0.065</v>
+        <v>0</v>
       </c>
       <c r="AI406">
         <v>0</v>
@@ -39823,13 +39820,13 @@
         <v>46</v>
       </c>
       <c r="AO406">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AP406">
         <v>0.2</v>
       </c>
       <c r="AQ406">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="AR406">
         <v>0.7</v>
@@ -39840,40 +39837,49 @@
         <v>824</v>
       </c>
       <c r="B407" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C407">
         <v>1.4</v>
       </c>
-      <c r="J407">
+      <c r="E407">
         <v>1.4</v>
       </c>
+      <c r="F407">
+        <v>1.4</v>
+      </c>
+      <c r="G407">
+        <v>1.4</v>
+      </c>
+      <c r="H407">
+        <v>1.4</v>
+      </c>
       <c r="K407">
         <v>0</v>
       </c>
       <c r="L407">
+        <v>0</v>
+      </c>
+      <c r="M407">
         <v>1.2</v>
       </c>
-      <c r="M407">
-        <v>0</v>
-      </c>
       <c r="N407">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="O407">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="P407">
         <v>0</v>
       </c>
       <c r="Q407">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="R407">
         <v>0</v>
       </c>
       <c r="S407">
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="T407">
         <v>1</v>
@@ -39900,7 +39906,7 @@
         <v>0</v>
       </c>
       <c r="AG407">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH407">
         <v>0.065</v>
@@ -39918,13 +39924,13 @@
         <v>46</v>
       </c>
       <c r="AO407">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="AP407">
         <v>0.2</v>
       </c>
       <c r="AQ407">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AR407">
         <v>0.7</v>
@@ -39935,12 +39941,12 @@
         <v>825</v>
       </c>
       <c r="B408" t="s">
-        <v>785</v>
-      </c>
-      <c r="D408">
-        <v>1</v>
-      </c>
-      <c r="I408">
+        <v>783</v>
+      </c>
+      <c r="C408">
+        <v>1.4</v>
+      </c>
+      <c r="J408">
         <v>1.4</v>
       </c>
       <c r="K408">
@@ -39959,23 +39965,20 @@
         <v>0</v>
       </c>
       <c r="P408">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="Q408">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="R408">
         <v>0</v>
       </c>
       <c r="S408">
-        <v>1.4</v>
+        <v>1.1</v>
       </c>
       <c r="T408">
         <v>1</v>
       </c>
-      <c r="U408">
-        <v>0.55</v>
-      </c>
       <c r="V408">
         <v>0.65</v>
       </c>
@@ -39992,10 +39995,10 @@
         <v>316</v>
       </c>
       <c r="AE408">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="AF408">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG408">
         <v>0</v>
@@ -40006,26 +40009,26 @@
       <c r="AI408">
         <v>0</v>
       </c>
-      <c r="AK408">
+      <c r="AL408">
         <v>1</v>
       </c>
       <c r="AM408">
-        <v>11500000000</v>
+        <v>10000000000</v>
       </c>
       <c r="AN408" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AO408">
-        <v>0.45</v>
+        <v>0.2</v>
       </c>
       <c r="AP408">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="AQ408">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="AR408">
-        <v>1.5</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="409" spans="1:44">
@@ -40033,47 +40036,47 @@
         <v>826</v>
       </c>
       <c r="B409" t="s">
-        <v>783</v>
-      </c>
-      <c r="C409">
+        <v>785</v>
+      </c>
+      <c r="D409">
+        <v>1</v>
+      </c>
+      <c r="I409">
         <v>1.4</v>
       </c>
-      <c r="D409">
-        <v>0.95</v>
-      </c>
-      <c r="H409">
+      <c r="K409">
+        <v>0</v>
+      </c>
+      <c r="L409">
+        <v>1.2</v>
+      </c>
+      <c r="M409">
+        <v>0</v>
+      </c>
+      <c r="N409">
+        <v>0</v>
+      </c>
+      <c r="O409">
+        <v>0</v>
+      </c>
+      <c r="P409">
         <v>1.4</v>
       </c>
-      <c r="K409">
-        <v>1.2</v>
-      </c>
-      <c r="L409">
-        <v>0</v>
-      </c>
-      <c r="M409">
-        <v>0</v>
-      </c>
-      <c r="N409">
-        <v>0</v>
-      </c>
-      <c r="O409">
-        <v>1.2</v>
-      </c>
-      <c r="P409">
-        <v>0</v>
-      </c>
       <c r="Q409">
         <v>0</v>
       </c>
       <c r="R409">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="S409">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="T409">
         <v>1</v>
       </c>
+      <c r="U409">
+        <v>0.55</v>
+      </c>
       <c r="V409">
         <v>0.65</v>
       </c>
@@ -40090,43 +40093,40 @@
         <v>316</v>
       </c>
       <c r="AE409">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="AF409">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AG409">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AH409">
         <v>0.065</v>
       </c>
       <c r="AI409">
-        <v>0.055</v>
+        <v>0</v>
       </c>
       <c r="AK409">
         <v>1</v>
       </c>
-      <c r="AL409">
-        <v>1</v>
-      </c>
       <c r="AM409">
-        <v>12800000000</v>
+        <v>11500000000</v>
       </c>
       <c r="AN409" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AO409">
-        <v>0.6</v>
+        <v>0.45</v>
       </c>
       <c r="AP409">
         <v>0.6</v>
       </c>
       <c r="AQ409">
-        <v>0.85</v>
+        <v>1.2</v>
       </c>
       <c r="AR409">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="410" spans="1:44">
@@ -40134,11 +40134,14 @@
         <v>827</v>
       </c>
       <c r="B410" t="s">
-        <v>788</v>
+        <v>828</v>
       </c>
       <c r="C410">
         <v>1.4</v>
       </c>
+      <c r="D410">
+        <v>0.95</v>
+      </c>
       <c r="H410">
         <v>1.4</v>
       </c>
@@ -40187,29 +40190,26 @@
       <c r="Z410">
         <v>316</v>
       </c>
-      <c r="AA410" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC410">
-        <v>1</v>
-      </c>
-      <c r="AD410">
-        <v>0.65</v>
-      </c>
       <c r="AE410">
-        <v>0.75</v>
+        <v>1.2</v>
       </c>
       <c r="AF410">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="AG410">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AH410">
         <v>0.065</v>
       </c>
       <c r="AI410">
-        <v>0.065</v>
+        <v>0.055</v>
+      </c>
+      <c r="AK410">
+        <v>1</v>
+      </c>
+      <c r="AL410">
+        <v>1</v>
       </c>
       <c r="AM410">
         <v>12800000000</v>
@@ -40218,36 +40218,33 @@
         <v>46</v>
       </c>
       <c r="AO410">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="AP410">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="AQ410">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="AR410">
-        <v>0</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="411" spans="1:44">
       <c r="A411" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B411" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C411">
         <v>1.4</v>
       </c>
-      <c r="D411">
-        <v>0.95</v>
-      </c>
-      <c r="G411">
+      <c r="H411">
         <v>1.4</v>
       </c>
       <c r="K411">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="L411">
         <v>0</v>
@@ -40256,11 +40253,11 @@
         <v>0</v>
       </c>
       <c r="N411">
+        <v>0</v>
+      </c>
+      <c r="O411">
         <v>1.2</v>
       </c>
-      <c r="O411">
-        <v>0</v>
-      </c>
       <c r="P411">
         <v>0</v>
       </c>
@@ -40268,7 +40265,7 @@
         <v>0</v>
       </c>
       <c r="R411">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="S411">
         <v>0</v>
@@ -40276,9 +40273,6 @@
       <c r="T411">
         <v>1</v>
       </c>
-      <c r="U411">
-        <v>0.75</v>
-      </c>
       <c r="V411">
         <v>0.65</v>
       </c>
@@ -40294,11 +40288,20 @@
       <c r="Z411">
         <v>316</v>
       </c>
+      <c r="AA411" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC411">
+        <v>1</v>
+      </c>
+      <c r="AD411">
+        <v>0.65</v>
+      </c>
       <c r="AE411">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="AF411">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="AG411">
         <v>0</v>
@@ -40307,7 +40310,7 @@
         <v>0.065</v>
       </c>
       <c r="AI411">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="AM411">
         <v>12800000000</v>
@@ -40330,37 +40333,31 @@
     </row>
     <row r="412" spans="1:44">
       <c r="A412" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="B412" t="s">
-        <v>830</v>
-      </c>
-      <c r="F412">
-        <v>1.45</v>
+        <v>790</v>
+      </c>
+      <c r="C412">
+        <v>1.4</v>
+      </c>
+      <c r="D412">
+        <v>0.95</v>
       </c>
       <c r="G412">
-        <v>1.45</v>
-      </c>
-      <c r="H412">
-        <v>1.45</v>
-      </c>
-      <c r="I412">
-        <v>1.45</v>
-      </c>
-      <c r="J412">
-        <v>1.45</v>
+        <v>1.4</v>
       </c>
       <c r="K412">
-        <v>1.45</v>
+        <v>0</v>
       </c>
       <c r="L412">
-        <v>1.45</v>
+        <v>0</v>
       </c>
       <c r="M412">
         <v>0</v>
       </c>
       <c r="N412">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="O412">
         <v>0</v>
@@ -40378,46 +40375,46 @@
         <v>0</v>
       </c>
       <c r="T412">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U412">
-        <v>0.35</v>
+        <v>0.75</v>
       </c>
       <c r="V412">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
       <c r="W412">
-        <v>6500000</v>
+        <v>1500000</v>
       </c>
       <c r="X412">
-        <v>130000</v>
+        <v>125000</v>
       </c>
       <c r="Y412">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="Z412">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="AE412">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AF412">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="AG412">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="AH412">
-        <v>0.066</v>
+        <v>0.065</v>
       </c>
       <c r="AI412">
-        <v>0.066</v>
+        <v>0</v>
       </c>
       <c r="AM412">
-        <v>13500000000</v>
+        <v>12800000000</v>
       </c>
       <c r="AN412" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AO412">
         <v>0</v>
@@ -40439,95 +40436,86 @@
       <c r="B413" t="s">
         <v>832</v>
       </c>
-      <c r="C413">
-        <v>1.2</v>
-      </c>
-      <c r="D413">
-        <v>0.55</v>
-      </c>
-      <c r="E413">
-        <v>0.8</v>
-      </c>
       <c r="F413">
-        <v>1.48</v>
+        <v>1.45</v>
       </c>
       <c r="G413">
-        <v>1.48</v>
+        <v>1.45</v>
       </c>
       <c r="H413">
-        <v>1.48</v>
+        <v>1.45</v>
       </c>
       <c r="I413">
-        <v>1.48</v>
+        <v>1.45</v>
       </c>
       <c r="J413">
-        <v>1.48</v>
+        <v>1.45</v>
       </c>
       <c r="K413">
-        <v>1.48</v>
+        <v>1.45</v>
       </c>
       <c r="L413">
-        <v>1.48</v>
+        <v>1.45</v>
       </c>
       <c r="M413">
-        <v>1.48</v>
+        <v>0</v>
       </c>
       <c r="N413">
-        <v>1.48</v>
+        <v>0</v>
       </c>
       <c r="O413">
-        <v>1.48</v>
+        <v>0</v>
       </c>
       <c r="P413">
-        <v>1.48</v>
+        <v>0</v>
       </c>
       <c r="Q413">
-        <v>1.48</v>
+        <v>0</v>
       </c>
       <c r="R413">
-        <v>1.48</v>
+        <v>0</v>
       </c>
       <c r="S413">
-        <v>1.48</v>
+        <v>0</v>
       </c>
       <c r="T413">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U413">
-        <v>0.45</v>
+        <v>0.35</v>
       </c>
       <c r="V413">
-        <v>1.48</v>
+        <v>0.6</v>
       </c>
       <c r="W413">
-        <v>6800000</v>
+        <v>6500000</v>
       </c>
       <c r="X413">
-        <v>140000</v>
+        <v>130000</v>
       </c>
       <c r="Y413">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="Z413">
         <v>325</v>
       </c>
       <c r="AE413">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="AF413">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="AG413">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="AH413">
-        <v>0.068</v>
+        <v>0.066</v>
       </c>
       <c r="AI413">
-        <v>0.068</v>
+        <v>0.066</v>
       </c>
       <c r="AM413">
-        <v>14000000000</v>
+        <v>13500000000</v>
       </c>
       <c r="AN413" t="s">
         <v>49</v>
@@ -40542,6 +40530,119 @@
         <v>0</v>
       </c>
       <c r="AR413">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="414" spans="1:44">
+      <c r="A414" t="s">
+        <v>833</v>
+      </c>
+      <c r="B414" t="s">
+        <v>834</v>
+      </c>
+      <c r="C414">
+        <v>1.2</v>
+      </c>
+      <c r="D414">
+        <v>0.55</v>
+      </c>
+      <c r="E414">
+        <v>0.8</v>
+      </c>
+      <c r="F414">
+        <v>1.48</v>
+      </c>
+      <c r="G414">
+        <v>1.48</v>
+      </c>
+      <c r="H414">
+        <v>1.48</v>
+      </c>
+      <c r="I414">
+        <v>1.48</v>
+      </c>
+      <c r="J414">
+        <v>1.48</v>
+      </c>
+      <c r="K414">
+        <v>1.48</v>
+      </c>
+      <c r="L414">
+        <v>1.48</v>
+      </c>
+      <c r="M414">
+        <v>1.48</v>
+      </c>
+      <c r="N414">
+        <v>1.48</v>
+      </c>
+      <c r="O414">
+        <v>1.48</v>
+      </c>
+      <c r="P414">
+        <v>1.48</v>
+      </c>
+      <c r="Q414">
+        <v>1.48</v>
+      </c>
+      <c r="R414">
+        <v>1.48</v>
+      </c>
+      <c r="S414">
+        <v>1.48</v>
+      </c>
+      <c r="T414">
+        <v>1</v>
+      </c>
+      <c r="U414">
+        <v>0.45</v>
+      </c>
+      <c r="V414">
+        <v>1.48</v>
+      </c>
+      <c r="W414">
+        <v>6800000</v>
+      </c>
+      <c r="X414">
+        <v>140000</v>
+      </c>
+      <c r="Y414">
+        <v>320</v>
+      </c>
+      <c r="Z414">
+        <v>325</v>
+      </c>
+      <c r="AE414">
+        <v>1.2</v>
+      </c>
+      <c r="AF414">
+        <v>0.8</v>
+      </c>
+      <c r="AG414">
+        <v>0.8</v>
+      </c>
+      <c r="AH414">
+        <v>0.068</v>
+      </c>
+      <c r="AI414">
+        <v>0.068</v>
+      </c>
+      <c r="AM414">
+        <v>14000000000</v>
+      </c>
+      <c r="AN414" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO414">
+        <v>0</v>
+      </c>
+      <c r="AP414">
+        <v>0</v>
+      </c>
+      <c r="AQ414">
+        <v>0</v>
+      </c>
+      <c r="AR414">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Managed to export out the quests.
- Lots of little fixes and changes.
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="861">
   <si>
     <t>name</t>
   </si>
@@ -2516,10 +2516,88 @@
     <t>Everything in time child. Everything must be balanced first.</t>
   </si>
   <si>
-    <t>Cosmic Interfearence</t>
+    <t>Cosmic Interference</t>
   </si>
   <si>
     <t>Let the cosmos interfere on your behalf.</t>
+  </si>
+  <si>
+    <t>Dragon Slayers Revenge</t>
+  </si>
+  <si>
+    <t>Take revenge and summon up the strength as a fighter to kill your foes in one fell swoop</t>
+  </si>
+  <si>
+    <t>Red Witches Flame</t>
+  </si>
+  <si>
+    <t>Heretical magic will flow through the veins of those seeking the power of the flames.</t>
+  </si>
+  <si>
+    <t>Hells Fighting Stance</t>
+  </si>
+  <si>
+    <t>Let the flames of hell wash over you as you take a stance against the hordes of Heaven.</t>
+  </si>
+  <si>
+    <t>Mothers Earthen Love</t>
+  </si>
+  <si>
+    <t>Let the mother of all guide you through the darkest of times child.</t>
+  </si>
+  <si>
+    <t>Shadows of Fear</t>
+  </si>
+  <si>
+    <t>Creep through the shadows of the enemies mind to infiltrate their darkest desire</t>
+  </si>
+  <si>
+    <t>Curse of the Insane Prophet</t>
+  </si>
+  <si>
+    <t>There is a cursed enchantment out there child .... oh this is it! Ha! this enchantment will make you go mad!! Mad with faith!</t>
+  </si>
+  <si>
+    <t>River of life</t>
+  </si>
+  <si>
+    <t>Let the river of life transcend you above all else child.</t>
+  </si>
+  <si>
+    <t>Shattered Intentions</t>
+  </si>
+  <si>
+    <t>Let the mind of the enemy rip apart before you.</t>
+  </si>
+  <si>
+    <t>Faithful Reincarnation</t>
+  </si>
+  <si>
+    <t>Let the gods reach down and make you whole again</t>
+  </si>
+  <si>
+    <t>Diseased Affliction of the Mind</t>
+  </si>
+  <si>
+    <t>Let the affliction take hold child. Don't fight it.</t>
+  </si>
+  <si>
+    <t>Raging Ancestor Spirit</t>
+  </si>
+  <si>
+    <t>Let the plight of the ancestors run through you as they rage with in your very soul.</t>
+  </si>
+  <si>
+    <t>Lifes Final Breath</t>
+  </si>
+  <si>
+    <t>Take a final breath child. Lash the damage out at the expense of all else.</t>
+  </si>
+  <si>
+    <t>End of Solace III</t>
+  </si>
+  <si>
+    <t>No one knows why it was titled "III", maybe it was the third attempt. Either way, with this you will transcend all space and time. The world is yours to own.</t>
   </si>
 </sst>
 </file>
@@ -2858,7 +2936,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AR414"/>
+  <dimension ref="A1:AR427"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -2888,7 +2966,7 @@
     <col min="20" max="20" width="23" bestFit="true" customWidth="true" style="0"/>
     <col min="21" max="21" width="21" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="23" max="23" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="10" bestFit="true" customWidth="true" style="0"/>
     <col min="24" max="24" width="15" bestFit="true" customWidth="true" style="0"/>
     <col min="25" max="25" width="24" bestFit="true" customWidth="true" style="0"/>
     <col min="26" max="26" width="23" bestFit="true" customWidth="true" style="0"/>
@@ -36807,7 +36885,7 @@
         <v>1</v>
       </c>
       <c r="AM377">
-        <v>4200000000</v>
+        <v>3500000000</v>
       </c>
       <c r="AN377" t="s">
         <v>46</v>
@@ -36816,13 +36894,13 @@
         <v>0</v>
       </c>
       <c r="AP377">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AQ377">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="AR377">
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="378" spans="1:44">
@@ -37454,13 +37532,13 @@
         <v>0</v>
       </c>
       <c r="M384">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="N384">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="O384">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="P384">
         <v>0</v>
@@ -37561,13 +37639,13 @@
         <v>0</v>
       </c>
       <c r="Q385">
-        <v>1.5</v>
+        <v>0.95</v>
       </c>
       <c r="R385">
         <v>0</v>
       </c>
       <c r="S385">
-        <v>1.8</v>
+        <v>0.95</v>
       </c>
       <c r="T385">
         <v>1</v>
@@ -37653,7 +37731,7 @@
         <v>0</v>
       </c>
       <c r="P386">
-        <v>1.8</v>
+        <v>0.95</v>
       </c>
       <c r="Q386">
         <v>0</v>
@@ -37662,7 +37740,7 @@
         <v>0</v>
       </c>
       <c r="S386">
-        <v>1.3</v>
+        <v>0.95</v>
       </c>
       <c r="T386">
         <v>1</v>
@@ -37748,7 +37826,7 @@
         <v>0</v>
       </c>
       <c r="O387">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="P387">
         <v>0</v>
@@ -37757,7 +37835,7 @@
         <v>0</v>
       </c>
       <c r="R387">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="S387">
         <v>0</v>
@@ -37840,7 +37918,7 @@
         <v>0</v>
       </c>
       <c r="O388">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="P388">
         <v>0</v>
@@ -37849,7 +37927,7 @@
         <v>0</v>
       </c>
       <c r="R388">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="S388">
         <v>0</v>
@@ -37944,7 +38022,7 @@
         <v>0</v>
       </c>
       <c r="N389">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="O389">
         <v>0</v>
@@ -38051,7 +38129,7 @@
         <v>0</v>
       </c>
       <c r="P390">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="Q390">
         <v>0</v>
@@ -38060,7 +38138,7 @@
         <v>0</v>
       </c>
       <c r="S390">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="T390">
         <v>1</v>
@@ -38476,25 +38554,25 @@
         <v>0.75</v>
       </c>
       <c r="M394">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="N394">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="O394">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="P394">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="Q394">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="R394">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="S394">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="T394">
         <v>1</v>
@@ -38993,25 +39071,25 @@
         <v>0</v>
       </c>
       <c r="M399">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="N399">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="O399">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="P399">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="Q399">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="R399">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="S399">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="T399">
         <v>1</v>
@@ -39216,25 +39294,25 @@
         <v>1.2</v>
       </c>
       <c r="M401">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="N401">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="O401">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="P401">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="Q401">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="R401">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="S401">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="T401">
         <v>1</v>
@@ -39555,16 +39633,16 @@
         <v>1.3</v>
       </c>
       <c r="P404">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="Q404">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="R404">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="S404">
-        <v>1.1</v>
+        <v>0.95</v>
       </c>
       <c r="T404">
         <v>1</v>
@@ -39861,13 +39939,13 @@
         <v>0</v>
       </c>
       <c r="M407">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="N407">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="O407">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="P407">
         <v>0</v>
@@ -39968,13 +40046,13 @@
         <v>0</v>
       </c>
       <c r="Q408">
-        <v>1.7</v>
+        <v>0.95</v>
       </c>
       <c r="R408">
         <v>0</v>
       </c>
       <c r="S408">
-        <v>1.1</v>
+        <v>0.95</v>
       </c>
       <c r="T408">
         <v>1</v>
@@ -40060,7 +40138,7 @@
         <v>0</v>
       </c>
       <c r="P409">
-        <v>1.4</v>
+        <v>0.95</v>
       </c>
       <c r="Q409">
         <v>0</v>
@@ -40069,7 +40147,7 @@
         <v>0</v>
       </c>
       <c r="S409">
-        <v>1.4</v>
+        <v>0.95</v>
       </c>
       <c r="T409">
         <v>1</v>
@@ -40158,7 +40236,7 @@
         <v>0</v>
       </c>
       <c r="O410">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="P410">
         <v>0</v>
@@ -40167,7 +40245,7 @@
         <v>0</v>
       </c>
       <c r="R410">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="S410">
         <v>0</v>
@@ -40256,7 +40334,7 @@
         <v>0</v>
       </c>
       <c r="O411">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="P411">
         <v>0</v>
@@ -40265,7 +40343,7 @@
         <v>0</v>
       </c>
       <c r="R411">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="S411">
         <v>0</v>
@@ -40357,7 +40435,7 @@
         <v>0</v>
       </c>
       <c r="N412">
-        <v>1.2</v>
+        <v>0.95</v>
       </c>
       <c r="O412">
         <v>0</v>
@@ -40571,25 +40649,25 @@
         <v>1.48</v>
       </c>
       <c r="M414">
-        <v>1.48</v>
+        <v>0.99</v>
       </c>
       <c r="N414">
-        <v>1.48</v>
+        <v>0.99</v>
       </c>
       <c r="O414">
-        <v>1.48</v>
+        <v>0.99</v>
       </c>
       <c r="P414">
-        <v>1.48</v>
+        <v>0.99</v>
       </c>
       <c r="Q414">
-        <v>1.48</v>
+        <v>0.99</v>
       </c>
       <c r="R414">
-        <v>1.48</v>
+        <v>0.99</v>
       </c>
       <c r="S414">
-        <v>1.48</v>
+        <v>0.99</v>
       </c>
       <c r="T414">
         <v>1</v>
@@ -40610,7 +40688,7 @@
         <v>320</v>
       </c>
       <c r="Z414">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="AE414">
         <v>1.2</v>
@@ -40644,6 +40722,1382 @@
       </c>
       <c r="AR414">
         <v>0</v>
+      </c>
+    </row>
+    <row r="415" spans="1:44">
+      <c r="A415" t="s">
+        <v>835</v>
+      </c>
+      <c r="B415" t="s">
+        <v>836</v>
+      </c>
+      <c r="K415">
+        <v>0</v>
+      </c>
+      <c r="L415">
+        <v>0</v>
+      </c>
+      <c r="M415">
+        <v>0</v>
+      </c>
+      <c r="N415">
+        <v>0</v>
+      </c>
+      <c r="O415">
+        <v>0</v>
+      </c>
+      <c r="P415">
+        <v>0</v>
+      </c>
+      <c r="Q415">
+        <v>0</v>
+      </c>
+      <c r="R415">
+        <v>0</v>
+      </c>
+      <c r="S415">
+        <v>0</v>
+      </c>
+      <c r="T415">
+        <v>0</v>
+      </c>
+      <c r="V415">
+        <v>0</v>
+      </c>
+      <c r="W415">
+        <v>7400000</v>
+      </c>
+      <c r="X415">
+        <v>150000</v>
+      </c>
+      <c r="Y415">
+        <v>320</v>
+      </c>
+      <c r="Z415">
+        <v>330</v>
+      </c>
+      <c r="AE415">
+        <v>0</v>
+      </c>
+      <c r="AF415">
+        <v>0</v>
+      </c>
+      <c r="AG415">
+        <v>0</v>
+      </c>
+      <c r="AH415">
+        <v>0</v>
+      </c>
+      <c r="AI415">
+        <v>0</v>
+      </c>
+      <c r="AL415">
+        <v>1</v>
+      </c>
+      <c r="AM415">
+        <v>15000000000</v>
+      </c>
+      <c r="AN415" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO415">
+        <v>0</v>
+      </c>
+      <c r="AQ415">
+        <v>0</v>
+      </c>
+      <c r="AR415">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="416" spans="1:44">
+      <c r="A416" t="s">
+        <v>837</v>
+      </c>
+      <c r="B416" t="s">
+        <v>838</v>
+      </c>
+      <c r="C416">
+        <v>1.6</v>
+      </c>
+      <c r="E416">
+        <v>1.0</v>
+      </c>
+      <c r="G416">
+        <v>0.5</v>
+      </c>
+      <c r="J416">
+        <v>1.65</v>
+      </c>
+      <c r="K416">
+        <v>0</v>
+      </c>
+      <c r="L416">
+        <v>1.6</v>
+      </c>
+      <c r="M416">
+        <v>0.95</v>
+      </c>
+      <c r="N416">
+        <v>0.95</v>
+      </c>
+      <c r="O416">
+        <v>0.95</v>
+      </c>
+      <c r="P416">
+        <v>0.95</v>
+      </c>
+      <c r="Q416">
+        <v>0.95</v>
+      </c>
+      <c r="R416">
+        <v>0.95</v>
+      </c>
+      <c r="S416">
+        <v>0.95</v>
+      </c>
+      <c r="T416">
+        <v>1</v>
+      </c>
+      <c r="U416">
+        <v>0.3</v>
+      </c>
+      <c r="V416">
+        <v>1</v>
+      </c>
+      <c r="W416">
+        <v>7400000</v>
+      </c>
+      <c r="X416">
+        <v>150000</v>
+      </c>
+      <c r="Y416">
+        <v>330</v>
+      </c>
+      <c r="Z416">
+        <v>340</v>
+      </c>
+      <c r="AC416">
+        <v>0</v>
+      </c>
+      <c r="AD416">
+        <v>0</v>
+      </c>
+      <c r="AE416">
+        <v>0.25</v>
+      </c>
+      <c r="AF416">
+        <v>0</v>
+      </c>
+      <c r="AG416">
+        <v>0.15</v>
+      </c>
+      <c r="AH416">
+        <v>0.015</v>
+      </c>
+      <c r="AI416">
+        <v>0.015</v>
+      </c>
+      <c r="AL416">
+        <v>1</v>
+      </c>
+      <c r="AM416">
+        <v>15000000000</v>
+      </c>
+      <c r="AN416" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO416">
+        <v>0.75</v>
+      </c>
+      <c r="AQ416">
+        <v>0.85</v>
+      </c>
+      <c r="AR416">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="417" spans="1:44">
+      <c r="A417" t="s">
+        <v>839</v>
+      </c>
+      <c r="B417" t="s">
+        <v>840</v>
+      </c>
+      <c r="C417">
+        <v>1.6</v>
+      </c>
+      <c r="E417">
+        <v>1.6</v>
+      </c>
+      <c r="F417">
+        <v>1.65</v>
+      </c>
+      <c r="G417">
+        <v>1</v>
+      </c>
+      <c r="H417">
+        <v>1.65</v>
+      </c>
+      <c r="K417">
+        <v>0</v>
+      </c>
+      <c r="L417">
+        <v>0</v>
+      </c>
+      <c r="M417">
+        <v>0.95</v>
+      </c>
+      <c r="N417">
+        <v>0.95</v>
+      </c>
+      <c r="O417">
+        <v>0.95</v>
+      </c>
+      <c r="P417">
+        <v>0.95</v>
+      </c>
+      <c r="Q417">
+        <v>0.95</v>
+      </c>
+      <c r="R417">
+        <v>0.95</v>
+      </c>
+      <c r="S417">
+        <v>0.95</v>
+      </c>
+      <c r="T417">
+        <v>1</v>
+      </c>
+      <c r="U417">
+        <v>0.3</v>
+      </c>
+      <c r="V417">
+        <v>1</v>
+      </c>
+      <c r="W417">
+        <v>7400000</v>
+      </c>
+      <c r="X417">
+        <v>150000</v>
+      </c>
+      <c r="Y417">
+        <v>330</v>
+      </c>
+      <c r="Z417">
+        <v>340</v>
+      </c>
+      <c r="AE417">
+        <v>0.5</v>
+      </c>
+      <c r="AF417">
+        <v>0</v>
+      </c>
+      <c r="AG417">
+        <v>0.25</v>
+      </c>
+      <c r="AH417">
+        <v>0.015</v>
+      </c>
+      <c r="AI417">
+        <v>0.015</v>
+      </c>
+      <c r="AL417">
+        <v>1</v>
+      </c>
+      <c r="AM417">
+        <v>15000000000</v>
+      </c>
+      <c r="AN417" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO417">
+        <v>0.75</v>
+      </c>
+      <c r="AQ417">
+        <v>0.85</v>
+      </c>
+      <c r="AR417">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="418" spans="1:44">
+      <c r="A418" t="s">
+        <v>841</v>
+      </c>
+      <c r="B418" t="s">
+        <v>842</v>
+      </c>
+      <c r="C418">
+        <v>1.6</v>
+      </c>
+      <c r="D418">
+        <v>0.15</v>
+      </c>
+      <c r="E418">
+        <v>0.75</v>
+      </c>
+      <c r="G418">
+        <v>0.8</v>
+      </c>
+      <c r="H418">
+        <v>1.6</v>
+      </c>
+      <c r="I418">
+        <v>0.5</v>
+      </c>
+      <c r="K418">
+        <v>1.5</v>
+      </c>
+      <c r="L418">
+        <v>0</v>
+      </c>
+      <c r="M418">
+        <v>0.95</v>
+      </c>
+      <c r="N418">
+        <v>0.95</v>
+      </c>
+      <c r="O418">
+        <v>0.95</v>
+      </c>
+      <c r="P418">
+        <v>0.95</v>
+      </c>
+      <c r="Q418">
+        <v>0.95</v>
+      </c>
+      <c r="R418">
+        <v>0.95</v>
+      </c>
+      <c r="S418">
+        <v>0.95</v>
+      </c>
+      <c r="T418">
+        <v>1</v>
+      </c>
+      <c r="U418">
+        <v>0.4</v>
+      </c>
+      <c r="V418">
+        <v>1</v>
+      </c>
+      <c r="W418">
+        <v>7400000</v>
+      </c>
+      <c r="X418">
+        <v>150000</v>
+      </c>
+      <c r="Y418">
+        <v>330</v>
+      </c>
+      <c r="Z418">
+        <v>340</v>
+      </c>
+      <c r="AE418">
+        <v>0.25</v>
+      </c>
+      <c r="AF418">
+        <v>0.1</v>
+      </c>
+      <c r="AG418">
+        <v>0.15</v>
+      </c>
+      <c r="AH418">
+        <v>0.015</v>
+      </c>
+      <c r="AI418">
+        <v>0.015</v>
+      </c>
+      <c r="AL418">
+        <v>1</v>
+      </c>
+      <c r="AM418">
+        <v>15000000000</v>
+      </c>
+      <c r="AN418" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO418">
+        <v>0.75</v>
+      </c>
+      <c r="AQ418">
+        <v>0.85</v>
+      </c>
+      <c r="AR418">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="419" spans="1:44">
+      <c r="A419" t="s">
+        <v>843</v>
+      </c>
+      <c r="B419" t="s">
+        <v>844</v>
+      </c>
+      <c r="C419">
+        <v>1.6</v>
+      </c>
+      <c r="E419">
+        <v>0.25</v>
+      </c>
+      <c r="G419">
+        <v>0.5</v>
+      </c>
+      <c r="H419">
+        <v>1.65</v>
+      </c>
+      <c r="K419">
+        <v>1.55</v>
+      </c>
+      <c r="L419">
+        <v>0</v>
+      </c>
+      <c r="M419">
+        <v>0.95</v>
+      </c>
+      <c r="N419">
+        <v>0.95</v>
+      </c>
+      <c r="O419">
+        <v>0.95</v>
+      </c>
+      <c r="P419">
+        <v>0.95</v>
+      </c>
+      <c r="Q419">
+        <v>0.95</v>
+      </c>
+      <c r="R419">
+        <v>0.95</v>
+      </c>
+      <c r="S419">
+        <v>0.95</v>
+      </c>
+      <c r="T419">
+        <v>1</v>
+      </c>
+      <c r="U419">
+        <v>0.45</v>
+      </c>
+      <c r="V419">
+        <v>1</v>
+      </c>
+      <c r="W419">
+        <v>7400000</v>
+      </c>
+      <c r="X419">
+        <v>150000</v>
+      </c>
+      <c r="Y419">
+        <v>330</v>
+      </c>
+      <c r="Z419">
+        <v>340</v>
+      </c>
+      <c r="AE419">
+        <v>0.25</v>
+      </c>
+      <c r="AF419">
+        <v>0</v>
+      </c>
+      <c r="AG419">
+        <v>0.05</v>
+      </c>
+      <c r="AH419">
+        <v>0.025</v>
+      </c>
+      <c r="AI419">
+        <v>0.025</v>
+      </c>
+      <c r="AL419">
+        <v>1</v>
+      </c>
+      <c r="AM419">
+        <v>15000000000</v>
+      </c>
+      <c r="AN419" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO419">
+        <v>0.85</v>
+      </c>
+      <c r="AQ419">
+        <v>0.9</v>
+      </c>
+      <c r="AR419">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="420" spans="1:44">
+      <c r="A420" t="s">
+        <v>845</v>
+      </c>
+      <c r="B420" t="s">
+        <v>846</v>
+      </c>
+      <c r="C420">
+        <v>1.6</v>
+      </c>
+      <c r="D420">
+        <v>1.75</v>
+      </c>
+      <c r="E420">
+        <v>0.6</v>
+      </c>
+      <c r="G420">
+        <v>0.55</v>
+      </c>
+      <c r="I420">
+        <v>1.65</v>
+      </c>
+      <c r="K420">
+        <v>0</v>
+      </c>
+      <c r="L420">
+        <v>1.6</v>
+      </c>
+      <c r="M420">
+        <v>0.95</v>
+      </c>
+      <c r="N420">
+        <v>0.95</v>
+      </c>
+      <c r="O420">
+        <v>0.95</v>
+      </c>
+      <c r="P420">
+        <v>0.95</v>
+      </c>
+      <c r="Q420">
+        <v>0.95</v>
+      </c>
+      <c r="R420">
+        <v>0.95</v>
+      </c>
+      <c r="S420">
+        <v>0.95</v>
+      </c>
+      <c r="T420">
+        <v>1</v>
+      </c>
+      <c r="U420">
+        <v>0.3</v>
+      </c>
+      <c r="V420">
+        <v>1</v>
+      </c>
+      <c r="W420">
+        <v>7400000</v>
+      </c>
+      <c r="X420">
+        <v>150000</v>
+      </c>
+      <c r="Y420">
+        <v>330</v>
+      </c>
+      <c r="Z420">
+        <v>340</v>
+      </c>
+      <c r="AE420">
+        <v>0.15</v>
+      </c>
+      <c r="AF420">
+        <v>0.65</v>
+      </c>
+      <c r="AG420">
+        <v>0.15</v>
+      </c>
+      <c r="AH420">
+        <v>0.015</v>
+      </c>
+      <c r="AI420">
+        <v>0.015</v>
+      </c>
+      <c r="AL420">
+        <v>1</v>
+      </c>
+      <c r="AM420">
+        <v>15000000000</v>
+      </c>
+      <c r="AN420" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO420">
+        <v>0.75</v>
+      </c>
+      <c r="AQ420">
+        <v>0.85</v>
+      </c>
+      <c r="AR420">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="421" spans="1:44">
+      <c r="A421" t="s">
+        <v>847</v>
+      </c>
+      <c r="B421" t="s">
+        <v>848</v>
+      </c>
+      <c r="C421">
+        <v>1.6</v>
+      </c>
+      <c r="D421">
+        <v>0.4</v>
+      </c>
+      <c r="E421">
+        <v>0.6</v>
+      </c>
+      <c r="G421">
+        <v>1.65</v>
+      </c>
+      <c r="K421">
+        <v>0</v>
+      </c>
+      <c r="L421">
+        <v>0</v>
+      </c>
+      <c r="M421">
+        <v>0.95</v>
+      </c>
+      <c r="N421">
+        <v>1</v>
+      </c>
+      <c r="O421">
+        <v>0.95</v>
+      </c>
+      <c r="P421">
+        <v>0.95</v>
+      </c>
+      <c r="Q421">
+        <v>0.95</v>
+      </c>
+      <c r="R421">
+        <v>0.95</v>
+      </c>
+      <c r="S421">
+        <v>0.95</v>
+      </c>
+      <c r="T421">
+        <v>1</v>
+      </c>
+      <c r="U421">
+        <v>0.99</v>
+      </c>
+      <c r="V421">
+        <v>1</v>
+      </c>
+      <c r="W421">
+        <v>7400000</v>
+      </c>
+      <c r="X421">
+        <v>150000</v>
+      </c>
+      <c r="Y421">
+        <v>330</v>
+      </c>
+      <c r="Z421">
+        <v>340</v>
+      </c>
+      <c r="AE421">
+        <v>0.25</v>
+      </c>
+      <c r="AF421">
+        <v>0.25</v>
+      </c>
+      <c r="AG421">
+        <v>0.25</v>
+      </c>
+      <c r="AH421">
+        <v>0.015</v>
+      </c>
+      <c r="AI421">
+        <v>0.015</v>
+      </c>
+      <c r="AL421">
+        <v>1</v>
+      </c>
+      <c r="AM421">
+        <v>15000000000</v>
+      </c>
+      <c r="AN421" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO421">
+        <v>0.75</v>
+      </c>
+      <c r="AQ421">
+        <v>0.85</v>
+      </c>
+      <c r="AR421">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="422" spans="1:44">
+      <c r="A422" t="s">
+        <v>849</v>
+      </c>
+      <c r="B422" t="s">
+        <v>850</v>
+      </c>
+      <c r="C422">
+        <v>1.68</v>
+      </c>
+      <c r="D422">
+        <v>1.68</v>
+      </c>
+      <c r="E422">
+        <v>1.68</v>
+      </c>
+      <c r="K422">
+        <v>0</v>
+      </c>
+      <c r="L422">
+        <v>0</v>
+      </c>
+      <c r="M422">
+        <v>0</v>
+      </c>
+      <c r="N422">
+        <v>1.68</v>
+      </c>
+      <c r="O422">
+        <v>0</v>
+      </c>
+      <c r="P422">
+        <v>0</v>
+      </c>
+      <c r="Q422">
+        <v>0</v>
+      </c>
+      <c r="R422">
+        <v>0</v>
+      </c>
+      <c r="S422">
+        <v>0</v>
+      </c>
+      <c r="T422">
+        <v>1</v>
+      </c>
+      <c r="U422">
+        <v>0.56</v>
+      </c>
+      <c r="V422">
+        <v>0</v>
+      </c>
+      <c r="W422">
+        <v>3500000</v>
+      </c>
+      <c r="X422">
+        <v>160000</v>
+      </c>
+      <c r="Y422">
+        <v>340</v>
+      </c>
+      <c r="Z422">
+        <v>350</v>
+      </c>
+      <c r="AE422">
+        <v>0.15</v>
+      </c>
+      <c r="AF422">
+        <v>0.15</v>
+      </c>
+      <c r="AG422">
+        <v>0.15</v>
+      </c>
+      <c r="AH422">
+        <v>0</v>
+      </c>
+      <c r="AI422">
+        <v>0</v>
+      </c>
+      <c r="AK422">
+        <v>1</v>
+      </c>
+      <c r="AL422">
+        <v>1</v>
+      </c>
+      <c r="AM422">
+        <v>18000000000</v>
+      </c>
+      <c r="AN422" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO422">
+        <v>0.67</v>
+      </c>
+      <c r="AP422">
+        <v>0.78</v>
+      </c>
+      <c r="AQ422">
+        <v>0.87</v>
+      </c>
+      <c r="AR422">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="423" spans="1:44">
+      <c r="A423" t="s">
+        <v>851</v>
+      </c>
+      <c r="B423" t="s">
+        <v>852</v>
+      </c>
+      <c r="C423">
+        <v>1.35</v>
+      </c>
+      <c r="D423">
+        <v>1.35</v>
+      </c>
+      <c r="E423">
+        <v>1.35</v>
+      </c>
+      <c r="F423">
+        <v>1</v>
+      </c>
+      <c r="G423">
+        <v>1</v>
+      </c>
+      <c r="H423">
+        <v>1</v>
+      </c>
+      <c r="I423">
+        <v>1</v>
+      </c>
+      <c r="J423">
+        <v>1</v>
+      </c>
+      <c r="K423">
+        <v>1</v>
+      </c>
+      <c r="L423">
+        <v>1</v>
+      </c>
+      <c r="M423">
+        <v>0</v>
+      </c>
+      <c r="N423">
+        <v>0</v>
+      </c>
+      <c r="O423">
+        <v>0</v>
+      </c>
+      <c r="P423">
+        <v>0</v>
+      </c>
+      <c r="Q423">
+        <v>0</v>
+      </c>
+      <c r="R423">
+        <v>0</v>
+      </c>
+      <c r="S423">
+        <v>0</v>
+      </c>
+      <c r="T423">
+        <v>0</v>
+      </c>
+      <c r="U423">
+        <v>0.99</v>
+      </c>
+      <c r="V423">
+        <v>1</v>
+      </c>
+      <c r="W423">
+        <v>4000000</v>
+      </c>
+      <c r="X423">
+        <v>175000</v>
+      </c>
+      <c r="Y423">
+        <v>350</v>
+      </c>
+      <c r="Z423">
+        <v>360</v>
+      </c>
+      <c r="AE423">
+        <v>0.1</v>
+      </c>
+      <c r="AF423">
+        <v>0.1</v>
+      </c>
+      <c r="AG423">
+        <v>0.1</v>
+      </c>
+      <c r="AH423">
+        <v>0.1</v>
+      </c>
+      <c r="AI423">
+        <v>0.1</v>
+      </c>
+      <c r="AK423">
+        <v>1</v>
+      </c>
+      <c r="AL423">
+        <v>1</v>
+      </c>
+      <c r="AM423">
+        <v>20000000000</v>
+      </c>
+      <c r="AN423" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO423">
+        <v>0.45</v>
+      </c>
+      <c r="AP423">
+        <v>0.5</v>
+      </c>
+      <c r="AQ423">
+        <v>0.87</v>
+      </c>
+      <c r="AR423">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="424" spans="1:44">
+      <c r="A424" t="s">
+        <v>853</v>
+      </c>
+      <c r="B424" t="s">
+        <v>854</v>
+      </c>
+      <c r="C424">
+        <v>1</v>
+      </c>
+      <c r="D424">
+        <v>1</v>
+      </c>
+      <c r="E424">
+        <v>1.0</v>
+      </c>
+      <c r="F424">
+        <v>0</v>
+      </c>
+      <c r="G424">
+        <v>0</v>
+      </c>
+      <c r="H424">
+        <v>0</v>
+      </c>
+      <c r="J424">
+        <v>0</v>
+      </c>
+      <c r="K424">
+        <v>0</v>
+      </c>
+      <c r="L424">
+        <v>0</v>
+      </c>
+      <c r="M424">
+        <v>0</v>
+      </c>
+      <c r="N424">
+        <v>0</v>
+      </c>
+      <c r="O424">
+        <v>0</v>
+      </c>
+      <c r="P424">
+        <v>0</v>
+      </c>
+      <c r="Q424">
+        <v>0</v>
+      </c>
+      <c r="R424">
+        <v>0</v>
+      </c>
+      <c r="S424">
+        <v>0</v>
+      </c>
+      <c r="T424">
+        <v>0</v>
+      </c>
+      <c r="U424">
+        <v>1</v>
+      </c>
+      <c r="V424">
+        <v>0</v>
+      </c>
+      <c r="W424">
+        <v>2800000</v>
+      </c>
+      <c r="X424">
+        <v>185000</v>
+      </c>
+      <c r="Y424">
+        <v>360</v>
+      </c>
+      <c r="Z424">
+        <v>370</v>
+      </c>
+      <c r="AE424">
+        <v>1.6</v>
+      </c>
+      <c r="AF424">
+        <v>1.6</v>
+      </c>
+      <c r="AG424">
+        <v>1.6</v>
+      </c>
+      <c r="AH424">
+        <v>0</v>
+      </c>
+      <c r="AI424">
+        <v>0</v>
+      </c>
+      <c r="AK424">
+        <v>1</v>
+      </c>
+      <c r="AL424">
+        <v>1</v>
+      </c>
+      <c r="AM424">
+        <v>21000000000</v>
+      </c>
+      <c r="AN424" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO424">
+        <v>1</v>
+      </c>
+      <c r="AP424">
+        <v>0.6</v>
+      </c>
+      <c r="AQ424">
+        <v>1.4</v>
+      </c>
+      <c r="AR424">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="425" spans="1:44">
+      <c r="A425" t="s">
+        <v>855</v>
+      </c>
+      <c r="B425" t="s">
+        <v>856</v>
+      </c>
+      <c r="C425">
+        <v>1.8</v>
+      </c>
+      <c r="D425">
+        <v>1.8</v>
+      </c>
+      <c r="E425">
+        <v>1.8</v>
+      </c>
+      <c r="F425">
+        <v>1.8</v>
+      </c>
+      <c r="G425">
+        <v>1.8</v>
+      </c>
+      <c r="H425">
+        <v>1.8</v>
+      </c>
+      <c r="I425">
+        <v>1.8</v>
+      </c>
+      <c r="J425">
+        <v>1.8</v>
+      </c>
+      <c r="K425">
+        <v>1.8</v>
+      </c>
+      <c r="L425">
+        <v>1.8</v>
+      </c>
+      <c r="M425">
+        <v>0</v>
+      </c>
+      <c r="N425">
+        <v>0</v>
+      </c>
+      <c r="O425">
+        <v>0</v>
+      </c>
+      <c r="P425">
+        <v>0</v>
+      </c>
+      <c r="Q425">
+        <v>0</v>
+      </c>
+      <c r="R425">
+        <v>0</v>
+      </c>
+      <c r="S425">
+        <v>0</v>
+      </c>
+      <c r="T425">
+        <v>0</v>
+      </c>
+      <c r="U425">
+        <v>0.65</v>
+      </c>
+      <c r="V425">
+        <v>1</v>
+      </c>
+      <c r="W425">
+        <v>1567000</v>
+      </c>
+      <c r="X425">
+        <v>190000</v>
+      </c>
+      <c r="Y425">
+        <v>380</v>
+      </c>
+      <c r="Z425">
+        <v>390</v>
+      </c>
+      <c r="AE425">
+        <v>0.65</v>
+      </c>
+      <c r="AF425">
+        <v>0.65</v>
+      </c>
+      <c r="AG425">
+        <v>0.65</v>
+      </c>
+      <c r="AH425">
+        <v>0.06</v>
+      </c>
+      <c r="AI425">
+        <v>0.06</v>
+      </c>
+      <c r="AK425">
+        <v>1</v>
+      </c>
+      <c r="AL425">
+        <v>1</v>
+      </c>
+      <c r="AM425">
+        <v>23000000000</v>
+      </c>
+      <c r="AN425" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO425">
+        <v>0.65</v>
+      </c>
+      <c r="AQ425">
+        <v>0.65</v>
+      </c>
+      <c r="AR425">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="426" spans="1:44">
+      <c r="A426" t="s">
+        <v>857</v>
+      </c>
+      <c r="B426" t="s">
+        <v>858</v>
+      </c>
+      <c r="C426">
+        <v>1.95</v>
+      </c>
+      <c r="K426">
+        <v>0</v>
+      </c>
+      <c r="L426">
+        <v>0</v>
+      </c>
+      <c r="M426">
+        <v>0</v>
+      </c>
+      <c r="N426">
+        <v>0</v>
+      </c>
+      <c r="O426">
+        <v>0</v>
+      </c>
+      <c r="P426">
+        <v>0</v>
+      </c>
+      <c r="Q426">
+        <v>0</v>
+      </c>
+      <c r="R426">
+        <v>0</v>
+      </c>
+      <c r="S426">
+        <v>0</v>
+      </c>
+      <c r="T426">
+        <v>0</v>
+      </c>
+      <c r="V426">
+        <v>0</v>
+      </c>
+      <c r="W426">
+        <v>2000000</v>
+      </c>
+      <c r="X426">
+        <v>210000</v>
+      </c>
+      <c r="Y426">
+        <v>390</v>
+      </c>
+      <c r="Z426">
+        <v>400</v>
+      </c>
+      <c r="AE426">
+        <v>1.95</v>
+      </c>
+      <c r="AF426">
+        <v>0</v>
+      </c>
+      <c r="AG426">
+        <v>0</v>
+      </c>
+      <c r="AH426">
+        <v>0</v>
+      </c>
+      <c r="AI426">
+        <v>0</v>
+      </c>
+      <c r="AK426">
+        <v>1</v>
+      </c>
+      <c r="AL426">
+        <v>1</v>
+      </c>
+      <c r="AM426">
+        <v>28000000000</v>
+      </c>
+      <c r="AN426" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO426">
+        <v>0</v>
+      </c>
+      <c r="AP426">
+        <v>1</v>
+      </c>
+      <c r="AQ426">
+        <v>0</v>
+      </c>
+      <c r="AR426">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="427" spans="1:44">
+      <c r="A427" t="s">
+        <v>859</v>
+      </c>
+      <c r="B427" t="s">
+        <v>860</v>
+      </c>
+      <c r="C427">
+        <v>2</v>
+      </c>
+      <c r="D427">
+        <v>2</v>
+      </c>
+      <c r="E427">
+        <v>2.0</v>
+      </c>
+      <c r="F427">
+        <v>2</v>
+      </c>
+      <c r="G427">
+        <v>2</v>
+      </c>
+      <c r="H427">
+        <v>2</v>
+      </c>
+      <c r="I427">
+        <v>2</v>
+      </c>
+      <c r="J427">
+        <v>2</v>
+      </c>
+      <c r="K427">
+        <v>2</v>
+      </c>
+      <c r="L427">
+        <v>2</v>
+      </c>
+      <c r="M427">
+        <v>0</v>
+      </c>
+      <c r="N427">
+        <v>0</v>
+      </c>
+      <c r="O427">
+        <v>0</v>
+      </c>
+      <c r="P427">
+        <v>0</v>
+      </c>
+      <c r="Q427">
+        <v>0</v>
+      </c>
+      <c r="R427">
+        <v>0</v>
+      </c>
+      <c r="S427">
+        <v>0</v>
+      </c>
+      <c r="T427">
+        <v>0</v>
+      </c>
+      <c r="U427">
+        <v>1</v>
+      </c>
+      <c r="V427">
+        <v>1</v>
+      </c>
+      <c r="W427">
+        <v>10000000</v>
+      </c>
+      <c r="X427">
+        <v>250000</v>
+      </c>
+      <c r="Y427">
+        <v>400</v>
+      </c>
+      <c r="Z427">
+        <v>401</v>
+      </c>
+      <c r="AE427">
+        <v>1</v>
+      </c>
+      <c r="AF427">
+        <v>1</v>
+      </c>
+      <c r="AG427">
+        <v>1</v>
+      </c>
+      <c r="AH427">
+        <v>1</v>
+      </c>
+      <c r="AI427">
+        <v>1</v>
+      </c>
+      <c r="AL427">
+        <v>1</v>
+      </c>
+      <c r="AM427">
+        <v>34000000000</v>
+      </c>
+      <c r="AN427" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO427">
+        <v>1</v>
+      </c>
+      <c r="AP427">
+        <v>1</v>
+      </c>
+      <c r="AQ427">
+        <v>1.9</v>
+      </c>
+      <c r="AR427">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed how the crafting section works, added new quests for the new skill quest items to be upgraded.
</commit_message>
<xml_diff>
--- a/resources/data-imports/affixes.xlsx
+++ b/resources/data-imports/affixes.xlsx
@@ -27363,6 +27363,9 @@
       <c r="AO268">
         <v>0</v>
       </c>
+      <c r="AP268">
+        <v>0</v>
+      </c>
       <c r="AQ268">
         <v>0</v>
       </c>
@@ -29265,6 +29268,9 @@
       <c r="AO289">
         <v>0</v>
       </c>
+      <c r="AP289">
+        <v>0</v>
+      </c>
       <c r="AQ289">
         <v>0</v>
       </c>
@@ -32285,6 +32291,9 @@
       <c r="AO323">
         <v>0</v>
       </c>
+      <c r="AP323">
+        <v>0</v>
+      </c>
       <c r="AQ323">
         <v>0</v>
       </c>
@@ -33905,6 +33914,9 @@
       <c r="AO341">
         <v>0</v>
       </c>
+      <c r="AP341">
+        <v>0</v>
+      </c>
       <c r="AQ341">
         <v>0</v>
       </c>
@@ -35338,6 +35350,9 @@
       <c r="AO357">
         <v>0</v>
       </c>
+      <c r="AP357">
+        <v>0</v>
+      </c>
       <c r="AQ357">
         <v>0</v>
       </c>
@@ -36774,6 +36789,9 @@
       <c r="AO373">
         <v>0</v>
       </c>
+      <c r="AP373">
+        <v>0</v>
+      </c>
       <c r="AQ373">
         <v>0</v>
       </c>
@@ -37727,6 +37745,9 @@
       <c r="AO383">
         <v>0</v>
       </c>
+      <c r="AP383">
+        <v>0</v>
+      </c>
       <c r="AQ383">
         <v>0.5</v>
       </c>
@@ -38508,6 +38529,9 @@
       <c r="AO391">
         <v>0</v>
       </c>
+      <c r="AP391">
+        <v>0</v>
+      </c>
       <c r="AQ391">
         <v>0</v>
       </c>
@@ -40623,6 +40647,9 @@
       <c r="AO412">
         <v>0</v>
       </c>
+      <c r="AP412">
+        <v>0</v>
+      </c>
       <c r="AQ412">
         <v>0</v>
       </c>
@@ -42599,6 +42626,9 @@
       <c r="AO431">
         <v>0.5</v>
       </c>
+      <c r="AP431">
+        <v>0</v>
+      </c>
       <c r="AQ431">
         <v>0</v>
       </c>
@@ -44304,6 +44334,9 @@
       </c>
       <c r="AO447">
         <v>1</v>
+      </c>
+      <c r="AP447">
+        <v>0</v>
       </c>
       <c r="AQ447">
         <v>0</v>

</xml_diff>